<commit_message>
Loading Encoder 1's QKV Dense weights successfully
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D1ACAC-3872-5C46-92EA-81A5C0020457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70320C3A-7B12-B045-A55C-A1F330D12041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
@@ -1139,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
   <dimension ref="A1:BP67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AI78" sqref="AI78"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BP9" sqref="BP9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1741,7 +1741,7 @@
         <v>13</v>
       </c>
       <c r="BP7" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:68" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1816,7 +1816,7 @@
         <v>26</v>
       </c>
       <c r="BP8" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:68" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1974,7 +1974,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="76"/>
       <c r="D11" s="76"/>
@@ -2268,7 +2268,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="76"/>
       <c r="D15" s="76"/>

</xml_diff>

<commit_message>
Broadcast transpose works for post-LayerNorm
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70320C3A-7B12-B045-A55C-A1F330D12041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A483CC94-3640-2343-82FF-3CC6D8ADFD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>CiM PARAMETERS MEMORY MAP</t>
   </si>
@@ -173,7 +173,10 @@
     <t>CiM INTERMEDIATE RESULTS MEMORY MAP</t>
   </si>
   <si>
-    <t>enc0_layernorm[id][:]</t>
+    <t>enc0_layernorm_out[id][:]</t>
+  </si>
+  <si>
+    <t>enc0_layernorm_out[:][id]</t>
   </si>
 </sst>
 </file>
@@ -288,7 +291,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -770,6 +773,9 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -809,7 +815,34 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1137,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
-  <dimension ref="A1:BP67"/>
+  <dimension ref="A1:BP75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="BP9" sqref="BP9"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68:BG71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4970,11 +5003,11 @@
       <c r="BH60" s="45"/>
       <c r="BI60" s="45"/>
       <c r="BJ60" s="46"/>
-      <c r="BK60" s="113" t="s">
+      <c r="BK60" s="114" t="s">
         <v>45</v>
       </c>
-      <c r="BL60" s="114"/>
-      <c r="BM60" s="115"/>
+      <c r="BL60" s="115"/>
+      <c r="BM60" s="116"/>
       <c r="BO60" s="10" t="s">
         <v>42</v>
       </c>
@@ -5044,9 +5077,9 @@
       <c r="BH61" s="48"/>
       <c r="BI61" s="48"/>
       <c r="BJ61" s="49"/>
-      <c r="BK61" s="116"/>
-      <c r="BL61" s="117"/>
-      <c r="BM61" s="118"/>
+      <c r="BK61" s="117"/>
+      <c r="BL61" s="118"/>
+      <c r="BM61" s="119"/>
       <c r="BO61" s="10" t="s">
         <v>43</v>
       </c>
@@ -5116,9 +5149,9 @@
       <c r="BH62" s="48"/>
       <c r="BI62" s="48"/>
       <c r="BJ62" s="49"/>
-      <c r="BK62" s="116"/>
-      <c r="BL62" s="117"/>
-      <c r="BM62" s="118"/>
+      <c r="BK62" s="117"/>
+      <c r="BL62" s="118"/>
+      <c r="BM62" s="119"/>
     </row>
     <row r="63" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -5185,9 +5218,9 @@
       <c r="BH63" s="51"/>
       <c r="BI63" s="51"/>
       <c r="BJ63" s="52"/>
-      <c r="BK63" s="119"/>
-      <c r="BL63" s="120"/>
-      <c r="BM63" s="121"/>
+      <c r="BK63" s="120"/>
+      <c r="BL63" s="121"/>
+      <c r="BM63" s="122"/>
     </row>
     <row r="64" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
@@ -5256,207 +5289,496 @@
       <c r="BH64" s="106"/>
       <c r="BI64" s="106"/>
       <c r="BJ64" s="107"/>
-    </row>
-    <row r="65" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="BK64" s="123" t="s">
+        <v>46</v>
+      </c>
+      <c r="BL64" s="124"/>
+      <c r="BM64" s="125"/>
+    </row>
+    <row r="65" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>5</v>
       </c>
       <c r="B65" s="108"/>
-      <c r="C65" s="122"/>
-      <c r="D65" s="122"/>
-      <c r="E65" s="122"/>
-      <c r="F65" s="122"/>
-      <c r="G65" s="122"/>
-      <c r="H65" s="122"/>
-      <c r="I65" s="122"/>
-      <c r="J65" s="122"/>
-      <c r="K65" s="122"/>
-      <c r="L65" s="122"/>
-      <c r="M65" s="122"/>
-      <c r="N65" s="122"/>
-      <c r="O65" s="122"/>
-      <c r="P65" s="122"/>
-      <c r="Q65" s="122"/>
-      <c r="R65" s="122"/>
-      <c r="S65" s="122"/>
-      <c r="T65" s="122"/>
-      <c r="U65" s="122"/>
-      <c r="V65" s="122"/>
-      <c r="W65" s="122"/>
-      <c r="X65" s="122"/>
-      <c r="Y65" s="122"/>
-      <c r="Z65" s="122"/>
-      <c r="AA65" s="122"/>
-      <c r="AB65" s="122"/>
-      <c r="AC65" s="122"/>
-      <c r="AD65" s="122"/>
-      <c r="AE65" s="122"/>
-      <c r="AF65" s="122"/>
-      <c r="AG65" s="122"/>
-      <c r="AH65" s="122"/>
-      <c r="AI65" s="122"/>
-      <c r="AJ65" s="122"/>
-      <c r="AK65" s="122"/>
-      <c r="AL65" s="122"/>
-      <c r="AM65" s="122"/>
-      <c r="AN65" s="122"/>
-      <c r="AO65" s="122"/>
-      <c r="AP65" s="122"/>
-      <c r="AQ65" s="122"/>
-      <c r="AR65" s="122"/>
-      <c r="AS65" s="122"/>
-      <c r="AT65" s="122"/>
-      <c r="AU65" s="122"/>
-      <c r="AV65" s="122"/>
-      <c r="AW65" s="122"/>
-      <c r="AX65" s="122"/>
-      <c r="AY65" s="122"/>
-      <c r="AZ65" s="122"/>
-      <c r="BA65" s="122"/>
-      <c r="BB65" s="122"/>
-      <c r="BC65" s="122"/>
-      <c r="BD65" s="122"/>
-      <c r="BE65" s="122"/>
-      <c r="BF65" s="122"/>
-      <c r="BG65" s="122"/>
-      <c r="BH65" s="122"/>
-      <c r="BI65" s="122"/>
-      <c r="BJ65" s="109"/>
-    </row>
-    <row r="66" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="C65" s="109"/>
+      <c r="D65" s="109"/>
+      <c r="E65" s="109"/>
+      <c r="F65" s="109"/>
+      <c r="G65" s="109"/>
+      <c r="H65" s="109"/>
+      <c r="I65" s="109"/>
+      <c r="J65" s="109"/>
+      <c r="K65" s="109"/>
+      <c r="L65" s="109"/>
+      <c r="M65" s="109"/>
+      <c r="N65" s="109"/>
+      <c r="O65" s="109"/>
+      <c r="P65" s="109"/>
+      <c r="Q65" s="109"/>
+      <c r="R65" s="109"/>
+      <c r="S65" s="109"/>
+      <c r="T65" s="109"/>
+      <c r="U65" s="109"/>
+      <c r="V65" s="109"/>
+      <c r="W65" s="109"/>
+      <c r="X65" s="109"/>
+      <c r="Y65" s="109"/>
+      <c r="Z65" s="109"/>
+      <c r="AA65" s="109"/>
+      <c r="AB65" s="109"/>
+      <c r="AC65" s="109"/>
+      <c r="AD65" s="109"/>
+      <c r="AE65" s="109"/>
+      <c r="AF65" s="109"/>
+      <c r="AG65" s="109"/>
+      <c r="AH65" s="109"/>
+      <c r="AI65" s="109"/>
+      <c r="AJ65" s="109"/>
+      <c r="AK65" s="109"/>
+      <c r="AL65" s="109"/>
+      <c r="AM65" s="109"/>
+      <c r="AN65" s="109"/>
+      <c r="AO65" s="109"/>
+      <c r="AP65" s="109"/>
+      <c r="AQ65" s="109"/>
+      <c r="AR65" s="109"/>
+      <c r="AS65" s="109"/>
+      <c r="AT65" s="109"/>
+      <c r="AU65" s="109"/>
+      <c r="AV65" s="109"/>
+      <c r="AW65" s="109"/>
+      <c r="AX65" s="109"/>
+      <c r="AY65" s="109"/>
+      <c r="AZ65" s="109"/>
+      <c r="BA65" s="109"/>
+      <c r="BB65" s="109"/>
+      <c r="BC65" s="109"/>
+      <c r="BD65" s="109"/>
+      <c r="BE65" s="109"/>
+      <c r="BF65" s="109"/>
+      <c r="BG65" s="109"/>
+      <c r="BH65" s="109"/>
+      <c r="BI65" s="109"/>
+      <c r="BJ65" s="110"/>
+      <c r="BK65" s="126"/>
+      <c r="BL65" s="127"/>
+      <c r="BM65" s="128"/>
+    </row>
+    <row r="66" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>6</v>
       </c>
       <c r="B66" s="108"/>
-      <c r="C66" s="122"/>
-      <c r="D66" s="122"/>
-      <c r="E66" s="122"/>
-      <c r="F66" s="122"/>
-      <c r="G66" s="122"/>
-      <c r="H66" s="122"/>
-      <c r="I66" s="122"/>
-      <c r="J66" s="122"/>
-      <c r="K66" s="122"/>
-      <c r="L66" s="122"/>
-      <c r="M66" s="122"/>
-      <c r="N66" s="122"/>
-      <c r="O66" s="122"/>
-      <c r="P66" s="122"/>
-      <c r="Q66" s="122"/>
-      <c r="R66" s="122"/>
-      <c r="S66" s="122"/>
-      <c r="T66" s="122"/>
-      <c r="U66" s="122"/>
-      <c r="V66" s="122"/>
-      <c r="W66" s="122"/>
-      <c r="X66" s="122"/>
-      <c r="Y66" s="122"/>
-      <c r="Z66" s="122"/>
-      <c r="AA66" s="122"/>
-      <c r="AB66" s="122"/>
-      <c r="AC66" s="122"/>
-      <c r="AD66" s="122"/>
-      <c r="AE66" s="122"/>
-      <c r="AF66" s="122"/>
-      <c r="AG66" s="122"/>
-      <c r="AH66" s="122"/>
-      <c r="AI66" s="122"/>
-      <c r="AJ66" s="122"/>
-      <c r="AK66" s="122"/>
-      <c r="AL66" s="122"/>
-      <c r="AM66" s="122"/>
-      <c r="AN66" s="122"/>
-      <c r="AO66" s="122"/>
-      <c r="AP66" s="122"/>
-      <c r="AQ66" s="122"/>
-      <c r="AR66" s="122"/>
-      <c r="AS66" s="122"/>
-      <c r="AT66" s="122"/>
-      <c r="AU66" s="122"/>
-      <c r="AV66" s="122"/>
-      <c r="AW66" s="122"/>
-      <c r="AX66" s="122"/>
-      <c r="AY66" s="122"/>
-      <c r="AZ66" s="122"/>
-      <c r="BA66" s="122"/>
-      <c r="BB66" s="122"/>
-      <c r="BC66" s="122"/>
-      <c r="BD66" s="122"/>
-      <c r="BE66" s="122"/>
-      <c r="BF66" s="122"/>
-      <c r="BG66" s="122"/>
-      <c r="BH66" s="122"/>
-      <c r="BI66" s="122"/>
-      <c r="BJ66" s="109"/>
-    </row>
-    <row r="67" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="C66" s="109"/>
+      <c r="D66" s="109"/>
+      <c r="E66" s="109"/>
+      <c r="F66" s="109"/>
+      <c r="G66" s="109"/>
+      <c r="H66" s="109"/>
+      <c r="I66" s="109"/>
+      <c r="J66" s="109"/>
+      <c r="K66" s="109"/>
+      <c r="L66" s="109"/>
+      <c r="M66" s="109"/>
+      <c r="N66" s="109"/>
+      <c r="O66" s="109"/>
+      <c r="P66" s="109"/>
+      <c r="Q66" s="109"/>
+      <c r="R66" s="109"/>
+      <c r="S66" s="109"/>
+      <c r="T66" s="109"/>
+      <c r="U66" s="109"/>
+      <c r="V66" s="109"/>
+      <c r="W66" s="109"/>
+      <c r="X66" s="109"/>
+      <c r="Y66" s="109"/>
+      <c r="Z66" s="109"/>
+      <c r="AA66" s="109"/>
+      <c r="AB66" s="109"/>
+      <c r="AC66" s="109"/>
+      <c r="AD66" s="109"/>
+      <c r="AE66" s="109"/>
+      <c r="AF66" s="109"/>
+      <c r="AG66" s="109"/>
+      <c r="AH66" s="109"/>
+      <c r="AI66" s="109"/>
+      <c r="AJ66" s="109"/>
+      <c r="AK66" s="109"/>
+      <c r="AL66" s="109"/>
+      <c r="AM66" s="109"/>
+      <c r="AN66" s="109"/>
+      <c r="AO66" s="109"/>
+      <c r="AP66" s="109"/>
+      <c r="AQ66" s="109"/>
+      <c r="AR66" s="109"/>
+      <c r="AS66" s="109"/>
+      <c r="AT66" s="109"/>
+      <c r="AU66" s="109"/>
+      <c r="AV66" s="109"/>
+      <c r="AW66" s="109"/>
+      <c r="AX66" s="109"/>
+      <c r="AY66" s="109"/>
+      <c r="AZ66" s="109"/>
+      <c r="BA66" s="109"/>
+      <c r="BB66" s="109"/>
+      <c r="BC66" s="109"/>
+      <c r="BD66" s="109"/>
+      <c r="BE66" s="109"/>
+      <c r="BF66" s="109"/>
+      <c r="BG66" s="109"/>
+      <c r="BH66" s="109"/>
+      <c r="BI66" s="109"/>
+      <c r="BJ66" s="110"/>
+      <c r="BK66" s="126"/>
+      <c r="BL66" s="127"/>
+      <c r="BM66" s="128"/>
+    </row>
+    <row r="67" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>7</v>
       </c>
-      <c r="B67" s="110"/>
-      <c r="C67" s="111"/>
-      <c r="D67" s="111"/>
-      <c r="E67" s="111"/>
-      <c r="F67" s="111"/>
-      <c r="G67" s="111"/>
-      <c r="H67" s="111"/>
-      <c r="I67" s="111"/>
-      <c r="J67" s="111"/>
-      <c r="K67" s="111"/>
-      <c r="L67" s="111"/>
-      <c r="M67" s="111"/>
-      <c r="N67" s="111"/>
-      <c r="O67" s="111"/>
-      <c r="P67" s="111"/>
-      <c r="Q67" s="111"/>
-      <c r="R67" s="111"/>
-      <c r="S67" s="111"/>
-      <c r="T67" s="111"/>
-      <c r="U67" s="111"/>
-      <c r="V67" s="111"/>
-      <c r="W67" s="111"/>
-      <c r="X67" s="111"/>
-      <c r="Y67" s="111"/>
-      <c r="Z67" s="111"/>
-      <c r="AA67" s="111"/>
-      <c r="AB67" s="111"/>
-      <c r="AC67" s="111"/>
-      <c r="AD67" s="111"/>
-      <c r="AE67" s="111"/>
-      <c r="AF67" s="111"/>
-      <c r="AG67" s="111"/>
-      <c r="AH67" s="111"/>
-      <c r="AI67" s="111"/>
-      <c r="AJ67" s="111"/>
-      <c r="AK67" s="111"/>
-      <c r="AL67" s="111"/>
-      <c r="AM67" s="111"/>
-      <c r="AN67" s="111"/>
-      <c r="AO67" s="111"/>
-      <c r="AP67" s="111"/>
-      <c r="AQ67" s="111"/>
-      <c r="AR67" s="111"/>
-      <c r="AS67" s="111"/>
-      <c r="AT67" s="111"/>
-      <c r="AU67" s="111"/>
-      <c r="AV67" s="111"/>
-      <c r="AW67" s="111"/>
-      <c r="AX67" s="111"/>
-      <c r="AY67" s="111"/>
-      <c r="AZ67" s="111"/>
-      <c r="BA67" s="111"/>
-      <c r="BB67" s="111"/>
-      <c r="BC67" s="111"/>
-      <c r="BD67" s="111"/>
-      <c r="BE67" s="111"/>
-      <c r="BF67" s="111"/>
-      <c r="BG67" s="111"/>
-      <c r="BH67" s="111"/>
-      <c r="BI67" s="111"/>
-      <c r="BJ67" s="112"/>
+      <c r="B67" s="111"/>
+      <c r="C67" s="112"/>
+      <c r="D67" s="112"/>
+      <c r="E67" s="112"/>
+      <c r="F67" s="112"/>
+      <c r="G67" s="112"/>
+      <c r="H67" s="112"/>
+      <c r="I67" s="112"/>
+      <c r="J67" s="112"/>
+      <c r="K67" s="112"/>
+      <c r="L67" s="112"/>
+      <c r="M67" s="112"/>
+      <c r="N67" s="112"/>
+      <c r="O67" s="112"/>
+      <c r="P67" s="112"/>
+      <c r="Q67" s="112"/>
+      <c r="R67" s="112"/>
+      <c r="S67" s="112"/>
+      <c r="T67" s="112"/>
+      <c r="U67" s="112"/>
+      <c r="V67" s="112"/>
+      <c r="W67" s="112"/>
+      <c r="X67" s="112"/>
+      <c r="Y67" s="112"/>
+      <c r="Z67" s="112"/>
+      <c r="AA67" s="112"/>
+      <c r="AB67" s="112"/>
+      <c r="AC67" s="112"/>
+      <c r="AD67" s="112"/>
+      <c r="AE67" s="112"/>
+      <c r="AF67" s="112"/>
+      <c r="AG67" s="112"/>
+      <c r="AH67" s="112"/>
+      <c r="AI67" s="112"/>
+      <c r="AJ67" s="112"/>
+      <c r="AK67" s="112"/>
+      <c r="AL67" s="112"/>
+      <c r="AM67" s="112"/>
+      <c r="AN67" s="112"/>
+      <c r="AO67" s="112"/>
+      <c r="AP67" s="112"/>
+      <c r="AQ67" s="112"/>
+      <c r="AR67" s="112"/>
+      <c r="AS67" s="112"/>
+      <c r="AT67" s="112"/>
+      <c r="AU67" s="112"/>
+      <c r="AV67" s="112"/>
+      <c r="AW67" s="112"/>
+      <c r="AX67" s="112"/>
+      <c r="AY67" s="112"/>
+      <c r="AZ67" s="112"/>
+      <c r="BA67" s="112"/>
+      <c r="BB67" s="112"/>
+      <c r="BC67" s="112"/>
+      <c r="BD67" s="112"/>
+      <c r="BE67" s="112"/>
+      <c r="BF67" s="112"/>
+      <c r="BG67" s="112"/>
+      <c r="BH67" s="112"/>
+      <c r="BI67" s="112"/>
+      <c r="BJ67" s="113"/>
+      <c r="BK67" s="129"/>
+      <c r="BL67" s="130"/>
+      <c r="BM67" s="131"/>
+    </row>
+    <row r="68" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>8</v>
+      </c>
+      <c r="B68" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" s="45"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="45"/>
+      <c r="G68" s="45"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="45"/>
+      <c r="J68" s="45"/>
+      <c r="K68" s="45"/>
+      <c r="L68" s="45"/>
+      <c r="M68" s="45"/>
+      <c r="N68" s="45"/>
+      <c r="O68" s="45"/>
+      <c r="P68" s="45"/>
+      <c r="Q68" s="45"/>
+      <c r="R68" s="45"/>
+      <c r="S68" s="45"/>
+      <c r="T68" s="45"/>
+      <c r="U68" s="45"/>
+      <c r="V68" s="45"/>
+      <c r="W68" s="45"/>
+      <c r="X68" s="45"/>
+      <c r="Y68" s="45"/>
+      <c r="Z68" s="45"/>
+      <c r="AA68" s="45"/>
+      <c r="AB68" s="45"/>
+      <c r="AC68" s="45"/>
+      <c r="AD68" s="45"/>
+      <c r="AE68" s="45"/>
+      <c r="AF68" s="45"/>
+      <c r="AG68" s="45"/>
+      <c r="AH68" s="45"/>
+      <c r="AI68" s="45"/>
+      <c r="AJ68" s="45"/>
+      <c r="AK68" s="45"/>
+      <c r="AL68" s="45"/>
+      <c r="AM68" s="45"/>
+      <c r="AN68" s="45"/>
+      <c r="AO68" s="45"/>
+      <c r="AP68" s="45"/>
+      <c r="AQ68" s="45"/>
+      <c r="AR68" s="45"/>
+      <c r="AS68" s="45"/>
+      <c r="AT68" s="45"/>
+      <c r="AU68" s="45"/>
+      <c r="AV68" s="45"/>
+      <c r="AW68" s="45"/>
+      <c r="AX68" s="45"/>
+      <c r="AY68" s="45"/>
+      <c r="AZ68" s="45"/>
+      <c r="BA68" s="45"/>
+      <c r="BB68" s="45"/>
+      <c r="BC68" s="45"/>
+      <c r="BD68" s="45"/>
+      <c r="BE68" s="45"/>
+      <c r="BF68" s="45"/>
+      <c r="BG68" s="46"/>
+    </row>
+    <row r="69" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>9</v>
+      </c>
+      <c r="B69" s="47"/>
+      <c r="C69" s="132"/>
+      <c r="D69" s="132"/>
+      <c r="E69" s="132"/>
+      <c r="F69" s="132"/>
+      <c r="G69" s="132"/>
+      <c r="H69" s="132"/>
+      <c r="I69" s="132"/>
+      <c r="J69" s="132"/>
+      <c r="K69" s="132"/>
+      <c r="L69" s="132"/>
+      <c r="M69" s="132"/>
+      <c r="N69" s="132"/>
+      <c r="O69" s="132"/>
+      <c r="P69" s="132"/>
+      <c r="Q69" s="132"/>
+      <c r="R69" s="132"/>
+      <c r="S69" s="132"/>
+      <c r="T69" s="132"/>
+      <c r="U69" s="132"/>
+      <c r="V69" s="132"/>
+      <c r="W69" s="132"/>
+      <c r="X69" s="132"/>
+      <c r="Y69" s="132"/>
+      <c r="Z69" s="132"/>
+      <c r="AA69" s="132"/>
+      <c r="AB69" s="132"/>
+      <c r="AC69" s="132"/>
+      <c r="AD69" s="132"/>
+      <c r="AE69" s="132"/>
+      <c r="AF69" s="132"/>
+      <c r="AG69" s="132"/>
+      <c r="AH69" s="132"/>
+      <c r="AI69" s="132"/>
+      <c r="AJ69" s="132"/>
+      <c r="AK69" s="132"/>
+      <c r="AL69" s="132"/>
+      <c r="AM69" s="132"/>
+      <c r="AN69" s="132"/>
+      <c r="AO69" s="132"/>
+      <c r="AP69" s="132"/>
+      <c r="AQ69" s="132"/>
+      <c r="AR69" s="132"/>
+      <c r="AS69" s="132"/>
+      <c r="AT69" s="132"/>
+      <c r="AU69" s="132"/>
+      <c r="AV69" s="132"/>
+      <c r="AW69" s="132"/>
+      <c r="AX69" s="132"/>
+      <c r="AY69" s="132"/>
+      <c r="AZ69" s="132"/>
+      <c r="BA69" s="132"/>
+      <c r="BB69" s="132"/>
+      <c r="BC69" s="132"/>
+      <c r="BD69" s="132"/>
+      <c r="BE69" s="132"/>
+      <c r="BF69" s="132"/>
+      <c r="BG69" s="49"/>
+    </row>
+    <row r="70" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>10</v>
+      </c>
+      <c r="B70" s="47"/>
+      <c r="C70" s="132"/>
+      <c r="D70" s="132"/>
+      <c r="E70" s="132"/>
+      <c r="F70" s="132"/>
+      <c r="G70" s="132"/>
+      <c r="H70" s="132"/>
+      <c r="I70" s="132"/>
+      <c r="J70" s="132"/>
+      <c r="K70" s="132"/>
+      <c r="L70" s="132"/>
+      <c r="M70" s="132"/>
+      <c r="N70" s="132"/>
+      <c r="O70" s="132"/>
+      <c r="P70" s="132"/>
+      <c r="Q70" s="132"/>
+      <c r="R70" s="132"/>
+      <c r="S70" s="132"/>
+      <c r="T70" s="132"/>
+      <c r="U70" s="132"/>
+      <c r="V70" s="132"/>
+      <c r="W70" s="132"/>
+      <c r="X70" s="132"/>
+      <c r="Y70" s="132"/>
+      <c r="Z70" s="132"/>
+      <c r="AA70" s="132"/>
+      <c r="AB70" s="132"/>
+      <c r="AC70" s="132"/>
+      <c r="AD70" s="132"/>
+      <c r="AE70" s="132"/>
+      <c r="AF70" s="132"/>
+      <c r="AG70" s="132"/>
+      <c r="AH70" s="132"/>
+      <c r="AI70" s="132"/>
+      <c r="AJ70" s="132"/>
+      <c r="AK70" s="132"/>
+      <c r="AL70" s="132"/>
+      <c r="AM70" s="132"/>
+      <c r="AN70" s="132"/>
+      <c r="AO70" s="132"/>
+      <c r="AP70" s="132"/>
+      <c r="AQ70" s="132"/>
+      <c r="AR70" s="132"/>
+      <c r="AS70" s="132"/>
+      <c r="AT70" s="132"/>
+      <c r="AU70" s="132"/>
+      <c r="AV70" s="132"/>
+      <c r="AW70" s="132"/>
+      <c r="AX70" s="132"/>
+      <c r="AY70" s="132"/>
+      <c r="AZ70" s="132"/>
+      <c r="BA70" s="132"/>
+      <c r="BB70" s="132"/>
+      <c r="BC70" s="132"/>
+      <c r="BD70" s="132"/>
+      <c r="BE70" s="132"/>
+      <c r="BF70" s="132"/>
+      <c r="BG70" s="49"/>
+    </row>
+    <row r="71" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>11</v>
+      </c>
+      <c r="B71" s="50"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="51"/>
+      <c r="E71" s="51"/>
+      <c r="F71" s="51"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="51"/>
+      <c r="I71" s="51"/>
+      <c r="J71" s="51"/>
+      <c r="K71" s="51"/>
+      <c r="L71" s="51"/>
+      <c r="M71" s="51"/>
+      <c r="N71" s="51"/>
+      <c r="O71" s="51"/>
+      <c r="P71" s="51"/>
+      <c r="Q71" s="51"/>
+      <c r="R71" s="51"/>
+      <c r="S71" s="51"/>
+      <c r="T71" s="51"/>
+      <c r="U71" s="51"/>
+      <c r="V71" s="51"/>
+      <c r="W71" s="51"/>
+      <c r="X71" s="51"/>
+      <c r="Y71" s="51"/>
+      <c r="Z71" s="51"/>
+      <c r="AA71" s="51"/>
+      <c r="AB71" s="51"/>
+      <c r="AC71" s="51"/>
+      <c r="AD71" s="51"/>
+      <c r="AE71" s="51"/>
+      <c r="AF71" s="51"/>
+      <c r="AG71" s="51"/>
+      <c r="AH71" s="51"/>
+      <c r="AI71" s="51"/>
+      <c r="AJ71" s="51"/>
+      <c r="AK71" s="51"/>
+      <c r="AL71" s="51"/>
+      <c r="AM71" s="51"/>
+      <c r="AN71" s="51"/>
+      <c r="AO71" s="51"/>
+      <c r="AP71" s="51"/>
+      <c r="AQ71" s="51"/>
+      <c r="AR71" s="51"/>
+      <c r="AS71" s="51"/>
+      <c r="AT71" s="51"/>
+      <c r="AU71" s="51"/>
+      <c r="AV71" s="51"/>
+      <c r="AW71" s="51"/>
+      <c r="AX71" s="51"/>
+      <c r="AY71" s="51"/>
+      <c r="AZ71" s="51"/>
+      <c r="BA71" s="51"/>
+      <c r="BB71" s="51"/>
+      <c r="BC71" s="51"/>
+      <c r="BD71" s="51"/>
+      <c r="BE71" s="51"/>
+      <c r="BF71" s="51"/>
+      <c r="BG71" s="52"/>
+    </row>
+    <row r="72" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="28">
+    <mergeCell ref="B68:BG71"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="B3:BM6"/>
     <mergeCell ref="B11:BM14"/>
@@ -5483,6 +5805,7 @@
     <mergeCell ref="BO33:BP33"/>
     <mergeCell ref="A58:M58"/>
     <mergeCell ref="B64:BJ67"/>
+    <mergeCell ref="BK64:BM67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added broadcast transpose to prepare for QKV of encoder MHSA
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A483CC94-3640-2343-82FF-3CC6D8ADFD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0868CA2-8AC1-2543-9090-1F3A7DD43250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
@@ -800,9 +800,6 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -827,9 +824,6 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -844,6 +838,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1172,7 +1172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
   <dimension ref="A1:BP75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B68" sqref="B68:BG71"/>
     </sheetView>
   </sheetViews>
@@ -5003,11 +5003,11 @@
       <c r="BH60" s="45"/>
       <c r="BI60" s="45"/>
       <c r="BJ60" s="46"/>
-      <c r="BK60" s="114" t="s">
+      <c r="BK60" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="BL60" s="115"/>
-      <c r="BM60" s="116"/>
+      <c r="BL60" s="123"/>
+      <c r="BM60" s="124"/>
       <c r="BO60" s="10" t="s">
         <v>42</v>
       </c>
@@ -5077,9 +5077,9 @@
       <c r="BH61" s="48"/>
       <c r="BI61" s="48"/>
       <c r="BJ61" s="49"/>
-      <c r="BK61" s="117"/>
-      <c r="BL61" s="118"/>
-      <c r="BM61" s="119"/>
+      <c r="BK61" s="125"/>
+      <c r="BL61" s="131"/>
+      <c r="BM61" s="126"/>
       <c r="BO61" s="10" t="s">
         <v>43</v>
       </c>
@@ -5149,9 +5149,9 @@
       <c r="BH62" s="48"/>
       <c r="BI62" s="48"/>
       <c r="BJ62" s="49"/>
-      <c r="BK62" s="117"/>
-      <c r="BL62" s="118"/>
-      <c r="BM62" s="119"/>
+      <c r="BK62" s="125"/>
+      <c r="BL62" s="131"/>
+      <c r="BM62" s="126"/>
     </row>
     <row r="63" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -5218,543 +5218,543 @@
       <c r="BH63" s="51"/>
       <c r="BI63" s="51"/>
       <c r="BJ63" s="52"/>
-      <c r="BK63" s="120"/>
-      <c r="BL63" s="121"/>
-      <c r="BM63" s="122"/>
+      <c r="BK63" s="127"/>
+      <c r="BL63" s="128"/>
+      <c r="BM63" s="129"/>
     </row>
     <row r="64" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>4</v>
       </c>
-      <c r="B64" s="105" t="s">
+      <c r="B64" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C64" s="106"/>
-      <c r="D64" s="106"/>
-      <c r="E64" s="106"/>
-      <c r="F64" s="106"/>
-      <c r="G64" s="106"/>
-      <c r="H64" s="106"/>
-      <c r="I64" s="106"/>
-      <c r="J64" s="106"/>
-      <c r="K64" s="106"/>
-      <c r="L64" s="106"/>
-      <c r="M64" s="106"/>
-      <c r="N64" s="106"/>
-      <c r="O64" s="106"/>
-      <c r="P64" s="106"/>
-      <c r="Q64" s="106"/>
-      <c r="R64" s="106"/>
-      <c r="S64" s="106"/>
-      <c r="T64" s="106"/>
-      <c r="U64" s="106"/>
-      <c r="V64" s="106"/>
-      <c r="W64" s="106"/>
-      <c r="X64" s="106"/>
-      <c r="Y64" s="106"/>
-      <c r="Z64" s="106"/>
-      <c r="AA64" s="106"/>
-      <c r="AB64" s="106"/>
-      <c r="AC64" s="106"/>
-      <c r="AD64" s="106"/>
-      <c r="AE64" s="106"/>
-      <c r="AF64" s="106"/>
-      <c r="AG64" s="106"/>
-      <c r="AH64" s="106"/>
-      <c r="AI64" s="106"/>
-      <c r="AJ64" s="106"/>
-      <c r="AK64" s="106"/>
-      <c r="AL64" s="106"/>
-      <c r="AM64" s="106"/>
-      <c r="AN64" s="106"/>
-      <c r="AO64" s="106"/>
-      <c r="AP64" s="106"/>
-      <c r="AQ64" s="106"/>
-      <c r="AR64" s="106"/>
-      <c r="AS64" s="106"/>
-      <c r="AT64" s="106"/>
-      <c r="AU64" s="106"/>
-      <c r="AV64" s="106"/>
-      <c r="AW64" s="106"/>
-      <c r="AX64" s="106"/>
-      <c r="AY64" s="106"/>
-      <c r="AZ64" s="106"/>
-      <c r="BA64" s="106"/>
-      <c r="BB64" s="106"/>
-      <c r="BC64" s="106"/>
-      <c r="BD64" s="106"/>
-      <c r="BE64" s="106"/>
-      <c r="BF64" s="106"/>
-      <c r="BG64" s="106"/>
-      <c r="BH64" s="106"/>
-      <c r="BI64" s="106"/>
-      <c r="BJ64" s="107"/>
-      <c r="BK64" s="123" t="s">
+      <c r="C64" s="45"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="45"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="45"/>
+      <c r="L64" s="45"/>
+      <c r="M64" s="45"/>
+      <c r="N64" s="45"/>
+      <c r="O64" s="45"/>
+      <c r="P64" s="45"/>
+      <c r="Q64" s="45"/>
+      <c r="R64" s="45"/>
+      <c r="S64" s="45"/>
+      <c r="T64" s="45"/>
+      <c r="U64" s="45"/>
+      <c r="V64" s="45"/>
+      <c r="W64" s="45"/>
+      <c r="X64" s="45"/>
+      <c r="Y64" s="45"/>
+      <c r="Z64" s="45"/>
+      <c r="AA64" s="45"/>
+      <c r="AB64" s="45"/>
+      <c r="AC64" s="45"/>
+      <c r="AD64" s="45"/>
+      <c r="AE64" s="45"/>
+      <c r="AF64" s="45"/>
+      <c r="AG64" s="45"/>
+      <c r="AH64" s="45"/>
+      <c r="AI64" s="45"/>
+      <c r="AJ64" s="45"/>
+      <c r="AK64" s="45"/>
+      <c r="AL64" s="45"/>
+      <c r="AM64" s="45"/>
+      <c r="AN64" s="45"/>
+      <c r="AO64" s="45"/>
+      <c r="AP64" s="45"/>
+      <c r="AQ64" s="45"/>
+      <c r="AR64" s="45"/>
+      <c r="AS64" s="45"/>
+      <c r="AT64" s="45"/>
+      <c r="AU64" s="45"/>
+      <c r="AV64" s="45"/>
+      <c r="AW64" s="45"/>
+      <c r="AX64" s="45"/>
+      <c r="AY64" s="45"/>
+      <c r="AZ64" s="45"/>
+      <c r="BA64" s="45"/>
+      <c r="BB64" s="45"/>
+      <c r="BC64" s="45"/>
+      <c r="BD64" s="45"/>
+      <c r="BE64" s="45"/>
+      <c r="BF64" s="45"/>
+      <c r="BG64" s="45"/>
+      <c r="BH64" s="45"/>
+      <c r="BI64" s="45"/>
+      <c r="BJ64" s="46"/>
+      <c r="BK64" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="BL64" s="124"/>
-      <c r="BM64" s="125"/>
+      <c r="BL64" s="115"/>
+      <c r="BM64" s="116"/>
     </row>
     <row r="65" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>5</v>
       </c>
-      <c r="B65" s="108"/>
-      <c r="C65" s="109"/>
-      <c r="D65" s="109"/>
-      <c r="E65" s="109"/>
-      <c r="F65" s="109"/>
-      <c r="G65" s="109"/>
-      <c r="H65" s="109"/>
-      <c r="I65" s="109"/>
-      <c r="J65" s="109"/>
-      <c r="K65" s="109"/>
-      <c r="L65" s="109"/>
-      <c r="M65" s="109"/>
-      <c r="N65" s="109"/>
-      <c r="O65" s="109"/>
-      <c r="P65" s="109"/>
-      <c r="Q65" s="109"/>
-      <c r="R65" s="109"/>
-      <c r="S65" s="109"/>
-      <c r="T65" s="109"/>
-      <c r="U65" s="109"/>
-      <c r="V65" s="109"/>
-      <c r="W65" s="109"/>
-      <c r="X65" s="109"/>
-      <c r="Y65" s="109"/>
-      <c r="Z65" s="109"/>
-      <c r="AA65" s="109"/>
-      <c r="AB65" s="109"/>
-      <c r="AC65" s="109"/>
-      <c r="AD65" s="109"/>
-      <c r="AE65" s="109"/>
-      <c r="AF65" s="109"/>
-      <c r="AG65" s="109"/>
-      <c r="AH65" s="109"/>
-      <c r="AI65" s="109"/>
-      <c r="AJ65" s="109"/>
-      <c r="AK65" s="109"/>
-      <c r="AL65" s="109"/>
-      <c r="AM65" s="109"/>
-      <c r="AN65" s="109"/>
-      <c r="AO65" s="109"/>
-      <c r="AP65" s="109"/>
-      <c r="AQ65" s="109"/>
-      <c r="AR65" s="109"/>
-      <c r="AS65" s="109"/>
-      <c r="AT65" s="109"/>
-      <c r="AU65" s="109"/>
-      <c r="AV65" s="109"/>
-      <c r="AW65" s="109"/>
-      <c r="AX65" s="109"/>
-      <c r="AY65" s="109"/>
-      <c r="AZ65" s="109"/>
-      <c r="BA65" s="109"/>
-      <c r="BB65" s="109"/>
-      <c r="BC65" s="109"/>
-      <c r="BD65" s="109"/>
-      <c r="BE65" s="109"/>
-      <c r="BF65" s="109"/>
-      <c r="BG65" s="109"/>
-      <c r="BH65" s="109"/>
-      <c r="BI65" s="109"/>
-      <c r="BJ65" s="110"/>
-      <c r="BK65" s="126"/>
-      <c r="BL65" s="127"/>
-      <c r="BM65" s="128"/>
+      <c r="B65" s="47"/>
+      <c r="C65" s="130"/>
+      <c r="D65" s="130"/>
+      <c r="E65" s="130"/>
+      <c r="F65" s="130"/>
+      <c r="G65" s="130"/>
+      <c r="H65" s="130"/>
+      <c r="I65" s="130"/>
+      <c r="J65" s="130"/>
+      <c r="K65" s="130"/>
+      <c r="L65" s="130"/>
+      <c r="M65" s="130"/>
+      <c r="N65" s="130"/>
+      <c r="O65" s="130"/>
+      <c r="P65" s="130"/>
+      <c r="Q65" s="130"/>
+      <c r="R65" s="130"/>
+      <c r="S65" s="130"/>
+      <c r="T65" s="130"/>
+      <c r="U65" s="130"/>
+      <c r="V65" s="130"/>
+      <c r="W65" s="130"/>
+      <c r="X65" s="130"/>
+      <c r="Y65" s="130"/>
+      <c r="Z65" s="130"/>
+      <c r="AA65" s="130"/>
+      <c r="AB65" s="130"/>
+      <c r="AC65" s="130"/>
+      <c r="AD65" s="130"/>
+      <c r="AE65" s="130"/>
+      <c r="AF65" s="130"/>
+      <c r="AG65" s="130"/>
+      <c r="AH65" s="130"/>
+      <c r="AI65" s="130"/>
+      <c r="AJ65" s="130"/>
+      <c r="AK65" s="130"/>
+      <c r="AL65" s="130"/>
+      <c r="AM65" s="130"/>
+      <c r="AN65" s="130"/>
+      <c r="AO65" s="130"/>
+      <c r="AP65" s="130"/>
+      <c r="AQ65" s="130"/>
+      <c r="AR65" s="130"/>
+      <c r="AS65" s="130"/>
+      <c r="AT65" s="130"/>
+      <c r="AU65" s="130"/>
+      <c r="AV65" s="130"/>
+      <c r="AW65" s="130"/>
+      <c r="AX65" s="130"/>
+      <c r="AY65" s="130"/>
+      <c r="AZ65" s="130"/>
+      <c r="BA65" s="130"/>
+      <c r="BB65" s="130"/>
+      <c r="BC65" s="130"/>
+      <c r="BD65" s="130"/>
+      <c r="BE65" s="130"/>
+      <c r="BF65" s="130"/>
+      <c r="BG65" s="130"/>
+      <c r="BH65" s="130"/>
+      <c r="BI65" s="130"/>
+      <c r="BJ65" s="49"/>
+      <c r="BK65" s="117"/>
+      <c r="BL65" s="132"/>
+      <c r="BM65" s="118"/>
     </row>
     <row r="66" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>6</v>
       </c>
-      <c r="B66" s="108"/>
-      <c r="C66" s="109"/>
-      <c r="D66" s="109"/>
-      <c r="E66" s="109"/>
-      <c r="F66" s="109"/>
-      <c r="G66" s="109"/>
-      <c r="H66" s="109"/>
-      <c r="I66" s="109"/>
-      <c r="J66" s="109"/>
-      <c r="K66" s="109"/>
-      <c r="L66" s="109"/>
-      <c r="M66" s="109"/>
-      <c r="N66" s="109"/>
-      <c r="O66" s="109"/>
-      <c r="P66" s="109"/>
-      <c r="Q66" s="109"/>
-      <c r="R66" s="109"/>
-      <c r="S66" s="109"/>
-      <c r="T66" s="109"/>
-      <c r="U66" s="109"/>
-      <c r="V66" s="109"/>
-      <c r="W66" s="109"/>
-      <c r="X66" s="109"/>
-      <c r="Y66" s="109"/>
-      <c r="Z66" s="109"/>
-      <c r="AA66" s="109"/>
-      <c r="AB66" s="109"/>
-      <c r="AC66" s="109"/>
-      <c r="AD66" s="109"/>
-      <c r="AE66" s="109"/>
-      <c r="AF66" s="109"/>
-      <c r="AG66" s="109"/>
-      <c r="AH66" s="109"/>
-      <c r="AI66" s="109"/>
-      <c r="AJ66" s="109"/>
-      <c r="AK66" s="109"/>
-      <c r="AL66" s="109"/>
-      <c r="AM66" s="109"/>
-      <c r="AN66" s="109"/>
-      <c r="AO66" s="109"/>
-      <c r="AP66" s="109"/>
-      <c r="AQ66" s="109"/>
-      <c r="AR66" s="109"/>
-      <c r="AS66" s="109"/>
-      <c r="AT66" s="109"/>
-      <c r="AU66" s="109"/>
-      <c r="AV66" s="109"/>
-      <c r="AW66" s="109"/>
-      <c r="AX66" s="109"/>
-      <c r="AY66" s="109"/>
-      <c r="AZ66" s="109"/>
-      <c r="BA66" s="109"/>
-      <c r="BB66" s="109"/>
-      <c r="BC66" s="109"/>
-      <c r="BD66" s="109"/>
-      <c r="BE66" s="109"/>
-      <c r="BF66" s="109"/>
-      <c r="BG66" s="109"/>
-      <c r="BH66" s="109"/>
-      <c r="BI66" s="109"/>
-      <c r="BJ66" s="110"/>
-      <c r="BK66" s="126"/>
-      <c r="BL66" s="127"/>
-      <c r="BM66" s="128"/>
+      <c r="B66" s="47"/>
+      <c r="C66" s="130"/>
+      <c r="D66" s="130"/>
+      <c r="E66" s="130"/>
+      <c r="F66" s="130"/>
+      <c r="G66" s="130"/>
+      <c r="H66" s="130"/>
+      <c r="I66" s="130"/>
+      <c r="J66" s="130"/>
+      <c r="K66" s="130"/>
+      <c r="L66" s="130"/>
+      <c r="M66" s="130"/>
+      <c r="N66" s="130"/>
+      <c r="O66" s="130"/>
+      <c r="P66" s="130"/>
+      <c r="Q66" s="130"/>
+      <c r="R66" s="130"/>
+      <c r="S66" s="130"/>
+      <c r="T66" s="130"/>
+      <c r="U66" s="130"/>
+      <c r="V66" s="130"/>
+      <c r="W66" s="130"/>
+      <c r="X66" s="130"/>
+      <c r="Y66" s="130"/>
+      <c r="Z66" s="130"/>
+      <c r="AA66" s="130"/>
+      <c r="AB66" s="130"/>
+      <c r="AC66" s="130"/>
+      <c r="AD66" s="130"/>
+      <c r="AE66" s="130"/>
+      <c r="AF66" s="130"/>
+      <c r="AG66" s="130"/>
+      <c r="AH66" s="130"/>
+      <c r="AI66" s="130"/>
+      <c r="AJ66" s="130"/>
+      <c r="AK66" s="130"/>
+      <c r="AL66" s="130"/>
+      <c r="AM66" s="130"/>
+      <c r="AN66" s="130"/>
+      <c r="AO66" s="130"/>
+      <c r="AP66" s="130"/>
+      <c r="AQ66" s="130"/>
+      <c r="AR66" s="130"/>
+      <c r="AS66" s="130"/>
+      <c r="AT66" s="130"/>
+      <c r="AU66" s="130"/>
+      <c r="AV66" s="130"/>
+      <c r="AW66" s="130"/>
+      <c r="AX66" s="130"/>
+      <c r="AY66" s="130"/>
+      <c r="AZ66" s="130"/>
+      <c r="BA66" s="130"/>
+      <c r="BB66" s="130"/>
+      <c r="BC66" s="130"/>
+      <c r="BD66" s="130"/>
+      <c r="BE66" s="130"/>
+      <c r="BF66" s="130"/>
+      <c r="BG66" s="130"/>
+      <c r="BH66" s="130"/>
+      <c r="BI66" s="130"/>
+      <c r="BJ66" s="49"/>
+      <c r="BK66" s="117"/>
+      <c r="BL66" s="132"/>
+      <c r="BM66" s="118"/>
     </row>
     <row r="67" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>7</v>
       </c>
-      <c r="B67" s="111"/>
-      <c r="C67" s="112"/>
-      <c r="D67" s="112"/>
-      <c r="E67" s="112"/>
-      <c r="F67" s="112"/>
-      <c r="G67" s="112"/>
-      <c r="H67" s="112"/>
-      <c r="I67" s="112"/>
-      <c r="J67" s="112"/>
-      <c r="K67" s="112"/>
-      <c r="L67" s="112"/>
-      <c r="M67" s="112"/>
-      <c r="N67" s="112"/>
-      <c r="O67" s="112"/>
-      <c r="P67" s="112"/>
-      <c r="Q67" s="112"/>
-      <c r="R67" s="112"/>
-      <c r="S67" s="112"/>
-      <c r="T67" s="112"/>
-      <c r="U67" s="112"/>
-      <c r="V67" s="112"/>
-      <c r="W67" s="112"/>
-      <c r="X67" s="112"/>
-      <c r="Y67" s="112"/>
-      <c r="Z67" s="112"/>
-      <c r="AA67" s="112"/>
-      <c r="AB67" s="112"/>
-      <c r="AC67" s="112"/>
-      <c r="AD67" s="112"/>
-      <c r="AE67" s="112"/>
-      <c r="AF67" s="112"/>
-      <c r="AG67" s="112"/>
-      <c r="AH67" s="112"/>
-      <c r="AI67" s="112"/>
-      <c r="AJ67" s="112"/>
-      <c r="AK67" s="112"/>
-      <c r="AL67" s="112"/>
-      <c r="AM67" s="112"/>
-      <c r="AN67" s="112"/>
-      <c r="AO67" s="112"/>
-      <c r="AP67" s="112"/>
-      <c r="AQ67" s="112"/>
-      <c r="AR67" s="112"/>
-      <c r="AS67" s="112"/>
-      <c r="AT67" s="112"/>
-      <c r="AU67" s="112"/>
-      <c r="AV67" s="112"/>
-      <c r="AW67" s="112"/>
-      <c r="AX67" s="112"/>
-      <c r="AY67" s="112"/>
-      <c r="AZ67" s="112"/>
-      <c r="BA67" s="112"/>
-      <c r="BB67" s="112"/>
-      <c r="BC67" s="112"/>
-      <c r="BD67" s="112"/>
-      <c r="BE67" s="112"/>
-      <c r="BF67" s="112"/>
-      <c r="BG67" s="112"/>
-      <c r="BH67" s="112"/>
-      <c r="BI67" s="112"/>
-      <c r="BJ67" s="113"/>
-      <c r="BK67" s="129"/>
-      <c r="BL67" s="130"/>
-      <c r="BM67" s="131"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="51"/>
+      <c r="K67" s="51"/>
+      <c r="L67" s="51"/>
+      <c r="M67" s="51"/>
+      <c r="N67" s="51"/>
+      <c r="O67" s="51"/>
+      <c r="P67" s="51"/>
+      <c r="Q67" s="51"/>
+      <c r="R67" s="51"/>
+      <c r="S67" s="51"/>
+      <c r="T67" s="51"/>
+      <c r="U67" s="51"/>
+      <c r="V67" s="51"/>
+      <c r="W67" s="51"/>
+      <c r="X67" s="51"/>
+      <c r="Y67" s="51"/>
+      <c r="Z67" s="51"/>
+      <c r="AA67" s="51"/>
+      <c r="AB67" s="51"/>
+      <c r="AC67" s="51"/>
+      <c r="AD67" s="51"/>
+      <c r="AE67" s="51"/>
+      <c r="AF67" s="51"/>
+      <c r="AG67" s="51"/>
+      <c r="AH67" s="51"/>
+      <c r="AI67" s="51"/>
+      <c r="AJ67" s="51"/>
+      <c r="AK67" s="51"/>
+      <c r="AL67" s="51"/>
+      <c r="AM67" s="51"/>
+      <c r="AN67" s="51"/>
+      <c r="AO67" s="51"/>
+      <c r="AP67" s="51"/>
+      <c r="AQ67" s="51"/>
+      <c r="AR67" s="51"/>
+      <c r="AS67" s="51"/>
+      <c r="AT67" s="51"/>
+      <c r="AU67" s="51"/>
+      <c r="AV67" s="51"/>
+      <c r="AW67" s="51"/>
+      <c r="AX67" s="51"/>
+      <c r="AY67" s="51"/>
+      <c r="AZ67" s="51"/>
+      <c r="BA67" s="51"/>
+      <c r="BB67" s="51"/>
+      <c r="BC67" s="51"/>
+      <c r="BD67" s="51"/>
+      <c r="BE67" s="51"/>
+      <c r="BF67" s="51"/>
+      <c r="BG67" s="51"/>
+      <c r="BH67" s="51"/>
+      <c r="BI67" s="51"/>
+      <c r="BJ67" s="52"/>
+      <c r="BK67" s="119"/>
+      <c r="BL67" s="120"/>
+      <c r="BM67" s="121"/>
     </row>
     <row r="68" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>8</v>
       </c>
-      <c r="B68" s="44" t="s">
+      <c r="B68" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C68" s="45"/>
-      <c r="D68" s="45"/>
-      <c r="E68" s="45"/>
-      <c r="F68" s="45"/>
-      <c r="G68" s="45"/>
-      <c r="H68" s="45"/>
-      <c r="I68" s="45"/>
-      <c r="J68" s="45"/>
-      <c r="K68" s="45"/>
-      <c r="L68" s="45"/>
-      <c r="M68" s="45"/>
-      <c r="N68" s="45"/>
-      <c r="O68" s="45"/>
-      <c r="P68" s="45"/>
-      <c r="Q68" s="45"/>
-      <c r="R68" s="45"/>
-      <c r="S68" s="45"/>
-      <c r="T68" s="45"/>
-      <c r="U68" s="45"/>
-      <c r="V68" s="45"/>
-      <c r="W68" s="45"/>
-      <c r="X68" s="45"/>
-      <c r="Y68" s="45"/>
-      <c r="Z68" s="45"/>
-      <c r="AA68" s="45"/>
-      <c r="AB68" s="45"/>
-      <c r="AC68" s="45"/>
-      <c r="AD68" s="45"/>
-      <c r="AE68" s="45"/>
-      <c r="AF68" s="45"/>
-      <c r="AG68" s="45"/>
-      <c r="AH68" s="45"/>
-      <c r="AI68" s="45"/>
-      <c r="AJ68" s="45"/>
-      <c r="AK68" s="45"/>
-      <c r="AL68" s="45"/>
-      <c r="AM68" s="45"/>
-      <c r="AN68" s="45"/>
-      <c r="AO68" s="45"/>
-      <c r="AP68" s="45"/>
-      <c r="AQ68" s="45"/>
-      <c r="AR68" s="45"/>
-      <c r="AS68" s="45"/>
-      <c r="AT68" s="45"/>
-      <c r="AU68" s="45"/>
-      <c r="AV68" s="45"/>
-      <c r="AW68" s="45"/>
-      <c r="AX68" s="45"/>
-      <c r="AY68" s="45"/>
-      <c r="AZ68" s="45"/>
-      <c r="BA68" s="45"/>
-      <c r="BB68" s="45"/>
-      <c r="BC68" s="45"/>
-      <c r="BD68" s="45"/>
-      <c r="BE68" s="45"/>
-      <c r="BF68" s="45"/>
-      <c r="BG68" s="46"/>
+      <c r="C68" s="106"/>
+      <c r="D68" s="106"/>
+      <c r="E68" s="106"/>
+      <c r="F68" s="106"/>
+      <c r="G68" s="106"/>
+      <c r="H68" s="106"/>
+      <c r="I68" s="106"/>
+      <c r="J68" s="106"/>
+      <c r="K68" s="106"/>
+      <c r="L68" s="106"/>
+      <c r="M68" s="106"/>
+      <c r="N68" s="106"/>
+      <c r="O68" s="106"/>
+      <c r="P68" s="106"/>
+      <c r="Q68" s="106"/>
+      <c r="R68" s="106"/>
+      <c r="S68" s="106"/>
+      <c r="T68" s="106"/>
+      <c r="U68" s="106"/>
+      <c r="V68" s="106"/>
+      <c r="W68" s="106"/>
+      <c r="X68" s="106"/>
+      <c r="Y68" s="106"/>
+      <c r="Z68" s="106"/>
+      <c r="AA68" s="106"/>
+      <c r="AB68" s="106"/>
+      <c r="AC68" s="106"/>
+      <c r="AD68" s="106"/>
+      <c r="AE68" s="106"/>
+      <c r="AF68" s="106"/>
+      <c r="AG68" s="106"/>
+      <c r="AH68" s="106"/>
+      <c r="AI68" s="106"/>
+      <c r="AJ68" s="106"/>
+      <c r="AK68" s="106"/>
+      <c r="AL68" s="106"/>
+      <c r="AM68" s="106"/>
+      <c r="AN68" s="106"/>
+      <c r="AO68" s="106"/>
+      <c r="AP68" s="106"/>
+      <c r="AQ68" s="106"/>
+      <c r="AR68" s="106"/>
+      <c r="AS68" s="106"/>
+      <c r="AT68" s="106"/>
+      <c r="AU68" s="106"/>
+      <c r="AV68" s="106"/>
+      <c r="AW68" s="106"/>
+      <c r="AX68" s="106"/>
+      <c r="AY68" s="106"/>
+      <c r="AZ68" s="106"/>
+      <c r="BA68" s="106"/>
+      <c r="BB68" s="106"/>
+      <c r="BC68" s="106"/>
+      <c r="BD68" s="106"/>
+      <c r="BE68" s="106"/>
+      <c r="BF68" s="106"/>
+      <c r="BG68" s="107"/>
     </row>
     <row r="69" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>9</v>
       </c>
-      <c r="B69" s="47"/>
-      <c r="C69" s="132"/>
-      <c r="D69" s="132"/>
-      <c r="E69" s="132"/>
-      <c r="F69" s="132"/>
-      <c r="G69" s="132"/>
-      <c r="H69" s="132"/>
-      <c r="I69" s="132"/>
-      <c r="J69" s="132"/>
-      <c r="K69" s="132"/>
-      <c r="L69" s="132"/>
-      <c r="M69" s="132"/>
-      <c r="N69" s="132"/>
-      <c r="O69" s="132"/>
-      <c r="P69" s="132"/>
-      <c r="Q69" s="132"/>
-      <c r="R69" s="132"/>
-      <c r="S69" s="132"/>
-      <c r="T69" s="132"/>
-      <c r="U69" s="132"/>
-      <c r="V69" s="132"/>
-      <c r="W69" s="132"/>
-      <c r="X69" s="132"/>
-      <c r="Y69" s="132"/>
-      <c r="Z69" s="132"/>
-      <c r="AA69" s="132"/>
-      <c r="AB69" s="132"/>
-      <c r="AC69" s="132"/>
-      <c r="AD69" s="132"/>
-      <c r="AE69" s="132"/>
-      <c r="AF69" s="132"/>
-      <c r="AG69" s="132"/>
-      <c r="AH69" s="132"/>
-      <c r="AI69" s="132"/>
-      <c r="AJ69" s="132"/>
-      <c r="AK69" s="132"/>
-      <c r="AL69" s="132"/>
-      <c r="AM69" s="132"/>
-      <c r="AN69" s="132"/>
-      <c r="AO69" s="132"/>
-      <c r="AP69" s="132"/>
-      <c r="AQ69" s="132"/>
-      <c r="AR69" s="132"/>
-      <c r="AS69" s="132"/>
-      <c r="AT69" s="132"/>
-      <c r="AU69" s="132"/>
-      <c r="AV69" s="132"/>
-      <c r="AW69" s="132"/>
-      <c r="AX69" s="132"/>
-      <c r="AY69" s="132"/>
-      <c r="AZ69" s="132"/>
-      <c r="BA69" s="132"/>
-      <c r="BB69" s="132"/>
-      <c r="BC69" s="132"/>
-      <c r="BD69" s="132"/>
-      <c r="BE69" s="132"/>
-      <c r="BF69" s="132"/>
-      <c r="BG69" s="49"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="109"/>
+      <c r="D69" s="109"/>
+      <c r="E69" s="109"/>
+      <c r="F69" s="109"/>
+      <c r="G69" s="109"/>
+      <c r="H69" s="109"/>
+      <c r="I69" s="109"/>
+      <c r="J69" s="109"/>
+      <c r="K69" s="109"/>
+      <c r="L69" s="109"/>
+      <c r="M69" s="109"/>
+      <c r="N69" s="109"/>
+      <c r="O69" s="109"/>
+      <c r="P69" s="109"/>
+      <c r="Q69" s="109"/>
+      <c r="R69" s="109"/>
+      <c r="S69" s="109"/>
+      <c r="T69" s="109"/>
+      <c r="U69" s="109"/>
+      <c r="V69" s="109"/>
+      <c r="W69" s="109"/>
+      <c r="X69" s="109"/>
+      <c r="Y69" s="109"/>
+      <c r="Z69" s="109"/>
+      <c r="AA69" s="109"/>
+      <c r="AB69" s="109"/>
+      <c r="AC69" s="109"/>
+      <c r="AD69" s="109"/>
+      <c r="AE69" s="109"/>
+      <c r="AF69" s="109"/>
+      <c r="AG69" s="109"/>
+      <c r="AH69" s="109"/>
+      <c r="AI69" s="109"/>
+      <c r="AJ69" s="109"/>
+      <c r="AK69" s="109"/>
+      <c r="AL69" s="109"/>
+      <c r="AM69" s="109"/>
+      <c r="AN69" s="109"/>
+      <c r="AO69" s="109"/>
+      <c r="AP69" s="109"/>
+      <c r="AQ69" s="109"/>
+      <c r="AR69" s="109"/>
+      <c r="AS69" s="109"/>
+      <c r="AT69" s="109"/>
+      <c r="AU69" s="109"/>
+      <c r="AV69" s="109"/>
+      <c r="AW69" s="109"/>
+      <c r="AX69" s="109"/>
+      <c r="AY69" s="109"/>
+      <c r="AZ69" s="109"/>
+      <c r="BA69" s="109"/>
+      <c r="BB69" s="109"/>
+      <c r="BC69" s="109"/>
+      <c r="BD69" s="109"/>
+      <c r="BE69" s="109"/>
+      <c r="BF69" s="109"/>
+      <c r="BG69" s="110"/>
     </row>
     <row r="70" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>10</v>
       </c>
-      <c r="B70" s="47"/>
-      <c r="C70" s="132"/>
-      <c r="D70" s="132"/>
-      <c r="E70" s="132"/>
-      <c r="F70" s="132"/>
-      <c r="G70" s="132"/>
-      <c r="H70" s="132"/>
-      <c r="I70" s="132"/>
-      <c r="J70" s="132"/>
-      <c r="K70" s="132"/>
-      <c r="L70" s="132"/>
-      <c r="M70" s="132"/>
-      <c r="N70" s="132"/>
-      <c r="O70" s="132"/>
-      <c r="P70" s="132"/>
-      <c r="Q70" s="132"/>
-      <c r="R70" s="132"/>
-      <c r="S70" s="132"/>
-      <c r="T70" s="132"/>
-      <c r="U70" s="132"/>
-      <c r="V70" s="132"/>
-      <c r="W70" s="132"/>
-      <c r="X70" s="132"/>
-      <c r="Y70" s="132"/>
-      <c r="Z70" s="132"/>
-      <c r="AA70" s="132"/>
-      <c r="AB70" s="132"/>
-      <c r="AC70" s="132"/>
-      <c r="AD70" s="132"/>
-      <c r="AE70" s="132"/>
-      <c r="AF70" s="132"/>
-      <c r="AG70" s="132"/>
-      <c r="AH70" s="132"/>
-      <c r="AI70" s="132"/>
-      <c r="AJ70" s="132"/>
-      <c r="AK70" s="132"/>
-      <c r="AL70" s="132"/>
-      <c r="AM70" s="132"/>
-      <c r="AN70" s="132"/>
-      <c r="AO70" s="132"/>
-      <c r="AP70" s="132"/>
-      <c r="AQ70" s="132"/>
-      <c r="AR70" s="132"/>
-      <c r="AS70" s="132"/>
-      <c r="AT70" s="132"/>
-      <c r="AU70" s="132"/>
-      <c r="AV70" s="132"/>
-      <c r="AW70" s="132"/>
-      <c r="AX70" s="132"/>
-      <c r="AY70" s="132"/>
-      <c r="AZ70" s="132"/>
-      <c r="BA70" s="132"/>
-      <c r="BB70" s="132"/>
-      <c r="BC70" s="132"/>
-      <c r="BD70" s="132"/>
-      <c r="BE70" s="132"/>
-      <c r="BF70" s="132"/>
-      <c r="BG70" s="49"/>
+      <c r="B70" s="108"/>
+      <c r="C70" s="109"/>
+      <c r="D70" s="109"/>
+      <c r="E70" s="109"/>
+      <c r="F70" s="109"/>
+      <c r="G70" s="109"/>
+      <c r="H70" s="109"/>
+      <c r="I70" s="109"/>
+      <c r="J70" s="109"/>
+      <c r="K70" s="109"/>
+      <c r="L70" s="109"/>
+      <c r="M70" s="109"/>
+      <c r="N70" s="109"/>
+      <c r="O70" s="109"/>
+      <c r="P70" s="109"/>
+      <c r="Q70" s="109"/>
+      <c r="R70" s="109"/>
+      <c r="S70" s="109"/>
+      <c r="T70" s="109"/>
+      <c r="U70" s="109"/>
+      <c r="V70" s="109"/>
+      <c r="W70" s="109"/>
+      <c r="X70" s="109"/>
+      <c r="Y70" s="109"/>
+      <c r="Z70" s="109"/>
+      <c r="AA70" s="109"/>
+      <c r="AB70" s="109"/>
+      <c r="AC70" s="109"/>
+      <c r="AD70" s="109"/>
+      <c r="AE70" s="109"/>
+      <c r="AF70" s="109"/>
+      <c r="AG70" s="109"/>
+      <c r="AH70" s="109"/>
+      <c r="AI70" s="109"/>
+      <c r="AJ70" s="109"/>
+      <c r="AK70" s="109"/>
+      <c r="AL70" s="109"/>
+      <c r="AM70" s="109"/>
+      <c r="AN70" s="109"/>
+      <c r="AO70" s="109"/>
+      <c r="AP70" s="109"/>
+      <c r="AQ70" s="109"/>
+      <c r="AR70" s="109"/>
+      <c r="AS70" s="109"/>
+      <c r="AT70" s="109"/>
+      <c r="AU70" s="109"/>
+      <c r="AV70" s="109"/>
+      <c r="AW70" s="109"/>
+      <c r="AX70" s="109"/>
+      <c r="AY70" s="109"/>
+      <c r="AZ70" s="109"/>
+      <c r="BA70" s="109"/>
+      <c r="BB70" s="109"/>
+      <c r="BC70" s="109"/>
+      <c r="BD70" s="109"/>
+      <c r="BE70" s="109"/>
+      <c r="BF70" s="109"/>
+      <c r="BG70" s="110"/>
     </row>
     <row r="71" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>11</v>
       </c>
-      <c r="B71" s="50"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="51"/>
-      <c r="E71" s="51"/>
-      <c r="F71" s="51"/>
-      <c r="G71" s="51"/>
-      <c r="H71" s="51"/>
-      <c r="I71" s="51"/>
-      <c r="J71" s="51"/>
-      <c r="K71" s="51"/>
-      <c r="L71" s="51"/>
-      <c r="M71" s="51"/>
-      <c r="N71" s="51"/>
-      <c r="O71" s="51"/>
-      <c r="P71" s="51"/>
-      <c r="Q71" s="51"/>
-      <c r="R71" s="51"/>
-      <c r="S71" s="51"/>
-      <c r="T71" s="51"/>
-      <c r="U71" s="51"/>
-      <c r="V71" s="51"/>
-      <c r="W71" s="51"/>
-      <c r="X71" s="51"/>
-      <c r="Y71" s="51"/>
-      <c r="Z71" s="51"/>
-      <c r="AA71" s="51"/>
-      <c r="AB71" s="51"/>
-      <c r="AC71" s="51"/>
-      <c r="AD71" s="51"/>
-      <c r="AE71" s="51"/>
-      <c r="AF71" s="51"/>
-      <c r="AG71" s="51"/>
-      <c r="AH71" s="51"/>
-      <c r="AI71" s="51"/>
-      <c r="AJ71" s="51"/>
-      <c r="AK71" s="51"/>
-      <c r="AL71" s="51"/>
-      <c r="AM71" s="51"/>
-      <c r="AN71" s="51"/>
-      <c r="AO71" s="51"/>
-      <c r="AP71" s="51"/>
-      <c r="AQ71" s="51"/>
-      <c r="AR71" s="51"/>
-      <c r="AS71" s="51"/>
-      <c r="AT71" s="51"/>
-      <c r="AU71" s="51"/>
-      <c r="AV71" s="51"/>
-      <c r="AW71" s="51"/>
-      <c r="AX71" s="51"/>
-      <c r="AY71" s="51"/>
-      <c r="AZ71" s="51"/>
-      <c r="BA71" s="51"/>
-      <c r="BB71" s="51"/>
-      <c r="BC71" s="51"/>
-      <c r="BD71" s="51"/>
-      <c r="BE71" s="51"/>
-      <c r="BF71" s="51"/>
-      <c r="BG71" s="52"/>
+      <c r="B71" s="111"/>
+      <c r="C71" s="112"/>
+      <c r="D71" s="112"/>
+      <c r="E71" s="112"/>
+      <c r="F71" s="112"/>
+      <c r="G71" s="112"/>
+      <c r="H71" s="112"/>
+      <c r="I71" s="112"/>
+      <c r="J71" s="112"/>
+      <c r="K71" s="112"/>
+      <c r="L71" s="112"/>
+      <c r="M71" s="112"/>
+      <c r="N71" s="112"/>
+      <c r="O71" s="112"/>
+      <c r="P71" s="112"/>
+      <c r="Q71" s="112"/>
+      <c r="R71" s="112"/>
+      <c r="S71" s="112"/>
+      <c r="T71" s="112"/>
+      <c r="U71" s="112"/>
+      <c r="V71" s="112"/>
+      <c r="W71" s="112"/>
+      <c r="X71" s="112"/>
+      <c r="Y71" s="112"/>
+      <c r="Z71" s="112"/>
+      <c r="AA71" s="112"/>
+      <c r="AB71" s="112"/>
+      <c r="AC71" s="112"/>
+      <c r="AD71" s="112"/>
+      <c r="AE71" s="112"/>
+      <c r="AF71" s="112"/>
+      <c r="AG71" s="112"/>
+      <c r="AH71" s="112"/>
+      <c r="AI71" s="112"/>
+      <c r="AJ71" s="112"/>
+      <c r="AK71" s="112"/>
+      <c r="AL71" s="112"/>
+      <c r="AM71" s="112"/>
+      <c r="AN71" s="112"/>
+      <c r="AO71" s="112"/>
+      <c r="AP71" s="112"/>
+      <c r="AQ71" s="112"/>
+      <c r="AR71" s="112"/>
+      <c r="AS71" s="112"/>
+      <c r="AT71" s="112"/>
+      <c r="AU71" s="112"/>
+      <c r="AV71" s="112"/>
+      <c r="AW71" s="112"/>
+      <c r="AX71" s="112"/>
+      <c r="AY71" s="112"/>
+      <c r="AZ71" s="112"/>
+      <c r="BA71" s="112"/>
+      <c r="BB71" s="112"/>
+      <c r="BC71" s="112"/>
+      <c r="BD71" s="112"/>
+      <c r="BE71" s="112"/>
+      <c r="BF71" s="112"/>
+      <c r="BG71" s="113"/>
     </row>
     <row r="72" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A72" s="2">

</xml_diff>

<commit_message>
Can now perform encoder 1's QKV
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0868CA2-8AC1-2543-9090-1F3A7DD43250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21884B7B-00DC-074C-8359-416FDAA67868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>CiM PARAMETERS MEMORY MAP</t>
   </si>
@@ -176,7 +176,16 @@
     <t>enc0_layernorm_out[id][:]</t>
   </si>
   <si>
-    <t>enc0_layernorm_out[:][id]</t>
+    <t>res_Q[:][id]</t>
+  </si>
+  <si>
+    <t>res_K[:][id]</t>
+  </si>
+  <si>
+    <t>res_V[:][id]</t>
+  </si>
+  <si>
+    <t>temp_QKV_input_row</t>
   </si>
 </sst>
 </file>
@@ -222,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,12 +295,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -761,57 +764,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -824,6 +776,9 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -842,9 +797,16 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
-  <dimension ref="A1:BP75"/>
+  <dimension ref="A1:BP84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:BG71"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BL85" sqref="BL85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5003,11 +4965,11 @@
       <c r="BH60" s="45"/>
       <c r="BI60" s="45"/>
       <c r="BJ60" s="46"/>
-      <c r="BK60" s="122" t="s">
+      <c r="BK60" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="BL60" s="123"/>
-      <c r="BM60" s="124"/>
+      <c r="BL60" s="106"/>
+      <c r="BM60" s="107"/>
       <c r="BO60" s="10" t="s">
         <v>42</v>
       </c>
@@ -5077,9 +5039,9 @@
       <c r="BH61" s="48"/>
       <c r="BI61" s="48"/>
       <c r="BJ61" s="49"/>
-      <c r="BK61" s="125"/>
-      <c r="BL61" s="131"/>
-      <c r="BM61" s="126"/>
+      <c r="BK61" s="108"/>
+      <c r="BL61" s="115"/>
+      <c r="BM61" s="110"/>
       <c r="BO61" s="10" t="s">
         <v>43</v>
       </c>
@@ -5149,9 +5111,9 @@
       <c r="BH62" s="48"/>
       <c r="BI62" s="48"/>
       <c r="BJ62" s="49"/>
-      <c r="BK62" s="125"/>
-      <c r="BL62" s="131"/>
-      <c r="BM62" s="126"/>
+      <c r="BK62" s="108"/>
+      <c r="BL62" s="115"/>
+      <c r="BM62" s="110"/>
     </row>
     <row r="63" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -5218,9 +5180,9 @@
       <c r="BH63" s="51"/>
       <c r="BI63" s="51"/>
       <c r="BJ63" s="52"/>
-      <c r="BK63" s="127"/>
-      <c r="BL63" s="128"/>
-      <c r="BM63" s="129"/>
+      <c r="BK63" s="111"/>
+      <c r="BL63" s="112"/>
+      <c r="BM63" s="113"/>
     </row>
     <row r="64" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
@@ -5289,149 +5251,149 @@
       <c r="BH64" s="45"/>
       <c r="BI64" s="45"/>
       <c r="BJ64" s="46"/>
-      <c r="BK64" s="114" t="s">
-        <v>46</v>
-      </c>
-      <c r="BL64" s="115"/>
-      <c r="BM64" s="116"/>
+      <c r="BK64" s="105" t="s">
+        <v>49</v>
+      </c>
+      <c r="BL64" s="106"/>
+      <c r="BM64" s="107"/>
     </row>
     <row r="65" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>5</v>
       </c>
       <c r="B65" s="47"/>
-      <c r="C65" s="130"/>
-      <c r="D65" s="130"/>
-      <c r="E65" s="130"/>
-      <c r="F65" s="130"/>
-      <c r="G65" s="130"/>
-      <c r="H65" s="130"/>
-      <c r="I65" s="130"/>
-      <c r="J65" s="130"/>
-      <c r="K65" s="130"/>
-      <c r="L65" s="130"/>
-      <c r="M65" s="130"/>
-      <c r="N65" s="130"/>
-      <c r="O65" s="130"/>
-      <c r="P65" s="130"/>
-      <c r="Q65" s="130"/>
-      <c r="R65" s="130"/>
-      <c r="S65" s="130"/>
-      <c r="T65" s="130"/>
-      <c r="U65" s="130"/>
-      <c r="V65" s="130"/>
-      <c r="W65" s="130"/>
-      <c r="X65" s="130"/>
-      <c r="Y65" s="130"/>
-      <c r="Z65" s="130"/>
-      <c r="AA65" s="130"/>
-      <c r="AB65" s="130"/>
-      <c r="AC65" s="130"/>
-      <c r="AD65" s="130"/>
-      <c r="AE65" s="130"/>
-      <c r="AF65" s="130"/>
-      <c r="AG65" s="130"/>
-      <c r="AH65" s="130"/>
-      <c r="AI65" s="130"/>
-      <c r="AJ65" s="130"/>
-      <c r="AK65" s="130"/>
-      <c r="AL65" s="130"/>
-      <c r="AM65" s="130"/>
-      <c r="AN65" s="130"/>
-      <c r="AO65" s="130"/>
-      <c r="AP65" s="130"/>
-      <c r="AQ65" s="130"/>
-      <c r="AR65" s="130"/>
-      <c r="AS65" s="130"/>
-      <c r="AT65" s="130"/>
-      <c r="AU65" s="130"/>
-      <c r="AV65" s="130"/>
-      <c r="AW65" s="130"/>
-      <c r="AX65" s="130"/>
-      <c r="AY65" s="130"/>
-      <c r="AZ65" s="130"/>
-      <c r="BA65" s="130"/>
-      <c r="BB65" s="130"/>
-      <c r="BC65" s="130"/>
-      <c r="BD65" s="130"/>
-      <c r="BE65" s="130"/>
-      <c r="BF65" s="130"/>
-      <c r="BG65" s="130"/>
-      <c r="BH65" s="130"/>
-      <c r="BI65" s="130"/>
+      <c r="C65" s="114"/>
+      <c r="D65" s="114"/>
+      <c r="E65" s="114"/>
+      <c r="F65" s="114"/>
+      <c r="G65" s="114"/>
+      <c r="H65" s="114"/>
+      <c r="I65" s="114"/>
+      <c r="J65" s="114"/>
+      <c r="K65" s="114"/>
+      <c r="L65" s="114"/>
+      <c r="M65" s="114"/>
+      <c r="N65" s="114"/>
+      <c r="O65" s="114"/>
+      <c r="P65" s="114"/>
+      <c r="Q65" s="114"/>
+      <c r="R65" s="114"/>
+      <c r="S65" s="114"/>
+      <c r="T65" s="114"/>
+      <c r="U65" s="114"/>
+      <c r="V65" s="114"/>
+      <c r="W65" s="114"/>
+      <c r="X65" s="114"/>
+      <c r="Y65" s="114"/>
+      <c r="Z65" s="114"/>
+      <c r="AA65" s="114"/>
+      <c r="AB65" s="114"/>
+      <c r="AC65" s="114"/>
+      <c r="AD65" s="114"/>
+      <c r="AE65" s="114"/>
+      <c r="AF65" s="114"/>
+      <c r="AG65" s="114"/>
+      <c r="AH65" s="114"/>
+      <c r="AI65" s="114"/>
+      <c r="AJ65" s="114"/>
+      <c r="AK65" s="114"/>
+      <c r="AL65" s="114"/>
+      <c r="AM65" s="114"/>
+      <c r="AN65" s="114"/>
+      <c r="AO65" s="114"/>
+      <c r="AP65" s="114"/>
+      <c r="AQ65" s="114"/>
+      <c r="AR65" s="114"/>
+      <c r="AS65" s="114"/>
+      <c r="AT65" s="114"/>
+      <c r="AU65" s="114"/>
+      <c r="AV65" s="114"/>
+      <c r="AW65" s="114"/>
+      <c r="AX65" s="114"/>
+      <c r="AY65" s="114"/>
+      <c r="AZ65" s="114"/>
+      <c r="BA65" s="114"/>
+      <c r="BB65" s="114"/>
+      <c r="BC65" s="114"/>
+      <c r="BD65" s="114"/>
+      <c r="BE65" s="114"/>
+      <c r="BF65" s="114"/>
+      <c r="BG65" s="114"/>
+      <c r="BH65" s="114"/>
+      <c r="BI65" s="114"/>
       <c r="BJ65" s="49"/>
-      <c r="BK65" s="117"/>
-      <c r="BL65" s="132"/>
-      <c r="BM65" s="118"/>
+      <c r="BK65" s="108"/>
+      <c r="BL65" s="109"/>
+      <c r="BM65" s="110"/>
     </row>
     <row r="66" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>6</v>
       </c>
       <c r="B66" s="47"/>
-      <c r="C66" s="130"/>
-      <c r="D66" s="130"/>
-      <c r="E66" s="130"/>
-      <c r="F66" s="130"/>
-      <c r="G66" s="130"/>
-      <c r="H66" s="130"/>
-      <c r="I66" s="130"/>
-      <c r="J66" s="130"/>
-      <c r="K66" s="130"/>
-      <c r="L66" s="130"/>
-      <c r="M66" s="130"/>
-      <c r="N66" s="130"/>
-      <c r="O66" s="130"/>
-      <c r="P66" s="130"/>
-      <c r="Q66" s="130"/>
-      <c r="R66" s="130"/>
-      <c r="S66" s="130"/>
-      <c r="T66" s="130"/>
-      <c r="U66" s="130"/>
-      <c r="V66" s="130"/>
-      <c r="W66" s="130"/>
-      <c r="X66" s="130"/>
-      <c r="Y66" s="130"/>
-      <c r="Z66" s="130"/>
-      <c r="AA66" s="130"/>
-      <c r="AB66" s="130"/>
-      <c r="AC66" s="130"/>
-      <c r="AD66" s="130"/>
-      <c r="AE66" s="130"/>
-      <c r="AF66" s="130"/>
-      <c r="AG66" s="130"/>
-      <c r="AH66" s="130"/>
-      <c r="AI66" s="130"/>
-      <c r="AJ66" s="130"/>
-      <c r="AK66" s="130"/>
-      <c r="AL66" s="130"/>
-      <c r="AM66" s="130"/>
-      <c r="AN66" s="130"/>
-      <c r="AO66" s="130"/>
-      <c r="AP66" s="130"/>
-      <c r="AQ66" s="130"/>
-      <c r="AR66" s="130"/>
-      <c r="AS66" s="130"/>
-      <c r="AT66" s="130"/>
-      <c r="AU66" s="130"/>
-      <c r="AV66" s="130"/>
-      <c r="AW66" s="130"/>
-      <c r="AX66" s="130"/>
-      <c r="AY66" s="130"/>
-      <c r="AZ66" s="130"/>
-      <c r="BA66" s="130"/>
-      <c r="BB66" s="130"/>
-      <c r="BC66" s="130"/>
-      <c r="BD66" s="130"/>
-      <c r="BE66" s="130"/>
-      <c r="BF66" s="130"/>
-      <c r="BG66" s="130"/>
-      <c r="BH66" s="130"/>
-      <c r="BI66" s="130"/>
+      <c r="C66" s="114"/>
+      <c r="D66" s="114"/>
+      <c r="E66" s="114"/>
+      <c r="F66" s="114"/>
+      <c r="G66" s="114"/>
+      <c r="H66" s="114"/>
+      <c r="I66" s="114"/>
+      <c r="J66" s="114"/>
+      <c r="K66" s="114"/>
+      <c r="L66" s="114"/>
+      <c r="M66" s="114"/>
+      <c r="N66" s="114"/>
+      <c r="O66" s="114"/>
+      <c r="P66" s="114"/>
+      <c r="Q66" s="114"/>
+      <c r="R66" s="114"/>
+      <c r="S66" s="114"/>
+      <c r="T66" s="114"/>
+      <c r="U66" s="114"/>
+      <c r="V66" s="114"/>
+      <c r="W66" s="114"/>
+      <c r="X66" s="114"/>
+      <c r="Y66" s="114"/>
+      <c r="Z66" s="114"/>
+      <c r="AA66" s="114"/>
+      <c r="AB66" s="114"/>
+      <c r="AC66" s="114"/>
+      <c r="AD66" s="114"/>
+      <c r="AE66" s="114"/>
+      <c r="AF66" s="114"/>
+      <c r="AG66" s="114"/>
+      <c r="AH66" s="114"/>
+      <c r="AI66" s="114"/>
+      <c r="AJ66" s="114"/>
+      <c r="AK66" s="114"/>
+      <c r="AL66" s="114"/>
+      <c r="AM66" s="114"/>
+      <c r="AN66" s="114"/>
+      <c r="AO66" s="114"/>
+      <c r="AP66" s="114"/>
+      <c r="AQ66" s="114"/>
+      <c r="AR66" s="114"/>
+      <c r="AS66" s="114"/>
+      <c r="AT66" s="114"/>
+      <c r="AU66" s="114"/>
+      <c r="AV66" s="114"/>
+      <c r="AW66" s="114"/>
+      <c r="AX66" s="114"/>
+      <c r="AY66" s="114"/>
+      <c r="AZ66" s="114"/>
+      <c r="BA66" s="114"/>
+      <c r="BB66" s="114"/>
+      <c r="BC66" s="114"/>
+      <c r="BD66" s="114"/>
+      <c r="BE66" s="114"/>
+      <c r="BF66" s="114"/>
+      <c r="BG66" s="114"/>
+      <c r="BH66" s="114"/>
+      <c r="BI66" s="114"/>
       <c r="BJ66" s="49"/>
-      <c r="BK66" s="117"/>
-      <c r="BL66" s="132"/>
-      <c r="BM66" s="118"/>
+      <c r="BK66" s="108"/>
+      <c r="BL66" s="109"/>
+      <c r="BM66" s="110"/>
     </row>
     <row r="67" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -5498,287 +5460,1140 @@
       <c r="BH67" s="51"/>
       <c r="BI67" s="51"/>
       <c r="BJ67" s="52"/>
-      <c r="BK67" s="119"/>
-      <c r="BL67" s="120"/>
-      <c r="BM67" s="121"/>
-    </row>
-    <row r="68" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="BK67" s="111"/>
+      <c r="BL67" s="112"/>
+      <c r="BM67" s="113"/>
+    </row>
+    <row r="68" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>8</v>
       </c>
-      <c r="B68" s="105" t="s">
+      <c r="B68" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" s="45"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="45"/>
+      <c r="G68" s="45"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="45"/>
+      <c r="J68" s="45"/>
+      <c r="K68" s="45"/>
+      <c r="L68" s="45"/>
+      <c r="M68" s="45"/>
+      <c r="N68" s="45"/>
+      <c r="O68" s="45"/>
+      <c r="P68" s="45"/>
+      <c r="Q68" s="45"/>
+      <c r="R68" s="45"/>
+      <c r="S68" s="45"/>
+      <c r="T68" s="45"/>
+      <c r="U68" s="45"/>
+      <c r="V68" s="45"/>
+      <c r="W68" s="45"/>
+      <c r="X68" s="45"/>
+      <c r="Y68" s="45"/>
+      <c r="Z68" s="45"/>
+      <c r="AA68" s="45"/>
+      <c r="AB68" s="45"/>
+      <c r="AC68" s="45"/>
+      <c r="AD68" s="45"/>
+      <c r="AE68" s="45"/>
+      <c r="AF68" s="45"/>
+      <c r="AG68" s="45"/>
+      <c r="AH68" s="45"/>
+      <c r="AI68" s="45"/>
+      <c r="AJ68" s="45"/>
+      <c r="AK68" s="45"/>
+      <c r="AL68" s="45"/>
+      <c r="AM68" s="45"/>
+      <c r="AN68" s="45"/>
+      <c r="AO68" s="45"/>
+      <c r="AP68" s="45"/>
+      <c r="AQ68" s="45"/>
+      <c r="AR68" s="45"/>
+      <c r="AS68" s="45"/>
+      <c r="AT68" s="45"/>
+      <c r="AU68" s="45"/>
+      <c r="AV68" s="45"/>
+      <c r="AW68" s="45"/>
+      <c r="AX68" s="45"/>
+      <c r="AY68" s="45"/>
+      <c r="AZ68" s="45"/>
+      <c r="BA68" s="45"/>
+      <c r="BB68" s="45"/>
+      <c r="BC68" s="45"/>
+      <c r="BD68" s="45"/>
+      <c r="BE68" s="45"/>
+      <c r="BF68" s="45"/>
+      <c r="BG68" s="45"/>
+      <c r="BH68" s="45"/>
+      <c r="BI68" s="45"/>
+      <c r="BJ68" s="46"/>
+      <c r="BK68" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C68" s="106"/>
-      <c r="D68" s="106"/>
-      <c r="E68" s="106"/>
-      <c r="F68" s="106"/>
-      <c r="G68" s="106"/>
-      <c r="H68" s="106"/>
-      <c r="I68" s="106"/>
-      <c r="J68" s="106"/>
-      <c r="K68" s="106"/>
-      <c r="L68" s="106"/>
-      <c r="M68" s="106"/>
-      <c r="N68" s="106"/>
-      <c r="O68" s="106"/>
-      <c r="P68" s="106"/>
-      <c r="Q68" s="106"/>
-      <c r="R68" s="106"/>
-      <c r="S68" s="106"/>
-      <c r="T68" s="106"/>
-      <c r="U68" s="106"/>
-      <c r="V68" s="106"/>
-      <c r="W68" s="106"/>
-      <c r="X68" s="106"/>
-      <c r="Y68" s="106"/>
-      <c r="Z68" s="106"/>
-      <c r="AA68" s="106"/>
-      <c r="AB68" s="106"/>
-      <c r="AC68" s="106"/>
-      <c r="AD68" s="106"/>
-      <c r="AE68" s="106"/>
-      <c r="AF68" s="106"/>
-      <c r="AG68" s="106"/>
-      <c r="AH68" s="106"/>
-      <c r="AI68" s="106"/>
-      <c r="AJ68" s="106"/>
-      <c r="AK68" s="106"/>
-      <c r="AL68" s="106"/>
-      <c r="AM68" s="106"/>
-      <c r="AN68" s="106"/>
-      <c r="AO68" s="106"/>
-      <c r="AP68" s="106"/>
-      <c r="AQ68" s="106"/>
-      <c r="AR68" s="106"/>
-      <c r="AS68" s="106"/>
-      <c r="AT68" s="106"/>
-      <c r="AU68" s="106"/>
-      <c r="AV68" s="106"/>
-      <c r="AW68" s="106"/>
-      <c r="AX68" s="106"/>
-      <c r="AY68" s="106"/>
-      <c r="AZ68" s="106"/>
-      <c r="BA68" s="106"/>
-      <c r="BB68" s="106"/>
-      <c r="BC68" s="106"/>
-      <c r="BD68" s="106"/>
-      <c r="BE68" s="106"/>
-      <c r="BF68" s="106"/>
-      <c r="BG68" s="107"/>
+      <c r="BL68" s="106"/>
+      <c r="BM68" s="107"/>
     </row>
     <row r="69" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>9</v>
       </c>
-      <c r="B69" s="108"/>
-      <c r="C69" s="109"/>
-      <c r="D69" s="109"/>
-      <c r="E69" s="109"/>
-      <c r="F69" s="109"/>
-      <c r="G69" s="109"/>
-      <c r="H69" s="109"/>
-      <c r="I69" s="109"/>
-      <c r="J69" s="109"/>
-      <c r="K69" s="109"/>
-      <c r="L69" s="109"/>
-      <c r="M69" s="109"/>
-      <c r="N69" s="109"/>
-      <c r="O69" s="109"/>
-      <c r="P69" s="109"/>
-      <c r="Q69" s="109"/>
-      <c r="R69" s="109"/>
-      <c r="S69" s="109"/>
-      <c r="T69" s="109"/>
-      <c r="U69" s="109"/>
-      <c r="V69" s="109"/>
-      <c r="W69" s="109"/>
-      <c r="X69" s="109"/>
-      <c r="Y69" s="109"/>
-      <c r="Z69" s="109"/>
-      <c r="AA69" s="109"/>
-      <c r="AB69" s="109"/>
-      <c r="AC69" s="109"/>
-      <c r="AD69" s="109"/>
-      <c r="AE69" s="109"/>
-      <c r="AF69" s="109"/>
-      <c r="AG69" s="109"/>
-      <c r="AH69" s="109"/>
-      <c r="AI69" s="109"/>
-      <c r="AJ69" s="109"/>
-      <c r="AK69" s="109"/>
-      <c r="AL69" s="109"/>
-      <c r="AM69" s="109"/>
-      <c r="AN69" s="109"/>
-      <c r="AO69" s="109"/>
-      <c r="AP69" s="109"/>
-      <c r="AQ69" s="109"/>
-      <c r="AR69" s="109"/>
-      <c r="AS69" s="109"/>
-      <c r="AT69" s="109"/>
-      <c r="AU69" s="109"/>
-      <c r="AV69" s="109"/>
-      <c r="AW69" s="109"/>
-      <c r="AX69" s="109"/>
-      <c r="AY69" s="109"/>
-      <c r="AZ69" s="109"/>
-      <c r="BA69" s="109"/>
-      <c r="BB69" s="109"/>
-      <c r="BC69" s="109"/>
-      <c r="BD69" s="109"/>
-      <c r="BE69" s="109"/>
-      <c r="BF69" s="109"/>
-      <c r="BG69" s="110"/>
+      <c r="B69" s="47"/>
+      <c r="C69" s="114"/>
+      <c r="D69" s="114"/>
+      <c r="E69" s="114"/>
+      <c r="F69" s="114"/>
+      <c r="G69" s="114"/>
+      <c r="H69" s="114"/>
+      <c r="I69" s="114"/>
+      <c r="J69" s="114"/>
+      <c r="K69" s="114"/>
+      <c r="L69" s="114"/>
+      <c r="M69" s="114"/>
+      <c r="N69" s="114"/>
+      <c r="O69" s="114"/>
+      <c r="P69" s="114"/>
+      <c r="Q69" s="114"/>
+      <c r="R69" s="114"/>
+      <c r="S69" s="114"/>
+      <c r="T69" s="114"/>
+      <c r="U69" s="114"/>
+      <c r="V69" s="114"/>
+      <c r="W69" s="114"/>
+      <c r="X69" s="114"/>
+      <c r="Y69" s="114"/>
+      <c r="Z69" s="114"/>
+      <c r="AA69" s="114"/>
+      <c r="AB69" s="114"/>
+      <c r="AC69" s="114"/>
+      <c r="AD69" s="114"/>
+      <c r="AE69" s="114"/>
+      <c r="AF69" s="114"/>
+      <c r="AG69" s="114"/>
+      <c r="AH69" s="114"/>
+      <c r="AI69" s="114"/>
+      <c r="AJ69" s="114"/>
+      <c r="AK69" s="114"/>
+      <c r="AL69" s="114"/>
+      <c r="AM69" s="114"/>
+      <c r="AN69" s="114"/>
+      <c r="AO69" s="114"/>
+      <c r="AP69" s="114"/>
+      <c r="AQ69" s="114"/>
+      <c r="AR69" s="114"/>
+      <c r="AS69" s="114"/>
+      <c r="AT69" s="114"/>
+      <c r="AU69" s="114"/>
+      <c r="AV69" s="114"/>
+      <c r="AW69" s="114"/>
+      <c r="AX69" s="114"/>
+      <c r="AY69" s="114"/>
+      <c r="AZ69" s="114"/>
+      <c r="BA69" s="114"/>
+      <c r="BB69" s="114"/>
+      <c r="BC69" s="114"/>
+      <c r="BD69" s="114"/>
+      <c r="BE69" s="114"/>
+      <c r="BF69" s="114"/>
+      <c r="BG69" s="114"/>
+      <c r="BH69" s="114"/>
+      <c r="BI69" s="114"/>
+      <c r="BJ69" s="49"/>
+      <c r="BK69" s="108"/>
+      <c r="BL69" s="109"/>
+      <c r="BM69" s="110"/>
     </row>
     <row r="70" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>10</v>
       </c>
-      <c r="B70" s="108"/>
-      <c r="C70" s="109"/>
-      <c r="D70" s="109"/>
-      <c r="E70" s="109"/>
-      <c r="F70" s="109"/>
-      <c r="G70" s="109"/>
-      <c r="H70" s="109"/>
-      <c r="I70" s="109"/>
-      <c r="J70" s="109"/>
-      <c r="K70" s="109"/>
-      <c r="L70" s="109"/>
-      <c r="M70" s="109"/>
-      <c r="N70" s="109"/>
-      <c r="O70" s="109"/>
-      <c r="P70" s="109"/>
-      <c r="Q70" s="109"/>
-      <c r="R70" s="109"/>
-      <c r="S70" s="109"/>
-      <c r="T70" s="109"/>
-      <c r="U70" s="109"/>
-      <c r="V70" s="109"/>
-      <c r="W70" s="109"/>
-      <c r="X70" s="109"/>
-      <c r="Y70" s="109"/>
-      <c r="Z70" s="109"/>
-      <c r="AA70" s="109"/>
-      <c r="AB70" s="109"/>
-      <c r="AC70" s="109"/>
-      <c r="AD70" s="109"/>
-      <c r="AE70" s="109"/>
-      <c r="AF70" s="109"/>
-      <c r="AG70" s="109"/>
-      <c r="AH70" s="109"/>
-      <c r="AI70" s="109"/>
-      <c r="AJ70" s="109"/>
-      <c r="AK70" s="109"/>
-      <c r="AL70" s="109"/>
-      <c r="AM70" s="109"/>
-      <c r="AN70" s="109"/>
-      <c r="AO70" s="109"/>
-      <c r="AP70" s="109"/>
-      <c r="AQ70" s="109"/>
-      <c r="AR70" s="109"/>
-      <c r="AS70" s="109"/>
-      <c r="AT70" s="109"/>
-      <c r="AU70" s="109"/>
-      <c r="AV70" s="109"/>
-      <c r="AW70" s="109"/>
-      <c r="AX70" s="109"/>
-      <c r="AY70" s="109"/>
-      <c r="AZ70" s="109"/>
-      <c r="BA70" s="109"/>
-      <c r="BB70" s="109"/>
-      <c r="BC70" s="109"/>
-      <c r="BD70" s="109"/>
-      <c r="BE70" s="109"/>
-      <c r="BF70" s="109"/>
-      <c r="BG70" s="110"/>
+      <c r="B70" s="47"/>
+      <c r="C70" s="114"/>
+      <c r="D70" s="114"/>
+      <c r="E70" s="114"/>
+      <c r="F70" s="114"/>
+      <c r="G70" s="114"/>
+      <c r="H70" s="114"/>
+      <c r="I70" s="114"/>
+      <c r="J70" s="114"/>
+      <c r="K70" s="114"/>
+      <c r="L70" s="114"/>
+      <c r="M70" s="114"/>
+      <c r="N70" s="114"/>
+      <c r="O70" s="114"/>
+      <c r="P70" s="114"/>
+      <c r="Q70" s="114"/>
+      <c r="R70" s="114"/>
+      <c r="S70" s="114"/>
+      <c r="T70" s="114"/>
+      <c r="U70" s="114"/>
+      <c r="V70" s="114"/>
+      <c r="W70" s="114"/>
+      <c r="X70" s="114"/>
+      <c r="Y70" s="114"/>
+      <c r="Z70" s="114"/>
+      <c r="AA70" s="114"/>
+      <c r="AB70" s="114"/>
+      <c r="AC70" s="114"/>
+      <c r="AD70" s="114"/>
+      <c r="AE70" s="114"/>
+      <c r="AF70" s="114"/>
+      <c r="AG70" s="114"/>
+      <c r="AH70" s="114"/>
+      <c r="AI70" s="114"/>
+      <c r="AJ70" s="114"/>
+      <c r="AK70" s="114"/>
+      <c r="AL70" s="114"/>
+      <c r="AM70" s="114"/>
+      <c r="AN70" s="114"/>
+      <c r="AO70" s="114"/>
+      <c r="AP70" s="114"/>
+      <c r="AQ70" s="114"/>
+      <c r="AR70" s="114"/>
+      <c r="AS70" s="114"/>
+      <c r="AT70" s="114"/>
+      <c r="AU70" s="114"/>
+      <c r="AV70" s="114"/>
+      <c r="AW70" s="114"/>
+      <c r="AX70" s="114"/>
+      <c r="AY70" s="114"/>
+      <c r="AZ70" s="114"/>
+      <c r="BA70" s="114"/>
+      <c r="BB70" s="114"/>
+      <c r="BC70" s="114"/>
+      <c r="BD70" s="114"/>
+      <c r="BE70" s="114"/>
+      <c r="BF70" s="114"/>
+      <c r="BG70" s="114"/>
+      <c r="BH70" s="114"/>
+      <c r="BI70" s="114"/>
+      <c r="BJ70" s="49"/>
+      <c r="BK70" s="108"/>
+      <c r="BL70" s="109"/>
+      <c r="BM70" s="110"/>
     </row>
     <row r="71" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>11</v>
       </c>
-      <c r="B71" s="111"/>
-      <c r="C71" s="112"/>
-      <c r="D71" s="112"/>
-      <c r="E71" s="112"/>
-      <c r="F71" s="112"/>
-      <c r="G71" s="112"/>
-      <c r="H71" s="112"/>
-      <c r="I71" s="112"/>
-      <c r="J71" s="112"/>
-      <c r="K71" s="112"/>
-      <c r="L71" s="112"/>
-      <c r="M71" s="112"/>
-      <c r="N71" s="112"/>
-      <c r="O71" s="112"/>
-      <c r="P71" s="112"/>
-      <c r="Q71" s="112"/>
-      <c r="R71" s="112"/>
-      <c r="S71" s="112"/>
-      <c r="T71" s="112"/>
-      <c r="U71" s="112"/>
-      <c r="V71" s="112"/>
-      <c r="W71" s="112"/>
-      <c r="X71" s="112"/>
-      <c r="Y71" s="112"/>
-      <c r="Z71" s="112"/>
-      <c r="AA71" s="112"/>
-      <c r="AB71" s="112"/>
-      <c r="AC71" s="112"/>
-      <c r="AD71" s="112"/>
-      <c r="AE71" s="112"/>
-      <c r="AF71" s="112"/>
-      <c r="AG71" s="112"/>
-      <c r="AH71" s="112"/>
-      <c r="AI71" s="112"/>
-      <c r="AJ71" s="112"/>
-      <c r="AK71" s="112"/>
-      <c r="AL71" s="112"/>
-      <c r="AM71" s="112"/>
-      <c r="AN71" s="112"/>
-      <c r="AO71" s="112"/>
-      <c r="AP71" s="112"/>
-      <c r="AQ71" s="112"/>
-      <c r="AR71" s="112"/>
-      <c r="AS71" s="112"/>
-      <c r="AT71" s="112"/>
-      <c r="AU71" s="112"/>
-      <c r="AV71" s="112"/>
-      <c r="AW71" s="112"/>
-      <c r="AX71" s="112"/>
-      <c r="AY71" s="112"/>
-      <c r="AZ71" s="112"/>
-      <c r="BA71" s="112"/>
-      <c r="BB71" s="112"/>
-      <c r="BC71" s="112"/>
-      <c r="BD71" s="112"/>
-      <c r="BE71" s="112"/>
-      <c r="BF71" s="112"/>
-      <c r="BG71" s="113"/>
-    </row>
-    <row r="72" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="B71" s="50"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="51"/>
+      <c r="E71" s="51"/>
+      <c r="F71" s="51"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="51"/>
+      <c r="I71" s="51"/>
+      <c r="J71" s="51"/>
+      <c r="K71" s="51"/>
+      <c r="L71" s="51"/>
+      <c r="M71" s="51"/>
+      <c r="N71" s="51"/>
+      <c r="O71" s="51"/>
+      <c r="P71" s="51"/>
+      <c r="Q71" s="51"/>
+      <c r="R71" s="51"/>
+      <c r="S71" s="51"/>
+      <c r="T71" s="51"/>
+      <c r="U71" s="51"/>
+      <c r="V71" s="51"/>
+      <c r="W71" s="51"/>
+      <c r="X71" s="51"/>
+      <c r="Y71" s="51"/>
+      <c r="Z71" s="51"/>
+      <c r="AA71" s="51"/>
+      <c r="AB71" s="51"/>
+      <c r="AC71" s="51"/>
+      <c r="AD71" s="51"/>
+      <c r="AE71" s="51"/>
+      <c r="AF71" s="51"/>
+      <c r="AG71" s="51"/>
+      <c r="AH71" s="51"/>
+      <c r="AI71" s="51"/>
+      <c r="AJ71" s="51"/>
+      <c r="AK71" s="51"/>
+      <c r="AL71" s="51"/>
+      <c r="AM71" s="51"/>
+      <c r="AN71" s="51"/>
+      <c r="AO71" s="51"/>
+      <c r="AP71" s="51"/>
+      <c r="AQ71" s="51"/>
+      <c r="AR71" s="51"/>
+      <c r="AS71" s="51"/>
+      <c r="AT71" s="51"/>
+      <c r="AU71" s="51"/>
+      <c r="AV71" s="51"/>
+      <c r="AW71" s="51"/>
+      <c r="AX71" s="51"/>
+      <c r="AY71" s="51"/>
+      <c r="AZ71" s="51"/>
+      <c r="BA71" s="51"/>
+      <c r="BB71" s="51"/>
+      <c r="BC71" s="51"/>
+      <c r="BD71" s="51"/>
+      <c r="BE71" s="51"/>
+      <c r="BF71" s="51"/>
+      <c r="BG71" s="51"/>
+      <c r="BH71" s="51"/>
+      <c r="BI71" s="51"/>
+      <c r="BJ71" s="52"/>
+      <c r="BK71" s="111"/>
+      <c r="BL71" s="112"/>
+      <c r="BM71" s="113"/>
+    </row>
+    <row r="72" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>12</v>
       </c>
+      <c r="B72" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72" s="45"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="45"/>
+      <c r="F72" s="45"/>
+      <c r="G72" s="45"/>
+      <c r="H72" s="45"/>
+      <c r="I72" s="45"/>
+      <c r="J72" s="45"/>
+      <c r="K72" s="45"/>
+      <c r="L72" s="45"/>
+      <c r="M72" s="45"/>
+      <c r="N72" s="45"/>
+      <c r="O72" s="45"/>
+      <c r="P72" s="45"/>
+      <c r="Q72" s="45"/>
+      <c r="R72" s="45"/>
+      <c r="S72" s="45"/>
+      <c r="T72" s="45"/>
+      <c r="U72" s="45"/>
+      <c r="V72" s="45"/>
+      <c r="W72" s="45"/>
+      <c r="X72" s="45"/>
+      <c r="Y72" s="45"/>
+      <c r="Z72" s="45"/>
+      <c r="AA72" s="45"/>
+      <c r="AB72" s="45"/>
+      <c r="AC72" s="45"/>
+      <c r="AD72" s="45"/>
+      <c r="AE72" s="45"/>
+      <c r="AF72" s="45"/>
+      <c r="AG72" s="45"/>
+      <c r="AH72" s="45"/>
+      <c r="AI72" s="45"/>
+      <c r="AJ72" s="45"/>
+      <c r="AK72" s="45"/>
+      <c r="AL72" s="45"/>
+      <c r="AM72" s="45"/>
+      <c r="AN72" s="45"/>
+      <c r="AO72" s="45"/>
+      <c r="AP72" s="45"/>
+      <c r="AQ72" s="45"/>
+      <c r="AR72" s="45"/>
+      <c r="AS72" s="45"/>
+      <c r="AT72" s="45"/>
+      <c r="AU72" s="45"/>
+      <c r="AV72" s="45"/>
+      <c r="AW72" s="45"/>
+      <c r="AX72" s="45"/>
+      <c r="AY72" s="45"/>
+      <c r="AZ72" s="45"/>
+      <c r="BA72" s="45"/>
+      <c r="BB72" s="45"/>
+      <c r="BC72" s="45"/>
+      <c r="BD72" s="45"/>
+      <c r="BE72" s="45"/>
+      <c r="BF72" s="45"/>
+      <c r="BG72" s="46"/>
+      <c r="BH72" s="105" t="s">
+        <v>47</v>
+      </c>
+      <c r="BI72" s="106"/>
+      <c r="BJ72" s="106"/>
+      <c r="BK72" s="106"/>
+      <c r="BL72" s="106"/>
+      <c r="BM72" s="107"/>
     </row>
     <row r="73" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>13</v>
       </c>
+      <c r="B73" s="47"/>
+      <c r="C73" s="114"/>
+      <c r="D73" s="114"/>
+      <c r="E73" s="114"/>
+      <c r="F73" s="114"/>
+      <c r="G73" s="114"/>
+      <c r="H73" s="114"/>
+      <c r="I73" s="114"/>
+      <c r="J73" s="114"/>
+      <c r="K73" s="114"/>
+      <c r="L73" s="114"/>
+      <c r="M73" s="114"/>
+      <c r="N73" s="114"/>
+      <c r="O73" s="114"/>
+      <c r="P73" s="114"/>
+      <c r="Q73" s="114"/>
+      <c r="R73" s="114"/>
+      <c r="S73" s="114"/>
+      <c r="T73" s="114"/>
+      <c r="U73" s="114"/>
+      <c r="V73" s="114"/>
+      <c r="W73" s="114"/>
+      <c r="X73" s="114"/>
+      <c r="Y73" s="114"/>
+      <c r="Z73" s="114"/>
+      <c r="AA73" s="114"/>
+      <c r="AB73" s="114"/>
+      <c r="AC73" s="114"/>
+      <c r="AD73" s="114"/>
+      <c r="AE73" s="114"/>
+      <c r="AF73" s="114"/>
+      <c r="AG73" s="114"/>
+      <c r="AH73" s="114"/>
+      <c r="AI73" s="114"/>
+      <c r="AJ73" s="114"/>
+      <c r="AK73" s="114"/>
+      <c r="AL73" s="114"/>
+      <c r="AM73" s="114"/>
+      <c r="AN73" s="114"/>
+      <c r="AO73" s="114"/>
+      <c r="AP73" s="114"/>
+      <c r="AQ73" s="114"/>
+      <c r="AR73" s="114"/>
+      <c r="AS73" s="114"/>
+      <c r="AT73" s="114"/>
+      <c r="AU73" s="114"/>
+      <c r="AV73" s="114"/>
+      <c r="AW73" s="114"/>
+      <c r="AX73" s="114"/>
+      <c r="AY73" s="114"/>
+      <c r="AZ73" s="114"/>
+      <c r="BA73" s="114"/>
+      <c r="BB73" s="114"/>
+      <c r="BC73" s="114"/>
+      <c r="BD73" s="114"/>
+      <c r="BE73" s="114"/>
+      <c r="BF73" s="114"/>
+      <c r="BG73" s="49"/>
+      <c r="BH73" s="108"/>
+      <c r="BI73" s="109"/>
+      <c r="BJ73" s="109"/>
+      <c r="BK73" s="109"/>
+      <c r="BL73" s="109"/>
+      <c r="BM73" s="110"/>
     </row>
     <row r="74" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>14</v>
       </c>
+      <c r="B74" s="47"/>
+      <c r="C74" s="114"/>
+      <c r="D74" s="114"/>
+      <c r="E74" s="114"/>
+      <c r="F74" s="114"/>
+      <c r="G74" s="114"/>
+      <c r="H74" s="114"/>
+      <c r="I74" s="114"/>
+      <c r="J74" s="114"/>
+      <c r="K74" s="114"/>
+      <c r="L74" s="114"/>
+      <c r="M74" s="114"/>
+      <c r="N74" s="114"/>
+      <c r="O74" s="114"/>
+      <c r="P74" s="114"/>
+      <c r="Q74" s="114"/>
+      <c r="R74" s="114"/>
+      <c r="S74" s="114"/>
+      <c r="T74" s="114"/>
+      <c r="U74" s="114"/>
+      <c r="V74" s="114"/>
+      <c r="W74" s="114"/>
+      <c r="X74" s="114"/>
+      <c r="Y74" s="114"/>
+      <c r="Z74" s="114"/>
+      <c r="AA74" s="114"/>
+      <c r="AB74" s="114"/>
+      <c r="AC74" s="114"/>
+      <c r="AD74" s="114"/>
+      <c r="AE74" s="114"/>
+      <c r="AF74" s="114"/>
+      <c r="AG74" s="114"/>
+      <c r="AH74" s="114"/>
+      <c r="AI74" s="114"/>
+      <c r="AJ74" s="114"/>
+      <c r="AK74" s="114"/>
+      <c r="AL74" s="114"/>
+      <c r="AM74" s="114"/>
+      <c r="AN74" s="114"/>
+      <c r="AO74" s="114"/>
+      <c r="AP74" s="114"/>
+      <c r="AQ74" s="114"/>
+      <c r="AR74" s="114"/>
+      <c r="AS74" s="114"/>
+      <c r="AT74" s="114"/>
+      <c r="AU74" s="114"/>
+      <c r="AV74" s="114"/>
+      <c r="AW74" s="114"/>
+      <c r="AX74" s="114"/>
+      <c r="AY74" s="114"/>
+      <c r="AZ74" s="114"/>
+      <c r="BA74" s="114"/>
+      <c r="BB74" s="114"/>
+      <c r="BC74" s="114"/>
+      <c r="BD74" s="114"/>
+      <c r="BE74" s="114"/>
+      <c r="BF74" s="114"/>
+      <c r="BG74" s="49"/>
+      <c r="BH74" s="108"/>
+      <c r="BI74" s="109"/>
+      <c r="BJ74" s="109"/>
+      <c r="BK74" s="109"/>
+      <c r="BL74" s="109"/>
+      <c r="BM74" s="110"/>
     </row>
     <row r="75" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>15</v>
       </c>
+      <c r="B75" s="50"/>
+      <c r="C75" s="51"/>
+      <c r="D75" s="51"/>
+      <c r="E75" s="51"/>
+      <c r="F75" s="51"/>
+      <c r="G75" s="51"/>
+      <c r="H75" s="51"/>
+      <c r="I75" s="51"/>
+      <c r="J75" s="51"/>
+      <c r="K75" s="51"/>
+      <c r="L75" s="51"/>
+      <c r="M75" s="51"/>
+      <c r="N75" s="51"/>
+      <c r="O75" s="51"/>
+      <c r="P75" s="51"/>
+      <c r="Q75" s="51"/>
+      <c r="R75" s="51"/>
+      <c r="S75" s="51"/>
+      <c r="T75" s="51"/>
+      <c r="U75" s="51"/>
+      <c r="V75" s="51"/>
+      <c r="W75" s="51"/>
+      <c r="X75" s="51"/>
+      <c r="Y75" s="51"/>
+      <c r="Z75" s="51"/>
+      <c r="AA75" s="51"/>
+      <c r="AB75" s="51"/>
+      <c r="AC75" s="51"/>
+      <c r="AD75" s="51"/>
+      <c r="AE75" s="51"/>
+      <c r="AF75" s="51"/>
+      <c r="AG75" s="51"/>
+      <c r="AH75" s="51"/>
+      <c r="AI75" s="51"/>
+      <c r="AJ75" s="51"/>
+      <c r="AK75" s="51"/>
+      <c r="AL75" s="51"/>
+      <c r="AM75" s="51"/>
+      <c r="AN75" s="51"/>
+      <c r="AO75" s="51"/>
+      <c r="AP75" s="51"/>
+      <c r="AQ75" s="51"/>
+      <c r="AR75" s="51"/>
+      <c r="AS75" s="51"/>
+      <c r="AT75" s="51"/>
+      <c r="AU75" s="51"/>
+      <c r="AV75" s="51"/>
+      <c r="AW75" s="51"/>
+      <c r="AX75" s="51"/>
+      <c r="AY75" s="51"/>
+      <c r="AZ75" s="51"/>
+      <c r="BA75" s="51"/>
+      <c r="BB75" s="51"/>
+      <c r="BC75" s="51"/>
+      <c r="BD75" s="51"/>
+      <c r="BE75" s="51"/>
+      <c r="BF75" s="51"/>
+      <c r="BG75" s="52"/>
+      <c r="BH75" s="111"/>
+      <c r="BI75" s="112"/>
+      <c r="BJ75" s="112"/>
+      <c r="BK75" s="112"/>
+      <c r="BL75" s="112"/>
+      <c r="BM75" s="113"/>
+    </row>
+    <row r="76" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
+        <v>16</v>
+      </c>
+      <c r="B76" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C76" s="45"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="45"/>
+      <c r="G76" s="45"/>
+      <c r="H76" s="45"/>
+      <c r="I76" s="45"/>
+      <c r="J76" s="45"/>
+      <c r="K76" s="45"/>
+      <c r="L76" s="45"/>
+      <c r="M76" s="45"/>
+      <c r="N76" s="45"/>
+      <c r="O76" s="45"/>
+      <c r="P76" s="45"/>
+      <c r="Q76" s="45"/>
+      <c r="R76" s="45"/>
+      <c r="S76" s="45"/>
+      <c r="T76" s="45"/>
+      <c r="U76" s="45"/>
+      <c r="V76" s="45"/>
+      <c r="W76" s="45"/>
+      <c r="X76" s="45"/>
+      <c r="Y76" s="45"/>
+      <c r="Z76" s="45"/>
+      <c r="AA76" s="45"/>
+      <c r="AB76" s="45"/>
+      <c r="AC76" s="45"/>
+      <c r="AD76" s="45"/>
+      <c r="AE76" s="45"/>
+      <c r="AF76" s="45"/>
+      <c r="AG76" s="45"/>
+      <c r="AH76" s="45"/>
+      <c r="AI76" s="45"/>
+      <c r="AJ76" s="45"/>
+      <c r="AK76" s="45"/>
+      <c r="AL76" s="45"/>
+      <c r="AM76" s="45"/>
+      <c r="AN76" s="45"/>
+      <c r="AO76" s="45"/>
+      <c r="AP76" s="45"/>
+      <c r="AQ76" s="45"/>
+      <c r="AR76" s="45"/>
+      <c r="AS76" s="45"/>
+      <c r="AT76" s="45"/>
+      <c r="AU76" s="45"/>
+      <c r="AV76" s="45"/>
+      <c r="AW76" s="45"/>
+      <c r="AX76" s="45"/>
+      <c r="AY76" s="45"/>
+      <c r="AZ76" s="45"/>
+      <c r="BA76" s="45"/>
+      <c r="BB76" s="45"/>
+      <c r="BC76" s="45"/>
+      <c r="BD76" s="46"/>
+      <c r="BE76" s="105" t="s">
+        <v>48</v>
+      </c>
+      <c r="BF76" s="106"/>
+      <c r="BG76" s="106"/>
+      <c r="BH76" s="106"/>
+      <c r="BI76" s="106"/>
+      <c r="BJ76" s="106"/>
+      <c r="BK76" s="106"/>
+      <c r="BL76" s="106"/>
+      <c r="BM76" s="107"/>
+    </row>
+    <row r="77" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>17</v>
+      </c>
+      <c r="B77" s="47"/>
+      <c r="C77" s="114"/>
+      <c r="D77" s="114"/>
+      <c r="E77" s="114"/>
+      <c r="F77" s="114"/>
+      <c r="G77" s="114"/>
+      <c r="H77" s="114"/>
+      <c r="I77" s="114"/>
+      <c r="J77" s="114"/>
+      <c r="K77" s="114"/>
+      <c r="L77" s="114"/>
+      <c r="M77" s="114"/>
+      <c r="N77" s="114"/>
+      <c r="O77" s="114"/>
+      <c r="P77" s="114"/>
+      <c r="Q77" s="114"/>
+      <c r="R77" s="114"/>
+      <c r="S77" s="114"/>
+      <c r="T77" s="114"/>
+      <c r="U77" s="114"/>
+      <c r="V77" s="114"/>
+      <c r="W77" s="114"/>
+      <c r="X77" s="114"/>
+      <c r="Y77" s="114"/>
+      <c r="Z77" s="114"/>
+      <c r="AA77" s="114"/>
+      <c r="AB77" s="114"/>
+      <c r="AC77" s="114"/>
+      <c r="AD77" s="114"/>
+      <c r="AE77" s="114"/>
+      <c r="AF77" s="114"/>
+      <c r="AG77" s="114"/>
+      <c r="AH77" s="114"/>
+      <c r="AI77" s="114"/>
+      <c r="AJ77" s="114"/>
+      <c r="AK77" s="114"/>
+      <c r="AL77" s="114"/>
+      <c r="AM77" s="114"/>
+      <c r="AN77" s="114"/>
+      <c r="AO77" s="114"/>
+      <c r="AP77" s="114"/>
+      <c r="AQ77" s="114"/>
+      <c r="AR77" s="114"/>
+      <c r="AS77" s="114"/>
+      <c r="AT77" s="114"/>
+      <c r="AU77" s="114"/>
+      <c r="AV77" s="114"/>
+      <c r="AW77" s="114"/>
+      <c r="AX77" s="114"/>
+      <c r="AY77" s="114"/>
+      <c r="AZ77" s="114"/>
+      <c r="BA77" s="114"/>
+      <c r="BB77" s="114"/>
+      <c r="BC77" s="114"/>
+      <c r="BD77" s="49"/>
+      <c r="BE77" s="108"/>
+      <c r="BF77" s="109"/>
+      <c r="BG77" s="109"/>
+      <c r="BH77" s="109"/>
+      <c r="BI77" s="109"/>
+      <c r="BJ77" s="109"/>
+      <c r="BK77" s="109"/>
+      <c r="BL77" s="109"/>
+      <c r="BM77" s="110"/>
+    </row>
+    <row r="78" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
+        <v>18</v>
+      </c>
+      <c r="B78" s="47"/>
+      <c r="C78" s="114"/>
+      <c r="D78" s="114"/>
+      <c r="E78" s="114"/>
+      <c r="F78" s="114"/>
+      <c r="G78" s="114"/>
+      <c r="H78" s="114"/>
+      <c r="I78" s="114"/>
+      <c r="J78" s="114"/>
+      <c r="K78" s="114"/>
+      <c r="L78" s="114"/>
+      <c r="M78" s="114"/>
+      <c r="N78" s="114"/>
+      <c r="O78" s="114"/>
+      <c r="P78" s="114"/>
+      <c r="Q78" s="114"/>
+      <c r="R78" s="114"/>
+      <c r="S78" s="114"/>
+      <c r="T78" s="114"/>
+      <c r="U78" s="114"/>
+      <c r="V78" s="114"/>
+      <c r="W78" s="114"/>
+      <c r="X78" s="114"/>
+      <c r="Y78" s="114"/>
+      <c r="Z78" s="114"/>
+      <c r="AA78" s="114"/>
+      <c r="AB78" s="114"/>
+      <c r="AC78" s="114"/>
+      <c r="AD78" s="114"/>
+      <c r="AE78" s="114"/>
+      <c r="AF78" s="114"/>
+      <c r="AG78" s="114"/>
+      <c r="AH78" s="114"/>
+      <c r="AI78" s="114"/>
+      <c r="AJ78" s="114"/>
+      <c r="AK78" s="114"/>
+      <c r="AL78" s="114"/>
+      <c r="AM78" s="114"/>
+      <c r="AN78" s="114"/>
+      <c r="AO78" s="114"/>
+      <c r="AP78" s="114"/>
+      <c r="AQ78" s="114"/>
+      <c r="AR78" s="114"/>
+      <c r="AS78" s="114"/>
+      <c r="AT78" s="114"/>
+      <c r="AU78" s="114"/>
+      <c r="AV78" s="114"/>
+      <c r="AW78" s="114"/>
+      <c r="AX78" s="114"/>
+      <c r="AY78" s="114"/>
+      <c r="AZ78" s="114"/>
+      <c r="BA78" s="114"/>
+      <c r="BB78" s="114"/>
+      <c r="BC78" s="114"/>
+      <c r="BD78" s="49"/>
+      <c r="BE78" s="108"/>
+      <c r="BF78" s="109"/>
+      <c r="BG78" s="109"/>
+      <c r="BH78" s="109"/>
+      <c r="BI78" s="109"/>
+      <c r="BJ78" s="109"/>
+      <c r="BK78" s="109"/>
+      <c r="BL78" s="109"/>
+      <c r="BM78" s="110"/>
+    </row>
+    <row r="79" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>19</v>
+      </c>
+      <c r="B79" s="50"/>
+      <c r="C79" s="51"/>
+      <c r="D79" s="51"/>
+      <c r="E79" s="51"/>
+      <c r="F79" s="51"/>
+      <c r="G79" s="51"/>
+      <c r="H79" s="51"/>
+      <c r="I79" s="51"/>
+      <c r="J79" s="51"/>
+      <c r="K79" s="51"/>
+      <c r="L79" s="51"/>
+      <c r="M79" s="51"/>
+      <c r="N79" s="51"/>
+      <c r="O79" s="51"/>
+      <c r="P79" s="51"/>
+      <c r="Q79" s="51"/>
+      <c r="R79" s="51"/>
+      <c r="S79" s="51"/>
+      <c r="T79" s="51"/>
+      <c r="U79" s="51"/>
+      <c r="V79" s="51"/>
+      <c r="W79" s="51"/>
+      <c r="X79" s="51"/>
+      <c r="Y79" s="51"/>
+      <c r="Z79" s="51"/>
+      <c r="AA79" s="51"/>
+      <c r="AB79" s="51"/>
+      <c r="AC79" s="51"/>
+      <c r="AD79" s="51"/>
+      <c r="AE79" s="51"/>
+      <c r="AF79" s="51"/>
+      <c r="AG79" s="51"/>
+      <c r="AH79" s="51"/>
+      <c r="AI79" s="51"/>
+      <c r="AJ79" s="51"/>
+      <c r="AK79" s="51"/>
+      <c r="AL79" s="51"/>
+      <c r="AM79" s="51"/>
+      <c r="AN79" s="51"/>
+      <c r="AO79" s="51"/>
+      <c r="AP79" s="51"/>
+      <c r="AQ79" s="51"/>
+      <c r="AR79" s="51"/>
+      <c r="AS79" s="51"/>
+      <c r="AT79" s="51"/>
+      <c r="AU79" s="51"/>
+      <c r="AV79" s="51"/>
+      <c r="AW79" s="51"/>
+      <c r="AX79" s="51"/>
+      <c r="AY79" s="51"/>
+      <c r="AZ79" s="51"/>
+      <c r="BA79" s="51"/>
+      <c r="BB79" s="51"/>
+      <c r="BC79" s="51"/>
+      <c r="BD79" s="52"/>
+      <c r="BE79" s="111"/>
+      <c r="BF79" s="112"/>
+      <c r="BG79" s="112"/>
+      <c r="BH79" s="112"/>
+      <c r="BI79" s="112"/>
+      <c r="BJ79" s="112"/>
+      <c r="BK79" s="112"/>
+      <c r="BL79" s="112"/>
+      <c r="BM79" s="113"/>
+    </row>
+    <row r="80" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>20</v>
+      </c>
+      <c r="B80" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C80" s="45"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="45"/>
+      <c r="F80" s="45"/>
+      <c r="G80" s="45"/>
+      <c r="H80" s="45"/>
+      <c r="I80" s="45"/>
+      <c r="J80" s="45"/>
+      <c r="K80" s="45"/>
+      <c r="L80" s="45"/>
+      <c r="M80" s="45"/>
+      <c r="N80" s="45"/>
+      <c r="O80" s="45"/>
+      <c r="P80" s="45"/>
+      <c r="Q80" s="45"/>
+      <c r="R80" s="45"/>
+      <c r="S80" s="45"/>
+      <c r="T80" s="45"/>
+      <c r="U80" s="45"/>
+      <c r="V80" s="45"/>
+      <c r="W80" s="45"/>
+      <c r="X80" s="45"/>
+      <c r="Y80" s="45"/>
+      <c r="Z80" s="45"/>
+      <c r="AA80" s="45"/>
+      <c r="AB80" s="45"/>
+      <c r="AC80" s="45"/>
+      <c r="AD80" s="45"/>
+      <c r="AE80" s="45"/>
+      <c r="AF80" s="45"/>
+      <c r="AG80" s="45"/>
+      <c r="AH80" s="45"/>
+      <c r="AI80" s="45"/>
+      <c r="AJ80" s="45"/>
+      <c r="AK80" s="45"/>
+      <c r="AL80" s="45"/>
+      <c r="AM80" s="45"/>
+      <c r="AN80" s="45"/>
+      <c r="AO80" s="45"/>
+      <c r="AP80" s="45"/>
+      <c r="AQ80" s="45"/>
+      <c r="AR80" s="45"/>
+      <c r="AS80" s="45"/>
+      <c r="AT80" s="45"/>
+      <c r="AU80" s="45"/>
+      <c r="AV80" s="45"/>
+      <c r="AW80" s="45"/>
+      <c r="AX80" s="45"/>
+      <c r="AY80" s="45"/>
+      <c r="AZ80" s="45"/>
+      <c r="BA80" s="46"/>
+      <c r="BB80" s="116"/>
+      <c r="BC80" s="116"/>
+      <c r="BD80" s="116"/>
+      <c r="BE80" s="116"/>
+      <c r="BF80" s="116"/>
+      <c r="BG80" s="116"/>
+      <c r="BH80" s="116"/>
+      <c r="BI80" s="116"/>
+      <c r="BJ80" s="116"/>
+      <c r="BK80" s="116"/>
+      <c r="BL80" s="118"/>
+      <c r="BM80" s="118"/>
+    </row>
+    <row r="81" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>21</v>
+      </c>
+      <c r="B81" s="47"/>
+      <c r="C81" s="114"/>
+      <c r="D81" s="114"/>
+      <c r="E81" s="114"/>
+      <c r="F81" s="114"/>
+      <c r="G81" s="114"/>
+      <c r="H81" s="114"/>
+      <c r="I81" s="114"/>
+      <c r="J81" s="114"/>
+      <c r="K81" s="114"/>
+      <c r="L81" s="114"/>
+      <c r="M81" s="114"/>
+      <c r="N81" s="114"/>
+      <c r="O81" s="114"/>
+      <c r="P81" s="114"/>
+      <c r="Q81" s="114"/>
+      <c r="R81" s="114"/>
+      <c r="S81" s="114"/>
+      <c r="T81" s="114"/>
+      <c r="U81" s="114"/>
+      <c r="V81" s="114"/>
+      <c r="W81" s="114"/>
+      <c r="X81" s="114"/>
+      <c r="Y81" s="114"/>
+      <c r="Z81" s="114"/>
+      <c r="AA81" s="114"/>
+      <c r="AB81" s="114"/>
+      <c r="AC81" s="114"/>
+      <c r="AD81" s="114"/>
+      <c r="AE81" s="114"/>
+      <c r="AF81" s="114"/>
+      <c r="AG81" s="114"/>
+      <c r="AH81" s="114"/>
+      <c r="AI81" s="114"/>
+      <c r="AJ81" s="114"/>
+      <c r="AK81" s="114"/>
+      <c r="AL81" s="114"/>
+      <c r="AM81" s="114"/>
+      <c r="AN81" s="114"/>
+      <c r="AO81" s="114"/>
+      <c r="AP81" s="114"/>
+      <c r="AQ81" s="114"/>
+      <c r="AR81" s="114"/>
+      <c r="AS81" s="114"/>
+      <c r="AT81" s="114"/>
+      <c r="AU81" s="114"/>
+      <c r="AV81" s="114"/>
+      <c r="AW81" s="114"/>
+      <c r="AX81" s="114"/>
+      <c r="AY81" s="114"/>
+      <c r="AZ81" s="114"/>
+      <c r="BA81" s="49"/>
+      <c r="BB81" s="118"/>
+      <c r="BC81" s="118"/>
+      <c r="BD81" s="118"/>
+      <c r="BE81" s="118"/>
+      <c r="BF81" s="118"/>
+      <c r="BG81" s="118"/>
+      <c r="BH81" s="118"/>
+      <c r="BI81" s="118"/>
+      <c r="BJ81" s="118"/>
+      <c r="BK81" s="118"/>
+      <c r="BL81" s="118"/>
+      <c r="BM81" s="118"/>
+    </row>
+    <row r="82" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
+        <v>22</v>
+      </c>
+      <c r="B82" s="47"/>
+      <c r="C82" s="114"/>
+      <c r="D82" s="114"/>
+      <c r="E82" s="114"/>
+      <c r="F82" s="114"/>
+      <c r="G82" s="114"/>
+      <c r="H82" s="114"/>
+      <c r="I82" s="114"/>
+      <c r="J82" s="114"/>
+      <c r="K82" s="114"/>
+      <c r="L82" s="114"/>
+      <c r="M82" s="114"/>
+      <c r="N82" s="114"/>
+      <c r="O82" s="114"/>
+      <c r="P82" s="114"/>
+      <c r="Q82" s="114"/>
+      <c r="R82" s="114"/>
+      <c r="S82" s="114"/>
+      <c r="T82" s="114"/>
+      <c r="U82" s="114"/>
+      <c r="V82" s="114"/>
+      <c r="W82" s="114"/>
+      <c r="X82" s="114"/>
+      <c r="Y82" s="114"/>
+      <c r="Z82" s="114"/>
+      <c r="AA82" s="114"/>
+      <c r="AB82" s="114"/>
+      <c r="AC82" s="114"/>
+      <c r="AD82" s="114"/>
+      <c r="AE82" s="114"/>
+      <c r="AF82" s="114"/>
+      <c r="AG82" s="114"/>
+      <c r="AH82" s="114"/>
+      <c r="AI82" s="114"/>
+      <c r="AJ82" s="114"/>
+      <c r="AK82" s="114"/>
+      <c r="AL82" s="114"/>
+      <c r="AM82" s="114"/>
+      <c r="AN82" s="114"/>
+      <c r="AO82" s="114"/>
+      <c r="AP82" s="114"/>
+      <c r="AQ82" s="114"/>
+      <c r="AR82" s="114"/>
+      <c r="AS82" s="114"/>
+      <c r="AT82" s="114"/>
+      <c r="AU82" s="114"/>
+      <c r="AV82" s="114"/>
+      <c r="AW82" s="114"/>
+      <c r="AX82" s="114"/>
+      <c r="AY82" s="114"/>
+      <c r="AZ82" s="114"/>
+      <c r="BA82" s="49"/>
+      <c r="BB82" s="118"/>
+      <c r="BC82" s="118"/>
+      <c r="BD82" s="118"/>
+      <c r="BE82" s="118"/>
+      <c r="BF82" s="118"/>
+      <c r="BG82" s="118"/>
+      <c r="BH82" s="118"/>
+      <c r="BI82" s="118"/>
+      <c r="BJ82" s="118"/>
+      <c r="BK82" s="118"/>
+      <c r="BL82" s="118"/>
+      <c r="BM82" s="118"/>
+    </row>
+    <row r="83" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>23</v>
+      </c>
+      <c r="B83" s="50"/>
+      <c r="C83" s="51"/>
+      <c r="D83" s="51"/>
+      <c r="E83" s="51"/>
+      <c r="F83" s="51"/>
+      <c r="G83" s="51"/>
+      <c r="H83" s="51"/>
+      <c r="I83" s="51"/>
+      <c r="J83" s="51"/>
+      <c r="K83" s="51"/>
+      <c r="L83" s="51"/>
+      <c r="M83" s="51"/>
+      <c r="N83" s="51"/>
+      <c r="O83" s="51"/>
+      <c r="P83" s="51"/>
+      <c r="Q83" s="51"/>
+      <c r="R83" s="51"/>
+      <c r="S83" s="51"/>
+      <c r="T83" s="51"/>
+      <c r="U83" s="51"/>
+      <c r="V83" s="51"/>
+      <c r="W83" s="51"/>
+      <c r="X83" s="51"/>
+      <c r="Y83" s="51"/>
+      <c r="Z83" s="51"/>
+      <c r="AA83" s="51"/>
+      <c r="AB83" s="51"/>
+      <c r="AC83" s="51"/>
+      <c r="AD83" s="51"/>
+      <c r="AE83" s="51"/>
+      <c r="AF83" s="51"/>
+      <c r="AG83" s="51"/>
+      <c r="AH83" s="51"/>
+      <c r="AI83" s="51"/>
+      <c r="AJ83" s="51"/>
+      <c r="AK83" s="51"/>
+      <c r="AL83" s="51"/>
+      <c r="AM83" s="51"/>
+      <c r="AN83" s="51"/>
+      <c r="AO83" s="51"/>
+      <c r="AP83" s="51"/>
+      <c r="AQ83" s="51"/>
+      <c r="AR83" s="51"/>
+      <c r="AS83" s="51"/>
+      <c r="AT83" s="51"/>
+      <c r="AU83" s="51"/>
+      <c r="AV83" s="51"/>
+      <c r="AW83" s="51"/>
+      <c r="AX83" s="51"/>
+      <c r="AY83" s="51"/>
+      <c r="AZ83" s="51"/>
+      <c r="BA83" s="52"/>
+      <c r="BB83" s="117"/>
+      <c r="BC83" s="118"/>
+      <c r="BD83" s="118"/>
+      <c r="BE83" s="118"/>
+      <c r="BF83" s="118"/>
+      <c r="BG83" s="118"/>
+      <c r="BH83" s="118"/>
+      <c r="BI83" s="118"/>
+      <c r="BJ83" s="118"/>
+      <c r="BK83" s="118"/>
+      <c r="BL83" s="118"/>
+      <c r="BM83" s="118"/>
+    </row>
+    <row r="84" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="BB84" s="119"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B68:BG71"/>
+  <mergeCells count="34">
+    <mergeCell ref="B76:BD79"/>
+    <mergeCell ref="BE76:BM79"/>
+    <mergeCell ref="B80:BA83"/>
+    <mergeCell ref="B72:BG75"/>
+    <mergeCell ref="BK68:BM71"/>
+    <mergeCell ref="B68:BJ71"/>
+    <mergeCell ref="BH72:BM75"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="B3:BM6"/>
     <mergeCell ref="B11:BM14"/>

</xml_diff>

<commit_message>
Now performs encoders' MHSA's softmax
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418EA029-7BF0-DF4D-9D62-527231A1DBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84708801-29E3-9241-A4EB-A88BF70AE8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
+    <workbookView xWindow="8580" yWindow="2080" windowWidth="33600" windowHeight="26620" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,28 +186,28 @@
     <t>res_K_T_broadcast[:][id]</t>
   </si>
   <si>
-    <t>res_QK_T_0[id][:]</t>
+    <t>softmax[0][id][:]</t>
   </si>
   <si>
-    <t>res_QK_T_1[id][:]</t>
+    <t>softmax[1][id][:]</t>
   </si>
   <si>
-    <t>res_QK_T_2[id][:]</t>
+    <t>softmax[2][id][:]</t>
   </si>
   <si>
-    <t>res_QK_T_3[id][:]</t>
+    <t>softmax[3][id][:]</t>
   </si>
   <si>
-    <t>res_QK_T_4[id][:]</t>
+    <t>softmax[4][id][:]</t>
   </si>
   <si>
-    <t>res_QK_T_5[id][:]</t>
+    <t>softmax[5][id][:]</t>
   </si>
   <si>
-    <t>res_QK_T_6[id][:]</t>
+    <t>softmax[6][id][:]</t>
   </si>
   <si>
-    <t>res_QK_T_7[id][:]</t>
+    <t>softmax[7][id][:]</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -912,13 +912,16 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1248,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
   <dimension ref="A1:BP111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AP111" sqref="AP111"/>
+    <sheetView tabSelected="1" topLeftCell="B55" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5922,14 +5925,14 @@
       <c r="BE72" s="114"/>
       <c r="BF72" s="114"/>
       <c r="BG72" s="115"/>
-      <c r="BH72" s="51" t="s">
+      <c r="BH72" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="BI72" s="52"/>
-      <c r="BJ72" s="52"/>
-      <c r="BK72" s="52"/>
-      <c r="BL72" s="52"/>
-      <c r="BM72" s="53"/>
+      <c r="BI72" s="132"/>
+      <c r="BJ72" s="132"/>
+      <c r="BK72" s="132"/>
+      <c r="BL72" s="132"/>
+      <c r="BM72" s="133"/>
     </row>
     <row r="73" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
@@ -5993,12 +5996,12 @@
       <c r="BE73" s="117"/>
       <c r="BF73" s="117"/>
       <c r="BG73" s="118"/>
-      <c r="BH73" s="54"/>
+      <c r="BH73" s="134"/>
       <c r="BI73" s="140"/>
       <c r="BJ73" s="140"/>
       <c r="BK73" s="140"/>
       <c r="BL73" s="140"/>
-      <c r="BM73" s="56"/>
+      <c r="BM73" s="136"/>
     </row>
     <row r="74" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
@@ -6062,12 +6065,12 @@
       <c r="BE74" s="117"/>
       <c r="BF74" s="117"/>
       <c r="BG74" s="118"/>
-      <c r="BH74" s="54"/>
+      <c r="BH74" s="134"/>
       <c r="BI74" s="140"/>
       <c r="BJ74" s="140"/>
       <c r="BK74" s="140"/>
       <c r="BL74" s="140"/>
-      <c r="BM74" s="56"/>
+      <c r="BM74" s="136"/>
     </row>
     <row r="75" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
@@ -6131,74 +6134,74 @@
       <c r="BE75" s="120"/>
       <c r="BF75" s="120"/>
       <c r="BG75" s="121"/>
-      <c r="BH75" s="57"/>
-      <c r="BI75" s="58"/>
-      <c r="BJ75" s="58"/>
-      <c r="BK75" s="58"/>
-      <c r="BL75" s="58"/>
-      <c r="BM75" s="59"/>
+      <c r="BH75" s="137"/>
+      <c r="BI75" s="138"/>
+      <c r="BJ75" s="138"/>
+      <c r="BK75" s="138"/>
+      <c r="BL75" s="138"/>
+      <c r="BM75" s="139"/>
     </row>
     <row r="76" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>16</v>
       </c>
-      <c r="B76" s="51" t="s">
+      <c r="B76" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="C76" s="43"/>
-      <c r="D76" s="43"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="43"/>
-      <c r="H76" s="43"/>
-      <c r="I76" s="43"/>
-      <c r="J76" s="43"/>
-      <c r="K76" s="43"/>
-      <c r="L76" s="43"/>
-      <c r="M76" s="43"/>
-      <c r="N76" s="43"/>
-      <c r="O76" s="43"/>
-      <c r="P76" s="43"/>
-      <c r="Q76" s="43"/>
-      <c r="R76" s="43"/>
-      <c r="S76" s="43"/>
-      <c r="T76" s="43"/>
-      <c r="U76" s="43"/>
-      <c r="V76" s="43"/>
-      <c r="W76" s="43"/>
-      <c r="X76" s="43"/>
-      <c r="Y76" s="43"/>
-      <c r="Z76" s="43"/>
-      <c r="AA76" s="43"/>
-      <c r="AB76" s="43"/>
-      <c r="AC76" s="43"/>
-      <c r="AD76" s="43"/>
-      <c r="AE76" s="43"/>
-      <c r="AF76" s="43"/>
-      <c r="AG76" s="43"/>
-      <c r="AH76" s="43"/>
-      <c r="AI76" s="43"/>
-      <c r="AJ76" s="43"/>
-      <c r="AK76" s="43"/>
-      <c r="AL76" s="43"/>
-      <c r="AM76" s="43"/>
-      <c r="AN76" s="43"/>
-      <c r="AO76" s="43"/>
-      <c r="AP76" s="43"/>
-      <c r="AQ76" s="43"/>
-      <c r="AR76" s="43"/>
-      <c r="AS76" s="43"/>
-      <c r="AT76" s="43"/>
-      <c r="AU76" s="43"/>
-      <c r="AV76" s="43"/>
-      <c r="AW76" s="43"/>
-      <c r="AX76" s="43"/>
-      <c r="AY76" s="43"/>
-      <c r="AZ76" s="43"/>
-      <c r="BA76" s="43"/>
-      <c r="BB76" s="43"/>
-      <c r="BC76" s="43"/>
-      <c r="BD76" s="44"/>
+      <c r="C76" s="123"/>
+      <c r="D76" s="123"/>
+      <c r="E76" s="123"/>
+      <c r="F76" s="123"/>
+      <c r="G76" s="123"/>
+      <c r="H76" s="123"/>
+      <c r="I76" s="123"/>
+      <c r="J76" s="123"/>
+      <c r="K76" s="123"/>
+      <c r="L76" s="123"/>
+      <c r="M76" s="123"/>
+      <c r="N76" s="123"/>
+      <c r="O76" s="123"/>
+      <c r="P76" s="123"/>
+      <c r="Q76" s="123"/>
+      <c r="R76" s="123"/>
+      <c r="S76" s="123"/>
+      <c r="T76" s="123"/>
+      <c r="U76" s="123"/>
+      <c r="V76" s="123"/>
+      <c r="W76" s="123"/>
+      <c r="X76" s="123"/>
+      <c r="Y76" s="123"/>
+      <c r="Z76" s="123"/>
+      <c r="AA76" s="123"/>
+      <c r="AB76" s="123"/>
+      <c r="AC76" s="123"/>
+      <c r="AD76" s="123"/>
+      <c r="AE76" s="123"/>
+      <c r="AF76" s="123"/>
+      <c r="AG76" s="123"/>
+      <c r="AH76" s="123"/>
+      <c r="AI76" s="123"/>
+      <c r="AJ76" s="123"/>
+      <c r="AK76" s="123"/>
+      <c r="AL76" s="123"/>
+      <c r="AM76" s="123"/>
+      <c r="AN76" s="123"/>
+      <c r="AO76" s="123"/>
+      <c r="AP76" s="123"/>
+      <c r="AQ76" s="123"/>
+      <c r="AR76" s="123"/>
+      <c r="AS76" s="123"/>
+      <c r="AT76" s="123"/>
+      <c r="AU76" s="123"/>
+      <c r="AV76" s="123"/>
+      <c r="AW76" s="123"/>
+      <c r="AX76" s="123"/>
+      <c r="AY76" s="123"/>
+      <c r="AZ76" s="123"/>
+      <c r="BA76" s="123"/>
+      <c r="BB76" s="123"/>
+      <c r="BC76" s="123"/>
+      <c r="BD76" s="124"/>
       <c r="BE76" s="51" t="s">
         <v>49</v>
       </c>
@@ -6215,61 +6218,61 @@
       <c r="A77" s="1">
         <v>17</v>
       </c>
-      <c r="B77" s="45"/>
-      <c r="C77" s="141"/>
-      <c r="D77" s="141"/>
-      <c r="E77" s="141"/>
-      <c r="F77" s="141"/>
-      <c r="G77" s="141"/>
-      <c r="H77" s="141"/>
-      <c r="I77" s="141"/>
-      <c r="J77" s="141"/>
-      <c r="K77" s="141"/>
-      <c r="L77" s="141"/>
-      <c r="M77" s="141"/>
-      <c r="N77" s="141"/>
-      <c r="O77" s="141"/>
-      <c r="P77" s="141"/>
-      <c r="Q77" s="141"/>
-      <c r="R77" s="141"/>
-      <c r="S77" s="141"/>
-      <c r="T77" s="141"/>
-      <c r="U77" s="141"/>
-      <c r="V77" s="141"/>
-      <c r="W77" s="141"/>
-      <c r="X77" s="141"/>
-      <c r="Y77" s="141"/>
-      <c r="Z77" s="141"/>
-      <c r="AA77" s="141"/>
-      <c r="AB77" s="141"/>
-      <c r="AC77" s="141"/>
-      <c r="AD77" s="141"/>
-      <c r="AE77" s="141"/>
-      <c r="AF77" s="141"/>
-      <c r="AG77" s="141"/>
-      <c r="AH77" s="141"/>
-      <c r="AI77" s="141"/>
-      <c r="AJ77" s="141"/>
-      <c r="AK77" s="141"/>
-      <c r="AL77" s="141"/>
-      <c r="AM77" s="141"/>
-      <c r="AN77" s="141"/>
-      <c r="AO77" s="141"/>
-      <c r="AP77" s="141"/>
-      <c r="AQ77" s="141"/>
-      <c r="AR77" s="141"/>
-      <c r="AS77" s="141"/>
-      <c r="AT77" s="141"/>
-      <c r="AU77" s="141"/>
-      <c r="AV77" s="141"/>
-      <c r="AW77" s="141"/>
-      <c r="AX77" s="141"/>
-      <c r="AY77" s="141"/>
-      <c r="AZ77" s="141"/>
-      <c r="BA77" s="141"/>
-      <c r="BB77" s="141"/>
-      <c r="BC77" s="141"/>
-      <c r="BD77" s="47"/>
+      <c r="B77" s="125"/>
+      <c r="C77" s="143"/>
+      <c r="D77" s="143"/>
+      <c r="E77" s="143"/>
+      <c r="F77" s="143"/>
+      <c r="G77" s="143"/>
+      <c r="H77" s="143"/>
+      <c r="I77" s="143"/>
+      <c r="J77" s="143"/>
+      <c r="K77" s="143"/>
+      <c r="L77" s="143"/>
+      <c r="M77" s="143"/>
+      <c r="N77" s="143"/>
+      <c r="O77" s="143"/>
+      <c r="P77" s="143"/>
+      <c r="Q77" s="143"/>
+      <c r="R77" s="143"/>
+      <c r="S77" s="143"/>
+      <c r="T77" s="143"/>
+      <c r="U77" s="143"/>
+      <c r="V77" s="143"/>
+      <c r="W77" s="143"/>
+      <c r="X77" s="143"/>
+      <c r="Y77" s="143"/>
+      <c r="Z77" s="143"/>
+      <c r="AA77" s="143"/>
+      <c r="AB77" s="143"/>
+      <c r="AC77" s="143"/>
+      <c r="AD77" s="143"/>
+      <c r="AE77" s="143"/>
+      <c r="AF77" s="143"/>
+      <c r="AG77" s="143"/>
+      <c r="AH77" s="143"/>
+      <c r="AI77" s="143"/>
+      <c r="AJ77" s="143"/>
+      <c r="AK77" s="143"/>
+      <c r="AL77" s="143"/>
+      <c r="AM77" s="143"/>
+      <c r="AN77" s="143"/>
+      <c r="AO77" s="143"/>
+      <c r="AP77" s="143"/>
+      <c r="AQ77" s="143"/>
+      <c r="AR77" s="143"/>
+      <c r="AS77" s="143"/>
+      <c r="AT77" s="143"/>
+      <c r="AU77" s="143"/>
+      <c r="AV77" s="143"/>
+      <c r="AW77" s="143"/>
+      <c r="AX77" s="143"/>
+      <c r="AY77" s="143"/>
+      <c r="AZ77" s="143"/>
+      <c r="BA77" s="143"/>
+      <c r="BB77" s="143"/>
+      <c r="BC77" s="143"/>
+      <c r="BD77" s="127"/>
       <c r="BE77" s="54"/>
       <c r="BF77" s="55"/>
       <c r="BG77" s="55"/>
@@ -6284,61 +6287,61 @@
       <c r="A78" s="2">
         <v>18</v>
       </c>
-      <c r="B78" s="45"/>
-      <c r="C78" s="141"/>
-      <c r="D78" s="141"/>
-      <c r="E78" s="141"/>
-      <c r="F78" s="141"/>
-      <c r="G78" s="141"/>
-      <c r="H78" s="141"/>
-      <c r="I78" s="141"/>
-      <c r="J78" s="141"/>
-      <c r="K78" s="141"/>
-      <c r="L78" s="141"/>
-      <c r="M78" s="141"/>
-      <c r="N78" s="141"/>
-      <c r="O78" s="141"/>
-      <c r="P78" s="141"/>
-      <c r="Q78" s="141"/>
-      <c r="R78" s="141"/>
-      <c r="S78" s="141"/>
-      <c r="T78" s="141"/>
-      <c r="U78" s="141"/>
-      <c r="V78" s="141"/>
-      <c r="W78" s="141"/>
-      <c r="X78" s="141"/>
-      <c r="Y78" s="141"/>
-      <c r="Z78" s="141"/>
-      <c r="AA78" s="141"/>
-      <c r="AB78" s="141"/>
-      <c r="AC78" s="141"/>
-      <c r="AD78" s="141"/>
-      <c r="AE78" s="141"/>
-      <c r="AF78" s="141"/>
-      <c r="AG78" s="141"/>
-      <c r="AH78" s="141"/>
-      <c r="AI78" s="141"/>
-      <c r="AJ78" s="141"/>
-      <c r="AK78" s="141"/>
-      <c r="AL78" s="141"/>
-      <c r="AM78" s="141"/>
-      <c r="AN78" s="141"/>
-      <c r="AO78" s="141"/>
-      <c r="AP78" s="141"/>
-      <c r="AQ78" s="141"/>
-      <c r="AR78" s="141"/>
-      <c r="AS78" s="141"/>
-      <c r="AT78" s="141"/>
-      <c r="AU78" s="141"/>
-      <c r="AV78" s="141"/>
-      <c r="AW78" s="141"/>
-      <c r="AX78" s="141"/>
-      <c r="AY78" s="141"/>
-      <c r="AZ78" s="141"/>
-      <c r="BA78" s="141"/>
-      <c r="BB78" s="141"/>
-      <c r="BC78" s="141"/>
-      <c r="BD78" s="47"/>
+      <c r="B78" s="125"/>
+      <c r="C78" s="143"/>
+      <c r="D78" s="143"/>
+      <c r="E78" s="143"/>
+      <c r="F78" s="143"/>
+      <c r="G78" s="143"/>
+      <c r="H78" s="143"/>
+      <c r="I78" s="143"/>
+      <c r="J78" s="143"/>
+      <c r="K78" s="143"/>
+      <c r="L78" s="143"/>
+      <c r="M78" s="143"/>
+      <c r="N78" s="143"/>
+      <c r="O78" s="143"/>
+      <c r="P78" s="143"/>
+      <c r="Q78" s="143"/>
+      <c r="R78" s="143"/>
+      <c r="S78" s="143"/>
+      <c r="T78" s="143"/>
+      <c r="U78" s="143"/>
+      <c r="V78" s="143"/>
+      <c r="W78" s="143"/>
+      <c r="X78" s="143"/>
+      <c r="Y78" s="143"/>
+      <c r="Z78" s="143"/>
+      <c r="AA78" s="143"/>
+      <c r="AB78" s="143"/>
+      <c r="AC78" s="143"/>
+      <c r="AD78" s="143"/>
+      <c r="AE78" s="143"/>
+      <c r="AF78" s="143"/>
+      <c r="AG78" s="143"/>
+      <c r="AH78" s="143"/>
+      <c r="AI78" s="143"/>
+      <c r="AJ78" s="143"/>
+      <c r="AK78" s="143"/>
+      <c r="AL78" s="143"/>
+      <c r="AM78" s="143"/>
+      <c r="AN78" s="143"/>
+      <c r="AO78" s="143"/>
+      <c r="AP78" s="143"/>
+      <c r="AQ78" s="143"/>
+      <c r="AR78" s="143"/>
+      <c r="AS78" s="143"/>
+      <c r="AT78" s="143"/>
+      <c r="AU78" s="143"/>
+      <c r="AV78" s="143"/>
+      <c r="AW78" s="143"/>
+      <c r="AX78" s="143"/>
+      <c r="AY78" s="143"/>
+      <c r="AZ78" s="143"/>
+      <c r="BA78" s="143"/>
+      <c r="BB78" s="143"/>
+      <c r="BC78" s="143"/>
+      <c r="BD78" s="127"/>
       <c r="BE78" s="54"/>
       <c r="BF78" s="55"/>
       <c r="BG78" s="55"/>
@@ -6353,61 +6356,61 @@
       <c r="A79" s="1">
         <v>19</v>
       </c>
-      <c r="B79" s="48"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
-      <c r="E79" s="49"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="49"/>
-      <c r="H79" s="49"/>
-      <c r="I79" s="49"/>
-      <c r="J79" s="49"/>
-      <c r="K79" s="49"/>
-      <c r="L79" s="49"/>
-      <c r="M79" s="49"/>
-      <c r="N79" s="49"/>
-      <c r="O79" s="49"/>
-      <c r="P79" s="49"/>
-      <c r="Q79" s="49"/>
-      <c r="R79" s="49"/>
-      <c r="S79" s="49"/>
-      <c r="T79" s="49"/>
-      <c r="U79" s="49"/>
-      <c r="V79" s="49"/>
-      <c r="W79" s="49"/>
-      <c r="X79" s="49"/>
-      <c r="Y79" s="49"/>
-      <c r="Z79" s="49"/>
-      <c r="AA79" s="49"/>
-      <c r="AB79" s="49"/>
-      <c r="AC79" s="49"/>
-      <c r="AD79" s="49"/>
-      <c r="AE79" s="49"/>
-      <c r="AF79" s="49"/>
-      <c r="AG79" s="49"/>
-      <c r="AH79" s="49"/>
-      <c r="AI79" s="49"/>
-      <c r="AJ79" s="49"/>
-      <c r="AK79" s="49"/>
-      <c r="AL79" s="49"/>
-      <c r="AM79" s="49"/>
-      <c r="AN79" s="49"/>
-      <c r="AO79" s="49"/>
-      <c r="AP79" s="49"/>
-      <c r="AQ79" s="49"/>
-      <c r="AR79" s="49"/>
-      <c r="AS79" s="49"/>
-      <c r="AT79" s="49"/>
-      <c r="AU79" s="49"/>
-      <c r="AV79" s="49"/>
-      <c r="AW79" s="49"/>
-      <c r="AX79" s="49"/>
-      <c r="AY79" s="49"/>
-      <c r="AZ79" s="49"/>
-      <c r="BA79" s="49"/>
-      <c r="BB79" s="49"/>
-      <c r="BC79" s="49"/>
-      <c r="BD79" s="50"/>
+      <c r="B79" s="128"/>
+      <c r="C79" s="129"/>
+      <c r="D79" s="129"/>
+      <c r="E79" s="129"/>
+      <c r="F79" s="129"/>
+      <c r="G79" s="129"/>
+      <c r="H79" s="129"/>
+      <c r="I79" s="129"/>
+      <c r="J79" s="129"/>
+      <c r="K79" s="129"/>
+      <c r="L79" s="129"/>
+      <c r="M79" s="129"/>
+      <c r="N79" s="129"/>
+      <c r="O79" s="129"/>
+      <c r="P79" s="129"/>
+      <c r="Q79" s="129"/>
+      <c r="R79" s="129"/>
+      <c r="S79" s="129"/>
+      <c r="T79" s="129"/>
+      <c r="U79" s="129"/>
+      <c r="V79" s="129"/>
+      <c r="W79" s="129"/>
+      <c r="X79" s="129"/>
+      <c r="Y79" s="129"/>
+      <c r="Z79" s="129"/>
+      <c r="AA79" s="129"/>
+      <c r="AB79" s="129"/>
+      <c r="AC79" s="129"/>
+      <c r="AD79" s="129"/>
+      <c r="AE79" s="129"/>
+      <c r="AF79" s="129"/>
+      <c r="AG79" s="129"/>
+      <c r="AH79" s="129"/>
+      <c r="AI79" s="129"/>
+      <c r="AJ79" s="129"/>
+      <c r="AK79" s="129"/>
+      <c r="AL79" s="129"/>
+      <c r="AM79" s="129"/>
+      <c r="AN79" s="129"/>
+      <c r="AO79" s="129"/>
+      <c r="AP79" s="129"/>
+      <c r="AQ79" s="129"/>
+      <c r="AR79" s="129"/>
+      <c r="AS79" s="129"/>
+      <c r="AT79" s="129"/>
+      <c r="AU79" s="129"/>
+      <c r="AV79" s="129"/>
+      <c r="AW79" s="129"/>
+      <c r="AX79" s="129"/>
+      <c r="AY79" s="129"/>
+      <c r="AZ79" s="129"/>
+      <c r="BA79" s="129"/>
+      <c r="BB79" s="129"/>
+      <c r="BC79" s="129"/>
+      <c r="BD79" s="130"/>
       <c r="BE79" s="57"/>
       <c r="BF79" s="58"/>
       <c r="BG79" s="58"/>
@@ -6548,16 +6551,16 @@
       <c r="AZ81" s="46"/>
       <c r="BA81" s="47"/>
       <c r="BB81" s="54"/>
-      <c r="BC81" s="140"/>
-      <c r="BD81" s="140"/>
-      <c r="BE81" s="140"/>
-      <c r="BF81" s="140"/>
-      <c r="BG81" s="140"/>
-      <c r="BH81" s="140"/>
-      <c r="BI81" s="140"/>
-      <c r="BJ81" s="140"/>
-      <c r="BK81" s="140"/>
-      <c r="BL81" s="140"/>
+      <c r="BC81" s="141"/>
+      <c r="BD81" s="141"/>
+      <c r="BE81" s="141"/>
+      <c r="BF81" s="141"/>
+      <c r="BG81" s="141"/>
+      <c r="BH81" s="141"/>
+      <c r="BI81" s="141"/>
+      <c r="BJ81" s="141"/>
+      <c r="BK81" s="141"/>
+      <c r="BL81" s="141"/>
       <c r="BM81" s="56"/>
     </row>
     <row r="82" spans="1:65" x14ac:dyDescent="0.2">
@@ -6617,16 +6620,16 @@
       <c r="AZ82" s="46"/>
       <c r="BA82" s="47"/>
       <c r="BB82" s="54"/>
-      <c r="BC82" s="140"/>
-      <c r="BD82" s="140"/>
-      <c r="BE82" s="140"/>
-      <c r="BF82" s="140"/>
-      <c r="BG82" s="140"/>
-      <c r="BH82" s="140"/>
-      <c r="BI82" s="140"/>
-      <c r="BJ82" s="140"/>
-      <c r="BK82" s="140"/>
-      <c r="BL82" s="140"/>
+      <c r="BC82" s="141"/>
+      <c r="BD82" s="141"/>
+      <c r="BE82" s="141"/>
+      <c r="BF82" s="141"/>
+      <c r="BG82" s="141"/>
+      <c r="BH82" s="141"/>
+      <c r="BI82" s="141"/>
+      <c r="BJ82" s="141"/>
+      <c r="BK82" s="141"/>
+      <c r="BL82" s="141"/>
       <c r="BM82" s="56"/>
     </row>
     <row r="83" spans="1:65" x14ac:dyDescent="0.2">
@@ -6776,68 +6779,68 @@
         <v>25</v>
       </c>
       <c r="B85" s="54"/>
-      <c r="C85" s="140"/>
-      <c r="D85" s="140"/>
-      <c r="E85" s="140"/>
-      <c r="F85" s="140"/>
-      <c r="G85" s="140"/>
-      <c r="H85" s="140"/>
-      <c r="I85" s="140"/>
-      <c r="J85" s="140"/>
-      <c r="K85" s="140"/>
-      <c r="L85" s="140"/>
-      <c r="M85" s="140"/>
-      <c r="N85" s="140"/>
-      <c r="O85" s="140"/>
-      <c r="P85" s="140"/>
-      <c r="Q85" s="140"/>
-      <c r="R85" s="140"/>
-      <c r="S85" s="140"/>
-      <c r="T85" s="140"/>
-      <c r="U85" s="140"/>
-      <c r="V85" s="140"/>
-      <c r="W85" s="140"/>
-      <c r="X85" s="140"/>
-      <c r="Y85" s="140"/>
-      <c r="Z85" s="140"/>
-      <c r="AA85" s="140"/>
-      <c r="AB85" s="140"/>
-      <c r="AC85" s="140"/>
-      <c r="AD85" s="140"/>
-      <c r="AE85" s="140"/>
-      <c r="AF85" s="140"/>
-      <c r="AG85" s="140"/>
-      <c r="AH85" s="140"/>
-      <c r="AI85" s="140"/>
-      <c r="AJ85" s="140"/>
-      <c r="AK85" s="140"/>
-      <c r="AL85" s="140"/>
-      <c r="AM85" s="140"/>
-      <c r="AN85" s="140"/>
-      <c r="AO85" s="140"/>
-      <c r="AP85" s="140"/>
-      <c r="AQ85" s="140"/>
-      <c r="AR85" s="140"/>
-      <c r="AS85" s="140"/>
-      <c r="AT85" s="140"/>
-      <c r="AU85" s="140"/>
-      <c r="AV85" s="140"/>
-      <c r="AW85" s="140"/>
+      <c r="C85" s="141"/>
+      <c r="D85" s="141"/>
+      <c r="E85" s="141"/>
+      <c r="F85" s="141"/>
+      <c r="G85" s="141"/>
+      <c r="H85" s="141"/>
+      <c r="I85" s="141"/>
+      <c r="J85" s="141"/>
+      <c r="K85" s="141"/>
+      <c r="L85" s="141"/>
+      <c r="M85" s="141"/>
+      <c r="N85" s="141"/>
+      <c r="O85" s="141"/>
+      <c r="P85" s="141"/>
+      <c r="Q85" s="141"/>
+      <c r="R85" s="141"/>
+      <c r="S85" s="141"/>
+      <c r="T85" s="141"/>
+      <c r="U85" s="141"/>
+      <c r="V85" s="141"/>
+      <c r="W85" s="141"/>
+      <c r="X85" s="141"/>
+      <c r="Y85" s="141"/>
+      <c r="Z85" s="141"/>
+      <c r="AA85" s="141"/>
+      <c r="AB85" s="141"/>
+      <c r="AC85" s="141"/>
+      <c r="AD85" s="141"/>
+      <c r="AE85" s="141"/>
+      <c r="AF85" s="141"/>
+      <c r="AG85" s="141"/>
+      <c r="AH85" s="141"/>
+      <c r="AI85" s="141"/>
+      <c r="AJ85" s="141"/>
+      <c r="AK85" s="141"/>
+      <c r="AL85" s="141"/>
+      <c r="AM85" s="141"/>
+      <c r="AN85" s="141"/>
+      <c r="AO85" s="141"/>
+      <c r="AP85" s="141"/>
+      <c r="AQ85" s="141"/>
+      <c r="AR85" s="141"/>
+      <c r="AS85" s="141"/>
+      <c r="AT85" s="141"/>
+      <c r="AU85" s="141"/>
+      <c r="AV85" s="141"/>
+      <c r="AW85" s="141"/>
       <c r="AX85" s="56"/>
       <c r="AY85" s="54"/>
-      <c r="AZ85" s="140"/>
-      <c r="BA85" s="140"/>
-      <c r="BB85" s="140"/>
-      <c r="BC85" s="140"/>
-      <c r="BD85" s="140"/>
-      <c r="BE85" s="140"/>
-      <c r="BF85" s="140"/>
-      <c r="BG85" s="140"/>
-      <c r="BH85" s="140"/>
-      <c r="BI85" s="140"/>
-      <c r="BJ85" s="140"/>
-      <c r="BK85" s="140"/>
-      <c r="BL85" s="140"/>
+      <c r="AZ85" s="141"/>
+      <c r="BA85" s="141"/>
+      <c r="BB85" s="141"/>
+      <c r="BC85" s="141"/>
+      <c r="BD85" s="141"/>
+      <c r="BE85" s="141"/>
+      <c r="BF85" s="141"/>
+      <c r="BG85" s="141"/>
+      <c r="BH85" s="141"/>
+      <c r="BI85" s="141"/>
+      <c r="BJ85" s="141"/>
+      <c r="BK85" s="141"/>
+      <c r="BL85" s="141"/>
       <c r="BM85" s="56"/>
     </row>
     <row r="86" spans="1:65" x14ac:dyDescent="0.2">
@@ -6845,68 +6848,68 @@
         <v>26</v>
       </c>
       <c r="B86" s="54"/>
-      <c r="C86" s="140"/>
-      <c r="D86" s="140"/>
-      <c r="E86" s="140"/>
-      <c r="F86" s="140"/>
-      <c r="G86" s="140"/>
-      <c r="H86" s="140"/>
-      <c r="I86" s="140"/>
-      <c r="J86" s="140"/>
-      <c r="K86" s="140"/>
-      <c r="L86" s="140"/>
-      <c r="M86" s="140"/>
-      <c r="N86" s="140"/>
-      <c r="O86" s="140"/>
-      <c r="P86" s="140"/>
-      <c r="Q86" s="140"/>
-      <c r="R86" s="140"/>
-      <c r="S86" s="140"/>
-      <c r="T86" s="140"/>
-      <c r="U86" s="140"/>
-      <c r="V86" s="140"/>
-      <c r="W86" s="140"/>
-      <c r="X86" s="140"/>
-      <c r="Y86" s="140"/>
-      <c r="Z86" s="140"/>
-      <c r="AA86" s="140"/>
-      <c r="AB86" s="140"/>
-      <c r="AC86" s="140"/>
-      <c r="AD86" s="140"/>
-      <c r="AE86" s="140"/>
-      <c r="AF86" s="140"/>
-      <c r="AG86" s="140"/>
-      <c r="AH86" s="140"/>
-      <c r="AI86" s="140"/>
-      <c r="AJ86" s="140"/>
-      <c r="AK86" s="140"/>
-      <c r="AL86" s="140"/>
-      <c r="AM86" s="140"/>
-      <c r="AN86" s="140"/>
-      <c r="AO86" s="140"/>
-      <c r="AP86" s="140"/>
-      <c r="AQ86" s="140"/>
-      <c r="AR86" s="140"/>
-      <c r="AS86" s="140"/>
-      <c r="AT86" s="140"/>
-      <c r="AU86" s="140"/>
-      <c r="AV86" s="140"/>
-      <c r="AW86" s="140"/>
+      <c r="C86" s="141"/>
+      <c r="D86" s="141"/>
+      <c r="E86" s="141"/>
+      <c r="F86" s="141"/>
+      <c r="G86" s="141"/>
+      <c r="H86" s="141"/>
+      <c r="I86" s="141"/>
+      <c r="J86" s="141"/>
+      <c r="K86" s="141"/>
+      <c r="L86" s="141"/>
+      <c r="M86" s="141"/>
+      <c r="N86" s="141"/>
+      <c r="O86" s="141"/>
+      <c r="P86" s="141"/>
+      <c r="Q86" s="141"/>
+      <c r="R86" s="141"/>
+      <c r="S86" s="141"/>
+      <c r="T86" s="141"/>
+      <c r="U86" s="141"/>
+      <c r="V86" s="141"/>
+      <c r="W86" s="141"/>
+      <c r="X86" s="141"/>
+      <c r="Y86" s="141"/>
+      <c r="Z86" s="141"/>
+      <c r="AA86" s="141"/>
+      <c r="AB86" s="141"/>
+      <c r="AC86" s="141"/>
+      <c r="AD86" s="141"/>
+      <c r="AE86" s="141"/>
+      <c r="AF86" s="141"/>
+      <c r="AG86" s="141"/>
+      <c r="AH86" s="141"/>
+      <c r="AI86" s="141"/>
+      <c r="AJ86" s="141"/>
+      <c r="AK86" s="141"/>
+      <c r="AL86" s="141"/>
+      <c r="AM86" s="141"/>
+      <c r="AN86" s="141"/>
+      <c r="AO86" s="141"/>
+      <c r="AP86" s="141"/>
+      <c r="AQ86" s="141"/>
+      <c r="AR86" s="141"/>
+      <c r="AS86" s="141"/>
+      <c r="AT86" s="141"/>
+      <c r="AU86" s="141"/>
+      <c r="AV86" s="141"/>
+      <c r="AW86" s="141"/>
       <c r="AX86" s="56"/>
       <c r="AY86" s="54"/>
-      <c r="AZ86" s="140"/>
-      <c r="BA86" s="140"/>
-      <c r="BB86" s="140"/>
-      <c r="BC86" s="140"/>
-      <c r="BD86" s="140"/>
-      <c r="BE86" s="140"/>
-      <c r="BF86" s="140"/>
-      <c r="BG86" s="140"/>
-      <c r="BH86" s="140"/>
-      <c r="BI86" s="140"/>
-      <c r="BJ86" s="140"/>
-      <c r="BK86" s="140"/>
-      <c r="BL86" s="140"/>
+      <c r="AZ86" s="141"/>
+      <c r="BA86" s="141"/>
+      <c r="BB86" s="141"/>
+      <c r="BC86" s="141"/>
+      <c r="BD86" s="141"/>
+      <c r="BE86" s="141"/>
+      <c r="BF86" s="141"/>
+      <c r="BG86" s="141"/>
+      <c r="BH86" s="141"/>
+      <c r="BI86" s="141"/>
+      <c r="BJ86" s="141"/>
+      <c r="BK86" s="141"/>
+      <c r="BL86" s="141"/>
       <c r="BM86" s="56"/>
     </row>
     <row r="87" spans="1:65" x14ac:dyDescent="0.2">
@@ -7056,68 +7059,68 @@
         <v>29</v>
       </c>
       <c r="B89" s="54"/>
-      <c r="C89" s="140"/>
-      <c r="D89" s="140"/>
-      <c r="E89" s="140"/>
-      <c r="F89" s="140"/>
-      <c r="G89" s="140"/>
-      <c r="H89" s="140"/>
-      <c r="I89" s="140"/>
-      <c r="J89" s="140"/>
-      <c r="K89" s="140"/>
-      <c r="L89" s="140"/>
-      <c r="M89" s="140"/>
-      <c r="N89" s="140"/>
-      <c r="O89" s="140"/>
-      <c r="P89" s="140"/>
-      <c r="Q89" s="140"/>
-      <c r="R89" s="140"/>
-      <c r="S89" s="140"/>
-      <c r="T89" s="140"/>
-      <c r="U89" s="140"/>
-      <c r="V89" s="140"/>
-      <c r="W89" s="140"/>
-      <c r="X89" s="140"/>
-      <c r="Y89" s="140"/>
-      <c r="Z89" s="140"/>
-      <c r="AA89" s="140"/>
-      <c r="AB89" s="140"/>
-      <c r="AC89" s="140"/>
-      <c r="AD89" s="140"/>
-      <c r="AE89" s="140"/>
-      <c r="AF89" s="140"/>
-      <c r="AG89" s="140"/>
-      <c r="AH89" s="140"/>
-      <c r="AI89" s="140"/>
-      <c r="AJ89" s="140"/>
-      <c r="AK89" s="140"/>
-      <c r="AL89" s="140"/>
-      <c r="AM89" s="140"/>
-      <c r="AN89" s="140"/>
-      <c r="AO89" s="140"/>
-      <c r="AP89" s="140"/>
-      <c r="AQ89" s="140"/>
-      <c r="AR89" s="140"/>
-      <c r="AS89" s="140"/>
-      <c r="AT89" s="140"/>
+      <c r="C89" s="141"/>
+      <c r="D89" s="141"/>
+      <c r="E89" s="141"/>
+      <c r="F89" s="141"/>
+      <c r="G89" s="141"/>
+      <c r="H89" s="141"/>
+      <c r="I89" s="141"/>
+      <c r="J89" s="141"/>
+      <c r="K89" s="141"/>
+      <c r="L89" s="141"/>
+      <c r="M89" s="141"/>
+      <c r="N89" s="141"/>
+      <c r="O89" s="141"/>
+      <c r="P89" s="141"/>
+      <c r="Q89" s="141"/>
+      <c r="R89" s="141"/>
+      <c r="S89" s="141"/>
+      <c r="T89" s="141"/>
+      <c r="U89" s="141"/>
+      <c r="V89" s="141"/>
+      <c r="W89" s="141"/>
+      <c r="X89" s="141"/>
+      <c r="Y89" s="141"/>
+      <c r="Z89" s="141"/>
+      <c r="AA89" s="141"/>
+      <c r="AB89" s="141"/>
+      <c r="AC89" s="141"/>
+      <c r="AD89" s="141"/>
+      <c r="AE89" s="141"/>
+      <c r="AF89" s="141"/>
+      <c r="AG89" s="141"/>
+      <c r="AH89" s="141"/>
+      <c r="AI89" s="141"/>
+      <c r="AJ89" s="141"/>
+      <c r="AK89" s="141"/>
+      <c r="AL89" s="141"/>
+      <c r="AM89" s="141"/>
+      <c r="AN89" s="141"/>
+      <c r="AO89" s="141"/>
+      <c r="AP89" s="141"/>
+      <c r="AQ89" s="141"/>
+      <c r="AR89" s="141"/>
+      <c r="AS89" s="141"/>
+      <c r="AT89" s="141"/>
       <c r="AU89" s="56"/>
       <c r="AV89" s="54"/>
-      <c r="AW89" s="140"/>
-      <c r="AX89" s="140"/>
-      <c r="AY89" s="140"/>
-      <c r="AZ89" s="140"/>
-      <c r="BA89" s="140"/>
-      <c r="BB89" s="140"/>
-      <c r="BC89" s="140"/>
-      <c r="BD89" s="140"/>
-      <c r="BE89" s="140"/>
-      <c r="BF89" s="140"/>
-      <c r="BG89" s="140"/>
-      <c r="BH89" s="140"/>
-      <c r="BI89" s="140"/>
-      <c r="BJ89" s="140"/>
-      <c r="BK89" s="140"/>
-      <c r="BL89" s="140"/>
+      <c r="AW89" s="141"/>
+      <c r="AX89" s="141"/>
+      <c r="AY89" s="141"/>
+      <c r="AZ89" s="141"/>
+      <c r="BA89" s="141"/>
+      <c r="BB89" s="141"/>
+      <c r="BC89" s="141"/>
+      <c r="BD89" s="141"/>
+      <c r="BE89" s="141"/>
+      <c r="BF89" s="141"/>
+      <c r="BG89" s="141"/>
+      <c r="BH89" s="141"/>
+      <c r="BI89" s="141"/>
+      <c r="BJ89" s="141"/>
+      <c r="BK89" s="141"/>
+      <c r="BL89" s="141"/>
       <c r="BM89" s="56"/>
     </row>
     <row r="90" spans="1:65" x14ac:dyDescent="0.2">
@@ -7125,68 +7128,68 @@
         <v>30</v>
       </c>
       <c r="B90" s="54"/>
-      <c r="C90" s="140"/>
-      <c r="D90" s="140"/>
-      <c r="E90" s="140"/>
-      <c r="F90" s="140"/>
-      <c r="G90" s="140"/>
-      <c r="H90" s="140"/>
-      <c r="I90" s="140"/>
-      <c r="J90" s="140"/>
-      <c r="K90" s="140"/>
-      <c r="L90" s="140"/>
-      <c r="M90" s="140"/>
-      <c r="N90" s="140"/>
-      <c r="O90" s="140"/>
-      <c r="P90" s="140"/>
-      <c r="Q90" s="140"/>
-      <c r="R90" s="140"/>
-      <c r="S90" s="140"/>
-      <c r="T90" s="140"/>
-      <c r="U90" s="140"/>
-      <c r="V90" s="140"/>
-      <c r="W90" s="140"/>
-      <c r="X90" s="140"/>
-      <c r="Y90" s="140"/>
-      <c r="Z90" s="140"/>
-      <c r="AA90" s="140"/>
-      <c r="AB90" s="140"/>
-      <c r="AC90" s="140"/>
-      <c r="AD90" s="140"/>
-      <c r="AE90" s="140"/>
-      <c r="AF90" s="140"/>
-      <c r="AG90" s="140"/>
-      <c r="AH90" s="140"/>
-      <c r="AI90" s="140"/>
-      <c r="AJ90" s="140"/>
-      <c r="AK90" s="140"/>
-      <c r="AL90" s="140"/>
-      <c r="AM90" s="140"/>
-      <c r="AN90" s="140"/>
-      <c r="AO90" s="140"/>
-      <c r="AP90" s="140"/>
-      <c r="AQ90" s="140"/>
-      <c r="AR90" s="140"/>
-      <c r="AS90" s="140"/>
-      <c r="AT90" s="140"/>
+      <c r="C90" s="141"/>
+      <c r="D90" s="141"/>
+      <c r="E90" s="141"/>
+      <c r="F90" s="141"/>
+      <c r="G90" s="141"/>
+      <c r="H90" s="141"/>
+      <c r="I90" s="141"/>
+      <c r="J90" s="141"/>
+      <c r="K90" s="141"/>
+      <c r="L90" s="141"/>
+      <c r="M90" s="141"/>
+      <c r="N90" s="141"/>
+      <c r="O90" s="141"/>
+      <c r="P90" s="141"/>
+      <c r="Q90" s="141"/>
+      <c r="R90" s="141"/>
+      <c r="S90" s="141"/>
+      <c r="T90" s="141"/>
+      <c r="U90" s="141"/>
+      <c r="V90" s="141"/>
+      <c r="W90" s="141"/>
+      <c r="X90" s="141"/>
+      <c r="Y90" s="141"/>
+      <c r="Z90" s="141"/>
+      <c r="AA90" s="141"/>
+      <c r="AB90" s="141"/>
+      <c r="AC90" s="141"/>
+      <c r="AD90" s="141"/>
+      <c r="AE90" s="141"/>
+      <c r="AF90" s="141"/>
+      <c r="AG90" s="141"/>
+      <c r="AH90" s="141"/>
+      <c r="AI90" s="141"/>
+      <c r="AJ90" s="141"/>
+      <c r="AK90" s="141"/>
+      <c r="AL90" s="141"/>
+      <c r="AM90" s="141"/>
+      <c r="AN90" s="141"/>
+      <c r="AO90" s="141"/>
+      <c r="AP90" s="141"/>
+      <c r="AQ90" s="141"/>
+      <c r="AR90" s="141"/>
+      <c r="AS90" s="141"/>
+      <c r="AT90" s="141"/>
       <c r="AU90" s="56"/>
       <c r="AV90" s="54"/>
-      <c r="AW90" s="140"/>
-      <c r="AX90" s="140"/>
-      <c r="AY90" s="140"/>
-      <c r="AZ90" s="140"/>
-      <c r="BA90" s="140"/>
-      <c r="BB90" s="140"/>
-      <c r="BC90" s="140"/>
-      <c r="BD90" s="140"/>
-      <c r="BE90" s="140"/>
-      <c r="BF90" s="140"/>
-      <c r="BG90" s="140"/>
-      <c r="BH90" s="140"/>
-      <c r="BI90" s="140"/>
-      <c r="BJ90" s="140"/>
-      <c r="BK90" s="140"/>
-      <c r="BL90" s="140"/>
+      <c r="AW90" s="141"/>
+      <c r="AX90" s="141"/>
+      <c r="AY90" s="141"/>
+      <c r="AZ90" s="141"/>
+      <c r="BA90" s="141"/>
+      <c r="BB90" s="141"/>
+      <c r="BC90" s="141"/>
+      <c r="BD90" s="141"/>
+      <c r="BE90" s="141"/>
+      <c r="BF90" s="141"/>
+      <c r="BG90" s="141"/>
+      <c r="BH90" s="141"/>
+      <c r="BI90" s="141"/>
+      <c r="BJ90" s="141"/>
+      <c r="BK90" s="141"/>
+      <c r="BL90" s="141"/>
       <c r="BM90" s="56"/>
     </row>
     <row r="91" spans="1:65" x14ac:dyDescent="0.2">
@@ -7336,68 +7339,68 @@
         <v>33</v>
       </c>
       <c r="B93" s="54"/>
-      <c r="C93" s="140"/>
-      <c r="D93" s="140"/>
-      <c r="E93" s="140"/>
-      <c r="F93" s="140"/>
-      <c r="G93" s="140"/>
-      <c r="H93" s="140"/>
-      <c r="I93" s="140"/>
-      <c r="J93" s="140"/>
-      <c r="K93" s="140"/>
-      <c r="L93" s="140"/>
-      <c r="M93" s="140"/>
-      <c r="N93" s="140"/>
-      <c r="O93" s="140"/>
-      <c r="P93" s="140"/>
-      <c r="Q93" s="140"/>
-      <c r="R93" s="140"/>
-      <c r="S93" s="140"/>
-      <c r="T93" s="140"/>
-      <c r="U93" s="140"/>
-      <c r="V93" s="140"/>
-      <c r="W93" s="140"/>
-      <c r="X93" s="140"/>
-      <c r="Y93" s="140"/>
-      <c r="Z93" s="140"/>
-      <c r="AA93" s="140"/>
-      <c r="AB93" s="140"/>
-      <c r="AC93" s="140"/>
-      <c r="AD93" s="140"/>
-      <c r="AE93" s="140"/>
-      <c r="AF93" s="140"/>
-      <c r="AG93" s="140"/>
-      <c r="AH93" s="140"/>
-      <c r="AI93" s="140"/>
-      <c r="AJ93" s="140"/>
-      <c r="AK93" s="140"/>
-      <c r="AL93" s="140"/>
-      <c r="AM93" s="140"/>
-      <c r="AN93" s="140"/>
-      <c r="AO93" s="140"/>
-      <c r="AP93" s="140"/>
-      <c r="AQ93" s="140"/>
+      <c r="C93" s="141"/>
+      <c r="D93" s="141"/>
+      <c r="E93" s="141"/>
+      <c r="F93" s="141"/>
+      <c r="G93" s="141"/>
+      <c r="H93" s="141"/>
+      <c r="I93" s="141"/>
+      <c r="J93" s="141"/>
+      <c r="K93" s="141"/>
+      <c r="L93" s="141"/>
+      <c r="M93" s="141"/>
+      <c r="N93" s="141"/>
+      <c r="O93" s="141"/>
+      <c r="P93" s="141"/>
+      <c r="Q93" s="141"/>
+      <c r="R93" s="141"/>
+      <c r="S93" s="141"/>
+      <c r="T93" s="141"/>
+      <c r="U93" s="141"/>
+      <c r="V93" s="141"/>
+      <c r="W93" s="141"/>
+      <c r="X93" s="141"/>
+      <c r="Y93" s="141"/>
+      <c r="Z93" s="141"/>
+      <c r="AA93" s="141"/>
+      <c r="AB93" s="141"/>
+      <c r="AC93" s="141"/>
+      <c r="AD93" s="141"/>
+      <c r="AE93" s="141"/>
+      <c r="AF93" s="141"/>
+      <c r="AG93" s="141"/>
+      <c r="AH93" s="141"/>
+      <c r="AI93" s="141"/>
+      <c r="AJ93" s="141"/>
+      <c r="AK93" s="141"/>
+      <c r="AL93" s="141"/>
+      <c r="AM93" s="141"/>
+      <c r="AN93" s="141"/>
+      <c r="AO93" s="141"/>
+      <c r="AP93" s="141"/>
+      <c r="AQ93" s="141"/>
       <c r="AR93" s="56"/>
       <c r="AS93" s="54"/>
-      <c r="AT93" s="140"/>
-      <c r="AU93" s="140"/>
-      <c r="AV93" s="140"/>
-      <c r="AW93" s="140"/>
-      <c r="AX93" s="140"/>
-      <c r="AY93" s="140"/>
-      <c r="AZ93" s="140"/>
-      <c r="BA93" s="140"/>
-      <c r="BB93" s="140"/>
-      <c r="BC93" s="140"/>
-      <c r="BD93" s="140"/>
-      <c r="BE93" s="140"/>
-      <c r="BF93" s="140"/>
-      <c r="BG93" s="140"/>
-      <c r="BH93" s="140"/>
-      <c r="BI93" s="140"/>
-      <c r="BJ93" s="140"/>
-      <c r="BK93" s="140"/>
-      <c r="BL93" s="140"/>
+      <c r="AT93" s="141"/>
+      <c r="AU93" s="141"/>
+      <c r="AV93" s="141"/>
+      <c r="AW93" s="141"/>
+      <c r="AX93" s="141"/>
+      <c r="AY93" s="141"/>
+      <c r="AZ93" s="141"/>
+      <c r="BA93" s="141"/>
+      <c r="BB93" s="141"/>
+      <c r="BC93" s="141"/>
+      <c r="BD93" s="141"/>
+      <c r="BE93" s="141"/>
+      <c r="BF93" s="141"/>
+      <c r="BG93" s="141"/>
+      <c r="BH93" s="141"/>
+      <c r="BI93" s="141"/>
+      <c r="BJ93" s="141"/>
+      <c r="BK93" s="141"/>
+      <c r="BL93" s="141"/>
       <c r="BM93" s="56"/>
     </row>
     <row r="94" spans="1:65" x14ac:dyDescent="0.2">
@@ -7405,68 +7408,68 @@
         <v>34</v>
       </c>
       <c r="B94" s="54"/>
-      <c r="C94" s="140"/>
-      <c r="D94" s="140"/>
-      <c r="E94" s="140"/>
-      <c r="F94" s="140"/>
-      <c r="G94" s="140"/>
-      <c r="H94" s="140"/>
-      <c r="I94" s="140"/>
-      <c r="J94" s="140"/>
-      <c r="K94" s="140"/>
-      <c r="L94" s="140"/>
-      <c r="M94" s="140"/>
-      <c r="N94" s="140"/>
-      <c r="O94" s="140"/>
-      <c r="P94" s="140"/>
-      <c r="Q94" s="140"/>
-      <c r="R94" s="140"/>
-      <c r="S94" s="140"/>
-      <c r="T94" s="140"/>
-      <c r="U94" s="140"/>
-      <c r="V94" s="140"/>
-      <c r="W94" s="140"/>
-      <c r="X94" s="140"/>
-      <c r="Y94" s="140"/>
-      <c r="Z94" s="140"/>
-      <c r="AA94" s="140"/>
-      <c r="AB94" s="140"/>
-      <c r="AC94" s="140"/>
-      <c r="AD94" s="140"/>
-      <c r="AE94" s="140"/>
-      <c r="AF94" s="140"/>
-      <c r="AG94" s="140"/>
-      <c r="AH94" s="140"/>
-      <c r="AI94" s="140"/>
-      <c r="AJ94" s="140"/>
-      <c r="AK94" s="140"/>
-      <c r="AL94" s="140"/>
-      <c r="AM94" s="140"/>
-      <c r="AN94" s="140"/>
-      <c r="AO94" s="140"/>
-      <c r="AP94" s="140"/>
-      <c r="AQ94" s="140"/>
+      <c r="C94" s="141"/>
+      <c r="D94" s="141"/>
+      <c r="E94" s="141"/>
+      <c r="F94" s="141"/>
+      <c r="G94" s="141"/>
+      <c r="H94" s="141"/>
+      <c r="I94" s="141"/>
+      <c r="J94" s="141"/>
+      <c r="K94" s="141"/>
+      <c r="L94" s="141"/>
+      <c r="M94" s="141"/>
+      <c r="N94" s="141"/>
+      <c r="O94" s="141"/>
+      <c r="P94" s="141"/>
+      <c r="Q94" s="141"/>
+      <c r="R94" s="141"/>
+      <c r="S94" s="141"/>
+      <c r="T94" s="141"/>
+      <c r="U94" s="141"/>
+      <c r="V94" s="141"/>
+      <c r="W94" s="141"/>
+      <c r="X94" s="141"/>
+      <c r="Y94" s="141"/>
+      <c r="Z94" s="141"/>
+      <c r="AA94" s="141"/>
+      <c r="AB94" s="141"/>
+      <c r="AC94" s="141"/>
+      <c r="AD94" s="141"/>
+      <c r="AE94" s="141"/>
+      <c r="AF94" s="141"/>
+      <c r="AG94" s="141"/>
+      <c r="AH94" s="141"/>
+      <c r="AI94" s="141"/>
+      <c r="AJ94" s="141"/>
+      <c r="AK94" s="141"/>
+      <c r="AL94" s="141"/>
+      <c r="AM94" s="141"/>
+      <c r="AN94" s="141"/>
+      <c r="AO94" s="141"/>
+      <c r="AP94" s="141"/>
+      <c r="AQ94" s="141"/>
       <c r="AR94" s="56"/>
       <c r="AS94" s="54"/>
-      <c r="AT94" s="140"/>
-      <c r="AU94" s="140"/>
-      <c r="AV94" s="140"/>
-      <c r="AW94" s="140"/>
-      <c r="AX94" s="140"/>
-      <c r="AY94" s="140"/>
-      <c r="AZ94" s="140"/>
-      <c r="BA94" s="140"/>
-      <c r="BB94" s="140"/>
-      <c r="BC94" s="140"/>
-      <c r="BD94" s="140"/>
-      <c r="BE94" s="140"/>
-      <c r="BF94" s="140"/>
-      <c r="BG94" s="140"/>
-      <c r="BH94" s="140"/>
-      <c r="BI94" s="140"/>
-      <c r="BJ94" s="140"/>
-      <c r="BK94" s="140"/>
-      <c r="BL94" s="140"/>
+      <c r="AT94" s="141"/>
+      <c r="AU94" s="141"/>
+      <c r="AV94" s="141"/>
+      <c r="AW94" s="141"/>
+      <c r="AX94" s="141"/>
+      <c r="AY94" s="141"/>
+      <c r="AZ94" s="141"/>
+      <c r="BA94" s="141"/>
+      <c r="BB94" s="141"/>
+      <c r="BC94" s="141"/>
+      <c r="BD94" s="141"/>
+      <c r="BE94" s="141"/>
+      <c r="BF94" s="141"/>
+      <c r="BG94" s="141"/>
+      <c r="BH94" s="141"/>
+      <c r="BI94" s="141"/>
+      <c r="BJ94" s="141"/>
+      <c r="BK94" s="141"/>
+      <c r="BL94" s="141"/>
       <c r="BM94" s="56"/>
     </row>
     <row r="95" spans="1:65" x14ac:dyDescent="0.2">
@@ -7616,68 +7619,68 @@
         <v>37</v>
       </c>
       <c r="B97" s="54"/>
-      <c r="C97" s="140"/>
-      <c r="D97" s="140"/>
-      <c r="E97" s="140"/>
-      <c r="F97" s="140"/>
-      <c r="G97" s="140"/>
-      <c r="H97" s="140"/>
-      <c r="I97" s="140"/>
-      <c r="J97" s="140"/>
-      <c r="K97" s="140"/>
-      <c r="L97" s="140"/>
-      <c r="M97" s="140"/>
-      <c r="N97" s="140"/>
-      <c r="O97" s="140"/>
-      <c r="P97" s="140"/>
-      <c r="Q97" s="140"/>
-      <c r="R97" s="140"/>
-      <c r="S97" s="140"/>
-      <c r="T97" s="140"/>
-      <c r="U97" s="140"/>
-      <c r="V97" s="140"/>
-      <c r="W97" s="140"/>
-      <c r="X97" s="140"/>
-      <c r="Y97" s="140"/>
-      <c r="Z97" s="140"/>
-      <c r="AA97" s="140"/>
-      <c r="AB97" s="140"/>
-      <c r="AC97" s="140"/>
-      <c r="AD97" s="140"/>
-      <c r="AE97" s="140"/>
-      <c r="AF97" s="140"/>
-      <c r="AG97" s="140"/>
-      <c r="AH97" s="140"/>
-      <c r="AI97" s="140"/>
-      <c r="AJ97" s="140"/>
-      <c r="AK97" s="140"/>
-      <c r="AL97" s="140"/>
-      <c r="AM97" s="140"/>
-      <c r="AN97" s="140"/>
+      <c r="C97" s="141"/>
+      <c r="D97" s="141"/>
+      <c r="E97" s="141"/>
+      <c r="F97" s="141"/>
+      <c r="G97" s="141"/>
+      <c r="H97" s="141"/>
+      <c r="I97" s="141"/>
+      <c r="J97" s="141"/>
+      <c r="K97" s="141"/>
+      <c r="L97" s="141"/>
+      <c r="M97" s="141"/>
+      <c r="N97" s="141"/>
+      <c r="O97" s="141"/>
+      <c r="P97" s="141"/>
+      <c r="Q97" s="141"/>
+      <c r="R97" s="141"/>
+      <c r="S97" s="141"/>
+      <c r="T97" s="141"/>
+      <c r="U97" s="141"/>
+      <c r="V97" s="141"/>
+      <c r="W97" s="141"/>
+      <c r="X97" s="141"/>
+      <c r="Y97" s="141"/>
+      <c r="Z97" s="141"/>
+      <c r="AA97" s="141"/>
+      <c r="AB97" s="141"/>
+      <c r="AC97" s="141"/>
+      <c r="AD97" s="141"/>
+      <c r="AE97" s="141"/>
+      <c r="AF97" s="141"/>
+      <c r="AG97" s="141"/>
+      <c r="AH97" s="141"/>
+      <c r="AI97" s="141"/>
+      <c r="AJ97" s="141"/>
+      <c r="AK97" s="141"/>
+      <c r="AL97" s="141"/>
+      <c r="AM97" s="141"/>
+      <c r="AN97" s="141"/>
       <c r="AO97" s="56"/>
       <c r="AP97" s="54"/>
-      <c r="AQ97" s="140"/>
-      <c r="AR97" s="140"/>
-      <c r="AS97" s="140"/>
-      <c r="AT97" s="140"/>
-      <c r="AU97" s="140"/>
-      <c r="AV97" s="140"/>
-      <c r="AW97" s="140"/>
-      <c r="AX97" s="140"/>
-      <c r="AY97" s="140"/>
-      <c r="AZ97" s="140"/>
-      <c r="BA97" s="140"/>
-      <c r="BB97" s="140"/>
-      <c r="BC97" s="140"/>
-      <c r="BD97" s="140"/>
-      <c r="BE97" s="140"/>
-      <c r="BF97" s="140"/>
-      <c r="BG97" s="140"/>
-      <c r="BH97" s="140"/>
-      <c r="BI97" s="140"/>
-      <c r="BJ97" s="140"/>
-      <c r="BK97" s="140"/>
-      <c r="BL97" s="140"/>
+      <c r="AQ97" s="141"/>
+      <c r="AR97" s="141"/>
+      <c r="AS97" s="141"/>
+      <c r="AT97" s="141"/>
+      <c r="AU97" s="141"/>
+      <c r="AV97" s="141"/>
+      <c r="AW97" s="141"/>
+      <c r="AX97" s="141"/>
+      <c r="AY97" s="141"/>
+      <c r="AZ97" s="141"/>
+      <c r="BA97" s="141"/>
+      <c r="BB97" s="141"/>
+      <c r="BC97" s="141"/>
+      <c r="BD97" s="141"/>
+      <c r="BE97" s="141"/>
+      <c r="BF97" s="141"/>
+      <c r="BG97" s="141"/>
+      <c r="BH97" s="141"/>
+      <c r="BI97" s="141"/>
+      <c r="BJ97" s="141"/>
+      <c r="BK97" s="141"/>
+      <c r="BL97" s="141"/>
       <c r="BM97" s="56"/>
     </row>
     <row r="98" spans="1:65" x14ac:dyDescent="0.2">
@@ -7685,68 +7688,68 @@
         <v>38</v>
       </c>
       <c r="B98" s="54"/>
-      <c r="C98" s="140"/>
-      <c r="D98" s="140"/>
-      <c r="E98" s="140"/>
-      <c r="F98" s="140"/>
-      <c r="G98" s="140"/>
-      <c r="H98" s="140"/>
-      <c r="I98" s="140"/>
-      <c r="J98" s="140"/>
-      <c r="K98" s="140"/>
-      <c r="L98" s="140"/>
-      <c r="M98" s="140"/>
-      <c r="N98" s="140"/>
-      <c r="O98" s="140"/>
-      <c r="P98" s="140"/>
-      <c r="Q98" s="140"/>
-      <c r="R98" s="140"/>
-      <c r="S98" s="140"/>
-      <c r="T98" s="140"/>
-      <c r="U98" s="140"/>
-      <c r="V98" s="140"/>
-      <c r="W98" s="140"/>
-      <c r="X98" s="140"/>
-      <c r="Y98" s="140"/>
-      <c r="Z98" s="140"/>
-      <c r="AA98" s="140"/>
-      <c r="AB98" s="140"/>
-      <c r="AC98" s="140"/>
-      <c r="AD98" s="140"/>
-      <c r="AE98" s="140"/>
-      <c r="AF98" s="140"/>
-      <c r="AG98" s="140"/>
-      <c r="AH98" s="140"/>
-      <c r="AI98" s="140"/>
-      <c r="AJ98" s="140"/>
-      <c r="AK98" s="140"/>
-      <c r="AL98" s="140"/>
-      <c r="AM98" s="140"/>
-      <c r="AN98" s="140"/>
+      <c r="C98" s="141"/>
+      <c r="D98" s="141"/>
+      <c r="E98" s="141"/>
+      <c r="F98" s="141"/>
+      <c r="G98" s="141"/>
+      <c r="H98" s="141"/>
+      <c r="I98" s="141"/>
+      <c r="J98" s="141"/>
+      <c r="K98" s="141"/>
+      <c r="L98" s="141"/>
+      <c r="M98" s="141"/>
+      <c r="N98" s="141"/>
+      <c r="O98" s="141"/>
+      <c r="P98" s="141"/>
+      <c r="Q98" s="141"/>
+      <c r="R98" s="141"/>
+      <c r="S98" s="141"/>
+      <c r="T98" s="141"/>
+      <c r="U98" s="141"/>
+      <c r="V98" s="141"/>
+      <c r="W98" s="141"/>
+      <c r="X98" s="141"/>
+      <c r="Y98" s="141"/>
+      <c r="Z98" s="141"/>
+      <c r="AA98" s="141"/>
+      <c r="AB98" s="141"/>
+      <c r="AC98" s="141"/>
+      <c r="AD98" s="141"/>
+      <c r="AE98" s="141"/>
+      <c r="AF98" s="141"/>
+      <c r="AG98" s="141"/>
+      <c r="AH98" s="141"/>
+      <c r="AI98" s="141"/>
+      <c r="AJ98" s="141"/>
+      <c r="AK98" s="141"/>
+      <c r="AL98" s="141"/>
+      <c r="AM98" s="141"/>
+      <c r="AN98" s="141"/>
       <c r="AO98" s="56"/>
       <c r="AP98" s="54"/>
-      <c r="AQ98" s="140"/>
-      <c r="AR98" s="140"/>
-      <c r="AS98" s="140"/>
-      <c r="AT98" s="140"/>
-      <c r="AU98" s="140"/>
-      <c r="AV98" s="140"/>
-      <c r="AW98" s="140"/>
-      <c r="AX98" s="140"/>
-      <c r="AY98" s="140"/>
-      <c r="AZ98" s="140"/>
-      <c r="BA98" s="140"/>
-      <c r="BB98" s="140"/>
-      <c r="BC98" s="140"/>
-      <c r="BD98" s="140"/>
-      <c r="BE98" s="140"/>
-      <c r="BF98" s="140"/>
-      <c r="BG98" s="140"/>
-      <c r="BH98" s="140"/>
-      <c r="BI98" s="140"/>
-      <c r="BJ98" s="140"/>
-      <c r="BK98" s="140"/>
-      <c r="BL98" s="140"/>
+      <c r="AQ98" s="141"/>
+      <c r="AR98" s="141"/>
+      <c r="AS98" s="141"/>
+      <c r="AT98" s="141"/>
+      <c r="AU98" s="141"/>
+      <c r="AV98" s="141"/>
+      <c r="AW98" s="141"/>
+      <c r="AX98" s="141"/>
+      <c r="AY98" s="141"/>
+      <c r="AZ98" s="141"/>
+      <c r="BA98" s="141"/>
+      <c r="BB98" s="141"/>
+      <c r="BC98" s="141"/>
+      <c r="BD98" s="141"/>
+      <c r="BE98" s="141"/>
+      <c r="BF98" s="141"/>
+      <c r="BG98" s="141"/>
+      <c r="BH98" s="141"/>
+      <c r="BI98" s="141"/>
+      <c r="BJ98" s="141"/>
+      <c r="BK98" s="141"/>
+      <c r="BL98" s="141"/>
       <c r="BM98" s="56"/>
     </row>
     <row r="99" spans="1:65" x14ac:dyDescent="0.2">
@@ -7896,68 +7899,68 @@
         <v>41</v>
       </c>
       <c r="B101" s="54"/>
-      <c r="C101" s="140"/>
-      <c r="D101" s="140"/>
-      <c r="E101" s="140"/>
-      <c r="F101" s="140"/>
-      <c r="G101" s="140"/>
-      <c r="H101" s="140"/>
-      <c r="I101" s="140"/>
-      <c r="J101" s="140"/>
-      <c r="K101" s="140"/>
-      <c r="L101" s="140"/>
-      <c r="M101" s="140"/>
-      <c r="N101" s="140"/>
-      <c r="O101" s="140"/>
-      <c r="P101" s="140"/>
-      <c r="Q101" s="140"/>
-      <c r="R101" s="140"/>
-      <c r="S101" s="140"/>
-      <c r="T101" s="140"/>
-      <c r="U101" s="140"/>
-      <c r="V101" s="140"/>
-      <c r="W101" s="140"/>
-      <c r="X101" s="140"/>
-      <c r="Y101" s="140"/>
-      <c r="Z101" s="140"/>
-      <c r="AA101" s="140"/>
-      <c r="AB101" s="140"/>
-      <c r="AC101" s="140"/>
-      <c r="AD101" s="140"/>
-      <c r="AE101" s="140"/>
-      <c r="AF101" s="140"/>
-      <c r="AG101" s="140"/>
-      <c r="AH101" s="140"/>
-      <c r="AI101" s="140"/>
-      <c r="AJ101" s="140"/>
-      <c r="AK101" s="140"/>
+      <c r="C101" s="141"/>
+      <c r="D101" s="141"/>
+      <c r="E101" s="141"/>
+      <c r="F101" s="141"/>
+      <c r="G101" s="141"/>
+      <c r="H101" s="141"/>
+      <c r="I101" s="141"/>
+      <c r="J101" s="141"/>
+      <c r="K101" s="141"/>
+      <c r="L101" s="141"/>
+      <c r="M101" s="141"/>
+      <c r="N101" s="141"/>
+      <c r="O101" s="141"/>
+      <c r="P101" s="141"/>
+      <c r="Q101" s="141"/>
+      <c r="R101" s="141"/>
+      <c r="S101" s="141"/>
+      <c r="T101" s="141"/>
+      <c r="U101" s="141"/>
+      <c r="V101" s="141"/>
+      <c r="W101" s="141"/>
+      <c r="X101" s="141"/>
+      <c r="Y101" s="141"/>
+      <c r="Z101" s="141"/>
+      <c r="AA101" s="141"/>
+      <c r="AB101" s="141"/>
+      <c r="AC101" s="141"/>
+      <c r="AD101" s="141"/>
+      <c r="AE101" s="141"/>
+      <c r="AF101" s="141"/>
+      <c r="AG101" s="141"/>
+      <c r="AH101" s="141"/>
+      <c r="AI101" s="141"/>
+      <c r="AJ101" s="141"/>
+      <c r="AK101" s="141"/>
       <c r="AL101" s="56"/>
       <c r="AM101" s="54"/>
-      <c r="AN101" s="140"/>
-      <c r="AO101" s="140"/>
-      <c r="AP101" s="140"/>
-      <c r="AQ101" s="140"/>
-      <c r="AR101" s="140"/>
-      <c r="AS101" s="140"/>
-      <c r="AT101" s="140"/>
-      <c r="AU101" s="140"/>
-      <c r="AV101" s="140"/>
-      <c r="AW101" s="140"/>
-      <c r="AX101" s="140"/>
-      <c r="AY101" s="140"/>
-      <c r="AZ101" s="140"/>
-      <c r="BA101" s="140"/>
-      <c r="BB101" s="140"/>
-      <c r="BC101" s="140"/>
-      <c r="BD101" s="140"/>
-      <c r="BE101" s="140"/>
-      <c r="BF101" s="140"/>
-      <c r="BG101" s="140"/>
-      <c r="BH101" s="140"/>
-      <c r="BI101" s="140"/>
-      <c r="BJ101" s="140"/>
-      <c r="BK101" s="140"/>
-      <c r="BL101" s="140"/>
+      <c r="AN101" s="141"/>
+      <c r="AO101" s="141"/>
+      <c r="AP101" s="141"/>
+      <c r="AQ101" s="141"/>
+      <c r="AR101" s="141"/>
+      <c r="AS101" s="141"/>
+      <c r="AT101" s="141"/>
+      <c r="AU101" s="141"/>
+      <c r="AV101" s="141"/>
+      <c r="AW101" s="141"/>
+      <c r="AX101" s="141"/>
+      <c r="AY101" s="141"/>
+      <c r="AZ101" s="141"/>
+      <c r="BA101" s="141"/>
+      <c r="BB101" s="141"/>
+      <c r="BC101" s="141"/>
+      <c r="BD101" s="141"/>
+      <c r="BE101" s="141"/>
+      <c r="BF101" s="141"/>
+      <c r="BG101" s="141"/>
+      <c r="BH101" s="141"/>
+      <c r="BI101" s="141"/>
+      <c r="BJ101" s="141"/>
+      <c r="BK101" s="141"/>
+      <c r="BL101" s="141"/>
       <c r="BM101" s="56"/>
     </row>
     <row r="102" spans="1:65" x14ac:dyDescent="0.2">
@@ -7965,68 +7968,68 @@
         <v>42</v>
       </c>
       <c r="B102" s="54"/>
-      <c r="C102" s="140"/>
-      <c r="D102" s="140"/>
-      <c r="E102" s="140"/>
-      <c r="F102" s="140"/>
-      <c r="G102" s="140"/>
-      <c r="H102" s="140"/>
-      <c r="I102" s="140"/>
-      <c r="J102" s="140"/>
-      <c r="K102" s="140"/>
-      <c r="L102" s="140"/>
-      <c r="M102" s="140"/>
-      <c r="N102" s="140"/>
-      <c r="O102" s="140"/>
-      <c r="P102" s="140"/>
-      <c r="Q102" s="140"/>
-      <c r="R102" s="140"/>
-      <c r="S102" s="140"/>
-      <c r="T102" s="140"/>
-      <c r="U102" s="140"/>
-      <c r="V102" s="140"/>
-      <c r="W102" s="140"/>
-      <c r="X102" s="140"/>
-      <c r="Y102" s="140"/>
-      <c r="Z102" s="140"/>
-      <c r="AA102" s="140"/>
-      <c r="AB102" s="140"/>
-      <c r="AC102" s="140"/>
-      <c r="AD102" s="140"/>
-      <c r="AE102" s="140"/>
-      <c r="AF102" s="140"/>
-      <c r="AG102" s="140"/>
-      <c r="AH102" s="140"/>
-      <c r="AI102" s="140"/>
-      <c r="AJ102" s="140"/>
-      <c r="AK102" s="140"/>
+      <c r="C102" s="141"/>
+      <c r="D102" s="141"/>
+      <c r="E102" s="141"/>
+      <c r="F102" s="141"/>
+      <c r="G102" s="141"/>
+      <c r="H102" s="141"/>
+      <c r="I102" s="141"/>
+      <c r="J102" s="141"/>
+      <c r="K102" s="141"/>
+      <c r="L102" s="141"/>
+      <c r="M102" s="141"/>
+      <c r="N102" s="141"/>
+      <c r="O102" s="141"/>
+      <c r="P102" s="141"/>
+      <c r="Q102" s="141"/>
+      <c r="R102" s="141"/>
+      <c r="S102" s="141"/>
+      <c r="T102" s="141"/>
+      <c r="U102" s="141"/>
+      <c r="V102" s="141"/>
+      <c r="W102" s="141"/>
+      <c r="X102" s="141"/>
+      <c r="Y102" s="141"/>
+      <c r="Z102" s="141"/>
+      <c r="AA102" s="141"/>
+      <c r="AB102" s="141"/>
+      <c r="AC102" s="141"/>
+      <c r="AD102" s="141"/>
+      <c r="AE102" s="141"/>
+      <c r="AF102" s="141"/>
+      <c r="AG102" s="141"/>
+      <c r="AH102" s="141"/>
+      <c r="AI102" s="141"/>
+      <c r="AJ102" s="141"/>
+      <c r="AK102" s="141"/>
       <c r="AL102" s="56"/>
       <c r="AM102" s="54"/>
-      <c r="AN102" s="140"/>
-      <c r="AO102" s="140"/>
-      <c r="AP102" s="140"/>
-      <c r="AQ102" s="140"/>
-      <c r="AR102" s="140"/>
-      <c r="AS102" s="140"/>
-      <c r="AT102" s="140"/>
-      <c r="AU102" s="140"/>
-      <c r="AV102" s="140"/>
-      <c r="AW102" s="140"/>
-      <c r="AX102" s="140"/>
-      <c r="AY102" s="140"/>
-      <c r="AZ102" s="140"/>
-      <c r="BA102" s="140"/>
-      <c r="BB102" s="140"/>
-      <c r="BC102" s="140"/>
-      <c r="BD102" s="140"/>
-      <c r="BE102" s="140"/>
-      <c r="BF102" s="140"/>
-      <c r="BG102" s="140"/>
-      <c r="BH102" s="140"/>
-      <c r="BI102" s="140"/>
-      <c r="BJ102" s="140"/>
-      <c r="BK102" s="140"/>
-      <c r="BL102" s="140"/>
+      <c r="AN102" s="141"/>
+      <c r="AO102" s="141"/>
+      <c r="AP102" s="141"/>
+      <c r="AQ102" s="141"/>
+      <c r="AR102" s="141"/>
+      <c r="AS102" s="141"/>
+      <c r="AT102" s="141"/>
+      <c r="AU102" s="141"/>
+      <c r="AV102" s="141"/>
+      <c r="AW102" s="141"/>
+      <c r="AX102" s="141"/>
+      <c r="AY102" s="141"/>
+      <c r="AZ102" s="141"/>
+      <c r="BA102" s="141"/>
+      <c r="BB102" s="141"/>
+      <c r="BC102" s="141"/>
+      <c r="BD102" s="141"/>
+      <c r="BE102" s="141"/>
+      <c r="BF102" s="141"/>
+      <c r="BG102" s="141"/>
+      <c r="BH102" s="141"/>
+      <c r="BI102" s="141"/>
+      <c r="BJ102" s="141"/>
+      <c r="BK102" s="141"/>
+      <c r="BL102" s="141"/>
       <c r="BM102" s="56"/>
     </row>
     <row r="103" spans="1:65" x14ac:dyDescent="0.2">
@@ -8176,68 +8179,68 @@
         <v>45</v>
       </c>
       <c r="B105" s="54"/>
-      <c r="C105" s="140"/>
-      <c r="D105" s="140"/>
-      <c r="E105" s="140"/>
-      <c r="F105" s="140"/>
-      <c r="G105" s="140"/>
-      <c r="H105" s="140"/>
-      <c r="I105" s="140"/>
-      <c r="J105" s="140"/>
-      <c r="K105" s="140"/>
-      <c r="L105" s="140"/>
-      <c r="M105" s="140"/>
-      <c r="N105" s="140"/>
-      <c r="O105" s="140"/>
-      <c r="P105" s="140"/>
-      <c r="Q105" s="140"/>
-      <c r="R105" s="140"/>
-      <c r="S105" s="140"/>
-      <c r="T105" s="140"/>
-      <c r="U105" s="140"/>
-      <c r="V105" s="140"/>
-      <c r="W105" s="140"/>
-      <c r="X105" s="140"/>
-      <c r="Y105" s="140"/>
-      <c r="Z105" s="140"/>
-      <c r="AA105" s="140"/>
-      <c r="AB105" s="140"/>
-      <c r="AC105" s="140"/>
-      <c r="AD105" s="140"/>
-      <c r="AE105" s="140"/>
-      <c r="AF105" s="140"/>
-      <c r="AG105" s="140"/>
-      <c r="AH105" s="140"/>
+      <c r="C105" s="141"/>
+      <c r="D105" s="141"/>
+      <c r="E105" s="141"/>
+      <c r="F105" s="141"/>
+      <c r="G105" s="141"/>
+      <c r="H105" s="141"/>
+      <c r="I105" s="141"/>
+      <c r="J105" s="141"/>
+      <c r="K105" s="141"/>
+      <c r="L105" s="141"/>
+      <c r="M105" s="141"/>
+      <c r="N105" s="141"/>
+      <c r="O105" s="141"/>
+      <c r="P105" s="141"/>
+      <c r="Q105" s="141"/>
+      <c r="R105" s="141"/>
+      <c r="S105" s="141"/>
+      <c r="T105" s="141"/>
+      <c r="U105" s="141"/>
+      <c r="V105" s="141"/>
+      <c r="W105" s="141"/>
+      <c r="X105" s="141"/>
+      <c r="Y105" s="141"/>
+      <c r="Z105" s="141"/>
+      <c r="AA105" s="141"/>
+      <c r="AB105" s="141"/>
+      <c r="AC105" s="141"/>
+      <c r="AD105" s="141"/>
+      <c r="AE105" s="141"/>
+      <c r="AF105" s="141"/>
+      <c r="AG105" s="141"/>
+      <c r="AH105" s="141"/>
       <c r="AI105" s="56"/>
       <c r="AJ105" s="54"/>
-      <c r="AK105" s="140"/>
-      <c r="AL105" s="140"/>
-      <c r="AM105" s="140"/>
-      <c r="AN105" s="140"/>
-      <c r="AO105" s="140"/>
-      <c r="AP105" s="140"/>
-      <c r="AQ105" s="140"/>
-      <c r="AR105" s="140"/>
-      <c r="AS105" s="140"/>
-      <c r="AT105" s="140"/>
-      <c r="AU105" s="140"/>
-      <c r="AV105" s="140"/>
-      <c r="AW105" s="140"/>
-      <c r="AX105" s="140"/>
-      <c r="AY105" s="140"/>
-      <c r="AZ105" s="140"/>
-      <c r="BA105" s="140"/>
-      <c r="BB105" s="140"/>
-      <c r="BC105" s="140"/>
-      <c r="BD105" s="140"/>
-      <c r="BE105" s="140"/>
-      <c r="BF105" s="140"/>
-      <c r="BG105" s="140"/>
-      <c r="BH105" s="140"/>
-      <c r="BI105" s="140"/>
-      <c r="BJ105" s="140"/>
-      <c r="BK105" s="140"/>
-      <c r="BL105" s="140"/>
+      <c r="AK105" s="141"/>
+      <c r="AL105" s="141"/>
+      <c r="AM105" s="141"/>
+      <c r="AN105" s="141"/>
+      <c r="AO105" s="141"/>
+      <c r="AP105" s="141"/>
+      <c r="AQ105" s="141"/>
+      <c r="AR105" s="141"/>
+      <c r="AS105" s="141"/>
+      <c r="AT105" s="141"/>
+      <c r="AU105" s="141"/>
+      <c r="AV105" s="141"/>
+      <c r="AW105" s="141"/>
+      <c r="AX105" s="141"/>
+      <c r="AY105" s="141"/>
+      <c r="AZ105" s="141"/>
+      <c r="BA105" s="141"/>
+      <c r="BB105" s="141"/>
+      <c r="BC105" s="141"/>
+      <c r="BD105" s="141"/>
+      <c r="BE105" s="141"/>
+      <c r="BF105" s="141"/>
+      <c r="BG105" s="141"/>
+      <c r="BH105" s="141"/>
+      <c r="BI105" s="141"/>
+      <c r="BJ105" s="141"/>
+      <c r="BK105" s="141"/>
+      <c r="BL105" s="141"/>
       <c r="BM105" s="56"/>
     </row>
     <row r="106" spans="1:65" x14ac:dyDescent="0.2">
@@ -8245,68 +8248,68 @@
         <v>46</v>
       </c>
       <c r="B106" s="54"/>
-      <c r="C106" s="140"/>
-      <c r="D106" s="140"/>
-      <c r="E106" s="140"/>
-      <c r="F106" s="140"/>
-      <c r="G106" s="140"/>
-      <c r="H106" s="140"/>
-      <c r="I106" s="140"/>
-      <c r="J106" s="140"/>
-      <c r="K106" s="140"/>
-      <c r="L106" s="140"/>
-      <c r="M106" s="140"/>
-      <c r="N106" s="140"/>
-      <c r="O106" s="140"/>
-      <c r="P106" s="140"/>
-      <c r="Q106" s="140"/>
-      <c r="R106" s="140"/>
-      <c r="S106" s="140"/>
-      <c r="T106" s="140"/>
-      <c r="U106" s="140"/>
-      <c r="V106" s="140"/>
-      <c r="W106" s="140"/>
-      <c r="X106" s="140"/>
-      <c r="Y106" s="140"/>
-      <c r="Z106" s="140"/>
-      <c r="AA106" s="140"/>
-      <c r="AB106" s="140"/>
-      <c r="AC106" s="140"/>
-      <c r="AD106" s="140"/>
-      <c r="AE106" s="140"/>
-      <c r="AF106" s="140"/>
-      <c r="AG106" s="140"/>
-      <c r="AH106" s="140"/>
+      <c r="C106" s="141"/>
+      <c r="D106" s="141"/>
+      <c r="E106" s="141"/>
+      <c r="F106" s="141"/>
+      <c r="G106" s="141"/>
+      <c r="H106" s="141"/>
+      <c r="I106" s="141"/>
+      <c r="J106" s="141"/>
+      <c r="K106" s="141"/>
+      <c r="L106" s="141"/>
+      <c r="M106" s="141"/>
+      <c r="N106" s="141"/>
+      <c r="O106" s="141"/>
+      <c r="P106" s="141"/>
+      <c r="Q106" s="141"/>
+      <c r="R106" s="141"/>
+      <c r="S106" s="141"/>
+      <c r="T106" s="141"/>
+      <c r="U106" s="141"/>
+      <c r="V106" s="141"/>
+      <c r="W106" s="141"/>
+      <c r="X106" s="141"/>
+      <c r="Y106" s="141"/>
+      <c r="Z106" s="141"/>
+      <c r="AA106" s="141"/>
+      <c r="AB106" s="141"/>
+      <c r="AC106" s="141"/>
+      <c r="AD106" s="141"/>
+      <c r="AE106" s="141"/>
+      <c r="AF106" s="141"/>
+      <c r="AG106" s="141"/>
+      <c r="AH106" s="141"/>
       <c r="AI106" s="56"/>
       <c r="AJ106" s="54"/>
-      <c r="AK106" s="140"/>
-      <c r="AL106" s="140"/>
-      <c r="AM106" s="140"/>
-      <c r="AN106" s="140"/>
-      <c r="AO106" s="140"/>
-      <c r="AP106" s="140"/>
-      <c r="AQ106" s="140"/>
-      <c r="AR106" s="140"/>
-      <c r="AS106" s="140"/>
-      <c r="AT106" s="140"/>
-      <c r="AU106" s="140"/>
-      <c r="AV106" s="140"/>
-      <c r="AW106" s="140"/>
-      <c r="AX106" s="140"/>
-      <c r="AY106" s="140"/>
-      <c r="AZ106" s="140"/>
-      <c r="BA106" s="140"/>
-      <c r="BB106" s="140"/>
-      <c r="BC106" s="140"/>
-      <c r="BD106" s="140"/>
-      <c r="BE106" s="140"/>
-      <c r="BF106" s="140"/>
-      <c r="BG106" s="140"/>
-      <c r="BH106" s="140"/>
-      <c r="BI106" s="140"/>
-      <c r="BJ106" s="140"/>
-      <c r="BK106" s="140"/>
-      <c r="BL106" s="140"/>
+      <c r="AK106" s="141"/>
+      <c r="AL106" s="141"/>
+      <c r="AM106" s="141"/>
+      <c r="AN106" s="141"/>
+      <c r="AO106" s="141"/>
+      <c r="AP106" s="141"/>
+      <c r="AQ106" s="141"/>
+      <c r="AR106" s="141"/>
+      <c r="AS106" s="141"/>
+      <c r="AT106" s="141"/>
+      <c r="AU106" s="141"/>
+      <c r="AV106" s="141"/>
+      <c r="AW106" s="141"/>
+      <c r="AX106" s="141"/>
+      <c r="AY106" s="141"/>
+      <c r="AZ106" s="141"/>
+      <c r="BA106" s="141"/>
+      <c r="BB106" s="141"/>
+      <c r="BC106" s="141"/>
+      <c r="BD106" s="141"/>
+      <c r="BE106" s="141"/>
+      <c r="BF106" s="141"/>
+      <c r="BG106" s="141"/>
+      <c r="BH106" s="141"/>
+      <c r="BI106" s="141"/>
+      <c r="BJ106" s="141"/>
+      <c r="BK106" s="141"/>
+      <c r="BL106" s="141"/>
       <c r="BM106" s="56"/>
     </row>
     <row r="107" spans="1:65" x14ac:dyDescent="0.2">
@@ -8385,35 +8388,35 @@
       <c r="B108" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C108" s="140"/>
-      <c r="D108" s="140"/>
-      <c r="E108" s="140"/>
-      <c r="F108" s="140"/>
-      <c r="G108" s="140"/>
-      <c r="H108" s="140"/>
-      <c r="I108" s="140"/>
-      <c r="J108" s="140"/>
-      <c r="K108" s="140"/>
-      <c r="L108" s="140"/>
-      <c r="M108" s="140"/>
-      <c r="N108" s="140"/>
-      <c r="O108" s="140"/>
-      <c r="P108" s="140"/>
-      <c r="Q108" s="140"/>
-      <c r="R108" s="140"/>
-      <c r="S108" s="140"/>
-      <c r="T108" s="140"/>
-      <c r="U108" s="140"/>
-      <c r="V108" s="140"/>
-      <c r="W108" s="140"/>
-      <c r="X108" s="140"/>
-      <c r="Y108" s="140"/>
-      <c r="Z108" s="140"/>
-      <c r="AA108" s="140"/>
-      <c r="AB108" s="140"/>
-      <c r="AC108" s="140"/>
-      <c r="AD108" s="140"/>
-      <c r="AE108" s="140"/>
+      <c r="C108" s="141"/>
+      <c r="D108" s="141"/>
+      <c r="E108" s="141"/>
+      <c r="F108" s="141"/>
+      <c r="G108" s="141"/>
+      <c r="H108" s="141"/>
+      <c r="I108" s="141"/>
+      <c r="J108" s="141"/>
+      <c r="K108" s="141"/>
+      <c r="L108" s="141"/>
+      <c r="M108" s="141"/>
+      <c r="N108" s="141"/>
+      <c r="O108" s="141"/>
+      <c r="P108" s="141"/>
+      <c r="Q108" s="141"/>
+      <c r="R108" s="141"/>
+      <c r="S108" s="141"/>
+      <c r="T108" s="141"/>
+      <c r="U108" s="141"/>
+      <c r="V108" s="141"/>
+      <c r="W108" s="141"/>
+      <c r="X108" s="141"/>
+      <c r="Y108" s="141"/>
+      <c r="Z108" s="141"/>
+      <c r="AA108" s="141"/>
+      <c r="AB108" s="141"/>
+      <c r="AC108" s="141"/>
+      <c r="AD108" s="141"/>
+      <c r="AE108" s="141"/>
       <c r="AF108" s="56"/>
     </row>
     <row r="109" spans="1:65" x14ac:dyDescent="0.2">
@@ -8421,35 +8424,35 @@
         <v>49</v>
       </c>
       <c r="B109" s="54"/>
-      <c r="C109" s="140"/>
-      <c r="D109" s="140"/>
-      <c r="E109" s="140"/>
-      <c r="F109" s="140"/>
-      <c r="G109" s="140"/>
-      <c r="H109" s="140"/>
-      <c r="I109" s="140"/>
-      <c r="J109" s="140"/>
-      <c r="K109" s="140"/>
-      <c r="L109" s="140"/>
-      <c r="M109" s="140"/>
-      <c r="N109" s="140"/>
-      <c r="O109" s="140"/>
-      <c r="P109" s="140"/>
-      <c r="Q109" s="140"/>
-      <c r="R109" s="140"/>
-      <c r="S109" s="140"/>
-      <c r="T109" s="140"/>
-      <c r="U109" s="140"/>
-      <c r="V109" s="140"/>
-      <c r="W109" s="140"/>
-      <c r="X109" s="140"/>
-      <c r="Y109" s="140"/>
-      <c r="Z109" s="140"/>
-      <c r="AA109" s="140"/>
-      <c r="AB109" s="140"/>
-      <c r="AC109" s="140"/>
-      <c r="AD109" s="140"/>
-      <c r="AE109" s="140"/>
+      <c r="C109" s="141"/>
+      <c r="D109" s="141"/>
+      <c r="E109" s="141"/>
+      <c r="F109" s="141"/>
+      <c r="G109" s="141"/>
+      <c r="H109" s="141"/>
+      <c r="I109" s="141"/>
+      <c r="J109" s="141"/>
+      <c r="K109" s="141"/>
+      <c r="L109" s="141"/>
+      <c r="M109" s="141"/>
+      <c r="N109" s="141"/>
+      <c r="O109" s="141"/>
+      <c r="P109" s="141"/>
+      <c r="Q109" s="141"/>
+      <c r="R109" s="141"/>
+      <c r="S109" s="141"/>
+      <c r="T109" s="141"/>
+      <c r="U109" s="141"/>
+      <c r="V109" s="141"/>
+      <c r="W109" s="141"/>
+      <c r="X109" s="141"/>
+      <c r="Y109" s="141"/>
+      <c r="Z109" s="141"/>
+      <c r="AA109" s="141"/>
+      <c r="AB109" s="141"/>
+      <c r="AC109" s="141"/>
+      <c r="AD109" s="141"/>
+      <c r="AE109" s="141"/>
       <c r="AF109" s="56"/>
     </row>
     <row r="110" spans="1:65" x14ac:dyDescent="0.2">
@@ -8457,35 +8460,35 @@
         <v>50</v>
       </c>
       <c r="B110" s="54"/>
-      <c r="C110" s="140"/>
-      <c r="D110" s="140"/>
-      <c r="E110" s="140"/>
-      <c r="F110" s="140"/>
-      <c r="G110" s="140"/>
-      <c r="H110" s="140"/>
-      <c r="I110" s="140"/>
-      <c r="J110" s="140"/>
-      <c r="K110" s="140"/>
-      <c r="L110" s="140"/>
-      <c r="M110" s="140"/>
-      <c r="N110" s="140"/>
-      <c r="O110" s="140"/>
-      <c r="P110" s="140"/>
-      <c r="Q110" s="140"/>
-      <c r="R110" s="140"/>
-      <c r="S110" s="140"/>
-      <c r="T110" s="140"/>
-      <c r="U110" s="140"/>
-      <c r="V110" s="140"/>
-      <c r="W110" s="140"/>
-      <c r="X110" s="140"/>
-      <c r="Y110" s="140"/>
-      <c r="Z110" s="140"/>
-      <c r="AA110" s="140"/>
-      <c r="AB110" s="140"/>
-      <c r="AC110" s="140"/>
-      <c r="AD110" s="140"/>
-      <c r="AE110" s="140"/>
+      <c r="C110" s="141"/>
+      <c r="D110" s="141"/>
+      <c r="E110" s="141"/>
+      <c r="F110" s="141"/>
+      <c r="G110" s="141"/>
+      <c r="H110" s="141"/>
+      <c r="I110" s="141"/>
+      <c r="J110" s="141"/>
+      <c r="K110" s="141"/>
+      <c r="L110" s="141"/>
+      <c r="M110" s="141"/>
+      <c r="N110" s="141"/>
+      <c r="O110" s="141"/>
+      <c r="P110" s="141"/>
+      <c r="Q110" s="141"/>
+      <c r="R110" s="141"/>
+      <c r="S110" s="141"/>
+      <c r="T110" s="141"/>
+      <c r="U110" s="141"/>
+      <c r="V110" s="141"/>
+      <c r="W110" s="141"/>
+      <c r="X110" s="141"/>
+      <c r="Y110" s="141"/>
+      <c r="Z110" s="141"/>
+      <c r="AA110" s="141"/>
+      <c r="AB110" s="141"/>
+      <c r="AC110" s="141"/>
+      <c r="AD110" s="141"/>
+      <c r="AE110" s="141"/>
       <c r="AF110" s="56"/>
     </row>
     <row r="111" spans="1:65" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added sum with encoder input
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22385B80-A826-274A-AC35-637828D79804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9054FE-23A4-D045-99D5-DF55F96B1B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>CiM PARAMETERS MEMORY MAP</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>enc_softmax*V_transposed[id][:]</t>
+  </si>
+  <si>
+    <t>enc_out_+_enc_in[:][id]</t>
   </si>
 </sst>
 </file>
@@ -1329,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
   <dimension ref="A1:BP111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="BP71" sqref="BP71"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72:BG75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5674,7 +5677,7 @@
         <v>8</v>
       </c>
       <c r="B68" s="42" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C68" s="43"/>
       <c r="D68" s="43"/>

</xml_diff>

<commit_message>
Now performs LayerNorm #2 (after encoder)
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9054FE-23A4-D045-99D5-DF55F96B1B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACD9B70-2305-3C4C-8257-6215FCE3CFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>CiM PARAMETERS MEMORY MAP</t>
   </si>
@@ -210,13 +210,10 @@
     <t>encoder.mhsa_combine_head.bias[id] (1 x float32)</t>
   </si>
   <si>
-    <t>enc_out[:][id]</t>
+    <t>after_1st_half_LayerNorm_2[id][:]</t>
   </si>
   <si>
-    <t>enc_softmax*V_transposed[id][:]</t>
-  </si>
-  <si>
-    <t>enc_out_+_enc_in[:][id]</t>
+    <t>after_LayerNorm_2[:][id]</t>
   </si>
 </sst>
 </file>
@@ -277,7 +274,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,12 +338,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -849,91 +840,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -950,60 +941,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1332,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
   <dimension ref="A1:BP111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:BG75"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AN46" sqref="AN46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5173,11 +5110,11 @@
       <c r="BH60" s="43"/>
       <c r="BI60" s="43"/>
       <c r="BJ60" s="44"/>
-      <c r="BK60" s="148" t="s">
-        <v>58</v>
-      </c>
-      <c r="BL60" s="149"/>
-      <c r="BM60" s="150"/>
+      <c r="BK60" s="131" t="s">
+        <v>57</v>
+      </c>
+      <c r="BL60" s="132"/>
+      <c r="BM60" s="133"/>
       <c r="BO60" s="10" t="s">
         <v>26</v>
       </c>
@@ -5247,9 +5184,9 @@
       <c r="BH61" s="46"/>
       <c r="BI61" s="46"/>
       <c r="BJ61" s="47"/>
-      <c r="BK61" s="151"/>
-      <c r="BL61" s="152"/>
-      <c r="BM61" s="153"/>
+      <c r="BK61" s="134"/>
+      <c r="BL61" s="135"/>
+      <c r="BM61" s="136"/>
       <c r="BO61" s="10" t="s">
         <v>27</v>
       </c>
@@ -5319,9 +5256,9 @@
       <c r="BH62" s="46"/>
       <c r="BI62" s="46"/>
       <c r="BJ62" s="47"/>
-      <c r="BK62" s="151"/>
-      <c r="BL62" s="152"/>
-      <c r="BM62" s="153"/>
+      <c r="BK62" s="134"/>
+      <c r="BL62" s="135"/>
+      <c r="BM62" s="136"/>
     </row>
     <row r="63" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -5388,79 +5325,79 @@
       <c r="BH63" s="49"/>
       <c r="BI63" s="49"/>
       <c r="BJ63" s="50"/>
-      <c r="BK63" s="154"/>
-      <c r="BL63" s="155"/>
-      <c r="BM63" s="156"/>
+      <c r="BK63" s="137"/>
+      <c r="BL63" s="138"/>
+      <c r="BM63" s="139"/>
     </row>
     <row r="64" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>4</v>
       </c>
-      <c r="B64" s="157" t="s">
+      <c r="B64" s="122" t="s">
+        <v>57</v>
+      </c>
+      <c r="C64" s="123"/>
+      <c r="D64" s="123"/>
+      <c r="E64" s="123"/>
+      <c r="F64" s="123"/>
+      <c r="G64" s="123"/>
+      <c r="H64" s="123"/>
+      <c r="I64" s="123"/>
+      <c r="J64" s="123"/>
+      <c r="K64" s="123"/>
+      <c r="L64" s="123"/>
+      <c r="M64" s="123"/>
+      <c r="N64" s="123"/>
+      <c r="O64" s="123"/>
+      <c r="P64" s="123"/>
+      <c r="Q64" s="123"/>
+      <c r="R64" s="123"/>
+      <c r="S64" s="123"/>
+      <c r="T64" s="123"/>
+      <c r="U64" s="123"/>
+      <c r="V64" s="123"/>
+      <c r="W64" s="123"/>
+      <c r="X64" s="123"/>
+      <c r="Y64" s="123"/>
+      <c r="Z64" s="123"/>
+      <c r="AA64" s="123"/>
+      <c r="AB64" s="123"/>
+      <c r="AC64" s="123"/>
+      <c r="AD64" s="123"/>
+      <c r="AE64" s="123"/>
+      <c r="AF64" s="123"/>
+      <c r="AG64" s="123"/>
+      <c r="AH64" s="123"/>
+      <c r="AI64" s="123"/>
+      <c r="AJ64" s="123"/>
+      <c r="AK64" s="123"/>
+      <c r="AL64" s="123"/>
+      <c r="AM64" s="123"/>
+      <c r="AN64" s="123"/>
+      <c r="AO64" s="123"/>
+      <c r="AP64" s="123"/>
+      <c r="AQ64" s="123"/>
+      <c r="AR64" s="123"/>
+      <c r="AS64" s="123"/>
+      <c r="AT64" s="123"/>
+      <c r="AU64" s="123"/>
+      <c r="AV64" s="123"/>
+      <c r="AW64" s="123"/>
+      <c r="AX64" s="123"/>
+      <c r="AY64" s="123"/>
+      <c r="AZ64" s="123"/>
+      <c r="BA64" s="123"/>
+      <c r="BB64" s="123"/>
+      <c r="BC64" s="123"/>
+      <c r="BD64" s="123"/>
+      <c r="BE64" s="123"/>
+      <c r="BF64" s="123"/>
+      <c r="BG64" s="123"/>
+      <c r="BH64" s="123"/>
+      <c r="BI64" s="123"/>
+      <c r="BJ64" s="124"/>
+      <c r="BK64" s="51" t="s">
         <v>58</v>
-      </c>
-      <c r="C64" s="158"/>
-      <c r="D64" s="158"/>
-      <c r="E64" s="158"/>
-      <c r="F64" s="158"/>
-      <c r="G64" s="158"/>
-      <c r="H64" s="158"/>
-      <c r="I64" s="158"/>
-      <c r="J64" s="158"/>
-      <c r="K64" s="158"/>
-      <c r="L64" s="158"/>
-      <c r="M64" s="158"/>
-      <c r="N64" s="158"/>
-      <c r="O64" s="158"/>
-      <c r="P64" s="158"/>
-      <c r="Q64" s="158"/>
-      <c r="R64" s="158"/>
-      <c r="S64" s="158"/>
-      <c r="T64" s="158"/>
-      <c r="U64" s="158"/>
-      <c r="V64" s="158"/>
-      <c r="W64" s="158"/>
-      <c r="X64" s="158"/>
-      <c r="Y64" s="158"/>
-      <c r="Z64" s="158"/>
-      <c r="AA64" s="158"/>
-      <c r="AB64" s="158"/>
-      <c r="AC64" s="158"/>
-      <c r="AD64" s="158"/>
-      <c r="AE64" s="158"/>
-      <c r="AF64" s="158"/>
-      <c r="AG64" s="158"/>
-      <c r="AH64" s="158"/>
-      <c r="AI64" s="158"/>
-      <c r="AJ64" s="158"/>
-      <c r="AK64" s="158"/>
-      <c r="AL64" s="158"/>
-      <c r="AM64" s="158"/>
-      <c r="AN64" s="158"/>
-      <c r="AO64" s="158"/>
-      <c r="AP64" s="158"/>
-      <c r="AQ64" s="158"/>
-      <c r="AR64" s="158"/>
-      <c r="AS64" s="158"/>
-      <c r="AT64" s="158"/>
-      <c r="AU64" s="158"/>
-      <c r="AV64" s="158"/>
-      <c r="AW64" s="158"/>
-      <c r="AX64" s="158"/>
-      <c r="AY64" s="158"/>
-      <c r="AZ64" s="158"/>
-      <c r="BA64" s="158"/>
-      <c r="BB64" s="158"/>
-      <c r="BC64" s="158"/>
-      <c r="BD64" s="158"/>
-      <c r="BE64" s="158"/>
-      <c r="BF64" s="158"/>
-      <c r="BG64" s="158"/>
-      <c r="BH64" s="158"/>
-      <c r="BI64" s="158"/>
-      <c r="BJ64" s="159"/>
-      <c r="BK64" s="51" t="s">
-        <v>57</v>
       </c>
       <c r="BL64" s="52"/>
       <c r="BM64" s="53"/>
@@ -5469,67 +5406,67 @@
       <c r="A65" s="1">
         <v>5</v>
       </c>
-      <c r="B65" s="160"/>
-      <c r="C65" s="161"/>
-      <c r="D65" s="161"/>
-      <c r="E65" s="161"/>
-      <c r="F65" s="161"/>
-      <c r="G65" s="161"/>
-      <c r="H65" s="161"/>
-      <c r="I65" s="161"/>
-      <c r="J65" s="161"/>
-      <c r="K65" s="161"/>
-      <c r="L65" s="161"/>
-      <c r="M65" s="161"/>
-      <c r="N65" s="161"/>
-      <c r="O65" s="161"/>
-      <c r="P65" s="161"/>
-      <c r="Q65" s="161"/>
-      <c r="R65" s="161"/>
-      <c r="S65" s="161"/>
-      <c r="T65" s="161"/>
-      <c r="U65" s="161"/>
-      <c r="V65" s="161"/>
-      <c r="W65" s="161"/>
-      <c r="X65" s="161"/>
-      <c r="Y65" s="161"/>
-      <c r="Z65" s="161"/>
-      <c r="AA65" s="161"/>
-      <c r="AB65" s="161"/>
-      <c r="AC65" s="161"/>
-      <c r="AD65" s="161"/>
-      <c r="AE65" s="161"/>
-      <c r="AF65" s="161"/>
-      <c r="AG65" s="161"/>
-      <c r="AH65" s="161"/>
-      <c r="AI65" s="161"/>
-      <c r="AJ65" s="161"/>
-      <c r="AK65" s="161"/>
-      <c r="AL65" s="161"/>
-      <c r="AM65" s="161"/>
-      <c r="AN65" s="161"/>
-      <c r="AO65" s="161"/>
-      <c r="AP65" s="161"/>
-      <c r="AQ65" s="161"/>
-      <c r="AR65" s="161"/>
-      <c r="AS65" s="161"/>
-      <c r="AT65" s="161"/>
-      <c r="AU65" s="161"/>
-      <c r="AV65" s="161"/>
-      <c r="AW65" s="161"/>
-      <c r="AX65" s="161"/>
-      <c r="AY65" s="161"/>
-      <c r="AZ65" s="161"/>
-      <c r="BA65" s="161"/>
-      <c r="BB65" s="161"/>
-      <c r="BC65" s="161"/>
-      <c r="BD65" s="161"/>
-      <c r="BE65" s="161"/>
-      <c r="BF65" s="161"/>
-      <c r="BG65" s="161"/>
-      <c r="BH65" s="161"/>
-      <c r="BI65" s="161"/>
-      <c r="BJ65" s="162"/>
+      <c r="B65" s="125"/>
+      <c r="C65" s="126"/>
+      <c r="D65" s="126"/>
+      <c r="E65" s="126"/>
+      <c r="F65" s="126"/>
+      <c r="G65" s="126"/>
+      <c r="H65" s="126"/>
+      <c r="I65" s="126"/>
+      <c r="J65" s="126"/>
+      <c r="K65" s="126"/>
+      <c r="L65" s="126"/>
+      <c r="M65" s="126"/>
+      <c r="N65" s="126"/>
+      <c r="O65" s="126"/>
+      <c r="P65" s="126"/>
+      <c r="Q65" s="126"/>
+      <c r="R65" s="126"/>
+      <c r="S65" s="126"/>
+      <c r="T65" s="126"/>
+      <c r="U65" s="126"/>
+      <c r="V65" s="126"/>
+      <c r="W65" s="126"/>
+      <c r="X65" s="126"/>
+      <c r="Y65" s="126"/>
+      <c r="Z65" s="126"/>
+      <c r="AA65" s="126"/>
+      <c r="AB65" s="126"/>
+      <c r="AC65" s="126"/>
+      <c r="AD65" s="126"/>
+      <c r="AE65" s="126"/>
+      <c r="AF65" s="126"/>
+      <c r="AG65" s="126"/>
+      <c r="AH65" s="126"/>
+      <c r="AI65" s="126"/>
+      <c r="AJ65" s="126"/>
+      <c r="AK65" s="126"/>
+      <c r="AL65" s="126"/>
+      <c r="AM65" s="126"/>
+      <c r="AN65" s="126"/>
+      <c r="AO65" s="126"/>
+      <c r="AP65" s="126"/>
+      <c r="AQ65" s="126"/>
+      <c r="AR65" s="126"/>
+      <c r="AS65" s="126"/>
+      <c r="AT65" s="126"/>
+      <c r="AU65" s="126"/>
+      <c r="AV65" s="126"/>
+      <c r="AW65" s="126"/>
+      <c r="AX65" s="126"/>
+      <c r="AY65" s="126"/>
+      <c r="AZ65" s="126"/>
+      <c r="BA65" s="126"/>
+      <c r="BB65" s="126"/>
+      <c r="BC65" s="126"/>
+      <c r="BD65" s="126"/>
+      <c r="BE65" s="126"/>
+      <c r="BF65" s="126"/>
+      <c r="BG65" s="126"/>
+      <c r="BH65" s="126"/>
+      <c r="BI65" s="126"/>
+      <c r="BJ65" s="127"/>
       <c r="BK65" s="54"/>
       <c r="BL65" s="55"/>
       <c r="BM65" s="56"/>
@@ -5538,67 +5475,67 @@
       <c r="A66" s="2">
         <v>6</v>
       </c>
-      <c r="B66" s="160"/>
-      <c r="C66" s="161"/>
-      <c r="D66" s="161"/>
-      <c r="E66" s="161"/>
-      <c r="F66" s="161"/>
-      <c r="G66" s="161"/>
-      <c r="H66" s="161"/>
-      <c r="I66" s="161"/>
-      <c r="J66" s="161"/>
-      <c r="K66" s="161"/>
-      <c r="L66" s="161"/>
-      <c r="M66" s="161"/>
-      <c r="N66" s="161"/>
-      <c r="O66" s="161"/>
-      <c r="P66" s="161"/>
-      <c r="Q66" s="161"/>
-      <c r="R66" s="161"/>
-      <c r="S66" s="161"/>
-      <c r="T66" s="161"/>
-      <c r="U66" s="161"/>
-      <c r="V66" s="161"/>
-      <c r="W66" s="161"/>
-      <c r="X66" s="161"/>
-      <c r="Y66" s="161"/>
-      <c r="Z66" s="161"/>
-      <c r="AA66" s="161"/>
-      <c r="AB66" s="161"/>
-      <c r="AC66" s="161"/>
-      <c r="AD66" s="161"/>
-      <c r="AE66" s="161"/>
-      <c r="AF66" s="161"/>
-      <c r="AG66" s="161"/>
-      <c r="AH66" s="161"/>
-      <c r="AI66" s="161"/>
-      <c r="AJ66" s="161"/>
-      <c r="AK66" s="161"/>
-      <c r="AL66" s="161"/>
-      <c r="AM66" s="161"/>
-      <c r="AN66" s="161"/>
-      <c r="AO66" s="161"/>
-      <c r="AP66" s="161"/>
-      <c r="AQ66" s="161"/>
-      <c r="AR66" s="161"/>
-      <c r="AS66" s="161"/>
-      <c r="AT66" s="161"/>
-      <c r="AU66" s="161"/>
-      <c r="AV66" s="161"/>
-      <c r="AW66" s="161"/>
-      <c r="AX66" s="161"/>
-      <c r="AY66" s="161"/>
-      <c r="AZ66" s="161"/>
-      <c r="BA66" s="161"/>
-      <c r="BB66" s="161"/>
-      <c r="BC66" s="161"/>
-      <c r="BD66" s="161"/>
-      <c r="BE66" s="161"/>
-      <c r="BF66" s="161"/>
-      <c r="BG66" s="161"/>
-      <c r="BH66" s="161"/>
-      <c r="BI66" s="161"/>
-      <c r="BJ66" s="162"/>
+      <c r="B66" s="125"/>
+      <c r="C66" s="126"/>
+      <c r="D66" s="126"/>
+      <c r="E66" s="126"/>
+      <c r="F66" s="126"/>
+      <c r="G66" s="126"/>
+      <c r="H66" s="126"/>
+      <c r="I66" s="126"/>
+      <c r="J66" s="126"/>
+      <c r="K66" s="126"/>
+      <c r="L66" s="126"/>
+      <c r="M66" s="126"/>
+      <c r="N66" s="126"/>
+      <c r="O66" s="126"/>
+      <c r="P66" s="126"/>
+      <c r="Q66" s="126"/>
+      <c r="R66" s="126"/>
+      <c r="S66" s="126"/>
+      <c r="T66" s="126"/>
+      <c r="U66" s="126"/>
+      <c r="V66" s="126"/>
+      <c r="W66" s="126"/>
+      <c r="X66" s="126"/>
+      <c r="Y66" s="126"/>
+      <c r="Z66" s="126"/>
+      <c r="AA66" s="126"/>
+      <c r="AB66" s="126"/>
+      <c r="AC66" s="126"/>
+      <c r="AD66" s="126"/>
+      <c r="AE66" s="126"/>
+      <c r="AF66" s="126"/>
+      <c r="AG66" s="126"/>
+      <c r="AH66" s="126"/>
+      <c r="AI66" s="126"/>
+      <c r="AJ66" s="126"/>
+      <c r="AK66" s="126"/>
+      <c r="AL66" s="126"/>
+      <c r="AM66" s="126"/>
+      <c r="AN66" s="126"/>
+      <c r="AO66" s="126"/>
+      <c r="AP66" s="126"/>
+      <c r="AQ66" s="126"/>
+      <c r="AR66" s="126"/>
+      <c r="AS66" s="126"/>
+      <c r="AT66" s="126"/>
+      <c r="AU66" s="126"/>
+      <c r="AV66" s="126"/>
+      <c r="AW66" s="126"/>
+      <c r="AX66" s="126"/>
+      <c r="AY66" s="126"/>
+      <c r="AZ66" s="126"/>
+      <c r="BA66" s="126"/>
+      <c r="BB66" s="126"/>
+      <c r="BC66" s="126"/>
+      <c r="BD66" s="126"/>
+      <c r="BE66" s="126"/>
+      <c r="BF66" s="126"/>
+      <c r="BG66" s="126"/>
+      <c r="BH66" s="126"/>
+      <c r="BI66" s="126"/>
+      <c r="BJ66" s="127"/>
       <c r="BK66" s="54"/>
       <c r="BL66" s="55"/>
       <c r="BM66" s="56"/>
@@ -5607,67 +5544,67 @@
       <c r="A67" s="1">
         <v>7</v>
       </c>
-      <c r="B67" s="163"/>
-      <c r="C67" s="164"/>
-      <c r="D67" s="164"/>
-      <c r="E67" s="164"/>
-      <c r="F67" s="164"/>
-      <c r="G67" s="164"/>
-      <c r="H67" s="164"/>
-      <c r="I67" s="164"/>
-      <c r="J67" s="164"/>
-      <c r="K67" s="164"/>
-      <c r="L67" s="164"/>
-      <c r="M67" s="164"/>
-      <c r="N67" s="164"/>
-      <c r="O67" s="164"/>
-      <c r="P67" s="164"/>
-      <c r="Q67" s="164"/>
-      <c r="R67" s="164"/>
-      <c r="S67" s="164"/>
-      <c r="T67" s="164"/>
-      <c r="U67" s="164"/>
-      <c r="V67" s="164"/>
-      <c r="W67" s="164"/>
-      <c r="X67" s="164"/>
-      <c r="Y67" s="164"/>
-      <c r="Z67" s="164"/>
-      <c r="AA67" s="164"/>
-      <c r="AB67" s="164"/>
-      <c r="AC67" s="164"/>
-      <c r="AD67" s="164"/>
-      <c r="AE67" s="164"/>
-      <c r="AF67" s="164"/>
-      <c r="AG67" s="164"/>
-      <c r="AH67" s="164"/>
-      <c r="AI67" s="164"/>
-      <c r="AJ67" s="164"/>
-      <c r="AK67" s="164"/>
-      <c r="AL67" s="164"/>
-      <c r="AM67" s="164"/>
-      <c r="AN67" s="164"/>
-      <c r="AO67" s="164"/>
-      <c r="AP67" s="164"/>
-      <c r="AQ67" s="164"/>
-      <c r="AR67" s="164"/>
-      <c r="AS67" s="164"/>
-      <c r="AT67" s="164"/>
-      <c r="AU67" s="164"/>
-      <c r="AV67" s="164"/>
-      <c r="AW67" s="164"/>
-      <c r="AX67" s="164"/>
-      <c r="AY67" s="164"/>
-      <c r="AZ67" s="164"/>
-      <c r="BA67" s="164"/>
-      <c r="BB67" s="164"/>
-      <c r="BC67" s="164"/>
-      <c r="BD67" s="164"/>
-      <c r="BE67" s="164"/>
-      <c r="BF67" s="164"/>
-      <c r="BG67" s="164"/>
-      <c r="BH67" s="164"/>
-      <c r="BI67" s="164"/>
-      <c r="BJ67" s="165"/>
+      <c r="B67" s="128"/>
+      <c r="C67" s="129"/>
+      <c r="D67" s="129"/>
+      <c r="E67" s="129"/>
+      <c r="F67" s="129"/>
+      <c r="G67" s="129"/>
+      <c r="H67" s="129"/>
+      <c r="I67" s="129"/>
+      <c r="J67" s="129"/>
+      <c r="K67" s="129"/>
+      <c r="L67" s="129"/>
+      <c r="M67" s="129"/>
+      <c r="N67" s="129"/>
+      <c r="O67" s="129"/>
+      <c r="P67" s="129"/>
+      <c r="Q67" s="129"/>
+      <c r="R67" s="129"/>
+      <c r="S67" s="129"/>
+      <c r="T67" s="129"/>
+      <c r="U67" s="129"/>
+      <c r="V67" s="129"/>
+      <c r="W67" s="129"/>
+      <c r="X67" s="129"/>
+      <c r="Y67" s="129"/>
+      <c r="Z67" s="129"/>
+      <c r="AA67" s="129"/>
+      <c r="AB67" s="129"/>
+      <c r="AC67" s="129"/>
+      <c r="AD67" s="129"/>
+      <c r="AE67" s="129"/>
+      <c r="AF67" s="129"/>
+      <c r="AG67" s="129"/>
+      <c r="AH67" s="129"/>
+      <c r="AI67" s="129"/>
+      <c r="AJ67" s="129"/>
+      <c r="AK67" s="129"/>
+      <c r="AL67" s="129"/>
+      <c r="AM67" s="129"/>
+      <c r="AN67" s="129"/>
+      <c r="AO67" s="129"/>
+      <c r="AP67" s="129"/>
+      <c r="AQ67" s="129"/>
+      <c r="AR67" s="129"/>
+      <c r="AS67" s="129"/>
+      <c r="AT67" s="129"/>
+      <c r="AU67" s="129"/>
+      <c r="AV67" s="129"/>
+      <c r="AW67" s="129"/>
+      <c r="AX67" s="129"/>
+      <c r="AY67" s="129"/>
+      <c r="AZ67" s="129"/>
+      <c r="BA67" s="129"/>
+      <c r="BB67" s="129"/>
+      <c r="BC67" s="129"/>
+      <c r="BD67" s="129"/>
+      <c r="BE67" s="129"/>
+      <c r="BF67" s="129"/>
+      <c r="BG67" s="129"/>
+      <c r="BH67" s="129"/>
+      <c r="BI67" s="129"/>
+      <c r="BJ67" s="130"/>
       <c r="BK67" s="57"/>
       <c r="BL67" s="58"/>
       <c r="BM67" s="59"/>
@@ -5677,7 +5614,7 @@
         <v>8</v>
       </c>
       <c r="B68" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C68" s="43"/>
       <c r="D68" s="43"/>

</xml_diff>

<commit_message>
Finished encoder's MLP Dense 2
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897CF774-AB31-1946-8382-A4B246AD700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352FD67E-725F-CF41-ADD5-C990EFAA0B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -233,10 +233,10 @@
     <t>mlp.dense2.kernel[:][id] (32 x float32)*</t>
   </si>
   <si>
-    <t>enc_mlp_dense1_broadcast_temp[x][:]</t>
+    <t>enc_mlp_dense2_broadcast_temp[x][:]</t>
   </si>
   <si>
-    <t>enc_mlp_dense1_res[:][id]</t>
+    <t>enc_mlp_dense2_res[:][id]</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
   <dimension ref="A1:BP111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BD39" sqref="BD39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BH72" sqref="BH72:BM75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5486,11 +5486,11 @@
       <c r="BH64" s="88"/>
       <c r="BI64" s="88"/>
       <c r="BJ64" s="89"/>
-      <c r="BK64" s="76" t="s">
+      <c r="BK64" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="BL64" s="77"/>
-      <c r="BM64" s="78"/>
+      <c r="BL64" s="65"/>
+      <c r="BM64" s="66"/>
     </row>
     <row r="65" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
@@ -5557,9 +5557,9 @@
       <c r="BH65" s="91"/>
       <c r="BI65" s="91"/>
       <c r="BJ65" s="92"/>
-      <c r="BK65" s="79"/>
-      <c r="BL65" s="80"/>
-      <c r="BM65" s="81"/>
+      <c r="BK65" s="43"/>
+      <c r="BL65" s="44"/>
+      <c r="BM65" s="45"/>
     </row>
     <row r="66" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
@@ -5626,9 +5626,9 @@
       <c r="BH66" s="91"/>
       <c r="BI66" s="91"/>
       <c r="BJ66" s="92"/>
-      <c r="BK66" s="79"/>
-      <c r="BL66" s="80"/>
-      <c r="BM66" s="81"/>
+      <c r="BK66" s="43"/>
+      <c r="BL66" s="44"/>
+      <c r="BM66" s="45"/>
     </row>
     <row r="67" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -5695,77 +5695,77 @@
       <c r="BH67" s="94"/>
       <c r="BI67" s="94"/>
       <c r="BJ67" s="95"/>
-      <c r="BK67" s="82"/>
-      <c r="BL67" s="83"/>
-      <c r="BM67" s="84"/>
+      <c r="BK67" s="46"/>
+      <c r="BL67" s="47"/>
+      <c r="BM67" s="48"/>
     </row>
     <row r="68" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>8</v>
       </c>
-      <c r="B68" s="87" t="s">
+      <c r="B68" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="C68" s="88"/>
-      <c r="D68" s="88"/>
-      <c r="E68" s="88"/>
-      <c r="F68" s="88"/>
-      <c r="G68" s="88"/>
-      <c r="H68" s="88"/>
-      <c r="I68" s="88"/>
-      <c r="J68" s="88"/>
-      <c r="K68" s="88"/>
-      <c r="L68" s="88"/>
-      <c r="M68" s="88"/>
-      <c r="N68" s="88"/>
-      <c r="O68" s="88"/>
-      <c r="P68" s="88"/>
-      <c r="Q68" s="88"/>
-      <c r="R68" s="88"/>
-      <c r="S68" s="88"/>
-      <c r="T68" s="88"/>
-      <c r="U68" s="88"/>
-      <c r="V68" s="88"/>
-      <c r="W68" s="88"/>
-      <c r="X68" s="88"/>
-      <c r="Y68" s="88"/>
-      <c r="Z68" s="88"/>
-      <c r="AA68" s="88"/>
-      <c r="AB68" s="88"/>
-      <c r="AC68" s="88"/>
-      <c r="AD68" s="88"/>
-      <c r="AE68" s="88"/>
-      <c r="AF68" s="88"/>
-      <c r="AG68" s="88"/>
-      <c r="AH68" s="88"/>
-      <c r="AI68" s="88"/>
-      <c r="AJ68" s="88"/>
-      <c r="AK68" s="88"/>
-      <c r="AL68" s="88"/>
-      <c r="AM68" s="88"/>
-      <c r="AN68" s="88"/>
-      <c r="AO68" s="88"/>
-      <c r="AP68" s="88"/>
-      <c r="AQ68" s="88"/>
-      <c r="AR68" s="88"/>
-      <c r="AS68" s="88"/>
-      <c r="AT68" s="88"/>
-      <c r="AU68" s="88"/>
-      <c r="AV68" s="88"/>
-      <c r="AW68" s="88"/>
-      <c r="AX68" s="88"/>
-      <c r="AY68" s="88"/>
-      <c r="AZ68" s="88"/>
-      <c r="BA68" s="88"/>
-      <c r="BB68" s="88"/>
-      <c r="BC68" s="88"/>
-      <c r="BD68" s="88"/>
-      <c r="BE68" s="88"/>
-      <c r="BF68" s="88"/>
-      <c r="BG68" s="88"/>
-      <c r="BH68" s="88"/>
-      <c r="BI68" s="88"/>
-      <c r="BJ68" s="89"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="68"/>
+      <c r="H68" s="68"/>
+      <c r="I68" s="68"/>
+      <c r="J68" s="68"/>
+      <c r="K68" s="68"/>
+      <c r="L68" s="68"/>
+      <c r="M68" s="68"/>
+      <c r="N68" s="68"/>
+      <c r="O68" s="68"/>
+      <c r="P68" s="68"/>
+      <c r="Q68" s="68"/>
+      <c r="R68" s="68"/>
+      <c r="S68" s="68"/>
+      <c r="T68" s="68"/>
+      <c r="U68" s="68"/>
+      <c r="V68" s="68"/>
+      <c r="W68" s="68"/>
+      <c r="X68" s="68"/>
+      <c r="Y68" s="68"/>
+      <c r="Z68" s="68"/>
+      <c r="AA68" s="68"/>
+      <c r="AB68" s="68"/>
+      <c r="AC68" s="68"/>
+      <c r="AD68" s="68"/>
+      <c r="AE68" s="68"/>
+      <c r="AF68" s="68"/>
+      <c r="AG68" s="68"/>
+      <c r="AH68" s="68"/>
+      <c r="AI68" s="68"/>
+      <c r="AJ68" s="68"/>
+      <c r="AK68" s="68"/>
+      <c r="AL68" s="68"/>
+      <c r="AM68" s="68"/>
+      <c r="AN68" s="68"/>
+      <c r="AO68" s="68"/>
+      <c r="AP68" s="68"/>
+      <c r="AQ68" s="68"/>
+      <c r="AR68" s="68"/>
+      <c r="AS68" s="68"/>
+      <c r="AT68" s="68"/>
+      <c r="AU68" s="68"/>
+      <c r="AV68" s="68"/>
+      <c r="AW68" s="68"/>
+      <c r="AX68" s="68"/>
+      <c r="AY68" s="68"/>
+      <c r="AZ68" s="68"/>
+      <c r="BA68" s="68"/>
+      <c r="BB68" s="68"/>
+      <c r="BC68" s="68"/>
+      <c r="BD68" s="68"/>
+      <c r="BE68" s="68"/>
+      <c r="BF68" s="68"/>
+      <c r="BG68" s="68"/>
+      <c r="BH68" s="68"/>
+      <c r="BI68" s="68"/>
+      <c r="BJ68" s="69"/>
       <c r="BK68" s="76" t="s">
         <v>66</v>
       </c>
@@ -5776,67 +5776,67 @@
       <c r="A69" s="1">
         <v>9</v>
       </c>
-      <c r="B69" s="90"/>
-      <c r="C69" s="91"/>
-      <c r="D69" s="91"/>
-      <c r="E69" s="91"/>
-      <c r="F69" s="91"/>
-      <c r="G69" s="91"/>
-      <c r="H69" s="91"/>
-      <c r="I69" s="91"/>
-      <c r="J69" s="91"/>
-      <c r="K69" s="91"/>
-      <c r="L69" s="91"/>
-      <c r="M69" s="91"/>
-      <c r="N69" s="91"/>
-      <c r="O69" s="91"/>
-      <c r="P69" s="91"/>
-      <c r="Q69" s="91"/>
-      <c r="R69" s="91"/>
-      <c r="S69" s="91"/>
-      <c r="T69" s="91"/>
-      <c r="U69" s="91"/>
-      <c r="V69" s="91"/>
-      <c r="W69" s="91"/>
-      <c r="X69" s="91"/>
-      <c r="Y69" s="91"/>
-      <c r="Z69" s="91"/>
-      <c r="AA69" s="91"/>
-      <c r="AB69" s="91"/>
-      <c r="AC69" s="91"/>
-      <c r="AD69" s="91"/>
-      <c r="AE69" s="91"/>
-      <c r="AF69" s="91"/>
-      <c r="AG69" s="91"/>
-      <c r="AH69" s="91"/>
-      <c r="AI69" s="91"/>
-      <c r="AJ69" s="91"/>
-      <c r="AK69" s="91"/>
-      <c r="AL69" s="91"/>
-      <c r="AM69" s="91"/>
-      <c r="AN69" s="91"/>
-      <c r="AO69" s="91"/>
-      <c r="AP69" s="91"/>
-      <c r="AQ69" s="91"/>
-      <c r="AR69" s="91"/>
-      <c r="AS69" s="91"/>
-      <c r="AT69" s="91"/>
-      <c r="AU69" s="91"/>
-      <c r="AV69" s="91"/>
-      <c r="AW69" s="91"/>
-      <c r="AX69" s="91"/>
-      <c r="AY69" s="91"/>
-      <c r="AZ69" s="91"/>
-      <c r="BA69" s="91"/>
-      <c r="BB69" s="91"/>
-      <c r="BC69" s="91"/>
-      <c r="BD69" s="91"/>
-      <c r="BE69" s="91"/>
-      <c r="BF69" s="91"/>
-      <c r="BG69" s="91"/>
-      <c r="BH69" s="91"/>
-      <c r="BI69" s="91"/>
-      <c r="BJ69" s="92"/>
+      <c r="B69" s="70"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="71"/>
+      <c r="E69" s="71"/>
+      <c r="F69" s="71"/>
+      <c r="G69" s="71"/>
+      <c r="H69" s="71"/>
+      <c r="I69" s="71"/>
+      <c r="J69" s="71"/>
+      <c r="K69" s="71"/>
+      <c r="L69" s="71"/>
+      <c r="M69" s="71"/>
+      <c r="N69" s="71"/>
+      <c r="O69" s="71"/>
+      <c r="P69" s="71"/>
+      <c r="Q69" s="71"/>
+      <c r="R69" s="71"/>
+      <c r="S69" s="71"/>
+      <c r="T69" s="71"/>
+      <c r="U69" s="71"/>
+      <c r="V69" s="71"/>
+      <c r="W69" s="71"/>
+      <c r="X69" s="71"/>
+      <c r="Y69" s="71"/>
+      <c r="Z69" s="71"/>
+      <c r="AA69" s="71"/>
+      <c r="AB69" s="71"/>
+      <c r="AC69" s="71"/>
+      <c r="AD69" s="71"/>
+      <c r="AE69" s="71"/>
+      <c r="AF69" s="71"/>
+      <c r="AG69" s="71"/>
+      <c r="AH69" s="71"/>
+      <c r="AI69" s="71"/>
+      <c r="AJ69" s="71"/>
+      <c r="AK69" s="71"/>
+      <c r="AL69" s="71"/>
+      <c r="AM69" s="71"/>
+      <c r="AN69" s="71"/>
+      <c r="AO69" s="71"/>
+      <c r="AP69" s="71"/>
+      <c r="AQ69" s="71"/>
+      <c r="AR69" s="71"/>
+      <c r="AS69" s="71"/>
+      <c r="AT69" s="71"/>
+      <c r="AU69" s="71"/>
+      <c r="AV69" s="71"/>
+      <c r="AW69" s="71"/>
+      <c r="AX69" s="71"/>
+      <c r="AY69" s="71"/>
+      <c r="AZ69" s="71"/>
+      <c r="BA69" s="71"/>
+      <c r="BB69" s="71"/>
+      <c r="BC69" s="71"/>
+      <c r="BD69" s="71"/>
+      <c r="BE69" s="71"/>
+      <c r="BF69" s="71"/>
+      <c r="BG69" s="71"/>
+      <c r="BH69" s="71"/>
+      <c r="BI69" s="71"/>
+      <c r="BJ69" s="72"/>
       <c r="BK69" s="79"/>
       <c r="BL69" s="80"/>
       <c r="BM69" s="81"/>
@@ -5845,67 +5845,67 @@
       <c r="A70" s="2">
         <v>10</v>
       </c>
-      <c r="B70" s="90"/>
-      <c r="C70" s="91"/>
-      <c r="D70" s="91"/>
-      <c r="E70" s="91"/>
-      <c r="F70" s="91"/>
-      <c r="G70" s="91"/>
-      <c r="H70" s="91"/>
-      <c r="I70" s="91"/>
-      <c r="J70" s="91"/>
-      <c r="K70" s="91"/>
-      <c r="L70" s="91"/>
-      <c r="M70" s="91"/>
-      <c r="N70" s="91"/>
-      <c r="O70" s="91"/>
-      <c r="P70" s="91"/>
-      <c r="Q70" s="91"/>
-      <c r="R70" s="91"/>
-      <c r="S70" s="91"/>
-      <c r="T70" s="91"/>
-      <c r="U70" s="91"/>
-      <c r="V70" s="91"/>
-      <c r="W70" s="91"/>
-      <c r="X70" s="91"/>
-      <c r="Y70" s="91"/>
-      <c r="Z70" s="91"/>
-      <c r="AA70" s="91"/>
-      <c r="AB70" s="91"/>
-      <c r="AC70" s="91"/>
-      <c r="AD70" s="91"/>
-      <c r="AE70" s="91"/>
-      <c r="AF70" s="91"/>
-      <c r="AG70" s="91"/>
-      <c r="AH70" s="91"/>
-      <c r="AI70" s="91"/>
-      <c r="AJ70" s="91"/>
-      <c r="AK70" s="91"/>
-      <c r="AL70" s="91"/>
-      <c r="AM70" s="91"/>
-      <c r="AN70" s="91"/>
-      <c r="AO70" s="91"/>
-      <c r="AP70" s="91"/>
-      <c r="AQ70" s="91"/>
-      <c r="AR70" s="91"/>
-      <c r="AS70" s="91"/>
-      <c r="AT70" s="91"/>
-      <c r="AU70" s="91"/>
-      <c r="AV70" s="91"/>
-      <c r="AW70" s="91"/>
-      <c r="AX70" s="91"/>
-      <c r="AY70" s="91"/>
-      <c r="AZ70" s="91"/>
-      <c r="BA70" s="91"/>
-      <c r="BB70" s="91"/>
-      <c r="BC70" s="91"/>
-      <c r="BD70" s="91"/>
-      <c r="BE70" s="91"/>
-      <c r="BF70" s="91"/>
-      <c r="BG70" s="91"/>
-      <c r="BH70" s="91"/>
-      <c r="BI70" s="91"/>
-      <c r="BJ70" s="92"/>
+      <c r="B70" s="70"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="71"/>
+      <c r="E70" s="71"/>
+      <c r="F70" s="71"/>
+      <c r="G70" s="71"/>
+      <c r="H70" s="71"/>
+      <c r="I70" s="71"/>
+      <c r="J70" s="71"/>
+      <c r="K70" s="71"/>
+      <c r="L70" s="71"/>
+      <c r="M70" s="71"/>
+      <c r="N70" s="71"/>
+      <c r="O70" s="71"/>
+      <c r="P70" s="71"/>
+      <c r="Q70" s="71"/>
+      <c r="R70" s="71"/>
+      <c r="S70" s="71"/>
+      <c r="T70" s="71"/>
+      <c r="U70" s="71"/>
+      <c r="V70" s="71"/>
+      <c r="W70" s="71"/>
+      <c r="X70" s="71"/>
+      <c r="Y70" s="71"/>
+      <c r="Z70" s="71"/>
+      <c r="AA70" s="71"/>
+      <c r="AB70" s="71"/>
+      <c r="AC70" s="71"/>
+      <c r="AD70" s="71"/>
+      <c r="AE70" s="71"/>
+      <c r="AF70" s="71"/>
+      <c r="AG70" s="71"/>
+      <c r="AH70" s="71"/>
+      <c r="AI70" s="71"/>
+      <c r="AJ70" s="71"/>
+      <c r="AK70" s="71"/>
+      <c r="AL70" s="71"/>
+      <c r="AM70" s="71"/>
+      <c r="AN70" s="71"/>
+      <c r="AO70" s="71"/>
+      <c r="AP70" s="71"/>
+      <c r="AQ70" s="71"/>
+      <c r="AR70" s="71"/>
+      <c r="AS70" s="71"/>
+      <c r="AT70" s="71"/>
+      <c r="AU70" s="71"/>
+      <c r="AV70" s="71"/>
+      <c r="AW70" s="71"/>
+      <c r="AX70" s="71"/>
+      <c r="AY70" s="71"/>
+      <c r="AZ70" s="71"/>
+      <c r="BA70" s="71"/>
+      <c r="BB70" s="71"/>
+      <c r="BC70" s="71"/>
+      <c r="BD70" s="71"/>
+      <c r="BE70" s="71"/>
+      <c r="BF70" s="71"/>
+      <c r="BG70" s="71"/>
+      <c r="BH70" s="71"/>
+      <c r="BI70" s="71"/>
+      <c r="BJ70" s="72"/>
       <c r="BK70" s="79"/>
       <c r="BL70" s="80"/>
       <c r="BM70" s="81"/>
@@ -5914,67 +5914,67 @@
       <c r="A71" s="1">
         <v>11</v>
       </c>
-      <c r="B71" s="93"/>
-      <c r="C71" s="94"/>
-      <c r="D71" s="94"/>
-      <c r="E71" s="94"/>
-      <c r="F71" s="94"/>
-      <c r="G71" s="94"/>
-      <c r="H71" s="94"/>
-      <c r="I71" s="94"/>
-      <c r="J71" s="94"/>
-      <c r="K71" s="94"/>
-      <c r="L71" s="94"/>
-      <c r="M71" s="94"/>
-      <c r="N71" s="94"/>
-      <c r="O71" s="94"/>
-      <c r="P71" s="94"/>
-      <c r="Q71" s="94"/>
-      <c r="R71" s="94"/>
-      <c r="S71" s="94"/>
-      <c r="T71" s="94"/>
-      <c r="U71" s="94"/>
-      <c r="V71" s="94"/>
-      <c r="W71" s="94"/>
-      <c r="X71" s="94"/>
-      <c r="Y71" s="94"/>
-      <c r="Z71" s="94"/>
-      <c r="AA71" s="94"/>
-      <c r="AB71" s="94"/>
-      <c r="AC71" s="94"/>
-      <c r="AD71" s="94"/>
-      <c r="AE71" s="94"/>
-      <c r="AF71" s="94"/>
-      <c r="AG71" s="94"/>
-      <c r="AH71" s="94"/>
-      <c r="AI71" s="94"/>
-      <c r="AJ71" s="94"/>
-      <c r="AK71" s="94"/>
-      <c r="AL71" s="94"/>
-      <c r="AM71" s="94"/>
-      <c r="AN71" s="94"/>
-      <c r="AO71" s="94"/>
-      <c r="AP71" s="94"/>
-      <c r="AQ71" s="94"/>
-      <c r="AR71" s="94"/>
-      <c r="AS71" s="94"/>
-      <c r="AT71" s="94"/>
-      <c r="AU71" s="94"/>
-      <c r="AV71" s="94"/>
-      <c r="AW71" s="94"/>
-      <c r="AX71" s="94"/>
-      <c r="AY71" s="94"/>
-      <c r="AZ71" s="94"/>
-      <c r="BA71" s="94"/>
-      <c r="BB71" s="94"/>
-      <c r="BC71" s="94"/>
-      <c r="BD71" s="94"/>
-      <c r="BE71" s="94"/>
-      <c r="BF71" s="94"/>
-      <c r="BG71" s="94"/>
-      <c r="BH71" s="94"/>
-      <c r="BI71" s="94"/>
-      <c r="BJ71" s="95"/>
+      <c r="B71" s="73"/>
+      <c r="C71" s="74"/>
+      <c r="D71" s="74"/>
+      <c r="E71" s="74"/>
+      <c r="F71" s="74"/>
+      <c r="G71" s="74"/>
+      <c r="H71" s="74"/>
+      <c r="I71" s="74"/>
+      <c r="J71" s="74"/>
+      <c r="K71" s="74"/>
+      <c r="L71" s="74"/>
+      <c r="M71" s="74"/>
+      <c r="N71" s="74"/>
+      <c r="O71" s="74"/>
+      <c r="P71" s="74"/>
+      <c r="Q71" s="74"/>
+      <c r="R71" s="74"/>
+      <c r="S71" s="74"/>
+      <c r="T71" s="74"/>
+      <c r="U71" s="74"/>
+      <c r="V71" s="74"/>
+      <c r="W71" s="74"/>
+      <c r="X71" s="74"/>
+      <c r="Y71" s="74"/>
+      <c r="Z71" s="74"/>
+      <c r="AA71" s="74"/>
+      <c r="AB71" s="74"/>
+      <c r="AC71" s="74"/>
+      <c r="AD71" s="74"/>
+      <c r="AE71" s="74"/>
+      <c r="AF71" s="74"/>
+      <c r="AG71" s="74"/>
+      <c r="AH71" s="74"/>
+      <c r="AI71" s="74"/>
+      <c r="AJ71" s="74"/>
+      <c r="AK71" s="74"/>
+      <c r="AL71" s="74"/>
+      <c r="AM71" s="74"/>
+      <c r="AN71" s="74"/>
+      <c r="AO71" s="74"/>
+      <c r="AP71" s="74"/>
+      <c r="AQ71" s="74"/>
+      <c r="AR71" s="74"/>
+      <c r="AS71" s="74"/>
+      <c r="AT71" s="74"/>
+      <c r="AU71" s="74"/>
+      <c r="AV71" s="74"/>
+      <c r="AW71" s="74"/>
+      <c r="AX71" s="74"/>
+      <c r="AY71" s="74"/>
+      <c r="AZ71" s="74"/>
+      <c r="BA71" s="74"/>
+      <c r="BB71" s="74"/>
+      <c r="BC71" s="74"/>
+      <c r="BD71" s="74"/>
+      <c r="BE71" s="74"/>
+      <c r="BF71" s="74"/>
+      <c r="BG71" s="74"/>
+      <c r="BH71" s="74"/>
+      <c r="BI71" s="74"/>
+      <c r="BJ71" s="75"/>
       <c r="BK71" s="82"/>
       <c r="BL71" s="83"/>
       <c r="BM71" s="84"/>

</xml_diff>

<commit_message>
Starting IP verification folder, moved some requirements.txt and edited readmes
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F274CAB2-62DD-3B45-AA0F-7235F17A3C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480ABBD6-5C63-C94D-91BB-9A5E08A97E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Memory map" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>CiM PARAMETERS MEMORY MAP</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>mlp_head_softmax_out[0][:]</t>
+  </si>
+  <si>
+    <t>Memory</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1079,15 +1082,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1498,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
   <dimension ref="A1:BQ92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BP49" sqref="BP49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2926,10 +2920,10 @@
       <c r="BK18" s="129"/>
       <c r="BL18" s="129"/>
       <c r="BM18" s="130"/>
-      <c r="BO18" s="175" t="s">
+      <c r="BO18" s="172" t="s">
         <v>71</v>
       </c>
-      <c r="BP18" s="176" t="s">
+      <c r="BP18" s="173" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3003,8 +2997,8 @@
       <c r="BK19" s="123"/>
       <c r="BL19" s="123"/>
       <c r="BM19" s="124"/>
-      <c r="BO19" s="164"/>
-      <c r="BP19" s="164"/>
+      <c r="BO19" s="161"/>
+      <c r="BP19" s="161"/>
     </row>
     <row r="20" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -3074,9 +3068,9 @@
       <c r="BK20" s="126"/>
       <c r="BL20" s="126"/>
       <c r="BM20" s="127"/>
-      <c r="BO20" s="165"/>
-      <c r="BP20" s="162"/>
-      <c r="BQ20" s="163"/>
+      <c r="BO20" s="162"/>
+      <c r="BP20" s="159"/>
+      <c r="BQ20" s="160"/>
     </row>
     <row r="21" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -3864,40 +3858,40 @@
       <c r="AE31" s="46"/>
       <c r="AF31" s="46"/>
       <c r="AG31" s="47"/>
-      <c r="AH31" s="166" t="s">
+      <c r="AH31" s="163" t="s">
         <v>74</v>
       </c>
-      <c r="AI31" s="167"/>
-      <c r="AJ31" s="167"/>
-      <c r="AK31" s="167"/>
-      <c r="AL31" s="167"/>
-      <c r="AM31" s="167"/>
-      <c r="AN31" s="167"/>
-      <c r="AO31" s="167"/>
-      <c r="AP31" s="167"/>
-      <c r="AQ31" s="167"/>
-      <c r="AR31" s="167"/>
-      <c r="AS31" s="167"/>
-      <c r="AT31" s="167"/>
-      <c r="AU31" s="167"/>
-      <c r="AV31" s="167"/>
-      <c r="AW31" s="167"/>
-      <c r="AX31" s="167"/>
-      <c r="AY31" s="167"/>
-      <c r="AZ31" s="167"/>
-      <c r="BA31" s="167"/>
-      <c r="BB31" s="167"/>
-      <c r="BC31" s="167"/>
-      <c r="BD31" s="167"/>
-      <c r="BE31" s="167"/>
-      <c r="BF31" s="167"/>
-      <c r="BG31" s="167"/>
-      <c r="BH31" s="167"/>
-      <c r="BI31" s="167"/>
-      <c r="BJ31" s="167"/>
-      <c r="BK31" s="167"/>
-      <c r="BL31" s="167"/>
-      <c r="BM31" s="168"/>
+      <c r="AI31" s="164"/>
+      <c r="AJ31" s="164"/>
+      <c r="AK31" s="164"/>
+      <c r="AL31" s="164"/>
+      <c r="AM31" s="164"/>
+      <c r="AN31" s="164"/>
+      <c r="AO31" s="164"/>
+      <c r="AP31" s="164"/>
+      <c r="AQ31" s="164"/>
+      <c r="AR31" s="164"/>
+      <c r="AS31" s="164"/>
+      <c r="AT31" s="164"/>
+      <c r="AU31" s="164"/>
+      <c r="AV31" s="164"/>
+      <c r="AW31" s="164"/>
+      <c r="AX31" s="164"/>
+      <c r="AY31" s="164"/>
+      <c r="AZ31" s="164"/>
+      <c r="BA31" s="164"/>
+      <c r="BB31" s="164"/>
+      <c r="BC31" s="164"/>
+      <c r="BD31" s="164"/>
+      <c r="BE31" s="164"/>
+      <c r="BF31" s="164"/>
+      <c r="BG31" s="164"/>
+      <c r="BH31" s="164"/>
+      <c r="BI31" s="164"/>
+      <c r="BJ31" s="164"/>
+      <c r="BK31" s="164"/>
+      <c r="BL31" s="164"/>
+      <c r="BM31" s="165"/>
     </row>
     <row r="32" spans="1:69" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -3935,38 +3929,38 @@
       <c r="AE32" s="49"/>
       <c r="AF32" s="49"/>
       <c r="AG32" s="50"/>
-      <c r="AH32" s="169"/>
-      <c r="AI32" s="170"/>
-      <c r="AJ32" s="170"/>
-      <c r="AK32" s="170"/>
-      <c r="AL32" s="170"/>
-      <c r="AM32" s="170"/>
-      <c r="AN32" s="170"/>
-      <c r="AO32" s="170"/>
-      <c r="AP32" s="170"/>
-      <c r="AQ32" s="170"/>
-      <c r="AR32" s="170"/>
-      <c r="AS32" s="170"/>
-      <c r="AT32" s="170"/>
-      <c r="AU32" s="170"/>
-      <c r="AV32" s="170"/>
-      <c r="AW32" s="170"/>
-      <c r="AX32" s="170"/>
-      <c r="AY32" s="170"/>
-      <c r="AZ32" s="170"/>
-      <c r="BA32" s="170"/>
-      <c r="BB32" s="170"/>
-      <c r="BC32" s="170"/>
-      <c r="BD32" s="170"/>
-      <c r="BE32" s="170"/>
-      <c r="BF32" s="170"/>
-      <c r="BG32" s="170"/>
-      <c r="BH32" s="170"/>
-      <c r="BI32" s="170"/>
-      <c r="BJ32" s="170"/>
-      <c r="BK32" s="170"/>
-      <c r="BL32" s="170"/>
-      <c r="BM32" s="171"/>
+      <c r="AH32" s="166"/>
+      <c r="AI32" s="167"/>
+      <c r="AJ32" s="167"/>
+      <c r="AK32" s="167"/>
+      <c r="AL32" s="167"/>
+      <c r="AM32" s="167"/>
+      <c r="AN32" s="167"/>
+      <c r="AO32" s="167"/>
+      <c r="AP32" s="167"/>
+      <c r="AQ32" s="167"/>
+      <c r="AR32" s="167"/>
+      <c r="AS32" s="167"/>
+      <c r="AT32" s="167"/>
+      <c r="AU32" s="167"/>
+      <c r="AV32" s="167"/>
+      <c r="AW32" s="167"/>
+      <c r="AX32" s="167"/>
+      <c r="AY32" s="167"/>
+      <c r="AZ32" s="167"/>
+      <c r="BA32" s="167"/>
+      <c r="BB32" s="167"/>
+      <c r="BC32" s="167"/>
+      <c r="BD32" s="167"/>
+      <c r="BE32" s="167"/>
+      <c r="BF32" s="167"/>
+      <c r="BG32" s="167"/>
+      <c r="BH32" s="167"/>
+      <c r="BI32" s="167"/>
+      <c r="BJ32" s="167"/>
+      <c r="BK32" s="167"/>
+      <c r="BL32" s="167"/>
+      <c r="BM32" s="168"/>
       <c r="BO32" s="77" t="s">
         <v>5</v>
       </c>
@@ -4008,38 +4002,38 @@
       <c r="AE33" s="49"/>
       <c r="AF33" s="49"/>
       <c r="AG33" s="50"/>
-      <c r="AH33" s="169"/>
-      <c r="AI33" s="170"/>
-      <c r="AJ33" s="170"/>
-      <c r="AK33" s="170"/>
-      <c r="AL33" s="170"/>
-      <c r="AM33" s="170"/>
-      <c r="AN33" s="170"/>
-      <c r="AO33" s="170"/>
-      <c r="AP33" s="170"/>
-      <c r="AQ33" s="170"/>
-      <c r="AR33" s="170"/>
-      <c r="AS33" s="170"/>
-      <c r="AT33" s="170"/>
-      <c r="AU33" s="170"/>
-      <c r="AV33" s="170"/>
-      <c r="AW33" s="170"/>
-      <c r="AX33" s="170"/>
-      <c r="AY33" s="170"/>
-      <c r="AZ33" s="170"/>
-      <c r="BA33" s="170"/>
-      <c r="BB33" s="170"/>
-      <c r="BC33" s="170"/>
-      <c r="BD33" s="170"/>
-      <c r="BE33" s="170"/>
-      <c r="BF33" s="170"/>
-      <c r="BG33" s="170"/>
-      <c r="BH33" s="170"/>
-      <c r="BI33" s="170"/>
-      <c r="BJ33" s="170"/>
-      <c r="BK33" s="170"/>
-      <c r="BL33" s="170"/>
-      <c r="BM33" s="171"/>
+      <c r="AH33" s="166"/>
+      <c r="AI33" s="167"/>
+      <c r="AJ33" s="167"/>
+      <c r="AK33" s="167"/>
+      <c r="AL33" s="167"/>
+      <c r="AM33" s="167"/>
+      <c r="AN33" s="167"/>
+      <c r="AO33" s="167"/>
+      <c r="AP33" s="167"/>
+      <c r="AQ33" s="167"/>
+      <c r="AR33" s="167"/>
+      <c r="AS33" s="167"/>
+      <c r="AT33" s="167"/>
+      <c r="AU33" s="167"/>
+      <c r="AV33" s="167"/>
+      <c r="AW33" s="167"/>
+      <c r="AX33" s="167"/>
+      <c r="AY33" s="167"/>
+      <c r="AZ33" s="167"/>
+      <c r="BA33" s="167"/>
+      <c r="BB33" s="167"/>
+      <c r="BC33" s="167"/>
+      <c r="BD33" s="167"/>
+      <c r="BE33" s="167"/>
+      <c r="BF33" s="167"/>
+      <c r="BG33" s="167"/>
+      <c r="BH33" s="167"/>
+      <c r="BI33" s="167"/>
+      <c r="BJ33" s="167"/>
+      <c r="BK33" s="167"/>
+      <c r="BL33" s="167"/>
+      <c r="BM33" s="168"/>
       <c r="BO33" s="79" t="s">
         <v>6</v>
       </c>
@@ -4081,38 +4075,38 @@
       <c r="AE34" s="52"/>
       <c r="AF34" s="52"/>
       <c r="AG34" s="53"/>
-      <c r="AH34" s="172"/>
-      <c r="AI34" s="173"/>
-      <c r="AJ34" s="173"/>
-      <c r="AK34" s="173"/>
-      <c r="AL34" s="173"/>
-      <c r="AM34" s="173"/>
-      <c r="AN34" s="173"/>
-      <c r="AO34" s="173"/>
-      <c r="AP34" s="173"/>
-      <c r="AQ34" s="173"/>
-      <c r="AR34" s="173"/>
-      <c r="AS34" s="173"/>
-      <c r="AT34" s="173"/>
-      <c r="AU34" s="173"/>
-      <c r="AV34" s="173"/>
-      <c r="AW34" s="173"/>
-      <c r="AX34" s="173"/>
-      <c r="AY34" s="173"/>
-      <c r="AZ34" s="173"/>
-      <c r="BA34" s="173"/>
-      <c r="BB34" s="173"/>
-      <c r="BC34" s="173"/>
-      <c r="BD34" s="173"/>
-      <c r="BE34" s="173"/>
-      <c r="BF34" s="173"/>
-      <c r="BG34" s="173"/>
-      <c r="BH34" s="173"/>
-      <c r="BI34" s="173"/>
-      <c r="BJ34" s="173"/>
-      <c r="BK34" s="173"/>
-      <c r="BL34" s="173"/>
-      <c r="BM34" s="174"/>
+      <c r="AH34" s="169"/>
+      <c r="AI34" s="170"/>
+      <c r="AJ34" s="170"/>
+      <c r="AK34" s="170"/>
+      <c r="AL34" s="170"/>
+      <c r="AM34" s="170"/>
+      <c r="AN34" s="170"/>
+      <c r="AO34" s="170"/>
+      <c r="AP34" s="170"/>
+      <c r="AQ34" s="170"/>
+      <c r="AR34" s="170"/>
+      <c r="AS34" s="170"/>
+      <c r="AT34" s="170"/>
+      <c r="AU34" s="170"/>
+      <c r="AV34" s="170"/>
+      <c r="AW34" s="170"/>
+      <c r="AX34" s="170"/>
+      <c r="AY34" s="170"/>
+      <c r="AZ34" s="170"/>
+      <c r="BA34" s="170"/>
+      <c r="BB34" s="170"/>
+      <c r="BC34" s="170"/>
+      <c r="BD34" s="170"/>
+      <c r="BE34" s="170"/>
+      <c r="BF34" s="170"/>
+      <c r="BG34" s="170"/>
+      <c r="BH34" s="170"/>
+      <c r="BI34" s="170"/>
+      <c r="BJ34" s="170"/>
+      <c r="BK34" s="170"/>
+      <c r="BL34" s="170"/>
+      <c r="BM34" s="171"/>
       <c r="BO34" s="10" t="s">
         <v>7</v>
       </c>
@@ -4213,12 +4207,12 @@
       <c r="BG35" s="143"/>
       <c r="BH35" s="143"/>
       <c r="BI35" s="144"/>
-      <c r="BJ35" s="177" t="s">
+      <c r="BJ35" s="174" t="s">
         <v>71</v>
       </c>
-      <c r="BK35" s="178"/>
-      <c r="BL35" s="178"/>
-      <c r="BM35" s="179"/>
+      <c r="BK35" s="175"/>
+      <c r="BL35" s="175"/>
+      <c r="BM35" s="176"/>
       <c r="BO35" s="10" t="s">
         <v>9</v>
       </c>
@@ -4460,40 +4454,40 @@
       <c r="A41" s="2">
         <v>0</v>
       </c>
-      <c r="B41" s="159" t="s">
+      <c r="B41" s="179" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="185"/>
-      <c r="D41" s="185"/>
-      <c r="E41" s="185"/>
-      <c r="F41" s="185"/>
-      <c r="G41" s="185"/>
-      <c r="H41" s="185"/>
-      <c r="I41" s="185"/>
-      <c r="J41" s="185"/>
-      <c r="K41" s="185"/>
-      <c r="L41" s="185"/>
-      <c r="M41" s="185"/>
-      <c r="N41" s="185"/>
-      <c r="O41" s="185"/>
-      <c r="P41" s="185"/>
-      <c r="Q41" s="185"/>
-      <c r="R41" s="185"/>
-      <c r="S41" s="185"/>
-      <c r="T41" s="185"/>
-      <c r="U41" s="185"/>
-      <c r="V41" s="185"/>
-      <c r="W41" s="185"/>
-      <c r="X41" s="185"/>
-      <c r="Y41" s="185"/>
-      <c r="Z41" s="185"/>
-      <c r="AA41" s="185"/>
-      <c r="AB41" s="185"/>
-      <c r="AC41" s="185"/>
-      <c r="AD41" s="185"/>
-      <c r="AE41" s="185"/>
-      <c r="AF41" s="185"/>
-      <c r="AG41" s="188"/>
+      <c r="C41" s="182"/>
+      <c r="D41" s="182"/>
+      <c r="E41" s="182"/>
+      <c r="F41" s="182"/>
+      <c r="G41" s="182"/>
+      <c r="H41" s="182"/>
+      <c r="I41" s="182"/>
+      <c r="J41" s="182"/>
+      <c r="K41" s="182"/>
+      <c r="L41" s="182"/>
+      <c r="M41" s="182"/>
+      <c r="N41" s="182"/>
+      <c r="O41" s="182"/>
+      <c r="P41" s="182"/>
+      <c r="Q41" s="182"/>
+      <c r="R41" s="182"/>
+      <c r="S41" s="182"/>
+      <c r="T41" s="182"/>
+      <c r="U41" s="182"/>
+      <c r="V41" s="182"/>
+      <c r="W41" s="182"/>
+      <c r="X41" s="182"/>
+      <c r="Y41" s="182"/>
+      <c r="Z41" s="182"/>
+      <c r="AA41" s="182"/>
+      <c r="AB41" s="182"/>
+      <c r="AC41" s="182"/>
+      <c r="AD41" s="182"/>
+      <c r="AE41" s="182"/>
+      <c r="AF41" s="182"/>
+      <c r="AG41" s="185"/>
       <c r="AH41" s="69" t="s">
         <v>79</v>
       </c>
@@ -4501,30 +4495,30 @@
       <c r="AJ41" s="70"/>
       <c r="AK41" s="70"/>
       <c r="AL41" s="71"/>
-      <c r="AM41" s="185"/>
-      <c r="AN41" s="185"/>
-      <c r="AO41" s="185"/>
-      <c r="AP41" s="185"/>
-      <c r="AQ41" s="185"/>
-      <c r="AR41" s="185"/>
-      <c r="AS41" s="185"/>
-      <c r="AT41" s="185"/>
-      <c r="AU41" s="185"/>
-      <c r="AV41" s="185"/>
-      <c r="AW41" s="185"/>
-      <c r="AX41" s="185"/>
-      <c r="AY41" s="185"/>
-      <c r="AZ41" s="185"/>
-      <c r="BA41" s="185"/>
-      <c r="BB41" s="185"/>
-      <c r="BC41" s="185"/>
-      <c r="BD41" s="185"/>
-      <c r="BE41" s="185"/>
-      <c r="BF41" s="185"/>
-      <c r="BG41" s="185"/>
-      <c r="BH41" s="185"/>
-      <c r="BI41" s="185"/>
-      <c r="BJ41" s="185"/>
+      <c r="AM41" s="182"/>
+      <c r="AN41" s="182"/>
+      <c r="AO41" s="182"/>
+      <c r="AP41" s="182"/>
+      <c r="AQ41" s="182"/>
+      <c r="AR41" s="182"/>
+      <c r="AS41" s="182"/>
+      <c r="AT41" s="182"/>
+      <c r="AU41" s="182"/>
+      <c r="AV41" s="182"/>
+      <c r="AW41" s="182"/>
+      <c r="AX41" s="182"/>
+      <c r="AY41" s="182"/>
+      <c r="AZ41" s="182"/>
+      <c r="BA41" s="182"/>
+      <c r="BB41" s="182"/>
+      <c r="BC41" s="182"/>
+      <c r="BD41" s="182"/>
+      <c r="BE41" s="182"/>
+      <c r="BF41" s="182"/>
+      <c r="BG41" s="182"/>
+      <c r="BH41" s="182"/>
+      <c r="BI41" s="182"/>
+      <c r="BJ41" s="182"/>
       <c r="BK41" s="57" t="s">
         <v>66</v>
       </c>
@@ -4538,67 +4532,67 @@
       <c r="A42" s="1">
         <v>1</v>
       </c>
-      <c r="B42" s="160"/>
-      <c r="C42" s="186"/>
-      <c r="D42" s="186"/>
-      <c r="E42" s="186"/>
-      <c r="F42" s="186"/>
-      <c r="G42" s="186"/>
-      <c r="H42" s="186"/>
-      <c r="I42" s="186"/>
-      <c r="J42" s="186"/>
-      <c r="K42" s="186"/>
-      <c r="L42" s="186"/>
-      <c r="M42" s="186"/>
-      <c r="N42" s="186"/>
-      <c r="O42" s="186"/>
-      <c r="P42" s="186"/>
-      <c r="Q42" s="186"/>
-      <c r="R42" s="186"/>
-      <c r="S42" s="186"/>
-      <c r="T42" s="186"/>
-      <c r="U42" s="186"/>
-      <c r="V42" s="186"/>
-      <c r="W42" s="186"/>
-      <c r="X42" s="186"/>
-      <c r="Y42" s="186"/>
-      <c r="Z42" s="186"/>
-      <c r="AA42" s="186"/>
-      <c r="AB42" s="186"/>
-      <c r="AC42" s="186"/>
-      <c r="AD42" s="186"/>
-      <c r="AE42" s="186"/>
-      <c r="AF42" s="186"/>
-      <c r="AG42" s="189"/>
+      <c r="B42" s="180"/>
+      <c r="C42" s="183"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="183"/>
+      <c r="F42" s="183"/>
+      <c r="G42" s="183"/>
+      <c r="H42" s="183"/>
+      <c r="I42" s="183"/>
+      <c r="J42" s="183"/>
+      <c r="K42" s="183"/>
+      <c r="L42" s="183"/>
+      <c r="M42" s="183"/>
+      <c r="N42" s="183"/>
+      <c r="O42" s="183"/>
+      <c r="P42" s="183"/>
+      <c r="Q42" s="183"/>
+      <c r="R42" s="183"/>
+      <c r="S42" s="183"/>
+      <c r="T42" s="183"/>
+      <c r="U42" s="183"/>
+      <c r="V42" s="183"/>
+      <c r="W42" s="183"/>
+      <c r="X42" s="183"/>
+      <c r="Y42" s="183"/>
+      <c r="Z42" s="183"/>
+      <c r="AA42" s="183"/>
+      <c r="AB42" s="183"/>
+      <c r="AC42" s="183"/>
+      <c r="AD42" s="183"/>
+      <c r="AE42" s="183"/>
+      <c r="AF42" s="183"/>
+      <c r="AG42" s="186"/>
       <c r="AH42" s="72"/>
       <c r="AI42" s="158"/>
       <c r="AJ42" s="158"/>
       <c r="AK42" s="158"/>
       <c r="AL42" s="73"/>
-      <c r="AM42" s="186"/>
-      <c r="AN42" s="186"/>
-      <c r="AO42" s="186"/>
-      <c r="AP42" s="186"/>
-      <c r="AQ42" s="186"/>
-      <c r="AR42" s="186"/>
-      <c r="AS42" s="186"/>
-      <c r="AT42" s="186"/>
-      <c r="AU42" s="186"/>
-      <c r="AV42" s="186"/>
-      <c r="AW42" s="186"/>
-      <c r="AX42" s="186"/>
-      <c r="AY42" s="186"/>
-      <c r="AZ42" s="186"/>
-      <c r="BA42" s="186"/>
-      <c r="BB42" s="186"/>
-      <c r="BC42" s="186"/>
-      <c r="BD42" s="186"/>
-      <c r="BE42" s="186"/>
-      <c r="BF42" s="186"/>
-      <c r="BG42" s="186"/>
-      <c r="BH42" s="186"/>
-      <c r="BI42" s="186"/>
-      <c r="BJ42" s="186"/>
+      <c r="AM42" s="183"/>
+      <c r="AN42" s="183"/>
+      <c r="AO42" s="183"/>
+      <c r="AP42" s="183"/>
+      <c r="AQ42" s="183"/>
+      <c r="AR42" s="183"/>
+      <c r="AS42" s="183"/>
+      <c r="AT42" s="183"/>
+      <c r="AU42" s="183"/>
+      <c r="AV42" s="183"/>
+      <c r="AW42" s="183"/>
+      <c r="AX42" s="183"/>
+      <c r="AY42" s="183"/>
+      <c r="AZ42" s="183"/>
+      <c r="BA42" s="183"/>
+      <c r="BB42" s="183"/>
+      <c r="BC42" s="183"/>
+      <c r="BD42" s="183"/>
+      <c r="BE42" s="183"/>
+      <c r="BF42" s="183"/>
+      <c r="BG42" s="183"/>
+      <c r="BH42" s="183"/>
+      <c r="BI42" s="183"/>
+      <c r="BJ42" s="183"/>
       <c r="BK42" s="36"/>
       <c r="BL42" s="157"/>
       <c r="BM42" s="38"/>
@@ -4610,67 +4604,67 @@
       <c r="A43" s="2">
         <v>2</v>
       </c>
-      <c r="B43" s="160"/>
-      <c r="C43" s="186"/>
-      <c r="D43" s="186"/>
-      <c r="E43" s="186"/>
-      <c r="F43" s="186"/>
-      <c r="G43" s="186"/>
-      <c r="H43" s="186"/>
-      <c r="I43" s="186"/>
-      <c r="J43" s="186"/>
-      <c r="K43" s="186"/>
-      <c r="L43" s="186"/>
-      <c r="M43" s="186"/>
-      <c r="N43" s="186"/>
-      <c r="O43" s="186"/>
-      <c r="P43" s="186"/>
-      <c r="Q43" s="186"/>
-      <c r="R43" s="186"/>
-      <c r="S43" s="186"/>
-      <c r="T43" s="186"/>
-      <c r="U43" s="186"/>
-      <c r="V43" s="186"/>
-      <c r="W43" s="186"/>
-      <c r="X43" s="186"/>
-      <c r="Y43" s="186"/>
-      <c r="Z43" s="186"/>
-      <c r="AA43" s="186"/>
-      <c r="AB43" s="186"/>
-      <c r="AC43" s="186"/>
-      <c r="AD43" s="186"/>
-      <c r="AE43" s="186"/>
-      <c r="AF43" s="186"/>
-      <c r="AG43" s="189"/>
+      <c r="B43" s="180"/>
+      <c r="C43" s="183"/>
+      <c r="D43" s="183"/>
+      <c r="E43" s="183"/>
+      <c r="F43" s="183"/>
+      <c r="G43" s="183"/>
+      <c r="H43" s="183"/>
+      <c r="I43" s="183"/>
+      <c r="J43" s="183"/>
+      <c r="K43" s="183"/>
+      <c r="L43" s="183"/>
+      <c r="M43" s="183"/>
+      <c r="N43" s="183"/>
+      <c r="O43" s="183"/>
+      <c r="P43" s="183"/>
+      <c r="Q43" s="183"/>
+      <c r="R43" s="183"/>
+      <c r="S43" s="183"/>
+      <c r="T43" s="183"/>
+      <c r="U43" s="183"/>
+      <c r="V43" s="183"/>
+      <c r="W43" s="183"/>
+      <c r="X43" s="183"/>
+      <c r="Y43" s="183"/>
+      <c r="Z43" s="183"/>
+      <c r="AA43" s="183"/>
+      <c r="AB43" s="183"/>
+      <c r="AC43" s="183"/>
+      <c r="AD43" s="183"/>
+      <c r="AE43" s="183"/>
+      <c r="AF43" s="183"/>
+      <c r="AG43" s="186"/>
       <c r="AH43" s="72"/>
       <c r="AI43" s="158"/>
       <c r="AJ43" s="158"/>
       <c r="AK43" s="158"/>
       <c r="AL43" s="73"/>
-      <c r="AM43" s="186"/>
-      <c r="AN43" s="186"/>
-      <c r="AO43" s="186"/>
-      <c r="AP43" s="186"/>
-      <c r="AQ43" s="186"/>
-      <c r="AR43" s="186"/>
-      <c r="AS43" s="186"/>
-      <c r="AT43" s="186"/>
-      <c r="AU43" s="186"/>
-      <c r="AV43" s="186"/>
-      <c r="AW43" s="186"/>
-      <c r="AX43" s="186"/>
-      <c r="AY43" s="186"/>
-      <c r="AZ43" s="186"/>
-      <c r="BA43" s="186"/>
-      <c r="BB43" s="186"/>
-      <c r="BC43" s="186"/>
-      <c r="BD43" s="186"/>
-      <c r="BE43" s="186"/>
-      <c r="BF43" s="186"/>
-      <c r="BG43" s="186"/>
-      <c r="BH43" s="186"/>
-      <c r="BI43" s="186"/>
-      <c r="BJ43" s="186"/>
+      <c r="AM43" s="183"/>
+      <c r="AN43" s="183"/>
+      <c r="AO43" s="183"/>
+      <c r="AP43" s="183"/>
+      <c r="AQ43" s="183"/>
+      <c r="AR43" s="183"/>
+      <c r="AS43" s="183"/>
+      <c r="AT43" s="183"/>
+      <c r="AU43" s="183"/>
+      <c r="AV43" s="183"/>
+      <c r="AW43" s="183"/>
+      <c r="AX43" s="183"/>
+      <c r="AY43" s="183"/>
+      <c r="AZ43" s="183"/>
+      <c r="BA43" s="183"/>
+      <c r="BB43" s="183"/>
+      <c r="BC43" s="183"/>
+      <c r="BD43" s="183"/>
+      <c r="BE43" s="183"/>
+      <c r="BF43" s="183"/>
+      <c r="BG43" s="183"/>
+      <c r="BH43" s="183"/>
+      <c r="BI43" s="183"/>
+      <c r="BJ43" s="183"/>
       <c r="BK43" s="36"/>
       <c r="BL43" s="157"/>
       <c r="BM43" s="38"/>
@@ -4682,67 +4676,67 @@
       <c r="A44" s="1">
         <v>3</v>
       </c>
-      <c r="B44" s="161"/>
-      <c r="C44" s="187"/>
-      <c r="D44" s="187"/>
-      <c r="E44" s="187"/>
-      <c r="F44" s="187"/>
-      <c r="G44" s="187"/>
-      <c r="H44" s="187"/>
-      <c r="I44" s="187"/>
-      <c r="J44" s="187"/>
-      <c r="K44" s="187"/>
-      <c r="L44" s="187"/>
-      <c r="M44" s="187"/>
-      <c r="N44" s="187"/>
-      <c r="O44" s="187"/>
-      <c r="P44" s="187"/>
-      <c r="Q44" s="187"/>
-      <c r="R44" s="187"/>
-      <c r="S44" s="187"/>
-      <c r="T44" s="187"/>
-      <c r="U44" s="187"/>
-      <c r="V44" s="187"/>
-      <c r="W44" s="187"/>
-      <c r="X44" s="187"/>
-      <c r="Y44" s="187"/>
-      <c r="Z44" s="187"/>
-      <c r="AA44" s="187"/>
-      <c r="AB44" s="187"/>
-      <c r="AC44" s="187"/>
-      <c r="AD44" s="187"/>
-      <c r="AE44" s="187"/>
-      <c r="AF44" s="187"/>
-      <c r="AG44" s="190"/>
+      <c r="B44" s="181"/>
+      <c r="C44" s="184"/>
+      <c r="D44" s="184"/>
+      <c r="E44" s="184"/>
+      <c r="F44" s="184"/>
+      <c r="G44" s="184"/>
+      <c r="H44" s="184"/>
+      <c r="I44" s="184"/>
+      <c r="J44" s="184"/>
+      <c r="K44" s="184"/>
+      <c r="L44" s="184"/>
+      <c r="M44" s="184"/>
+      <c r="N44" s="184"/>
+      <c r="O44" s="184"/>
+      <c r="P44" s="184"/>
+      <c r="Q44" s="184"/>
+      <c r="R44" s="184"/>
+      <c r="S44" s="184"/>
+      <c r="T44" s="184"/>
+      <c r="U44" s="184"/>
+      <c r="V44" s="184"/>
+      <c r="W44" s="184"/>
+      <c r="X44" s="184"/>
+      <c r="Y44" s="184"/>
+      <c r="Z44" s="184"/>
+      <c r="AA44" s="184"/>
+      <c r="AB44" s="184"/>
+      <c r="AC44" s="184"/>
+      <c r="AD44" s="184"/>
+      <c r="AE44" s="184"/>
+      <c r="AF44" s="184"/>
+      <c r="AG44" s="187"/>
       <c r="AH44" s="74"/>
       <c r="AI44" s="75"/>
       <c r="AJ44" s="75"/>
       <c r="AK44" s="75"/>
       <c r="AL44" s="76"/>
-      <c r="AM44" s="187"/>
-      <c r="AN44" s="187"/>
-      <c r="AO44" s="187"/>
-      <c r="AP44" s="187"/>
-      <c r="AQ44" s="187"/>
-      <c r="AR44" s="187"/>
-      <c r="AS44" s="187"/>
-      <c r="AT44" s="187"/>
-      <c r="AU44" s="187"/>
-      <c r="AV44" s="187"/>
-      <c r="AW44" s="187"/>
-      <c r="AX44" s="187"/>
-      <c r="AY44" s="187"/>
-      <c r="AZ44" s="187"/>
-      <c r="BA44" s="187"/>
-      <c r="BB44" s="187"/>
-      <c r="BC44" s="187"/>
-      <c r="BD44" s="187"/>
-      <c r="BE44" s="187"/>
-      <c r="BF44" s="187"/>
-      <c r="BG44" s="187"/>
-      <c r="BH44" s="187"/>
-      <c r="BI44" s="187"/>
-      <c r="BJ44" s="187"/>
+      <c r="AM44" s="184"/>
+      <c r="AN44" s="184"/>
+      <c r="AO44" s="184"/>
+      <c r="AP44" s="184"/>
+      <c r="AQ44" s="184"/>
+      <c r="AR44" s="184"/>
+      <c r="AS44" s="184"/>
+      <c r="AT44" s="184"/>
+      <c r="AU44" s="184"/>
+      <c r="AV44" s="184"/>
+      <c r="AW44" s="184"/>
+      <c r="AX44" s="184"/>
+      <c r="AY44" s="184"/>
+      <c r="AZ44" s="184"/>
+      <c r="BA44" s="184"/>
+      <c r="BB44" s="184"/>
+      <c r="BC44" s="184"/>
+      <c r="BD44" s="184"/>
+      <c r="BE44" s="184"/>
+      <c r="BF44" s="184"/>
+      <c r="BG44" s="184"/>
+      <c r="BH44" s="184"/>
+      <c r="BI44" s="184"/>
+      <c r="BJ44" s="184"/>
       <c r="BK44" s="39"/>
       <c r="BL44" s="40"/>
       <c r="BM44" s="41"/>
@@ -4814,7 +4808,7 @@
       <c r="BH45" s="61"/>
       <c r="BI45" s="61"/>
       <c r="BJ45" s="62"/>
-      <c r="BK45" s="182" t="s">
+      <c r="BK45" s="179" t="s">
         <v>67</v>
       </c>
       <c r="BL45" s="145"/>
@@ -4885,8 +4879,8 @@
       <c r="BH46" s="64"/>
       <c r="BI46" s="64"/>
       <c r="BJ46" s="65"/>
-      <c r="BK46" s="183"/>
-      <c r="BL46" s="181"/>
+      <c r="BK46" s="180"/>
+      <c r="BL46" s="178"/>
       <c r="BM46" s="147"/>
     </row>
     <row r="47" spans="1:68" x14ac:dyDescent="0.2">
@@ -4954,8 +4948,8 @@
       <c r="BH47" s="64"/>
       <c r="BI47" s="64"/>
       <c r="BJ47" s="65"/>
-      <c r="BK47" s="183"/>
-      <c r="BL47" s="181"/>
+      <c r="BK47" s="180"/>
+      <c r="BL47" s="178"/>
       <c r="BM47" s="147"/>
     </row>
     <row r="48" spans="1:68" x14ac:dyDescent="0.2">
@@ -5023,11 +5017,11 @@
       <c r="BH48" s="67"/>
       <c r="BI48" s="67"/>
       <c r="BJ48" s="68"/>
-      <c r="BK48" s="184"/>
+      <c r="BK48" s="181"/>
       <c r="BL48" s="148"/>
       <c r="BM48" s="149"/>
     </row>
-    <row r="49" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:68" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>8</v>
       </c>
@@ -5099,8 +5093,11 @@
       </c>
       <c r="BL49" s="58"/>
       <c r="BM49" s="59"/>
-    </row>
-    <row r="50" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="BP49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>9</v>
       </c>
@@ -5169,7 +5166,7 @@
       <c r="BL50" s="37"/>
       <c r="BM50" s="38"/>
     </row>
-    <row r="51" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>10</v>
       </c>
@@ -5238,7 +5235,7 @@
       <c r="BL51" s="37"/>
       <c r="BM51" s="38"/>
     </row>
-    <row r="52" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>11</v>
       </c>
@@ -5307,7 +5304,7 @@
       <c r="BL52" s="40"/>
       <c r="BM52" s="41"/>
     </row>
-    <row r="53" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:68" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>12</v>
       </c>
@@ -5380,7 +5377,7 @@
       <c r="BL53" s="58"/>
       <c r="BM53" s="59"/>
     </row>
-    <row r="54" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>13</v>
       </c>
@@ -5449,7 +5446,7 @@
       <c r="BL54" s="37"/>
       <c r="BM54" s="38"/>
     </row>
-    <row r="55" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>14</v>
       </c>
@@ -5518,7 +5515,7 @@
       <c r="BL55" s="37"/>
       <c r="BM55" s="38"/>
     </row>
-    <row r="56" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>15</v>
       </c>
@@ -5587,7 +5584,7 @@
       <c r="BL56" s="40"/>
       <c r="BM56" s="41"/>
     </row>
-    <row r="57" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:68" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>16</v>
       </c>
@@ -5660,7 +5657,7 @@
       <c r="BL57" s="58"/>
       <c r="BM57" s="59"/>
     </row>
-    <row r="58" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>17</v>
       </c>
@@ -5729,7 +5726,7 @@
       <c r="BL58" s="37"/>
       <c r="BM58" s="38"/>
     </row>
-    <row r="59" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>18</v>
       </c>
@@ -5798,7 +5795,7 @@
       <c r="BL59" s="37"/>
       <c r="BM59" s="38"/>
     </row>
-    <row r="60" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>19</v>
       </c>
@@ -5867,7 +5864,7 @@
       <c r="BL60" s="40"/>
       <c r="BM60" s="41"/>
     </row>
-    <row r="61" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:68" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>20</v>
       </c>
@@ -5940,7 +5937,7 @@
       <c r="BL61" s="58"/>
       <c r="BM61" s="59"/>
     </row>
-    <row r="62" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>21</v>
       </c>
@@ -6009,7 +6006,7 @@
       <c r="BL62" s="37"/>
       <c r="BM62" s="38"/>
     </row>
-    <row r="63" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>22</v>
       </c>
@@ -6078,7 +6075,7 @@
       <c r="BL63" s="37"/>
       <c r="BM63" s="38"/>
     </row>
-    <row r="64" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>23</v>
       </c>
@@ -6426,8 +6423,8 @@
       <c r="BK68" s="40"/>
       <c r="BL68" s="40"/>
       <c r="BM68" s="41"/>
-      <c r="BP68" s="163"/>
-      <c r="BQ68" s="163"/>
+      <c r="BP68" s="160"/>
+      <c r="BQ68" s="160"/>
     </row>
     <row r="69" spans="1:69" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
@@ -6501,8 +6498,8 @@
       <c r="BK69" s="58"/>
       <c r="BL69" s="58"/>
       <c r="BM69" s="59"/>
-      <c r="BP69" s="164"/>
-      <c r="BQ69" s="164"/>
+      <c r="BP69" s="161"/>
+      <c r="BQ69" s="161"/>
     </row>
     <row r="70" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -6572,8 +6569,8 @@
       <c r="BK70" s="37"/>
       <c r="BL70" s="37"/>
       <c r="BM70" s="38"/>
-      <c r="BP70" s="180"/>
-      <c r="BQ70" s="180"/>
+      <c r="BP70" s="177"/>
+      <c r="BQ70" s="177"/>
     </row>
     <row r="71" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A71" s="1">

</xml_diff>

<commit_message>
All weights are properly loaded (manually checked). Started to add automatic checking of the inference step results. So far, patch load, positional embedding, classification token all have automatic results verification
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306289E8-2DB4-F448-9858-B268E4E93207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F85D494-4C2A-7B42-BBF4-E32396B3C0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
   <si>
     <t>CiM PARAMETERS MEMORY MAP</t>
   </si>
@@ -276,9 +276,6 @@
     <t>mlp_head_softmax_out[0][:]</t>
   </si>
   <si>
-    <t>Memory</t>
-  </si>
-  <si>
     <t>softmax_out_-1</t>
   </si>
   <si>
@@ -303,10 +300,10 @@
     <t>filtered_softmax[id]</t>
   </si>
   <si>
-    <t>mlp.dense1.bias[id] / mlp_head_dense_1.bias[id] (1x float32)</t>
-  </si>
-  <si>
     <t>mlp_head.LayerNorm2.gamma[id] (1 x float32)</t>
+  </si>
+  <si>
+    <t>mlp.dense1.bias[id] / mlp_head_dense_1.bias[id] (1 x float32)</t>
   </si>
 </sst>
 </file>
@@ -1537,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55CAFD0-475F-A04D-A042-FEAC302FFF8D}">
   <dimension ref="A1:BQ97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BP17" sqref="BP17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BP52" sqref="BP52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2818,7 +2815,7 @@
         <v>61</v>
       </c>
       <c r="BP16" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:69" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4274,7 +4271,7 @@
     </row>
     <row r="37" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A37" s="53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" s="54"/>
       <c r="C37" s="54"/>
@@ -4336,7 +4333,7 @@
       <c r="P38" s="59"/>
       <c r="Q38" s="59"/>
       <c r="BO38" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:68" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4344,14 +4341,14 @@
         <v>1</v>
       </c>
       <c r="B39" s="65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" s="66"/>
       <c r="D39" s="66"/>
       <c r="E39" s="66"/>
       <c r="F39" s="67"/>
       <c r="G39" s="65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H39" s="66"/>
       <c r="I39" s="66"/>
@@ -4360,7 +4357,7 @@
       <c r="L39" s="43"/>
       <c r="M39" s="43"/>
       <c r="BO39" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:68" x14ac:dyDescent="0.2">
@@ -4684,21 +4681,21 @@
       <c r="AK46" s="66"/>
       <c r="AL46" s="67"/>
       <c r="AM46" s="65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AN46" s="66"/>
       <c r="AO46" s="66"/>
       <c r="AP46" s="66"/>
       <c r="AQ46" s="67"/>
       <c r="AR46" s="65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AS46" s="66"/>
       <c r="AT46" s="66"/>
       <c r="AU46" s="66"/>
       <c r="AV46" s="67"/>
       <c r="AW46" s="65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AX46" s="66"/>
       <c r="AY46" s="66"/>
@@ -4866,7 +4863,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -4935,7 +4932,7 @@
       <c r="BL49" s="167"/>
       <c r="BM49" s="168"/>
     </row>
-    <row r="50" spans="1:68" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>4</v>
       </c>
@@ -5008,7 +5005,7 @@
       <c r="BL50" s="38"/>
       <c r="BM50" s="39"/>
     </row>
-    <row r="51" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>5</v>
       </c>
@@ -5077,7 +5074,7 @@
       <c r="BL51" s="46"/>
       <c r="BM51" s="40"/>
     </row>
-    <row r="52" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>6</v>
       </c>
@@ -5146,7 +5143,7 @@
       <c r="BL52" s="46"/>
       <c r="BM52" s="40"/>
     </row>
-    <row r="53" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>7</v>
       </c>
@@ -5215,7 +5212,7 @@
       <c r="BL53" s="41"/>
       <c r="BM53" s="42"/>
     </row>
-    <row r="54" spans="1:68" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>8</v>
       </c>
@@ -5287,11 +5284,8 @@
       </c>
       <c r="BL54" s="161"/>
       <c r="BM54" s="162"/>
-      <c r="BP54" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="1:68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>9</v>
       </c>
@@ -5360,7 +5354,7 @@
       <c r="BL55" s="164"/>
       <c r="BM55" s="165"/>
     </row>
-    <row r="56" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>10</v>
       </c>
@@ -5429,7 +5423,7 @@
       <c r="BL56" s="164"/>
       <c r="BM56" s="165"/>
     </row>
-    <row r="57" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>11</v>
       </c>
@@ -5498,7 +5492,7 @@
       <c r="BL57" s="167"/>
       <c r="BM57" s="168"/>
     </row>
-    <row r="58" spans="1:68" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>12</v>
       </c>
@@ -5571,7 +5565,7 @@
       <c r="BL58" s="161"/>
       <c r="BM58" s="162"/>
     </row>
-    <row r="59" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>13</v>
       </c>
@@ -5640,7 +5634,7 @@
       <c r="BL59" s="164"/>
       <c r="BM59" s="165"/>
     </row>
-    <row r="60" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>14</v>
       </c>
@@ -5709,7 +5703,7 @@
       <c r="BL60" s="164"/>
       <c r="BM60" s="165"/>
     </row>
-    <row r="61" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>15</v>
       </c>
@@ -5778,7 +5772,7 @@
       <c r="BL61" s="167"/>
       <c r="BM61" s="168"/>
     </row>
-    <row r="62" spans="1:68" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:65" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>16</v>
       </c>
@@ -5851,7 +5845,7 @@
       <c r="BL62" s="161"/>
       <c r="BM62" s="162"/>
     </row>
-    <row r="63" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>17</v>
       </c>
@@ -5920,7 +5914,7 @@
       <c r="BL63" s="164"/>
       <c r="BM63" s="165"/>
     </row>
-    <row r="64" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Added patch projectio dense
</commit_message>
<xml_diff>
--- a/asic/CiM_mem_map.xlsx
+++ b/asic/CiM_mem_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Developer/engsci-thesis/asic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7F9D9A-F33C-8F46-9535-50FE1F4590CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878B783E-58F0-034E-9684-7E1F48A0D133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="26780" windowWidth="33600" windowHeight="20500" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{8CF7BA68-15AC-A04C-9888-F9B48A0742FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory map" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>-Each cell is 1 byte</t>
   </si>
   <si>
     <t>-Matrix indexing is row-major: A[row][col]</t>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>1/sqrt(# heads) (1)</t>
+  </si>
+  <si>
+    <t>-Each cell is 1 word</t>
   </si>
 </sst>
 </file>
@@ -710,6 +710,195 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -773,15 +962,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,24 +971,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -834,168 +996,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1326,7 +1326,7 @@
   <dimension ref="A1:BQ119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BA38" sqref="BA38:BB38"/>
+      <selection activeCell="B23" sqref="B23:BM26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1339,18 +1339,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:68">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="120"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="114"/>
       <c r="K1" s="1"/>
       <c r="L1" s="2"/>
     </row>
@@ -1557,1281 +1557,1281 @@
       <c r="A3" s="5">
         <v>0</v>
       </c>
-      <c r="B3" s="94" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="95"/>
-      <c r="Z3" s="95"/>
-      <c r="AA3" s="95"/>
-      <c r="AB3" s="95"/>
-      <c r="AC3" s="95"/>
-      <c r="AD3" s="95"/>
-      <c r="AE3" s="95"/>
-      <c r="AF3" s="95"/>
-      <c r="AG3" s="95"/>
-      <c r="AH3" s="95"/>
-      <c r="AI3" s="95"/>
-      <c r="AJ3" s="95"/>
-      <c r="AK3" s="95"/>
-      <c r="AL3" s="95"/>
-      <c r="AM3" s="95"/>
-      <c r="AN3" s="95"/>
-      <c r="AO3" s="95"/>
-      <c r="AP3" s="95"/>
-      <c r="AQ3" s="95"/>
-      <c r="AR3" s="95"/>
-      <c r="AS3" s="95"/>
-      <c r="AT3" s="95"/>
-      <c r="AU3" s="95"/>
-      <c r="AV3" s="95"/>
-      <c r="AW3" s="95"/>
-      <c r="AX3" s="95"/>
-      <c r="AY3" s="95"/>
-      <c r="AZ3" s="95"/>
-      <c r="BA3" s="95"/>
-      <c r="BB3" s="95"/>
-      <c r="BC3" s="95"/>
-      <c r="BD3" s="95"/>
-      <c r="BE3" s="95"/>
-      <c r="BF3" s="95"/>
-      <c r="BG3" s="95"/>
-      <c r="BH3" s="95"/>
-      <c r="BI3" s="95"/>
-      <c r="BJ3" s="95"/>
-      <c r="BK3" s="95"/>
-      <c r="BL3" s="95"/>
-      <c r="BM3" s="96"/>
+      <c r="B3" s="148" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="149"/>
+      <c r="J3" s="149"/>
+      <c r="K3" s="149"/>
+      <c r="L3" s="149"/>
+      <c r="M3" s="149"/>
+      <c r="N3" s="149"/>
+      <c r="O3" s="149"/>
+      <c r="P3" s="149"/>
+      <c r="Q3" s="149"/>
+      <c r="R3" s="149"/>
+      <c r="S3" s="149"/>
+      <c r="T3" s="149"/>
+      <c r="U3" s="149"/>
+      <c r="V3" s="149"/>
+      <c r="W3" s="149"/>
+      <c r="X3" s="149"/>
+      <c r="Y3" s="149"/>
+      <c r="Z3" s="149"/>
+      <c r="AA3" s="149"/>
+      <c r="AB3" s="149"/>
+      <c r="AC3" s="149"/>
+      <c r="AD3" s="149"/>
+      <c r="AE3" s="149"/>
+      <c r="AF3" s="149"/>
+      <c r="AG3" s="149"/>
+      <c r="AH3" s="149"/>
+      <c r="AI3" s="149"/>
+      <c r="AJ3" s="149"/>
+      <c r="AK3" s="149"/>
+      <c r="AL3" s="149"/>
+      <c r="AM3" s="149"/>
+      <c r="AN3" s="149"/>
+      <c r="AO3" s="149"/>
+      <c r="AP3" s="149"/>
+      <c r="AQ3" s="149"/>
+      <c r="AR3" s="149"/>
+      <c r="AS3" s="149"/>
+      <c r="AT3" s="149"/>
+      <c r="AU3" s="149"/>
+      <c r="AV3" s="149"/>
+      <c r="AW3" s="149"/>
+      <c r="AX3" s="149"/>
+      <c r="AY3" s="149"/>
+      <c r="AZ3" s="149"/>
+      <c r="BA3" s="149"/>
+      <c r="BB3" s="149"/>
+      <c r="BC3" s="149"/>
+      <c r="BD3" s="149"/>
+      <c r="BE3" s="149"/>
+      <c r="BF3" s="149"/>
+      <c r="BG3" s="149"/>
+      <c r="BH3" s="149"/>
+      <c r="BI3" s="149"/>
+      <c r="BJ3" s="149"/>
+      <c r="BK3" s="149"/>
+      <c r="BL3" s="149"/>
+      <c r="BM3" s="150"/>
       <c r="BO3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="BP3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:68" ht="18" customHeight="1">
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="97"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="98"/>
-      <c r="P4" s="98"/>
-      <c r="Q4" s="98"/>
-      <c r="R4" s="98"/>
-      <c r="S4" s="98"/>
-      <c r="T4" s="98"/>
-      <c r="U4" s="98"/>
-      <c r="V4" s="98"/>
-      <c r="W4" s="98"/>
-      <c r="X4" s="98"/>
-      <c r="Y4" s="98"/>
-      <c r="Z4" s="98"/>
-      <c r="AA4" s="98"/>
-      <c r="AB4" s="98"/>
-      <c r="AC4" s="98"/>
-      <c r="AD4" s="98"/>
-      <c r="AE4" s="98"/>
-      <c r="AF4" s="98"/>
-      <c r="AG4" s="98"/>
-      <c r="AH4" s="98"/>
-      <c r="AI4" s="98"/>
-      <c r="AJ4" s="98"/>
-      <c r="AK4" s="98"/>
-      <c r="AL4" s="98"/>
-      <c r="AM4" s="98"/>
-      <c r="AN4" s="98"/>
-      <c r="AO4" s="98"/>
-      <c r="AP4" s="98"/>
-      <c r="AQ4" s="98"/>
-      <c r="AR4" s="98"/>
-      <c r="AS4" s="98"/>
-      <c r="AT4" s="98"/>
-      <c r="AU4" s="98"/>
-      <c r="AV4" s="98"/>
-      <c r="AW4" s="98"/>
-      <c r="AX4" s="98"/>
-      <c r="AY4" s="98"/>
-      <c r="AZ4" s="98"/>
-      <c r="BA4" s="98"/>
-      <c r="BB4" s="98"/>
-      <c r="BC4" s="98"/>
-      <c r="BD4" s="98"/>
-      <c r="BE4" s="98"/>
-      <c r="BF4" s="98"/>
-      <c r="BG4" s="98"/>
-      <c r="BH4" s="98"/>
-      <c r="BI4" s="98"/>
-      <c r="BJ4" s="98"/>
-      <c r="BK4" s="98"/>
-      <c r="BL4" s="98"/>
-      <c r="BM4" s="99"/>
+      <c r="B4" s="151"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+      <c r="L4" s="152"/>
+      <c r="M4" s="152"/>
+      <c r="N4" s="152"/>
+      <c r="O4" s="152"/>
+      <c r="P4" s="152"/>
+      <c r="Q4" s="152"/>
+      <c r="R4" s="152"/>
+      <c r="S4" s="152"/>
+      <c r="T4" s="152"/>
+      <c r="U4" s="152"/>
+      <c r="V4" s="152"/>
+      <c r="W4" s="152"/>
+      <c r="X4" s="152"/>
+      <c r="Y4" s="152"/>
+      <c r="Z4" s="152"/>
+      <c r="AA4" s="152"/>
+      <c r="AB4" s="152"/>
+      <c r="AC4" s="152"/>
+      <c r="AD4" s="152"/>
+      <c r="AE4" s="152"/>
+      <c r="AF4" s="152"/>
+      <c r="AG4" s="152"/>
+      <c r="AH4" s="152"/>
+      <c r="AI4" s="152"/>
+      <c r="AJ4" s="152"/>
+      <c r="AK4" s="152"/>
+      <c r="AL4" s="152"/>
+      <c r="AM4" s="152"/>
+      <c r="AN4" s="152"/>
+      <c r="AO4" s="152"/>
+      <c r="AP4" s="152"/>
+      <c r="AQ4" s="152"/>
+      <c r="AR4" s="152"/>
+      <c r="AS4" s="152"/>
+      <c r="AT4" s="152"/>
+      <c r="AU4" s="152"/>
+      <c r="AV4" s="152"/>
+      <c r="AW4" s="152"/>
+      <c r="AX4" s="152"/>
+      <c r="AY4" s="152"/>
+      <c r="AZ4" s="152"/>
+      <c r="BA4" s="152"/>
+      <c r="BB4" s="152"/>
+      <c r="BC4" s="152"/>
+      <c r="BD4" s="152"/>
+      <c r="BE4" s="152"/>
+      <c r="BF4" s="152"/>
+      <c r="BG4" s="152"/>
+      <c r="BH4" s="152"/>
+      <c r="BI4" s="152"/>
+      <c r="BJ4" s="152"/>
+      <c r="BK4" s="152"/>
+      <c r="BL4" s="152"/>
+      <c r="BM4" s="153"/>
       <c r="BO4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="BP4" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:68" ht="18" customHeight="1">
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="98"/>
-      <c r="Q5" s="98"/>
-      <c r="R5" s="98"/>
-      <c r="S5" s="98"/>
-      <c r="T5" s="98"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
-      <c r="W5" s="98"/>
-      <c r="X5" s="98"/>
-      <c r="Y5" s="98"/>
-      <c r="Z5" s="98"/>
-      <c r="AA5" s="98"/>
-      <c r="AB5" s="98"/>
-      <c r="AC5" s="98"/>
-      <c r="AD5" s="98"/>
-      <c r="AE5" s="98"/>
-      <c r="AF5" s="98"/>
-      <c r="AG5" s="98"/>
-      <c r="AH5" s="98"/>
-      <c r="AI5" s="98"/>
-      <c r="AJ5" s="98"/>
-      <c r="AK5" s="98"/>
-      <c r="AL5" s="98"/>
-      <c r="AM5" s="98"/>
-      <c r="AN5" s="98"/>
-      <c r="AO5" s="98"/>
-      <c r="AP5" s="98"/>
-      <c r="AQ5" s="98"/>
-      <c r="AR5" s="98"/>
-      <c r="AS5" s="98"/>
-      <c r="AT5" s="98"/>
-      <c r="AU5" s="98"/>
-      <c r="AV5" s="98"/>
-      <c r="AW5" s="98"/>
-      <c r="AX5" s="98"/>
-      <c r="AY5" s="98"/>
-      <c r="AZ5" s="98"/>
-      <c r="BA5" s="98"/>
-      <c r="BB5" s="98"/>
-      <c r="BC5" s="98"/>
-      <c r="BD5" s="98"/>
-      <c r="BE5" s="98"/>
-      <c r="BF5" s="98"/>
-      <c r="BG5" s="98"/>
-      <c r="BH5" s="98"/>
-      <c r="BI5" s="98"/>
-      <c r="BJ5" s="98"/>
-      <c r="BK5" s="98"/>
-      <c r="BL5" s="98"/>
-      <c r="BM5" s="99"/>
+      <c r="B5" s="151"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
+      <c r="E5" s="152"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="152"/>
+      <c r="H5" s="152"/>
+      <c r="I5" s="152"/>
+      <c r="J5" s="152"/>
+      <c r="K5" s="152"/>
+      <c r="L5" s="152"/>
+      <c r="M5" s="152"/>
+      <c r="N5" s="152"/>
+      <c r="O5" s="152"/>
+      <c r="P5" s="152"/>
+      <c r="Q5" s="152"/>
+      <c r="R5" s="152"/>
+      <c r="S5" s="152"/>
+      <c r="T5" s="152"/>
+      <c r="U5" s="152"/>
+      <c r="V5" s="152"/>
+      <c r="W5" s="152"/>
+      <c r="X5" s="152"/>
+      <c r="Y5" s="152"/>
+      <c r="Z5" s="152"/>
+      <c r="AA5" s="152"/>
+      <c r="AB5" s="152"/>
+      <c r="AC5" s="152"/>
+      <c r="AD5" s="152"/>
+      <c r="AE5" s="152"/>
+      <c r="AF5" s="152"/>
+      <c r="AG5" s="152"/>
+      <c r="AH5" s="152"/>
+      <c r="AI5" s="152"/>
+      <c r="AJ5" s="152"/>
+      <c r="AK5" s="152"/>
+      <c r="AL5" s="152"/>
+      <c r="AM5" s="152"/>
+      <c r="AN5" s="152"/>
+      <c r="AO5" s="152"/>
+      <c r="AP5" s="152"/>
+      <c r="AQ5" s="152"/>
+      <c r="AR5" s="152"/>
+      <c r="AS5" s="152"/>
+      <c r="AT5" s="152"/>
+      <c r="AU5" s="152"/>
+      <c r="AV5" s="152"/>
+      <c r="AW5" s="152"/>
+      <c r="AX5" s="152"/>
+      <c r="AY5" s="152"/>
+      <c r="AZ5" s="152"/>
+      <c r="BA5" s="152"/>
+      <c r="BB5" s="152"/>
+      <c r="BC5" s="152"/>
+      <c r="BD5" s="152"/>
+      <c r="BE5" s="152"/>
+      <c r="BF5" s="152"/>
+      <c r="BG5" s="152"/>
+      <c r="BH5" s="152"/>
+      <c r="BI5" s="152"/>
+      <c r="BJ5" s="152"/>
+      <c r="BK5" s="152"/>
+      <c r="BL5" s="152"/>
+      <c r="BM5" s="153"/>
       <c r="BO5" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BP5" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:68" ht="18" customHeight="1">
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="100"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="101"/>
-      <c r="P6" s="101"/>
-      <c r="Q6" s="101"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="101"/>
-      <c r="T6" s="101"/>
-      <c r="U6" s="101"/>
-      <c r="V6" s="101"/>
-      <c r="W6" s="101"/>
-      <c r="X6" s="101"/>
-      <c r="Y6" s="101"/>
-      <c r="Z6" s="101"/>
-      <c r="AA6" s="101"/>
-      <c r="AB6" s="101"/>
-      <c r="AC6" s="101"/>
-      <c r="AD6" s="101"/>
-      <c r="AE6" s="101"/>
-      <c r="AF6" s="101"/>
-      <c r="AG6" s="101"/>
-      <c r="AH6" s="101"/>
-      <c r="AI6" s="101"/>
-      <c r="AJ6" s="101"/>
-      <c r="AK6" s="101"/>
-      <c r="AL6" s="101"/>
-      <c r="AM6" s="101"/>
-      <c r="AN6" s="101"/>
-      <c r="AO6" s="101"/>
-      <c r="AP6" s="101"/>
-      <c r="AQ6" s="101"/>
-      <c r="AR6" s="101"/>
-      <c r="AS6" s="101"/>
-      <c r="AT6" s="101"/>
-      <c r="AU6" s="101"/>
-      <c r="AV6" s="101"/>
-      <c r="AW6" s="101"/>
-      <c r="AX6" s="101"/>
-      <c r="AY6" s="101"/>
-      <c r="AZ6" s="101"/>
-      <c r="BA6" s="101"/>
-      <c r="BB6" s="101"/>
-      <c r="BC6" s="101"/>
-      <c r="BD6" s="101"/>
-      <c r="BE6" s="101"/>
-      <c r="BF6" s="101"/>
-      <c r="BG6" s="101"/>
-      <c r="BH6" s="101"/>
-      <c r="BI6" s="101"/>
-      <c r="BJ6" s="101"/>
-      <c r="BK6" s="101"/>
-      <c r="BL6" s="101"/>
-      <c r="BM6" s="102"/>
+      <c r="B6" s="154"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="155"/>
+      <c r="F6" s="155"/>
+      <c r="G6" s="155"/>
+      <c r="H6" s="155"/>
+      <c r="I6" s="155"/>
+      <c r="J6" s="155"/>
+      <c r="K6" s="155"/>
+      <c r="L6" s="155"/>
+      <c r="M6" s="155"/>
+      <c r="N6" s="155"/>
+      <c r="O6" s="155"/>
+      <c r="P6" s="155"/>
+      <c r="Q6" s="155"/>
+      <c r="R6" s="155"/>
+      <c r="S6" s="155"/>
+      <c r="T6" s="155"/>
+      <c r="U6" s="155"/>
+      <c r="V6" s="155"/>
+      <c r="W6" s="155"/>
+      <c r="X6" s="155"/>
+      <c r="Y6" s="155"/>
+      <c r="Z6" s="155"/>
+      <c r="AA6" s="155"/>
+      <c r="AB6" s="155"/>
+      <c r="AC6" s="155"/>
+      <c r="AD6" s="155"/>
+      <c r="AE6" s="155"/>
+      <c r="AF6" s="155"/>
+      <c r="AG6" s="155"/>
+      <c r="AH6" s="155"/>
+      <c r="AI6" s="155"/>
+      <c r="AJ6" s="155"/>
+      <c r="AK6" s="155"/>
+      <c r="AL6" s="155"/>
+      <c r="AM6" s="155"/>
+      <c r="AN6" s="155"/>
+      <c r="AO6" s="155"/>
+      <c r="AP6" s="155"/>
+      <c r="AQ6" s="155"/>
+      <c r="AR6" s="155"/>
+      <c r="AS6" s="155"/>
+      <c r="AT6" s="155"/>
+      <c r="AU6" s="155"/>
+      <c r="AV6" s="155"/>
+      <c r="AW6" s="155"/>
+      <c r="AX6" s="155"/>
+      <c r="AY6" s="155"/>
+      <c r="AZ6" s="155"/>
+      <c r="BA6" s="155"/>
+      <c r="BB6" s="155"/>
+      <c r="BC6" s="155"/>
+      <c r="BD6" s="155"/>
+      <c r="BE6" s="155"/>
+      <c r="BF6" s="155"/>
+      <c r="BG6" s="155"/>
+      <c r="BH6" s="155"/>
+      <c r="BI6" s="155"/>
+      <c r="BJ6" s="155"/>
+      <c r="BK6" s="155"/>
+      <c r="BL6" s="155"/>
+      <c r="BM6" s="156"/>
       <c r="BO6" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BP6" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:68" ht="18" customHeight="1">
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="112" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="113"/>
-      <c r="M7" s="113"/>
-      <c r="N7" s="113"/>
-      <c r="O7" s="113"/>
-      <c r="P7" s="113"/>
-      <c r="Q7" s="113"/>
-      <c r="R7" s="113"/>
-      <c r="S7" s="113"/>
-      <c r="T7" s="113"/>
-      <c r="U7" s="113"/>
-      <c r="V7" s="113"/>
-      <c r="W7" s="113"/>
-      <c r="X7" s="113"/>
-      <c r="Y7" s="113"/>
-      <c r="Z7" s="113"/>
-      <c r="AA7" s="113"/>
-      <c r="AB7" s="113"/>
-      <c r="AC7" s="113"/>
-      <c r="AD7" s="113"/>
-      <c r="AE7" s="113"/>
-      <c r="AF7" s="113"/>
-      <c r="AG7" s="113"/>
-      <c r="AH7" s="113"/>
-      <c r="AI7" s="113"/>
-      <c r="AJ7" s="113"/>
-      <c r="AK7" s="113"/>
-      <c r="AL7" s="113"/>
-      <c r="AM7" s="113"/>
-      <c r="AN7" s="113"/>
-      <c r="AO7" s="113"/>
-      <c r="AP7" s="113"/>
-      <c r="AQ7" s="113"/>
-      <c r="AR7" s="113"/>
-      <c r="AS7" s="113"/>
-      <c r="AT7" s="113"/>
-      <c r="AU7" s="113"/>
-      <c r="AV7" s="113"/>
-      <c r="AW7" s="113"/>
-      <c r="AX7" s="113"/>
-      <c r="AY7" s="113"/>
-      <c r="AZ7" s="113"/>
-      <c r="BA7" s="113"/>
-      <c r="BB7" s="113"/>
-      <c r="BC7" s="113"/>
-      <c r="BD7" s="113"/>
-      <c r="BE7" s="113"/>
-      <c r="BF7" s="113"/>
-      <c r="BG7" s="113"/>
-      <c r="BH7" s="113"/>
-      <c r="BI7" s="113"/>
-      <c r="BJ7" s="114"/>
+      <c r="B7" s="106" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="107"/>
+      <c r="S7" s="107"/>
+      <c r="T7" s="107"/>
+      <c r="U7" s="107"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="107"/>
+      <c r="X7" s="107"/>
+      <c r="Y7" s="107"/>
+      <c r="Z7" s="107"/>
+      <c r="AA7" s="107"/>
+      <c r="AB7" s="107"/>
+      <c r="AC7" s="107"/>
+      <c r="AD7" s="107"/>
+      <c r="AE7" s="107"/>
+      <c r="AF7" s="107"/>
+      <c r="AG7" s="107"/>
+      <c r="AH7" s="107"/>
+      <c r="AI7" s="107"/>
+      <c r="AJ7" s="107"/>
+      <c r="AK7" s="107"/>
+      <c r="AL7" s="107"/>
+      <c r="AM7" s="107"/>
+      <c r="AN7" s="107"/>
+      <c r="AO7" s="107"/>
+      <c r="AP7" s="107"/>
+      <c r="AQ7" s="107"/>
+      <c r="AR7" s="107"/>
+      <c r="AS7" s="107"/>
+      <c r="AT7" s="107"/>
+      <c r="AU7" s="107"/>
+      <c r="AV7" s="107"/>
+      <c r="AW7" s="107"/>
+      <c r="AX7" s="107"/>
+      <c r="AY7" s="107"/>
+      <c r="AZ7" s="107"/>
+      <c r="BA7" s="107"/>
+      <c r="BB7" s="107"/>
+      <c r="BC7" s="107"/>
+      <c r="BD7" s="107"/>
+      <c r="BE7" s="107"/>
+      <c r="BF7" s="107"/>
+      <c r="BG7" s="107"/>
+      <c r="BH7" s="107"/>
+      <c r="BI7" s="107"/>
+      <c r="BJ7" s="108"/>
       <c r="BK7" s="12"/>
       <c r="BL7" s="12"/>
       <c r="BM7" s="12"/>
       <c r="BO7" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="BP7" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:68" ht="18" customHeight="1">
       <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="115"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="116"/>
-      <c r="M8" s="116"/>
-      <c r="N8" s="116"/>
-      <c r="O8" s="116"/>
-      <c r="P8" s="116"/>
-      <c r="Q8" s="116"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="116"/>
-      <c r="T8" s="116"/>
-      <c r="U8" s="116"/>
-      <c r="V8" s="116"/>
-      <c r="W8" s="116"/>
-      <c r="X8" s="116"/>
-      <c r="Y8" s="116"/>
-      <c r="Z8" s="116"/>
-      <c r="AA8" s="116"/>
-      <c r="AB8" s="116"/>
-      <c r="AC8" s="116"/>
-      <c r="AD8" s="116"/>
-      <c r="AE8" s="116"/>
-      <c r="AF8" s="116"/>
-      <c r="AG8" s="116"/>
-      <c r="AH8" s="116"/>
-      <c r="AI8" s="116"/>
-      <c r="AJ8" s="116"/>
-      <c r="AK8" s="116"/>
-      <c r="AL8" s="116"/>
-      <c r="AM8" s="116"/>
-      <c r="AN8" s="116"/>
-      <c r="AO8" s="116"/>
-      <c r="AP8" s="116"/>
-      <c r="AQ8" s="116"/>
-      <c r="AR8" s="116"/>
-      <c r="AS8" s="116"/>
-      <c r="AT8" s="116"/>
-      <c r="AU8" s="116"/>
-      <c r="AV8" s="116"/>
-      <c r="AW8" s="116"/>
-      <c r="AX8" s="116"/>
-      <c r="AY8" s="116"/>
-      <c r="AZ8" s="116"/>
-      <c r="BA8" s="116"/>
-      <c r="BB8" s="116"/>
-      <c r="BC8" s="116"/>
-      <c r="BD8" s="116"/>
-      <c r="BE8" s="116"/>
-      <c r="BF8" s="116"/>
-      <c r="BG8" s="116"/>
-      <c r="BH8" s="116"/>
-      <c r="BI8" s="116"/>
-      <c r="BJ8" s="117"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
+      <c r="K8" s="110"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="110"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="110"/>
+      <c r="S8" s="110"/>
+      <c r="T8" s="110"/>
+      <c r="U8" s="110"/>
+      <c r="V8" s="110"/>
+      <c r="W8" s="110"/>
+      <c r="X8" s="110"/>
+      <c r="Y8" s="110"/>
+      <c r="Z8" s="110"/>
+      <c r="AA8" s="110"/>
+      <c r="AB8" s="110"/>
+      <c r="AC8" s="110"/>
+      <c r="AD8" s="110"/>
+      <c r="AE8" s="110"/>
+      <c r="AF8" s="110"/>
+      <c r="AG8" s="110"/>
+      <c r="AH8" s="110"/>
+      <c r="AI8" s="110"/>
+      <c r="AJ8" s="110"/>
+      <c r="AK8" s="110"/>
+      <c r="AL8" s="110"/>
+      <c r="AM8" s="110"/>
+      <c r="AN8" s="110"/>
+      <c r="AO8" s="110"/>
+      <c r="AP8" s="110"/>
+      <c r="AQ8" s="110"/>
+      <c r="AR8" s="110"/>
+      <c r="AS8" s="110"/>
+      <c r="AT8" s="110"/>
+      <c r="AU8" s="110"/>
+      <c r="AV8" s="110"/>
+      <c r="AW8" s="110"/>
+      <c r="AX8" s="110"/>
+      <c r="AY8" s="110"/>
+      <c r="AZ8" s="110"/>
+      <c r="BA8" s="110"/>
+      <c r="BB8" s="110"/>
+      <c r="BC8" s="110"/>
+      <c r="BD8" s="110"/>
+      <c r="BE8" s="110"/>
+      <c r="BF8" s="110"/>
+      <c r="BG8" s="110"/>
+      <c r="BH8" s="110"/>
+      <c r="BI8" s="110"/>
+      <c r="BJ8" s="111"/>
       <c r="BK8" s="12"/>
       <c r="BL8" s="12"/>
       <c r="BM8" s="12"/>
       <c r="BO8" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="BP8" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:68" ht="18" customHeight="1">
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="115"/>
-      <c r="C9" s="116"/>
-      <c r="D9" s="116"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="116"/>
-      <c r="G9" s="116"/>
-      <c r="H9" s="116"/>
-      <c r="I9" s="116"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
-      <c r="M9" s="116"/>
-      <c r="N9" s="116"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="116"/>
-      <c r="Q9" s="116"/>
-      <c r="R9" s="116"/>
-      <c r="S9" s="116"/>
-      <c r="T9" s="116"/>
-      <c r="U9" s="116"/>
-      <c r="V9" s="116"/>
-      <c r="W9" s="116"/>
-      <c r="X9" s="116"/>
-      <c r="Y9" s="116"/>
-      <c r="Z9" s="116"/>
-      <c r="AA9" s="116"/>
-      <c r="AB9" s="116"/>
-      <c r="AC9" s="116"/>
-      <c r="AD9" s="116"/>
-      <c r="AE9" s="116"/>
-      <c r="AF9" s="116"/>
-      <c r="AG9" s="116"/>
-      <c r="AH9" s="116"/>
-      <c r="AI9" s="116"/>
-      <c r="AJ9" s="116"/>
-      <c r="AK9" s="116"/>
-      <c r="AL9" s="116"/>
-      <c r="AM9" s="116"/>
-      <c r="AN9" s="116"/>
-      <c r="AO9" s="116"/>
-      <c r="AP9" s="116"/>
-      <c r="AQ9" s="116"/>
-      <c r="AR9" s="116"/>
-      <c r="AS9" s="116"/>
-      <c r="AT9" s="116"/>
-      <c r="AU9" s="116"/>
-      <c r="AV9" s="116"/>
-      <c r="AW9" s="116"/>
-      <c r="AX9" s="116"/>
-      <c r="AY9" s="116"/>
-      <c r="AZ9" s="116"/>
-      <c r="BA9" s="116"/>
-      <c r="BB9" s="116"/>
-      <c r="BC9" s="116"/>
-      <c r="BD9" s="116"/>
-      <c r="BE9" s="116"/>
-      <c r="BF9" s="116"/>
-      <c r="BG9" s="116"/>
-      <c r="BH9" s="116"/>
-      <c r="BI9" s="116"/>
-      <c r="BJ9" s="117"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="110"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="110"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
+      <c r="J9" s="110"/>
+      <c r="K9" s="110"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="110"/>
+      <c r="N9" s="110"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="110"/>
+      <c r="Q9" s="110"/>
+      <c r="R9" s="110"/>
+      <c r="S9" s="110"/>
+      <c r="T9" s="110"/>
+      <c r="U9" s="110"/>
+      <c r="V9" s="110"/>
+      <c r="W9" s="110"/>
+      <c r="X9" s="110"/>
+      <c r="Y9" s="110"/>
+      <c r="Z9" s="110"/>
+      <c r="AA9" s="110"/>
+      <c r="AB9" s="110"/>
+      <c r="AC9" s="110"/>
+      <c r="AD9" s="110"/>
+      <c r="AE9" s="110"/>
+      <c r="AF9" s="110"/>
+      <c r="AG9" s="110"/>
+      <c r="AH9" s="110"/>
+      <c r="AI9" s="110"/>
+      <c r="AJ9" s="110"/>
+      <c r="AK9" s="110"/>
+      <c r="AL9" s="110"/>
+      <c r="AM9" s="110"/>
+      <c r="AN9" s="110"/>
+      <c r="AO9" s="110"/>
+      <c r="AP9" s="110"/>
+      <c r="AQ9" s="110"/>
+      <c r="AR9" s="110"/>
+      <c r="AS9" s="110"/>
+      <c r="AT9" s="110"/>
+      <c r="AU9" s="110"/>
+      <c r="AV9" s="110"/>
+      <c r="AW9" s="110"/>
+      <c r="AX9" s="110"/>
+      <c r="AY9" s="110"/>
+      <c r="AZ9" s="110"/>
+      <c r="BA9" s="110"/>
+      <c r="BB9" s="110"/>
+      <c r="BC9" s="110"/>
+      <c r="BD9" s="110"/>
+      <c r="BE9" s="110"/>
+      <c r="BF9" s="110"/>
+      <c r="BG9" s="110"/>
+      <c r="BH9" s="110"/>
+      <c r="BI9" s="110"/>
+      <c r="BJ9" s="111"/>
       <c r="BK9" s="12"/>
       <c r="BL9" s="12"/>
       <c r="BM9" s="12"/>
       <c r="BO9" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="BP9" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:68" ht="18" customHeight="1">
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="116"/>
-      <c r="G10" s="116"/>
-      <c r="H10" s="116"/>
-      <c r="I10" s="116"/>
-      <c r="J10" s="116"/>
-      <c r="K10" s="116"/>
-      <c r="L10" s="116"/>
-      <c r="M10" s="116"/>
-      <c r="N10" s="116"/>
-      <c r="O10" s="116"/>
-      <c r="P10" s="116"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="116"/>
-      <c r="S10" s="116"/>
-      <c r="T10" s="116"/>
-      <c r="U10" s="116"/>
-      <c r="V10" s="116"/>
-      <c r="W10" s="116"/>
-      <c r="X10" s="116"/>
-      <c r="Y10" s="116"/>
-      <c r="Z10" s="116"/>
-      <c r="AA10" s="116"/>
-      <c r="AB10" s="116"/>
-      <c r="AC10" s="116"/>
-      <c r="AD10" s="116"/>
-      <c r="AE10" s="116"/>
-      <c r="AF10" s="116"/>
-      <c r="AG10" s="116"/>
-      <c r="AH10" s="116"/>
-      <c r="AI10" s="116"/>
-      <c r="AJ10" s="116"/>
-      <c r="AK10" s="116"/>
-      <c r="AL10" s="116"/>
-      <c r="AM10" s="116"/>
-      <c r="AN10" s="116"/>
-      <c r="AO10" s="116"/>
-      <c r="AP10" s="116"/>
-      <c r="AQ10" s="116"/>
-      <c r="AR10" s="116"/>
-      <c r="AS10" s="116"/>
-      <c r="AT10" s="116"/>
-      <c r="AU10" s="116"/>
-      <c r="AV10" s="116"/>
-      <c r="AW10" s="116"/>
-      <c r="AX10" s="116"/>
-      <c r="AY10" s="116"/>
-      <c r="AZ10" s="116"/>
-      <c r="BA10" s="116"/>
-      <c r="BB10" s="116"/>
-      <c r="BC10" s="116"/>
-      <c r="BD10" s="116"/>
-      <c r="BE10" s="116"/>
-      <c r="BF10" s="116"/>
-      <c r="BG10" s="116"/>
-      <c r="BH10" s="116"/>
-      <c r="BI10" s="116"/>
-      <c r="BJ10" s="117"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="110"/>
+      <c r="J10" s="110"/>
+      <c r="K10" s="110"/>
+      <c r="L10" s="110"/>
+      <c r="M10" s="110"/>
+      <c r="N10" s="110"/>
+      <c r="O10" s="110"/>
+      <c r="P10" s="110"/>
+      <c r="Q10" s="110"/>
+      <c r="R10" s="110"/>
+      <c r="S10" s="110"/>
+      <c r="T10" s="110"/>
+      <c r="U10" s="110"/>
+      <c r="V10" s="110"/>
+      <c r="W10" s="110"/>
+      <c r="X10" s="110"/>
+      <c r="Y10" s="110"/>
+      <c r="Z10" s="110"/>
+      <c r="AA10" s="110"/>
+      <c r="AB10" s="110"/>
+      <c r="AC10" s="110"/>
+      <c r="AD10" s="110"/>
+      <c r="AE10" s="110"/>
+      <c r="AF10" s="110"/>
+      <c r="AG10" s="110"/>
+      <c r="AH10" s="110"/>
+      <c r="AI10" s="110"/>
+      <c r="AJ10" s="110"/>
+      <c r="AK10" s="110"/>
+      <c r="AL10" s="110"/>
+      <c r="AM10" s="110"/>
+      <c r="AN10" s="110"/>
+      <c r="AO10" s="110"/>
+      <c r="AP10" s="110"/>
+      <c r="AQ10" s="110"/>
+      <c r="AR10" s="110"/>
+      <c r="AS10" s="110"/>
+      <c r="AT10" s="110"/>
+      <c r="AU10" s="110"/>
+      <c r="AV10" s="110"/>
+      <c r="AW10" s="110"/>
+      <c r="AX10" s="110"/>
+      <c r="AY10" s="110"/>
+      <c r="AZ10" s="110"/>
+      <c r="BA10" s="110"/>
+      <c r="BB10" s="110"/>
+      <c r="BC10" s="110"/>
+      <c r="BD10" s="110"/>
+      <c r="BE10" s="110"/>
+      <c r="BF10" s="110"/>
+      <c r="BG10" s="110"/>
+      <c r="BH10" s="110"/>
+      <c r="BI10" s="110"/>
+      <c r="BJ10" s="111"/>
       <c r="BK10" s="12"/>
       <c r="BL10" s="12"/>
       <c r="BM10" s="12"/>
       <c r="BO10" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BP10" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:68" ht="18" customHeight="1">
       <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="103" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="104"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="104"/>
-      <c r="F11" s="104"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="104"/>
-      <c r="M11" s="104"/>
-      <c r="N11" s="104"/>
-      <c r="O11" s="104"/>
-      <c r="P11" s="104"/>
-      <c r="Q11" s="104"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="104"/>
-      <c r="T11" s="104"/>
-      <c r="U11" s="104"/>
-      <c r="V11" s="104"/>
-      <c r="W11" s="104"/>
-      <c r="X11" s="104"/>
-      <c r="Y11" s="104"/>
-      <c r="Z11" s="104"/>
-      <c r="AA11" s="104"/>
-      <c r="AB11" s="104"/>
-      <c r="AC11" s="104"/>
-      <c r="AD11" s="104"/>
-      <c r="AE11" s="104"/>
-      <c r="AF11" s="104"/>
-      <c r="AG11" s="104"/>
-      <c r="AH11" s="104"/>
-      <c r="AI11" s="104"/>
-      <c r="AJ11" s="104"/>
-      <c r="AK11" s="104"/>
-      <c r="AL11" s="104"/>
-      <c r="AM11" s="104"/>
-      <c r="AN11" s="104"/>
-      <c r="AO11" s="104"/>
-      <c r="AP11" s="104"/>
-      <c r="AQ11" s="104"/>
-      <c r="AR11" s="104"/>
-      <c r="AS11" s="104"/>
-      <c r="AT11" s="104"/>
-      <c r="AU11" s="104"/>
-      <c r="AV11" s="104"/>
-      <c r="AW11" s="104"/>
-      <c r="AX11" s="104"/>
-      <c r="AY11" s="104"/>
-      <c r="AZ11" s="104"/>
-      <c r="BA11" s="104"/>
-      <c r="BB11" s="104"/>
-      <c r="BC11" s="104"/>
-      <c r="BD11" s="104"/>
-      <c r="BE11" s="104"/>
-      <c r="BF11" s="104"/>
-      <c r="BG11" s="104"/>
-      <c r="BH11" s="104"/>
-      <c r="BI11" s="104"/>
-      <c r="BJ11" s="104"/>
-      <c r="BK11" s="104"/>
-      <c r="BL11" s="104"/>
-      <c r="BM11" s="105"/>
+      <c r="B11" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="98"/>
+      <c r="P11" s="98"/>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="98"/>
+      <c r="T11" s="98"/>
+      <c r="U11" s="98"/>
+      <c r="V11" s="98"/>
+      <c r="W11" s="98"/>
+      <c r="X11" s="98"/>
+      <c r="Y11" s="98"/>
+      <c r="Z11" s="98"/>
+      <c r="AA11" s="98"/>
+      <c r="AB11" s="98"/>
+      <c r="AC11" s="98"/>
+      <c r="AD11" s="98"/>
+      <c r="AE11" s="98"/>
+      <c r="AF11" s="98"/>
+      <c r="AG11" s="98"/>
+      <c r="AH11" s="98"/>
+      <c r="AI11" s="98"/>
+      <c r="AJ11" s="98"/>
+      <c r="AK11" s="98"/>
+      <c r="AL11" s="98"/>
+      <c r="AM11" s="98"/>
+      <c r="AN11" s="98"/>
+      <c r="AO11" s="98"/>
+      <c r="AP11" s="98"/>
+      <c r="AQ11" s="98"/>
+      <c r="AR11" s="98"/>
+      <c r="AS11" s="98"/>
+      <c r="AT11" s="98"/>
+      <c r="AU11" s="98"/>
+      <c r="AV11" s="98"/>
+      <c r="AW11" s="98"/>
+      <c r="AX11" s="98"/>
+      <c r="AY11" s="98"/>
+      <c r="AZ11" s="98"/>
+      <c r="BA11" s="98"/>
+      <c r="BB11" s="98"/>
+      <c r="BC11" s="98"/>
+      <c r="BD11" s="98"/>
+      <c r="BE11" s="98"/>
+      <c r="BF11" s="98"/>
+      <c r="BG11" s="98"/>
+      <c r="BH11" s="98"/>
+      <c r="BI11" s="98"/>
+      <c r="BJ11" s="98"/>
+      <c r="BK11" s="98"/>
+      <c r="BL11" s="98"/>
+      <c r="BM11" s="99"/>
       <c r="BO11" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="BP11" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:68" ht="18" customHeight="1">
       <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="106"/>
-      <c r="C12" s="107"/>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107"/>
-      <c r="J12" s="107"/>
-      <c r="K12" s="107"/>
-      <c r="L12" s="107"/>
-      <c r="M12" s="107"/>
-      <c r="N12" s="107"/>
-      <c r="O12" s="107"/>
-      <c r="P12" s="107"/>
-      <c r="Q12" s="107"/>
-      <c r="R12" s="107"/>
-      <c r="S12" s="107"/>
-      <c r="T12" s="107"/>
-      <c r="U12" s="107"/>
-      <c r="V12" s="107"/>
-      <c r="W12" s="107"/>
-      <c r="X12" s="107"/>
-      <c r="Y12" s="107"/>
-      <c r="Z12" s="107"/>
-      <c r="AA12" s="107"/>
-      <c r="AB12" s="107"/>
-      <c r="AC12" s="107"/>
-      <c r="AD12" s="107"/>
-      <c r="AE12" s="107"/>
-      <c r="AF12" s="107"/>
-      <c r="AG12" s="107"/>
-      <c r="AH12" s="107"/>
-      <c r="AI12" s="107"/>
-      <c r="AJ12" s="107"/>
-      <c r="AK12" s="107"/>
-      <c r="AL12" s="107"/>
-      <c r="AM12" s="107"/>
-      <c r="AN12" s="107"/>
-      <c r="AO12" s="107"/>
-      <c r="AP12" s="107"/>
-      <c r="AQ12" s="107"/>
-      <c r="AR12" s="107"/>
-      <c r="AS12" s="107"/>
-      <c r="AT12" s="107"/>
-      <c r="AU12" s="107"/>
-      <c r="AV12" s="107"/>
-      <c r="AW12" s="107"/>
-      <c r="AX12" s="107"/>
-      <c r="AY12" s="107"/>
-      <c r="AZ12" s="107"/>
-      <c r="BA12" s="107"/>
-      <c r="BB12" s="107"/>
-      <c r="BC12" s="107"/>
-      <c r="BD12" s="107"/>
-      <c r="BE12" s="107"/>
-      <c r="BF12" s="107"/>
-      <c r="BG12" s="107"/>
-      <c r="BH12" s="107"/>
-      <c r="BI12" s="107"/>
-      <c r="BJ12" s="107"/>
-      <c r="BK12" s="107"/>
-      <c r="BL12" s="107"/>
-      <c r="BM12" s="108"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="101"/>
+      <c r="F12" s="101"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="101"/>
+      <c r="L12" s="101"/>
+      <c r="M12" s="101"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="101"/>
+      <c r="P12" s="101"/>
+      <c r="Q12" s="101"/>
+      <c r="R12" s="101"/>
+      <c r="S12" s="101"/>
+      <c r="T12" s="101"/>
+      <c r="U12" s="101"/>
+      <c r="V12" s="101"/>
+      <c r="W12" s="101"/>
+      <c r="X12" s="101"/>
+      <c r="Y12" s="101"/>
+      <c r="Z12" s="101"/>
+      <c r="AA12" s="101"/>
+      <c r="AB12" s="101"/>
+      <c r="AC12" s="101"/>
+      <c r="AD12" s="101"/>
+      <c r="AE12" s="101"/>
+      <c r="AF12" s="101"/>
+      <c r="AG12" s="101"/>
+      <c r="AH12" s="101"/>
+      <c r="AI12" s="101"/>
+      <c r="AJ12" s="101"/>
+      <c r="AK12" s="101"/>
+      <c r="AL12" s="101"/>
+      <c r="AM12" s="101"/>
+      <c r="AN12" s="101"/>
+      <c r="AO12" s="101"/>
+      <c r="AP12" s="101"/>
+      <c r="AQ12" s="101"/>
+      <c r="AR12" s="101"/>
+      <c r="AS12" s="101"/>
+      <c r="AT12" s="101"/>
+      <c r="AU12" s="101"/>
+      <c r="AV12" s="101"/>
+      <c r="AW12" s="101"/>
+      <c r="AX12" s="101"/>
+      <c r="AY12" s="101"/>
+      <c r="AZ12" s="101"/>
+      <c r="BA12" s="101"/>
+      <c r="BB12" s="101"/>
+      <c r="BC12" s="101"/>
+      <c r="BD12" s="101"/>
+      <c r="BE12" s="101"/>
+      <c r="BF12" s="101"/>
+      <c r="BG12" s="101"/>
+      <c r="BH12" s="101"/>
+      <c r="BI12" s="101"/>
+      <c r="BJ12" s="101"/>
+      <c r="BK12" s="101"/>
+      <c r="BL12" s="101"/>
+      <c r="BM12" s="102"/>
       <c r="BO12" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="BP12" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:68" ht="18" customHeight="1">
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="106"/>
-      <c r="C13" s="107"/>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="107"/>
-      <c r="K13" s="107"/>
-      <c r="L13" s="107"/>
-      <c r="M13" s="107"/>
-      <c r="N13" s="107"/>
-      <c r="O13" s="107"/>
-      <c r="P13" s="107"/>
-      <c r="Q13" s="107"/>
-      <c r="R13" s="107"/>
-      <c r="S13" s="107"/>
-      <c r="T13" s="107"/>
-      <c r="U13" s="107"/>
-      <c r="V13" s="107"/>
-      <c r="W13" s="107"/>
-      <c r="X13" s="107"/>
-      <c r="Y13" s="107"/>
-      <c r="Z13" s="107"/>
-      <c r="AA13" s="107"/>
-      <c r="AB13" s="107"/>
-      <c r="AC13" s="107"/>
-      <c r="AD13" s="107"/>
-      <c r="AE13" s="107"/>
-      <c r="AF13" s="107"/>
-      <c r="AG13" s="107"/>
-      <c r="AH13" s="107"/>
-      <c r="AI13" s="107"/>
-      <c r="AJ13" s="107"/>
-      <c r="AK13" s="107"/>
-      <c r="AL13" s="107"/>
-      <c r="AM13" s="107"/>
-      <c r="AN13" s="107"/>
-      <c r="AO13" s="107"/>
-      <c r="AP13" s="107"/>
-      <c r="AQ13" s="107"/>
-      <c r="AR13" s="107"/>
-      <c r="AS13" s="107"/>
-      <c r="AT13" s="107"/>
-      <c r="AU13" s="107"/>
-      <c r="AV13" s="107"/>
-      <c r="AW13" s="107"/>
-      <c r="AX13" s="107"/>
-      <c r="AY13" s="107"/>
-      <c r="AZ13" s="107"/>
-      <c r="BA13" s="107"/>
-      <c r="BB13" s="107"/>
-      <c r="BC13" s="107"/>
-      <c r="BD13" s="107"/>
-      <c r="BE13" s="107"/>
-      <c r="BF13" s="107"/>
-      <c r="BG13" s="107"/>
-      <c r="BH13" s="107"/>
-      <c r="BI13" s="107"/>
-      <c r="BJ13" s="107"/>
-      <c r="BK13" s="107"/>
-      <c r="BL13" s="107"/>
-      <c r="BM13" s="108"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101"/>
+      <c r="K13" s="101"/>
+      <c r="L13" s="101"/>
+      <c r="M13" s="101"/>
+      <c r="N13" s="101"/>
+      <c r="O13" s="101"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="101"/>
+      <c r="R13" s="101"/>
+      <c r="S13" s="101"/>
+      <c r="T13" s="101"/>
+      <c r="U13" s="101"/>
+      <c r="V13" s="101"/>
+      <c r="W13" s="101"/>
+      <c r="X13" s="101"/>
+      <c r="Y13" s="101"/>
+      <c r="Z13" s="101"/>
+      <c r="AA13" s="101"/>
+      <c r="AB13" s="101"/>
+      <c r="AC13" s="101"/>
+      <c r="AD13" s="101"/>
+      <c r="AE13" s="101"/>
+      <c r="AF13" s="101"/>
+      <c r="AG13" s="101"/>
+      <c r="AH13" s="101"/>
+      <c r="AI13" s="101"/>
+      <c r="AJ13" s="101"/>
+      <c r="AK13" s="101"/>
+      <c r="AL13" s="101"/>
+      <c r="AM13" s="101"/>
+      <c r="AN13" s="101"/>
+      <c r="AO13" s="101"/>
+      <c r="AP13" s="101"/>
+      <c r="AQ13" s="101"/>
+      <c r="AR13" s="101"/>
+      <c r="AS13" s="101"/>
+      <c r="AT13" s="101"/>
+      <c r="AU13" s="101"/>
+      <c r="AV13" s="101"/>
+      <c r="AW13" s="101"/>
+      <c r="AX13" s="101"/>
+      <c r="AY13" s="101"/>
+      <c r="AZ13" s="101"/>
+      <c r="BA13" s="101"/>
+      <c r="BB13" s="101"/>
+      <c r="BC13" s="101"/>
+      <c r="BD13" s="101"/>
+      <c r="BE13" s="101"/>
+      <c r="BF13" s="101"/>
+      <c r="BG13" s="101"/>
+      <c r="BH13" s="101"/>
+      <c r="BI13" s="101"/>
+      <c r="BJ13" s="101"/>
+      <c r="BK13" s="101"/>
+      <c r="BL13" s="101"/>
+      <c r="BM13" s="102"/>
       <c r="BO13" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="BP13" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:68" ht="18" customHeight="1">
       <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="109"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="110"/>
-      <c r="L14" s="110"/>
-      <c r="M14" s="110"/>
-      <c r="N14" s="110"/>
-      <c r="O14" s="110"/>
-      <c r="P14" s="110"/>
-      <c r="Q14" s="110"/>
-      <c r="R14" s="110"/>
-      <c r="S14" s="110"/>
-      <c r="T14" s="110"/>
-      <c r="U14" s="110"/>
-      <c r="V14" s="110"/>
-      <c r="W14" s="110"/>
-      <c r="X14" s="110"/>
-      <c r="Y14" s="110"/>
-      <c r="Z14" s="110"/>
-      <c r="AA14" s="110"/>
-      <c r="AB14" s="110"/>
-      <c r="AC14" s="110"/>
-      <c r="AD14" s="110"/>
-      <c r="AE14" s="110"/>
-      <c r="AF14" s="110"/>
-      <c r="AG14" s="110"/>
-      <c r="AH14" s="110"/>
-      <c r="AI14" s="110"/>
-      <c r="AJ14" s="110"/>
-      <c r="AK14" s="110"/>
-      <c r="AL14" s="110"/>
-      <c r="AM14" s="110"/>
-      <c r="AN14" s="110"/>
-      <c r="AO14" s="110"/>
-      <c r="AP14" s="110"/>
-      <c r="AQ14" s="110"/>
-      <c r="AR14" s="110"/>
-      <c r="AS14" s="110"/>
-      <c r="AT14" s="110"/>
-      <c r="AU14" s="110"/>
-      <c r="AV14" s="110"/>
-      <c r="AW14" s="110"/>
-      <c r="AX14" s="110"/>
-      <c r="AY14" s="110"/>
-      <c r="AZ14" s="110"/>
-      <c r="BA14" s="110"/>
-      <c r="BB14" s="110"/>
-      <c r="BC14" s="110"/>
-      <c r="BD14" s="110"/>
-      <c r="BE14" s="110"/>
-      <c r="BF14" s="110"/>
-      <c r="BG14" s="110"/>
-      <c r="BH14" s="110"/>
-      <c r="BI14" s="110"/>
-      <c r="BJ14" s="110"/>
-      <c r="BK14" s="110"/>
-      <c r="BL14" s="110"/>
-      <c r="BM14" s="111"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="104"/>
+      <c r="L14" s="104"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="104"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
+      <c r="U14" s="104"/>
+      <c r="V14" s="104"/>
+      <c r="W14" s="104"/>
+      <c r="X14" s="104"/>
+      <c r="Y14" s="104"/>
+      <c r="Z14" s="104"/>
+      <c r="AA14" s="104"/>
+      <c r="AB14" s="104"/>
+      <c r="AC14" s="104"/>
+      <c r="AD14" s="104"/>
+      <c r="AE14" s="104"/>
+      <c r="AF14" s="104"/>
+      <c r="AG14" s="104"/>
+      <c r="AH14" s="104"/>
+      <c r="AI14" s="104"/>
+      <c r="AJ14" s="104"/>
+      <c r="AK14" s="104"/>
+      <c r="AL14" s="104"/>
+      <c r="AM14" s="104"/>
+      <c r="AN14" s="104"/>
+      <c r="AO14" s="104"/>
+      <c r="AP14" s="104"/>
+      <c r="AQ14" s="104"/>
+      <c r="AR14" s="104"/>
+      <c r="AS14" s="104"/>
+      <c r="AT14" s="104"/>
+      <c r="AU14" s="104"/>
+      <c r="AV14" s="104"/>
+      <c r="AW14" s="104"/>
+      <c r="AX14" s="104"/>
+      <c r="AY14" s="104"/>
+      <c r="AZ14" s="104"/>
+      <c r="BA14" s="104"/>
+      <c r="BB14" s="104"/>
+      <c r="BC14" s="104"/>
+      <c r="BD14" s="104"/>
+      <c r="BE14" s="104"/>
+      <c r="BF14" s="104"/>
+      <c r="BG14" s="104"/>
+      <c r="BH14" s="104"/>
+      <c r="BI14" s="104"/>
+      <c r="BJ14" s="104"/>
+      <c r="BK14" s="104"/>
+      <c r="BL14" s="104"/>
+      <c r="BM14" s="105"/>
       <c r="BO14" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="BP14" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:68" ht="18" customHeight="1">
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="B15" s="103" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="104"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="104"/>
-      <c r="J15" s="104"/>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="104"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
-      <c r="U15" s="104"/>
-      <c r="V15" s="104"/>
-      <c r="W15" s="104"/>
-      <c r="X15" s="104"/>
-      <c r="Y15" s="104"/>
-      <c r="Z15" s="104"/>
-      <c r="AA15" s="104"/>
-      <c r="AB15" s="104"/>
-      <c r="AC15" s="104"/>
-      <c r="AD15" s="104"/>
-      <c r="AE15" s="104"/>
-      <c r="AF15" s="104"/>
-      <c r="AG15" s="104"/>
-      <c r="AH15" s="104"/>
-      <c r="AI15" s="104"/>
-      <c r="AJ15" s="104"/>
-      <c r="AK15" s="104"/>
-      <c r="AL15" s="104"/>
-      <c r="AM15" s="104"/>
-      <c r="AN15" s="104"/>
-      <c r="AO15" s="104"/>
-      <c r="AP15" s="104"/>
-      <c r="AQ15" s="104"/>
-      <c r="AR15" s="104"/>
-      <c r="AS15" s="104"/>
-      <c r="AT15" s="104"/>
-      <c r="AU15" s="104"/>
-      <c r="AV15" s="104"/>
-      <c r="AW15" s="104"/>
-      <c r="AX15" s="104"/>
-      <c r="AY15" s="104"/>
-      <c r="AZ15" s="104"/>
-      <c r="BA15" s="104"/>
-      <c r="BB15" s="104"/>
-      <c r="BC15" s="104"/>
-      <c r="BD15" s="104"/>
-      <c r="BE15" s="104"/>
-      <c r="BF15" s="104"/>
-      <c r="BG15" s="104"/>
-      <c r="BH15" s="104"/>
-      <c r="BI15" s="104"/>
-      <c r="BJ15" s="104"/>
-      <c r="BK15" s="104"/>
-      <c r="BL15" s="104"/>
-      <c r="BM15" s="105"/>
+      <c r="B15" s="97" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="98"/>
+      <c r="P15" s="98"/>
+      <c r="Q15" s="98"/>
+      <c r="R15" s="98"/>
+      <c r="S15" s="98"/>
+      <c r="T15" s="98"/>
+      <c r="U15" s="98"/>
+      <c r="V15" s="98"/>
+      <c r="W15" s="98"/>
+      <c r="X15" s="98"/>
+      <c r="Y15" s="98"/>
+      <c r="Z15" s="98"/>
+      <c r="AA15" s="98"/>
+      <c r="AB15" s="98"/>
+      <c r="AC15" s="98"/>
+      <c r="AD15" s="98"/>
+      <c r="AE15" s="98"/>
+      <c r="AF15" s="98"/>
+      <c r="AG15" s="98"/>
+      <c r="AH15" s="98"/>
+      <c r="AI15" s="98"/>
+      <c r="AJ15" s="98"/>
+      <c r="AK15" s="98"/>
+      <c r="AL15" s="98"/>
+      <c r="AM15" s="98"/>
+      <c r="AN15" s="98"/>
+      <c r="AO15" s="98"/>
+      <c r="AP15" s="98"/>
+      <c r="AQ15" s="98"/>
+      <c r="AR15" s="98"/>
+      <c r="AS15" s="98"/>
+      <c r="AT15" s="98"/>
+      <c r="AU15" s="98"/>
+      <c r="AV15" s="98"/>
+      <c r="AW15" s="98"/>
+      <c r="AX15" s="98"/>
+      <c r="AY15" s="98"/>
+      <c r="AZ15" s="98"/>
+      <c r="BA15" s="98"/>
+      <c r="BB15" s="98"/>
+      <c r="BC15" s="98"/>
+      <c r="BD15" s="98"/>
+      <c r="BE15" s="98"/>
+      <c r="BF15" s="98"/>
+      <c r="BG15" s="98"/>
+      <c r="BH15" s="98"/>
+      <c r="BI15" s="98"/>
+      <c r="BJ15" s="98"/>
+      <c r="BK15" s="98"/>
+      <c r="BL15" s="98"/>
+      <c r="BM15" s="99"/>
       <c r="BO15" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="BP15" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:68" ht="18" customHeight="1">
       <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="106"/>
-      <c r="C16" s="107"/>
-      <c r="D16" s="107"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="107"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107"/>
-      <c r="J16" s="107"/>
-      <c r="K16" s="107"/>
-      <c r="L16" s="107"/>
-      <c r="M16" s="107"/>
-      <c r="N16" s="107"/>
-      <c r="O16" s="107"/>
-      <c r="P16" s="107"/>
-      <c r="Q16" s="107"/>
-      <c r="R16" s="107"/>
-      <c r="S16" s="107"/>
-      <c r="T16" s="107"/>
-      <c r="U16" s="107"/>
-      <c r="V16" s="107"/>
-      <c r="W16" s="107"/>
-      <c r="X16" s="107"/>
-      <c r="Y16" s="107"/>
-      <c r="Z16" s="107"/>
-      <c r="AA16" s="107"/>
-      <c r="AB16" s="107"/>
-      <c r="AC16" s="107"/>
-      <c r="AD16" s="107"/>
-      <c r="AE16" s="107"/>
-      <c r="AF16" s="107"/>
-      <c r="AG16" s="107"/>
-      <c r="AH16" s="107"/>
-      <c r="AI16" s="107"/>
-      <c r="AJ16" s="107"/>
-      <c r="AK16" s="107"/>
-      <c r="AL16" s="107"/>
-      <c r="AM16" s="107"/>
-      <c r="AN16" s="107"/>
-      <c r="AO16" s="107"/>
-      <c r="AP16" s="107"/>
-      <c r="AQ16" s="107"/>
-      <c r="AR16" s="107"/>
-      <c r="AS16" s="107"/>
-      <c r="AT16" s="107"/>
-      <c r="AU16" s="107"/>
-      <c r="AV16" s="107"/>
-      <c r="AW16" s="107"/>
-      <c r="AX16" s="107"/>
-      <c r="AY16" s="107"/>
-      <c r="AZ16" s="107"/>
-      <c r="BA16" s="107"/>
-      <c r="BB16" s="107"/>
-      <c r="BC16" s="107"/>
-      <c r="BD16" s="107"/>
-      <c r="BE16" s="107"/>
-      <c r="BF16" s="107"/>
-      <c r="BG16" s="107"/>
-      <c r="BH16" s="107"/>
-      <c r="BI16" s="107"/>
-      <c r="BJ16" s="107"/>
-      <c r="BK16" s="107"/>
-      <c r="BL16" s="107"/>
-      <c r="BM16" s="108"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="101"/>
+      <c r="J16" s="101"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="101"/>
+      <c r="N16" s="101"/>
+      <c r="O16" s="101"/>
+      <c r="P16" s="101"/>
+      <c r="Q16" s="101"/>
+      <c r="R16" s="101"/>
+      <c r="S16" s="101"/>
+      <c r="T16" s="101"/>
+      <c r="U16" s="101"/>
+      <c r="V16" s="101"/>
+      <c r="W16" s="101"/>
+      <c r="X16" s="101"/>
+      <c r="Y16" s="101"/>
+      <c r="Z16" s="101"/>
+      <c r="AA16" s="101"/>
+      <c r="AB16" s="101"/>
+      <c r="AC16" s="101"/>
+      <c r="AD16" s="101"/>
+      <c r="AE16" s="101"/>
+      <c r="AF16" s="101"/>
+      <c r="AG16" s="101"/>
+      <c r="AH16" s="101"/>
+      <c r="AI16" s="101"/>
+      <c r="AJ16" s="101"/>
+      <c r="AK16" s="101"/>
+      <c r="AL16" s="101"/>
+      <c r="AM16" s="101"/>
+      <c r="AN16" s="101"/>
+      <c r="AO16" s="101"/>
+      <c r="AP16" s="101"/>
+      <c r="AQ16" s="101"/>
+      <c r="AR16" s="101"/>
+      <c r="AS16" s="101"/>
+      <c r="AT16" s="101"/>
+      <c r="AU16" s="101"/>
+      <c r="AV16" s="101"/>
+      <c r="AW16" s="101"/>
+      <c r="AX16" s="101"/>
+      <c r="AY16" s="101"/>
+      <c r="AZ16" s="101"/>
+      <c r="BA16" s="101"/>
+      <c r="BB16" s="101"/>
+      <c r="BC16" s="101"/>
+      <c r="BD16" s="101"/>
+      <c r="BE16" s="101"/>
+      <c r="BF16" s="101"/>
+      <c r="BG16" s="101"/>
+      <c r="BH16" s="101"/>
+      <c r="BI16" s="101"/>
+      <c r="BJ16" s="101"/>
+      <c r="BK16" s="101"/>
+      <c r="BL16" s="101"/>
+      <c r="BM16" s="102"/>
       <c r="BO16" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BP16" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:69" ht="18" customHeight="1">
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="106"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="107"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="107"/>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107"/>
-      <c r="J17" s="107"/>
-      <c r="K17" s="107"/>
-      <c r="L17" s="107"/>
-      <c r="M17" s="107"/>
-      <c r="N17" s="107"/>
-      <c r="O17" s="107"/>
-      <c r="P17" s="107"/>
-      <c r="Q17" s="107"/>
-      <c r="R17" s="107"/>
-      <c r="S17" s="107"/>
-      <c r="T17" s="107"/>
-      <c r="U17" s="107"/>
-      <c r="V17" s="107"/>
-      <c r="W17" s="107"/>
-      <c r="X17" s="107"/>
-      <c r="Y17" s="107"/>
-      <c r="Z17" s="107"/>
-      <c r="AA17" s="107"/>
-      <c r="AB17" s="107"/>
-      <c r="AC17" s="107"/>
-      <c r="AD17" s="107"/>
-      <c r="AE17" s="107"/>
-      <c r="AF17" s="107"/>
-      <c r="AG17" s="107"/>
-      <c r="AH17" s="107"/>
-      <c r="AI17" s="107"/>
-      <c r="AJ17" s="107"/>
-      <c r="AK17" s="107"/>
-      <c r="AL17" s="107"/>
-      <c r="AM17" s="107"/>
-      <c r="AN17" s="107"/>
-      <c r="AO17" s="107"/>
-      <c r="AP17" s="107"/>
-      <c r="AQ17" s="107"/>
-      <c r="AR17" s="107"/>
-      <c r="AS17" s="107"/>
-      <c r="AT17" s="107"/>
-      <c r="AU17" s="107"/>
-      <c r="AV17" s="107"/>
-      <c r="AW17" s="107"/>
-      <c r="AX17" s="107"/>
-      <c r="AY17" s="107"/>
-      <c r="AZ17" s="107"/>
-      <c r="BA17" s="107"/>
-      <c r="BB17" s="107"/>
-      <c r="BC17" s="107"/>
-      <c r="BD17" s="107"/>
-      <c r="BE17" s="107"/>
-      <c r="BF17" s="107"/>
-      <c r="BG17" s="107"/>
-      <c r="BH17" s="107"/>
-      <c r="BI17" s="107"/>
-      <c r="BJ17" s="107"/>
-      <c r="BK17" s="107"/>
-      <c r="BL17" s="107"/>
-      <c r="BM17" s="108"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="101"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="101"/>
+      <c r="J17" s="101"/>
+      <c r="K17" s="101"/>
+      <c r="L17" s="101"/>
+      <c r="M17" s="101"/>
+      <c r="N17" s="101"/>
+      <c r="O17" s="101"/>
+      <c r="P17" s="101"/>
+      <c r="Q17" s="101"/>
+      <c r="R17" s="101"/>
+      <c r="S17" s="101"/>
+      <c r="T17" s="101"/>
+      <c r="U17" s="101"/>
+      <c r="V17" s="101"/>
+      <c r="W17" s="101"/>
+      <c r="X17" s="101"/>
+      <c r="Y17" s="101"/>
+      <c r="Z17" s="101"/>
+      <c r="AA17" s="101"/>
+      <c r="AB17" s="101"/>
+      <c r="AC17" s="101"/>
+      <c r="AD17" s="101"/>
+      <c r="AE17" s="101"/>
+      <c r="AF17" s="101"/>
+      <c r="AG17" s="101"/>
+      <c r="AH17" s="101"/>
+      <c r="AI17" s="101"/>
+      <c r="AJ17" s="101"/>
+      <c r="AK17" s="101"/>
+      <c r="AL17" s="101"/>
+      <c r="AM17" s="101"/>
+      <c r="AN17" s="101"/>
+      <c r="AO17" s="101"/>
+      <c r="AP17" s="101"/>
+      <c r="AQ17" s="101"/>
+      <c r="AR17" s="101"/>
+      <c r="AS17" s="101"/>
+      <c r="AT17" s="101"/>
+      <c r="AU17" s="101"/>
+      <c r="AV17" s="101"/>
+      <c r="AW17" s="101"/>
+      <c r="AX17" s="101"/>
+      <c r="AY17" s="101"/>
+      <c r="AZ17" s="101"/>
+      <c r="BA17" s="101"/>
+      <c r="BB17" s="101"/>
+      <c r="BC17" s="101"/>
+      <c r="BD17" s="101"/>
+      <c r="BE17" s="101"/>
+      <c r="BF17" s="101"/>
+      <c r="BG17" s="101"/>
+      <c r="BH17" s="101"/>
+      <c r="BI17" s="101"/>
+      <c r="BJ17" s="101"/>
+      <c r="BK17" s="101"/>
+      <c r="BL17" s="101"/>
+      <c r="BM17" s="102"/>
       <c r="BN17" s="25"/>
       <c r="BO17" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="BP17" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:69" ht="18" customHeight="1">
       <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="110"/>
-      <c r="D18" s="110"/>
-      <c r="E18" s="110"/>
-      <c r="F18" s="110"/>
-      <c r="G18" s="110"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="110"/>
-      <c r="J18" s="110"/>
-      <c r="K18" s="110"/>
-      <c r="L18" s="110"/>
-      <c r="M18" s="110"/>
-      <c r="N18" s="110"/>
-      <c r="O18" s="110"/>
-      <c r="P18" s="110"/>
-      <c r="Q18" s="110"/>
-      <c r="R18" s="110"/>
-      <c r="S18" s="110"/>
-      <c r="T18" s="110"/>
-      <c r="U18" s="110"/>
-      <c r="V18" s="110"/>
-      <c r="W18" s="110"/>
-      <c r="X18" s="110"/>
-      <c r="Y18" s="110"/>
-      <c r="Z18" s="110"/>
-      <c r="AA18" s="110"/>
-      <c r="AB18" s="110"/>
-      <c r="AC18" s="110"/>
-      <c r="AD18" s="110"/>
-      <c r="AE18" s="110"/>
-      <c r="AF18" s="110"/>
-      <c r="AG18" s="110"/>
-      <c r="AH18" s="110"/>
-      <c r="AI18" s="110"/>
-      <c r="AJ18" s="110"/>
-      <c r="AK18" s="110"/>
-      <c r="AL18" s="110"/>
-      <c r="AM18" s="110"/>
-      <c r="AN18" s="110"/>
-      <c r="AO18" s="110"/>
-      <c r="AP18" s="110"/>
-      <c r="AQ18" s="110"/>
-      <c r="AR18" s="110"/>
-      <c r="AS18" s="110"/>
-      <c r="AT18" s="110"/>
-      <c r="AU18" s="110"/>
-      <c r="AV18" s="110"/>
-      <c r="AW18" s="110"/>
-      <c r="AX18" s="110"/>
-      <c r="AY18" s="110"/>
-      <c r="AZ18" s="110"/>
-      <c r="BA18" s="110"/>
-      <c r="BB18" s="110"/>
-      <c r="BC18" s="110"/>
-      <c r="BD18" s="110"/>
-      <c r="BE18" s="110"/>
-      <c r="BF18" s="110"/>
-      <c r="BG18" s="110"/>
-      <c r="BH18" s="110"/>
-      <c r="BI18" s="110"/>
-      <c r="BJ18" s="110"/>
-      <c r="BK18" s="110"/>
-      <c r="BL18" s="110"/>
-      <c r="BM18" s="111"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="104"/>
+      <c r="L18" s="104"/>
+      <c r="M18" s="104"/>
+      <c r="N18" s="104"/>
+      <c r="O18" s="104"/>
+      <c r="P18" s="104"/>
+      <c r="Q18" s="104"/>
+      <c r="R18" s="104"/>
+      <c r="S18" s="104"/>
+      <c r="T18" s="104"/>
+      <c r="U18" s="104"/>
+      <c r="V18" s="104"/>
+      <c r="W18" s="104"/>
+      <c r="X18" s="104"/>
+      <c r="Y18" s="104"/>
+      <c r="Z18" s="104"/>
+      <c r="AA18" s="104"/>
+      <c r="AB18" s="104"/>
+      <c r="AC18" s="104"/>
+      <c r="AD18" s="104"/>
+      <c r="AE18" s="104"/>
+      <c r="AF18" s="104"/>
+      <c r="AG18" s="104"/>
+      <c r="AH18" s="104"/>
+      <c r="AI18" s="104"/>
+      <c r="AJ18" s="104"/>
+      <c r="AK18" s="104"/>
+      <c r="AL18" s="104"/>
+      <c r="AM18" s="104"/>
+      <c r="AN18" s="104"/>
+      <c r="AO18" s="104"/>
+      <c r="AP18" s="104"/>
+      <c r="AQ18" s="104"/>
+      <c r="AR18" s="104"/>
+      <c r="AS18" s="104"/>
+      <c r="AT18" s="104"/>
+      <c r="AU18" s="104"/>
+      <c r="AV18" s="104"/>
+      <c r="AW18" s="104"/>
+      <c r="AX18" s="104"/>
+      <c r="AY18" s="104"/>
+      <c r="AZ18" s="104"/>
+      <c r="BA18" s="104"/>
+      <c r="BB18" s="104"/>
+      <c r="BC18" s="104"/>
+      <c r="BD18" s="104"/>
+      <c r="BE18" s="104"/>
+      <c r="BF18" s="104"/>
+      <c r="BG18" s="104"/>
+      <c r="BH18" s="104"/>
+      <c r="BI18" s="104"/>
+      <c r="BJ18" s="104"/>
+      <c r="BK18" s="104"/>
+      <c r="BL18" s="104"/>
+      <c r="BM18" s="105"/>
       <c r="BO18" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="BP18" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:69">
       <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="104"/>
-      <c r="G19" s="104"/>
-      <c r="H19" s="104"/>
-      <c r="I19" s="104"/>
-      <c r="J19" s="104"/>
-      <c r="K19" s="104"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="104"/>
-      <c r="N19" s="104"/>
-      <c r="O19" s="104"/>
-      <c r="P19" s="104"/>
-      <c r="Q19" s="104"/>
-      <c r="R19" s="104"/>
-      <c r="S19" s="104"/>
-      <c r="T19" s="104"/>
-      <c r="U19" s="104"/>
-      <c r="V19" s="104"/>
-      <c r="W19" s="104"/>
-      <c r="X19" s="104"/>
-      <c r="Y19" s="104"/>
-      <c r="Z19" s="104"/>
-      <c r="AA19" s="104"/>
-      <c r="AB19" s="104"/>
-      <c r="AC19" s="104"/>
-      <c r="AD19" s="104"/>
-      <c r="AE19" s="104"/>
-      <c r="AF19" s="104"/>
-      <c r="AG19" s="104"/>
-      <c r="AH19" s="104"/>
-      <c r="AI19" s="104"/>
-      <c r="AJ19" s="104"/>
-      <c r="AK19" s="104"/>
-      <c r="AL19" s="104"/>
-      <c r="AM19" s="104"/>
-      <c r="AN19" s="104"/>
-      <c r="AO19" s="104"/>
-      <c r="AP19" s="104"/>
-      <c r="AQ19" s="104"/>
-      <c r="AR19" s="104"/>
-      <c r="AS19" s="104"/>
-      <c r="AT19" s="104"/>
-      <c r="AU19" s="104"/>
-      <c r="AV19" s="104"/>
-      <c r="AW19" s="104"/>
-      <c r="AX19" s="104"/>
-      <c r="AY19" s="104"/>
-      <c r="AZ19" s="104"/>
-      <c r="BA19" s="104"/>
-      <c r="BB19" s="104"/>
-      <c r="BC19" s="104"/>
-      <c r="BD19" s="104"/>
-      <c r="BE19" s="104"/>
-      <c r="BF19" s="104"/>
-      <c r="BG19" s="104"/>
-      <c r="BH19" s="104"/>
-      <c r="BI19" s="104"/>
-      <c r="BJ19" s="104"/>
-      <c r="BK19" s="104"/>
-      <c r="BL19" s="104"/>
-      <c r="BM19" s="105"/>
+      <c r="B19" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="98"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="98"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="98"/>
+      <c r="O19" s="98"/>
+      <c r="P19" s="98"/>
+      <c r="Q19" s="98"/>
+      <c r="R19" s="98"/>
+      <c r="S19" s="98"/>
+      <c r="T19" s="98"/>
+      <c r="U19" s="98"/>
+      <c r="V19" s="98"/>
+      <c r="W19" s="98"/>
+      <c r="X19" s="98"/>
+      <c r="Y19" s="98"/>
+      <c r="Z19" s="98"/>
+      <c r="AA19" s="98"/>
+      <c r="AB19" s="98"/>
+      <c r="AC19" s="98"/>
+      <c r="AD19" s="98"/>
+      <c r="AE19" s="98"/>
+      <c r="AF19" s="98"/>
+      <c r="AG19" s="98"/>
+      <c r="AH19" s="98"/>
+      <c r="AI19" s="98"/>
+      <c r="AJ19" s="98"/>
+      <c r="AK19" s="98"/>
+      <c r="AL19" s="98"/>
+      <c r="AM19" s="98"/>
+      <c r="AN19" s="98"/>
+      <c r="AO19" s="98"/>
+      <c r="AP19" s="98"/>
+      <c r="AQ19" s="98"/>
+      <c r="AR19" s="98"/>
+      <c r="AS19" s="98"/>
+      <c r="AT19" s="98"/>
+      <c r="AU19" s="98"/>
+      <c r="AV19" s="98"/>
+      <c r="AW19" s="98"/>
+      <c r="AX19" s="98"/>
+      <c r="AY19" s="98"/>
+      <c r="AZ19" s="98"/>
+      <c r="BA19" s="98"/>
+      <c r="BB19" s="98"/>
+      <c r="BC19" s="98"/>
+      <c r="BD19" s="98"/>
+      <c r="BE19" s="98"/>
+      <c r="BF19" s="98"/>
+      <c r="BG19" s="98"/>
+      <c r="BH19" s="98"/>
+      <c r="BI19" s="98"/>
+      <c r="BJ19" s="98"/>
+      <c r="BK19" s="98"/>
+      <c r="BL19" s="98"/>
+      <c r="BM19" s="99"/>
       <c r="BO19" s="28"/>
       <c r="BP19" s="28"/>
     </row>
@@ -2839,70 +2839,70 @@
       <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="106"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="107"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="107"/>
-      <c r="J20" s="107"/>
-      <c r="K20" s="107"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="107"/>
-      <c r="N20" s="107"/>
-      <c r="O20" s="107"/>
-      <c r="P20" s="107"/>
-      <c r="Q20" s="107"/>
-      <c r="R20" s="107"/>
-      <c r="S20" s="107"/>
-      <c r="T20" s="107"/>
-      <c r="U20" s="107"/>
-      <c r="V20" s="107"/>
-      <c r="W20" s="107"/>
-      <c r="X20" s="107"/>
-      <c r="Y20" s="107"/>
-      <c r="Z20" s="107"/>
-      <c r="AA20" s="107"/>
-      <c r="AB20" s="107"/>
-      <c r="AC20" s="107"/>
-      <c r="AD20" s="107"/>
-      <c r="AE20" s="107"/>
-      <c r="AF20" s="107"/>
-      <c r="AG20" s="107"/>
-      <c r="AH20" s="107"/>
-      <c r="AI20" s="107"/>
-      <c r="AJ20" s="107"/>
-      <c r="AK20" s="107"/>
-      <c r="AL20" s="107"/>
-      <c r="AM20" s="107"/>
-      <c r="AN20" s="107"/>
-      <c r="AO20" s="107"/>
-      <c r="AP20" s="107"/>
-      <c r="AQ20" s="107"/>
-      <c r="AR20" s="107"/>
-      <c r="AS20" s="107"/>
-      <c r="AT20" s="107"/>
-      <c r="AU20" s="107"/>
-      <c r="AV20" s="107"/>
-      <c r="AW20" s="107"/>
-      <c r="AX20" s="107"/>
-      <c r="AY20" s="107"/>
-      <c r="AZ20" s="107"/>
-      <c r="BA20" s="107"/>
-      <c r="BB20" s="107"/>
-      <c r="BC20" s="107"/>
-      <c r="BD20" s="107"/>
-      <c r="BE20" s="107"/>
-      <c r="BF20" s="107"/>
-      <c r="BG20" s="107"/>
-      <c r="BH20" s="107"/>
-      <c r="BI20" s="107"/>
-      <c r="BJ20" s="107"/>
-      <c r="BK20" s="107"/>
-      <c r="BL20" s="107"/>
-      <c r="BM20" s="108"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="101"/>
+      <c r="I20" s="101"/>
+      <c r="J20" s="101"/>
+      <c r="K20" s="101"/>
+      <c r="L20" s="101"/>
+      <c r="M20" s="101"/>
+      <c r="N20" s="101"/>
+      <c r="O20" s="101"/>
+      <c r="P20" s="101"/>
+      <c r="Q20" s="101"/>
+      <c r="R20" s="101"/>
+      <c r="S20" s="101"/>
+      <c r="T20" s="101"/>
+      <c r="U20" s="101"/>
+      <c r="V20" s="101"/>
+      <c r="W20" s="101"/>
+      <c r="X20" s="101"/>
+      <c r="Y20" s="101"/>
+      <c r="Z20" s="101"/>
+      <c r="AA20" s="101"/>
+      <c r="AB20" s="101"/>
+      <c r="AC20" s="101"/>
+      <c r="AD20" s="101"/>
+      <c r="AE20" s="101"/>
+      <c r="AF20" s="101"/>
+      <c r="AG20" s="101"/>
+      <c r="AH20" s="101"/>
+      <c r="AI20" s="101"/>
+      <c r="AJ20" s="101"/>
+      <c r="AK20" s="101"/>
+      <c r="AL20" s="101"/>
+      <c r="AM20" s="101"/>
+      <c r="AN20" s="101"/>
+      <c r="AO20" s="101"/>
+      <c r="AP20" s="101"/>
+      <c r="AQ20" s="101"/>
+      <c r="AR20" s="101"/>
+      <c r="AS20" s="101"/>
+      <c r="AT20" s="101"/>
+      <c r="AU20" s="101"/>
+      <c r="AV20" s="101"/>
+      <c r="AW20" s="101"/>
+      <c r="AX20" s="101"/>
+      <c r="AY20" s="101"/>
+      <c r="AZ20" s="101"/>
+      <c r="BA20" s="101"/>
+      <c r="BB20" s="101"/>
+      <c r="BC20" s="101"/>
+      <c r="BD20" s="101"/>
+      <c r="BE20" s="101"/>
+      <c r="BF20" s="101"/>
+      <c r="BG20" s="101"/>
+      <c r="BH20" s="101"/>
+      <c r="BI20" s="101"/>
+      <c r="BJ20" s="101"/>
+      <c r="BK20" s="101"/>
+      <c r="BL20" s="101"/>
+      <c r="BM20" s="102"/>
       <c r="BO20" s="59" t="s">
         <v>2</v>
       </c>
@@ -2912,452 +2912,452 @@
       <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="106"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="107"/>
-      <c r="K21" s="107"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="107"/>
-      <c r="N21" s="107"/>
-      <c r="O21" s="107"/>
-      <c r="P21" s="107"/>
-      <c r="Q21" s="107"/>
-      <c r="R21" s="107"/>
-      <c r="S21" s="107"/>
-      <c r="T21" s="107"/>
-      <c r="U21" s="107"/>
-      <c r="V21" s="107"/>
-      <c r="W21" s="107"/>
-      <c r="X21" s="107"/>
-      <c r="Y21" s="107"/>
-      <c r="Z21" s="107"/>
-      <c r="AA21" s="107"/>
-      <c r="AB21" s="107"/>
-      <c r="AC21" s="107"/>
-      <c r="AD21" s="107"/>
-      <c r="AE21" s="107"/>
-      <c r="AF21" s="107"/>
-      <c r="AG21" s="107"/>
-      <c r="AH21" s="107"/>
-      <c r="AI21" s="107"/>
-      <c r="AJ21" s="107"/>
-      <c r="AK21" s="107"/>
-      <c r="AL21" s="107"/>
-      <c r="AM21" s="107"/>
-      <c r="AN21" s="107"/>
-      <c r="AO21" s="107"/>
-      <c r="AP21" s="107"/>
-      <c r="AQ21" s="107"/>
-      <c r="AR21" s="107"/>
-      <c r="AS21" s="107"/>
-      <c r="AT21" s="107"/>
-      <c r="AU21" s="107"/>
-      <c r="AV21" s="107"/>
-      <c r="AW21" s="107"/>
-      <c r="AX21" s="107"/>
-      <c r="AY21" s="107"/>
-      <c r="AZ21" s="107"/>
-      <c r="BA21" s="107"/>
-      <c r="BB21" s="107"/>
-      <c r="BC21" s="107"/>
-      <c r="BD21" s="107"/>
-      <c r="BE21" s="107"/>
-      <c r="BF21" s="107"/>
-      <c r="BG21" s="107"/>
-      <c r="BH21" s="107"/>
-      <c r="BI21" s="107"/>
-      <c r="BJ21" s="107"/>
-      <c r="BK21" s="107"/>
-      <c r="BL21" s="107"/>
-      <c r="BM21" s="108"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="101"/>
+      <c r="J21" s="101"/>
+      <c r="K21" s="101"/>
+      <c r="L21" s="101"/>
+      <c r="M21" s="101"/>
+      <c r="N21" s="101"/>
+      <c r="O21" s="101"/>
+      <c r="P21" s="101"/>
+      <c r="Q21" s="101"/>
+      <c r="R21" s="101"/>
+      <c r="S21" s="101"/>
+      <c r="T21" s="101"/>
+      <c r="U21" s="101"/>
+      <c r="V21" s="101"/>
+      <c r="W21" s="101"/>
+      <c r="X21" s="101"/>
+      <c r="Y21" s="101"/>
+      <c r="Z21" s="101"/>
+      <c r="AA21" s="101"/>
+      <c r="AB21" s="101"/>
+      <c r="AC21" s="101"/>
+      <c r="AD21" s="101"/>
+      <c r="AE21" s="101"/>
+      <c r="AF21" s="101"/>
+      <c r="AG21" s="101"/>
+      <c r="AH21" s="101"/>
+      <c r="AI21" s="101"/>
+      <c r="AJ21" s="101"/>
+      <c r="AK21" s="101"/>
+      <c r="AL21" s="101"/>
+      <c r="AM21" s="101"/>
+      <c r="AN21" s="101"/>
+      <c r="AO21" s="101"/>
+      <c r="AP21" s="101"/>
+      <c r="AQ21" s="101"/>
+      <c r="AR21" s="101"/>
+      <c r="AS21" s="101"/>
+      <c r="AT21" s="101"/>
+      <c r="AU21" s="101"/>
+      <c r="AV21" s="101"/>
+      <c r="AW21" s="101"/>
+      <c r="AX21" s="101"/>
+      <c r="AY21" s="101"/>
+      <c r="AZ21" s="101"/>
+      <c r="BA21" s="101"/>
+      <c r="BB21" s="101"/>
+      <c r="BC21" s="101"/>
+      <c r="BD21" s="101"/>
+      <c r="BE21" s="101"/>
+      <c r="BF21" s="101"/>
+      <c r="BG21" s="101"/>
+      <c r="BH21" s="101"/>
+      <c r="BI21" s="101"/>
+      <c r="BJ21" s="101"/>
+      <c r="BK21" s="101"/>
+      <c r="BL21" s="101"/>
+      <c r="BM21" s="102"/>
       <c r="BO21" s="29">
         <v>1</v>
       </c>
       <c r="BP21" s="30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:69">
       <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="109"/>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="110"/>
-      <c r="M22" s="110"/>
-      <c r="N22" s="110"/>
-      <c r="O22" s="110"/>
-      <c r="P22" s="110"/>
-      <c r="Q22" s="110"/>
-      <c r="R22" s="110"/>
-      <c r="S22" s="110"/>
-      <c r="T22" s="110"/>
-      <c r="U22" s="110"/>
-      <c r="V22" s="110"/>
-      <c r="W22" s="110"/>
-      <c r="X22" s="110"/>
-      <c r="Y22" s="110"/>
-      <c r="Z22" s="110"/>
-      <c r="AA22" s="110"/>
-      <c r="AB22" s="110"/>
-      <c r="AC22" s="110"/>
-      <c r="AD22" s="110"/>
-      <c r="AE22" s="110"/>
-      <c r="AF22" s="110"/>
-      <c r="AG22" s="110"/>
-      <c r="AH22" s="110"/>
-      <c r="AI22" s="110"/>
-      <c r="AJ22" s="110"/>
-      <c r="AK22" s="110"/>
-      <c r="AL22" s="110"/>
-      <c r="AM22" s="110"/>
-      <c r="AN22" s="110"/>
-      <c r="AO22" s="110"/>
-      <c r="AP22" s="110"/>
-      <c r="AQ22" s="110"/>
-      <c r="AR22" s="110"/>
-      <c r="AS22" s="110"/>
-      <c r="AT22" s="110"/>
-      <c r="AU22" s="110"/>
-      <c r="AV22" s="110"/>
-      <c r="AW22" s="110"/>
-      <c r="AX22" s="110"/>
-      <c r="AY22" s="110"/>
-      <c r="AZ22" s="110"/>
-      <c r="BA22" s="110"/>
-      <c r="BB22" s="110"/>
-      <c r="BC22" s="110"/>
-      <c r="BD22" s="110"/>
-      <c r="BE22" s="110"/>
-      <c r="BF22" s="110"/>
-      <c r="BG22" s="110"/>
-      <c r="BH22" s="110"/>
-      <c r="BI22" s="110"/>
-      <c r="BJ22" s="110"/>
-      <c r="BK22" s="110"/>
-      <c r="BL22" s="110"/>
-      <c r="BM22" s="111"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="104"/>
+      <c r="O22" s="104"/>
+      <c r="P22" s="104"/>
+      <c r="Q22" s="104"/>
+      <c r="R22" s="104"/>
+      <c r="S22" s="104"/>
+      <c r="T22" s="104"/>
+      <c r="U22" s="104"/>
+      <c r="V22" s="104"/>
+      <c r="W22" s="104"/>
+      <c r="X22" s="104"/>
+      <c r="Y22" s="104"/>
+      <c r="Z22" s="104"/>
+      <c r="AA22" s="104"/>
+      <c r="AB22" s="104"/>
+      <c r="AC22" s="104"/>
+      <c r="AD22" s="104"/>
+      <c r="AE22" s="104"/>
+      <c r="AF22" s="104"/>
+      <c r="AG22" s="104"/>
+      <c r="AH22" s="104"/>
+      <c r="AI22" s="104"/>
+      <c r="AJ22" s="104"/>
+      <c r="AK22" s="104"/>
+      <c r="AL22" s="104"/>
+      <c r="AM22" s="104"/>
+      <c r="AN22" s="104"/>
+      <c r="AO22" s="104"/>
+      <c r="AP22" s="104"/>
+      <c r="AQ22" s="104"/>
+      <c r="AR22" s="104"/>
+      <c r="AS22" s="104"/>
+      <c r="AT22" s="104"/>
+      <c r="AU22" s="104"/>
+      <c r="AV22" s="104"/>
+      <c r="AW22" s="104"/>
+      <c r="AX22" s="104"/>
+      <c r="AY22" s="104"/>
+      <c r="AZ22" s="104"/>
+      <c r="BA22" s="104"/>
+      <c r="BB22" s="104"/>
+      <c r="BC22" s="104"/>
+      <c r="BD22" s="104"/>
+      <c r="BE22" s="104"/>
+      <c r="BF22" s="104"/>
+      <c r="BG22" s="104"/>
+      <c r="BH22" s="104"/>
+      <c r="BI22" s="104"/>
+      <c r="BJ22" s="104"/>
+      <c r="BK22" s="104"/>
+      <c r="BL22" s="104"/>
+      <c r="BM22" s="105"/>
       <c r="BO22" s="31">
         <v>2</v>
       </c>
       <c r="BP22" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:69">
       <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="B23" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="62"/>
-      <c r="V23" s="62"/>
-      <c r="W23" s="62"/>
-      <c r="X23" s="62"/>
-      <c r="Y23" s="62"/>
-      <c r="Z23" s="62"/>
-      <c r="AA23" s="62"/>
-      <c r="AB23" s="62"/>
-      <c r="AC23" s="62"/>
-      <c r="AD23" s="62"/>
-      <c r="AE23" s="62"/>
-      <c r="AF23" s="62"/>
-      <c r="AG23" s="62"/>
-      <c r="AH23" s="62"/>
-      <c r="AI23" s="62"/>
-      <c r="AJ23" s="62"/>
-      <c r="AK23" s="62"/>
-      <c r="AL23" s="62"/>
-      <c r="AM23" s="62"/>
-      <c r="AN23" s="62"/>
-      <c r="AO23" s="62"/>
-      <c r="AP23" s="62"/>
-      <c r="AQ23" s="62"/>
-      <c r="AR23" s="62"/>
-      <c r="AS23" s="62"/>
-      <c r="AT23" s="62"/>
-      <c r="AU23" s="62"/>
-      <c r="AV23" s="62"/>
-      <c r="AW23" s="62"/>
-      <c r="AX23" s="62"/>
-      <c r="AY23" s="62"/>
-      <c r="AZ23" s="62"/>
-      <c r="BA23" s="62"/>
-      <c r="BB23" s="62"/>
-      <c r="BC23" s="62"/>
-      <c r="BD23" s="62"/>
-      <c r="BE23" s="62"/>
-      <c r="BF23" s="62"/>
-      <c r="BG23" s="62"/>
-      <c r="BH23" s="62"/>
-      <c r="BI23" s="62"/>
-      <c r="BJ23" s="62"/>
-      <c r="BK23" s="62"/>
-      <c r="BL23" s="62"/>
-      <c r="BM23" s="63"/>
+      <c r="B23" s="124" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="125"/>
+      <c r="D23" s="125"/>
+      <c r="E23" s="125"/>
+      <c r="F23" s="125"/>
+      <c r="G23" s="125"/>
+      <c r="H23" s="125"/>
+      <c r="I23" s="125"/>
+      <c r="J23" s="125"/>
+      <c r="K23" s="125"/>
+      <c r="L23" s="125"/>
+      <c r="M23" s="125"/>
+      <c r="N23" s="125"/>
+      <c r="O23" s="125"/>
+      <c r="P23" s="125"/>
+      <c r="Q23" s="125"/>
+      <c r="R23" s="125"/>
+      <c r="S23" s="125"/>
+      <c r="T23" s="125"/>
+      <c r="U23" s="125"/>
+      <c r="V23" s="125"/>
+      <c r="W23" s="125"/>
+      <c r="X23" s="125"/>
+      <c r="Y23" s="125"/>
+      <c r="Z23" s="125"/>
+      <c r="AA23" s="125"/>
+      <c r="AB23" s="125"/>
+      <c r="AC23" s="125"/>
+      <c r="AD23" s="125"/>
+      <c r="AE23" s="125"/>
+      <c r="AF23" s="125"/>
+      <c r="AG23" s="125"/>
+      <c r="AH23" s="125"/>
+      <c r="AI23" s="125"/>
+      <c r="AJ23" s="125"/>
+      <c r="AK23" s="125"/>
+      <c r="AL23" s="125"/>
+      <c r="AM23" s="125"/>
+      <c r="AN23" s="125"/>
+      <c r="AO23" s="125"/>
+      <c r="AP23" s="125"/>
+      <c r="AQ23" s="125"/>
+      <c r="AR23" s="125"/>
+      <c r="AS23" s="125"/>
+      <c r="AT23" s="125"/>
+      <c r="AU23" s="125"/>
+      <c r="AV23" s="125"/>
+      <c r="AW23" s="125"/>
+      <c r="AX23" s="125"/>
+      <c r="AY23" s="125"/>
+      <c r="AZ23" s="125"/>
+      <c r="BA23" s="125"/>
+      <c r="BB23" s="125"/>
+      <c r="BC23" s="125"/>
+      <c r="BD23" s="125"/>
+      <c r="BE23" s="125"/>
+      <c r="BF23" s="125"/>
+      <c r="BG23" s="125"/>
+      <c r="BH23" s="125"/>
+      <c r="BI23" s="125"/>
+      <c r="BJ23" s="125"/>
+      <c r="BK23" s="125"/>
+      <c r="BL23" s="125"/>
+      <c r="BM23" s="126"/>
       <c r="BO23" s="33">
         <v>3</v>
       </c>
       <c r="BP23" s="34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:69">
       <c r="A24" s="4">
         <v>21</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="65"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="65"/>
-      <c r="P24" s="65"/>
-      <c r="Q24" s="65"/>
-      <c r="R24" s="65"/>
-      <c r="S24" s="65"/>
-      <c r="T24" s="65"/>
-      <c r="U24" s="65"/>
-      <c r="V24" s="65"/>
-      <c r="W24" s="65"/>
-      <c r="X24" s="65"/>
-      <c r="Y24" s="65"/>
-      <c r="Z24" s="65"/>
-      <c r="AA24" s="65"/>
-      <c r="AB24" s="65"/>
-      <c r="AC24" s="65"/>
-      <c r="AD24" s="65"/>
-      <c r="AE24" s="65"/>
-      <c r="AF24" s="65"/>
-      <c r="AG24" s="65"/>
-      <c r="AH24" s="65"/>
-      <c r="AI24" s="65"/>
-      <c r="AJ24" s="65"/>
-      <c r="AK24" s="65"/>
-      <c r="AL24" s="65"/>
-      <c r="AM24" s="65"/>
-      <c r="AN24" s="65"/>
-      <c r="AO24" s="65"/>
-      <c r="AP24" s="65"/>
-      <c r="AQ24" s="65"/>
-      <c r="AR24" s="65"/>
-      <c r="AS24" s="65"/>
-      <c r="AT24" s="65"/>
-      <c r="AU24" s="65"/>
-      <c r="AV24" s="65"/>
-      <c r="AW24" s="65"/>
-      <c r="AX24" s="65"/>
-      <c r="AY24" s="65"/>
-      <c r="AZ24" s="65"/>
-      <c r="BA24" s="65"/>
-      <c r="BB24" s="65"/>
-      <c r="BC24" s="65"/>
-      <c r="BD24" s="65"/>
-      <c r="BE24" s="65"/>
-      <c r="BF24" s="65"/>
-      <c r="BG24" s="65"/>
-      <c r="BH24" s="65"/>
-      <c r="BI24" s="65"/>
-      <c r="BJ24" s="65"/>
-      <c r="BK24" s="65"/>
-      <c r="BL24" s="65"/>
-      <c r="BM24" s="66"/>
+      <c r="B24" s="127"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128"/>
+      <c r="F24" s="128"/>
+      <c r="G24" s="128"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="128"/>
+      <c r="J24" s="128"/>
+      <c r="K24" s="128"/>
+      <c r="L24" s="128"/>
+      <c r="M24" s="128"/>
+      <c r="N24" s="128"/>
+      <c r="O24" s="128"/>
+      <c r="P24" s="128"/>
+      <c r="Q24" s="128"/>
+      <c r="R24" s="128"/>
+      <c r="S24" s="128"/>
+      <c r="T24" s="128"/>
+      <c r="U24" s="128"/>
+      <c r="V24" s="128"/>
+      <c r="W24" s="128"/>
+      <c r="X24" s="128"/>
+      <c r="Y24" s="128"/>
+      <c r="Z24" s="128"/>
+      <c r="AA24" s="128"/>
+      <c r="AB24" s="128"/>
+      <c r="AC24" s="128"/>
+      <c r="AD24" s="128"/>
+      <c r="AE24" s="128"/>
+      <c r="AF24" s="128"/>
+      <c r="AG24" s="128"/>
+      <c r="AH24" s="128"/>
+      <c r="AI24" s="128"/>
+      <c r="AJ24" s="128"/>
+      <c r="AK24" s="128"/>
+      <c r="AL24" s="128"/>
+      <c r="AM24" s="128"/>
+      <c r="AN24" s="128"/>
+      <c r="AO24" s="128"/>
+      <c r="AP24" s="128"/>
+      <c r="AQ24" s="128"/>
+      <c r="AR24" s="128"/>
+      <c r="AS24" s="128"/>
+      <c r="AT24" s="128"/>
+      <c r="AU24" s="128"/>
+      <c r="AV24" s="128"/>
+      <c r="AW24" s="128"/>
+      <c r="AX24" s="128"/>
+      <c r="AY24" s="128"/>
+      <c r="AZ24" s="128"/>
+      <c r="BA24" s="128"/>
+      <c r="BB24" s="128"/>
+      <c r="BC24" s="128"/>
+      <c r="BD24" s="128"/>
+      <c r="BE24" s="128"/>
+      <c r="BF24" s="128"/>
+      <c r="BG24" s="128"/>
+      <c r="BH24" s="128"/>
+      <c r="BI24" s="128"/>
+      <c r="BJ24" s="128"/>
+      <c r="BK24" s="128"/>
+      <c r="BL24" s="128"/>
+      <c r="BM24" s="129"/>
       <c r="BO24" s="35">
         <v>4</v>
       </c>
       <c r="BP24" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:69">
       <c r="A25" s="4">
         <v>22</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="65"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="65"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="65"/>
-      <c r="R25" s="65"/>
-      <c r="S25" s="65"/>
-      <c r="T25" s="65"/>
-      <c r="U25" s="65"/>
-      <c r="V25" s="65"/>
-      <c r="W25" s="65"/>
-      <c r="X25" s="65"/>
-      <c r="Y25" s="65"/>
-      <c r="Z25" s="65"/>
-      <c r="AA25" s="65"/>
-      <c r="AB25" s="65"/>
-      <c r="AC25" s="65"/>
-      <c r="AD25" s="65"/>
-      <c r="AE25" s="65"/>
-      <c r="AF25" s="65"/>
-      <c r="AG25" s="65"/>
-      <c r="AH25" s="65"/>
-      <c r="AI25" s="65"/>
-      <c r="AJ25" s="65"/>
-      <c r="AK25" s="65"/>
-      <c r="AL25" s="65"/>
-      <c r="AM25" s="65"/>
-      <c r="AN25" s="65"/>
-      <c r="AO25" s="65"/>
-      <c r="AP25" s="65"/>
-      <c r="AQ25" s="65"/>
-      <c r="AR25" s="65"/>
-      <c r="AS25" s="65"/>
-      <c r="AT25" s="65"/>
-      <c r="AU25" s="65"/>
-      <c r="AV25" s="65"/>
-      <c r="AW25" s="65"/>
-      <c r="AX25" s="65"/>
-      <c r="AY25" s="65"/>
-      <c r="AZ25" s="65"/>
-      <c r="BA25" s="65"/>
-      <c r="BB25" s="65"/>
-      <c r="BC25" s="65"/>
-      <c r="BD25" s="65"/>
-      <c r="BE25" s="65"/>
-      <c r="BF25" s="65"/>
-      <c r="BG25" s="65"/>
-      <c r="BH25" s="65"/>
-      <c r="BI25" s="65"/>
-      <c r="BJ25" s="65"/>
-      <c r="BK25" s="65"/>
-      <c r="BL25" s="65"/>
-      <c r="BM25" s="66"/>
+      <c r="B25" s="127"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="128"/>
+      <c r="L25" s="128"/>
+      <c r="M25" s="128"/>
+      <c r="N25" s="128"/>
+      <c r="O25" s="128"/>
+      <c r="P25" s="128"/>
+      <c r="Q25" s="128"/>
+      <c r="R25" s="128"/>
+      <c r="S25" s="128"/>
+      <c r="T25" s="128"/>
+      <c r="U25" s="128"/>
+      <c r="V25" s="128"/>
+      <c r="W25" s="128"/>
+      <c r="X25" s="128"/>
+      <c r="Y25" s="128"/>
+      <c r="Z25" s="128"/>
+      <c r="AA25" s="128"/>
+      <c r="AB25" s="128"/>
+      <c r="AC25" s="128"/>
+      <c r="AD25" s="128"/>
+      <c r="AE25" s="128"/>
+      <c r="AF25" s="128"/>
+      <c r="AG25" s="128"/>
+      <c r="AH25" s="128"/>
+      <c r="AI25" s="128"/>
+      <c r="AJ25" s="128"/>
+      <c r="AK25" s="128"/>
+      <c r="AL25" s="128"/>
+      <c r="AM25" s="128"/>
+      <c r="AN25" s="128"/>
+      <c r="AO25" s="128"/>
+      <c r="AP25" s="128"/>
+      <c r="AQ25" s="128"/>
+      <c r="AR25" s="128"/>
+      <c r="AS25" s="128"/>
+      <c r="AT25" s="128"/>
+      <c r="AU25" s="128"/>
+      <c r="AV25" s="128"/>
+      <c r="AW25" s="128"/>
+      <c r="AX25" s="128"/>
+      <c r="AY25" s="128"/>
+      <c r="AZ25" s="128"/>
+      <c r="BA25" s="128"/>
+      <c r="BB25" s="128"/>
+      <c r="BC25" s="128"/>
+      <c r="BD25" s="128"/>
+      <c r="BE25" s="128"/>
+      <c r="BF25" s="128"/>
+      <c r="BG25" s="128"/>
+      <c r="BH25" s="128"/>
+      <c r="BI25" s="128"/>
+      <c r="BJ25" s="128"/>
+      <c r="BK25" s="128"/>
+      <c r="BL25" s="128"/>
+      <c r="BM25" s="129"/>
       <c r="BO25" s="37">
         <v>5</v>
       </c>
       <c r="BP25" s="38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:69">
       <c r="A26" s="4">
         <v>23</v>
       </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
-      <c r="M26" s="68"/>
-      <c r="N26" s="68"/>
-      <c r="O26" s="68"/>
-      <c r="P26" s="68"/>
-      <c r="Q26" s="68"/>
-      <c r="R26" s="68"/>
-      <c r="S26" s="68"/>
-      <c r="T26" s="68"/>
-      <c r="U26" s="68"/>
-      <c r="V26" s="68"/>
-      <c r="W26" s="68"/>
-      <c r="X26" s="68"/>
-      <c r="Y26" s="68"/>
-      <c r="Z26" s="68"/>
-      <c r="AA26" s="68"/>
-      <c r="AB26" s="68"/>
-      <c r="AC26" s="68"/>
-      <c r="AD26" s="68"/>
-      <c r="AE26" s="68"/>
-      <c r="AF26" s="68"/>
-      <c r="AG26" s="68"/>
-      <c r="AH26" s="68"/>
-      <c r="AI26" s="68"/>
-      <c r="AJ26" s="68"/>
-      <c r="AK26" s="68"/>
-      <c r="AL26" s="68"/>
-      <c r="AM26" s="68"/>
-      <c r="AN26" s="68"/>
-      <c r="AO26" s="68"/>
-      <c r="AP26" s="68"/>
-      <c r="AQ26" s="68"/>
-      <c r="AR26" s="68"/>
-      <c r="AS26" s="68"/>
-      <c r="AT26" s="68"/>
-      <c r="AU26" s="68"/>
-      <c r="AV26" s="68"/>
-      <c r="AW26" s="68"/>
-      <c r="AX26" s="68"/>
-      <c r="AY26" s="68"/>
-      <c r="AZ26" s="68"/>
-      <c r="BA26" s="68"/>
-      <c r="BB26" s="68"/>
-      <c r="BC26" s="68"/>
-      <c r="BD26" s="68"/>
-      <c r="BE26" s="68"/>
-      <c r="BF26" s="68"/>
-      <c r="BG26" s="68"/>
-      <c r="BH26" s="68"/>
-      <c r="BI26" s="68"/>
-      <c r="BJ26" s="68"/>
-      <c r="BK26" s="68"/>
-      <c r="BL26" s="68"/>
-      <c r="BM26" s="69"/>
+      <c r="B26" s="130"/>
+      <c r="C26" s="131"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="131"/>
+      <c r="F26" s="131"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="131"/>
+      <c r="I26" s="131"/>
+      <c r="J26" s="131"/>
+      <c r="K26" s="131"/>
+      <c r="L26" s="131"/>
+      <c r="M26" s="131"/>
+      <c r="N26" s="131"/>
+      <c r="O26" s="131"/>
+      <c r="P26" s="131"/>
+      <c r="Q26" s="131"/>
+      <c r="R26" s="131"/>
+      <c r="S26" s="131"/>
+      <c r="T26" s="131"/>
+      <c r="U26" s="131"/>
+      <c r="V26" s="131"/>
+      <c r="W26" s="131"/>
+      <c r="X26" s="131"/>
+      <c r="Y26" s="131"/>
+      <c r="Z26" s="131"/>
+      <c r="AA26" s="131"/>
+      <c r="AB26" s="131"/>
+      <c r="AC26" s="131"/>
+      <c r="AD26" s="131"/>
+      <c r="AE26" s="131"/>
+      <c r="AF26" s="131"/>
+      <c r="AG26" s="131"/>
+      <c r="AH26" s="131"/>
+      <c r="AI26" s="131"/>
+      <c r="AJ26" s="131"/>
+      <c r="AK26" s="131"/>
+      <c r="AL26" s="131"/>
+      <c r="AM26" s="131"/>
+      <c r="AN26" s="131"/>
+      <c r="AO26" s="131"/>
+      <c r="AP26" s="131"/>
+      <c r="AQ26" s="131"/>
+      <c r="AR26" s="131"/>
+      <c r="AS26" s="131"/>
+      <c r="AT26" s="131"/>
+      <c r="AU26" s="131"/>
+      <c r="AV26" s="131"/>
+      <c r="AW26" s="131"/>
+      <c r="AX26" s="131"/>
+      <c r="AY26" s="131"/>
+      <c r="AZ26" s="131"/>
+      <c r="BA26" s="131"/>
+      <c r="BB26" s="131"/>
+      <c r="BC26" s="131"/>
+      <c r="BD26" s="131"/>
+      <c r="BE26" s="131"/>
+      <c r="BF26" s="131"/>
+      <c r="BG26" s="131"/>
+      <c r="BH26" s="131"/>
+      <c r="BI26" s="131"/>
+      <c r="BJ26" s="131"/>
+      <c r="BK26" s="131"/>
+      <c r="BL26" s="131"/>
+      <c r="BM26" s="132"/>
       <c r="BO26" s="17">
         <v>7</v>
       </c>
       <c r="BP26" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:69" ht="16" customHeight="1">
@@ -3365,7 +3365,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="88" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="89"/>
       <c r="D27" s="89"/>
@@ -3434,7 +3434,7 @@
         <v>10</v>
       </c>
       <c r="BP27" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:69" ht="16" customHeight="1">
@@ -3509,7 +3509,7 @@
         <v>11</v>
       </c>
       <c r="BP28" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="BQ28" s="25"/>
     </row>
@@ -3517,72 +3517,72 @@
       <c r="A29" s="4">
         <v>26</v>
       </c>
-      <c r="B29" s="142" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="143"/>
-      <c r="D29" s="143"/>
-      <c r="E29" s="143"/>
-      <c r="F29" s="143"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="143"/>
-      <c r="I29" s="143"/>
-      <c r="J29" s="143"/>
-      <c r="K29" s="143"/>
-      <c r="L29" s="143"/>
-      <c r="M29" s="143"/>
-      <c r="N29" s="143"/>
-      <c r="O29" s="143"/>
-      <c r="P29" s="143"/>
-      <c r="Q29" s="143"/>
-      <c r="R29" s="143"/>
-      <c r="S29" s="143"/>
-      <c r="T29" s="143"/>
-      <c r="U29" s="143"/>
-      <c r="V29" s="143"/>
-      <c r="W29" s="143"/>
-      <c r="X29" s="143"/>
-      <c r="Y29" s="143"/>
-      <c r="Z29" s="143"/>
-      <c r="AA29" s="143"/>
-      <c r="AB29" s="143"/>
-      <c r="AC29" s="143"/>
-      <c r="AD29" s="143"/>
-      <c r="AE29" s="143"/>
-      <c r="AF29" s="143"/>
-      <c r="AG29" s="143"/>
-      <c r="AH29" s="143"/>
-      <c r="AI29" s="143"/>
-      <c r="AJ29" s="143"/>
-      <c r="AK29" s="143"/>
-      <c r="AL29" s="143"/>
-      <c r="AM29" s="143"/>
-      <c r="AN29" s="143"/>
-      <c r="AO29" s="143"/>
-      <c r="AP29" s="143"/>
-      <c r="AQ29" s="143"/>
-      <c r="AR29" s="143"/>
-      <c r="AS29" s="143"/>
-      <c r="AT29" s="143"/>
-      <c r="AU29" s="143"/>
-      <c r="AV29" s="143"/>
-      <c r="AW29" s="143"/>
-      <c r="AX29" s="143"/>
-      <c r="AY29" s="143"/>
-      <c r="AZ29" s="143"/>
-      <c r="BA29" s="143"/>
-      <c r="BB29" s="143"/>
-      <c r="BC29" s="143"/>
-      <c r="BD29" s="143"/>
-      <c r="BE29" s="143"/>
-      <c r="BF29" s="143"/>
-      <c r="BG29" s="143"/>
-      <c r="BH29" s="143"/>
-      <c r="BI29" s="143"/>
-      <c r="BJ29" s="143"/>
-      <c r="BK29" s="143"/>
-      <c r="BL29" s="143"/>
-      <c r="BM29" s="144"/>
+      <c r="B29" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="74"/>
+      <c r="O29" s="74"/>
+      <c r="P29" s="74"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="74"/>
+      <c r="S29" s="74"/>
+      <c r="T29" s="74"/>
+      <c r="U29" s="74"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="74"/>
+      <c r="X29" s="74"/>
+      <c r="Y29" s="74"/>
+      <c r="Z29" s="74"/>
+      <c r="AA29" s="74"/>
+      <c r="AB29" s="74"/>
+      <c r="AC29" s="74"/>
+      <c r="AD29" s="74"/>
+      <c r="AE29" s="74"/>
+      <c r="AF29" s="74"/>
+      <c r="AG29" s="74"/>
+      <c r="AH29" s="74"/>
+      <c r="AI29" s="74"/>
+      <c r="AJ29" s="74"/>
+      <c r="AK29" s="74"/>
+      <c r="AL29" s="74"/>
+      <c r="AM29" s="74"/>
+      <c r="AN29" s="74"/>
+      <c r="AO29" s="74"/>
+      <c r="AP29" s="74"/>
+      <c r="AQ29" s="74"/>
+      <c r="AR29" s="74"/>
+      <c r="AS29" s="74"/>
+      <c r="AT29" s="74"/>
+      <c r="AU29" s="74"/>
+      <c r="AV29" s="74"/>
+      <c r="AW29" s="74"/>
+      <c r="AX29" s="74"/>
+      <c r="AY29" s="74"/>
+      <c r="AZ29" s="74"/>
+      <c r="BA29" s="74"/>
+      <c r="BB29" s="74"/>
+      <c r="BC29" s="74"/>
+      <c r="BD29" s="74"/>
+      <c r="BE29" s="74"/>
+      <c r="BF29" s="74"/>
+      <c r="BG29" s="74"/>
+      <c r="BH29" s="74"/>
+      <c r="BI29" s="74"/>
+      <c r="BJ29" s="74"/>
+      <c r="BK29" s="74"/>
+      <c r="BL29" s="74"/>
+      <c r="BM29" s="75"/>
       <c r="BO29" s="40"/>
       <c r="BP29" s="41"/>
     </row>
@@ -3590,70 +3590,70 @@
       <c r="A30" s="4">
         <v>27</v>
       </c>
-      <c r="B30" s="145"/>
-      <c r="C30" s="146"/>
-      <c r="D30" s="146"/>
-      <c r="E30" s="146"/>
-      <c r="F30" s="146"/>
-      <c r="G30" s="146"/>
-      <c r="H30" s="146"/>
-      <c r="I30" s="146"/>
-      <c r="J30" s="146"/>
-      <c r="K30" s="146"/>
-      <c r="L30" s="146"/>
-      <c r="M30" s="146"/>
-      <c r="N30" s="146"/>
-      <c r="O30" s="146"/>
-      <c r="P30" s="146"/>
-      <c r="Q30" s="146"/>
-      <c r="R30" s="146"/>
-      <c r="S30" s="146"/>
-      <c r="T30" s="146"/>
-      <c r="U30" s="146"/>
-      <c r="V30" s="146"/>
-      <c r="W30" s="146"/>
-      <c r="X30" s="146"/>
-      <c r="Y30" s="146"/>
-      <c r="Z30" s="146"/>
-      <c r="AA30" s="146"/>
-      <c r="AB30" s="146"/>
-      <c r="AC30" s="146"/>
-      <c r="AD30" s="146"/>
-      <c r="AE30" s="146"/>
-      <c r="AF30" s="146"/>
-      <c r="AG30" s="146"/>
-      <c r="AH30" s="146"/>
-      <c r="AI30" s="146"/>
-      <c r="AJ30" s="146"/>
-      <c r="AK30" s="146"/>
-      <c r="AL30" s="146"/>
-      <c r="AM30" s="146"/>
-      <c r="AN30" s="146"/>
-      <c r="AO30" s="146"/>
-      <c r="AP30" s="146"/>
-      <c r="AQ30" s="146"/>
-      <c r="AR30" s="146"/>
-      <c r="AS30" s="146"/>
-      <c r="AT30" s="146"/>
-      <c r="AU30" s="146"/>
-      <c r="AV30" s="146"/>
-      <c r="AW30" s="146"/>
-      <c r="AX30" s="146"/>
-      <c r="AY30" s="146"/>
-      <c r="AZ30" s="146"/>
-      <c r="BA30" s="146"/>
-      <c r="BB30" s="146"/>
-      <c r="BC30" s="146"/>
-      <c r="BD30" s="146"/>
-      <c r="BE30" s="146"/>
-      <c r="BF30" s="146"/>
-      <c r="BG30" s="146"/>
-      <c r="BH30" s="146"/>
-      <c r="BI30" s="146"/>
-      <c r="BJ30" s="146"/>
-      <c r="BK30" s="146"/>
-      <c r="BL30" s="146"/>
-      <c r="BM30" s="147"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77"/>
+      <c r="N30" s="77"/>
+      <c r="O30" s="77"/>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="77"/>
+      <c r="R30" s="77"/>
+      <c r="S30" s="77"/>
+      <c r="T30" s="77"/>
+      <c r="U30" s="77"/>
+      <c r="V30" s="77"/>
+      <c r="W30" s="77"/>
+      <c r="X30" s="77"/>
+      <c r="Y30" s="77"/>
+      <c r="Z30" s="77"/>
+      <c r="AA30" s="77"/>
+      <c r="AB30" s="77"/>
+      <c r="AC30" s="77"/>
+      <c r="AD30" s="77"/>
+      <c r="AE30" s="77"/>
+      <c r="AF30" s="77"/>
+      <c r="AG30" s="77"/>
+      <c r="AH30" s="77"/>
+      <c r="AI30" s="77"/>
+      <c r="AJ30" s="77"/>
+      <c r="AK30" s="77"/>
+      <c r="AL30" s="77"/>
+      <c r="AM30" s="77"/>
+      <c r="AN30" s="77"/>
+      <c r="AO30" s="77"/>
+      <c r="AP30" s="77"/>
+      <c r="AQ30" s="77"/>
+      <c r="AR30" s="77"/>
+      <c r="AS30" s="77"/>
+      <c r="AT30" s="77"/>
+      <c r="AU30" s="77"/>
+      <c r="AV30" s="77"/>
+      <c r="AW30" s="77"/>
+      <c r="AX30" s="77"/>
+      <c r="AY30" s="77"/>
+      <c r="AZ30" s="77"/>
+      <c r="BA30" s="77"/>
+      <c r="BB30" s="77"/>
+      <c r="BC30" s="77"/>
+      <c r="BD30" s="77"/>
+      <c r="BE30" s="77"/>
+      <c r="BF30" s="77"/>
+      <c r="BG30" s="77"/>
+      <c r="BH30" s="77"/>
+      <c r="BI30" s="77"/>
+      <c r="BJ30" s="77"/>
+      <c r="BK30" s="77"/>
+      <c r="BL30" s="77"/>
+      <c r="BM30" s="78"/>
       <c r="BO30" s="59" t="s">
         <v>5</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="88" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="89"/>
       <c r="D31" s="89"/>
@@ -3697,42 +3697,42 @@
       <c r="AE31" s="89"/>
       <c r="AF31" s="89"/>
       <c r="AG31" s="90"/>
-      <c r="AH31" s="130" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI31" s="131"/>
-      <c r="AJ31" s="131"/>
-      <c r="AK31" s="131"/>
-      <c r="AL31" s="131"/>
-      <c r="AM31" s="131"/>
-      <c r="AN31" s="131"/>
-      <c r="AO31" s="131"/>
-      <c r="AP31" s="131"/>
-      <c r="AQ31" s="131"/>
-      <c r="AR31" s="131"/>
-      <c r="AS31" s="131"/>
-      <c r="AT31" s="131"/>
-      <c r="AU31" s="131"/>
-      <c r="AV31" s="131"/>
-      <c r="AW31" s="131"/>
-      <c r="AX31" s="131"/>
-      <c r="AY31" s="131"/>
-      <c r="AZ31" s="131"/>
-      <c r="BA31" s="131"/>
-      <c r="BB31" s="131"/>
-      <c r="BC31" s="131"/>
-      <c r="BD31" s="131"/>
-      <c r="BE31" s="131"/>
-      <c r="BF31" s="131"/>
-      <c r="BG31" s="131"/>
-      <c r="BH31" s="131"/>
-      <c r="BI31" s="131"/>
-      <c r="BJ31" s="131"/>
-      <c r="BK31" s="131"/>
-      <c r="BL31" s="131"/>
-      <c r="BM31" s="132"/>
+      <c r="AH31" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI31" s="62"/>
+      <c r="AJ31" s="62"/>
+      <c r="AK31" s="62"/>
+      <c r="AL31" s="62"/>
+      <c r="AM31" s="62"/>
+      <c r="AN31" s="62"/>
+      <c r="AO31" s="62"/>
+      <c r="AP31" s="62"/>
+      <c r="AQ31" s="62"/>
+      <c r="AR31" s="62"/>
+      <c r="AS31" s="62"/>
+      <c r="AT31" s="62"/>
+      <c r="AU31" s="62"/>
+      <c r="AV31" s="62"/>
+      <c r="AW31" s="62"/>
+      <c r="AX31" s="62"/>
+      <c r="AY31" s="62"/>
+      <c r="AZ31" s="62"/>
+      <c r="BA31" s="62"/>
+      <c r="BB31" s="62"/>
+      <c r="BC31" s="62"/>
+      <c r="BD31" s="62"/>
+      <c r="BE31" s="62"/>
+      <c r="BF31" s="62"/>
+      <c r="BG31" s="62"/>
+      <c r="BH31" s="62"/>
+      <c r="BI31" s="62"/>
+      <c r="BJ31" s="62"/>
+      <c r="BK31" s="62"/>
+      <c r="BL31" s="62"/>
+      <c r="BM31" s="63"/>
       <c r="BO31" s="42" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="BP31" s="42"/>
     </row>
@@ -3772,40 +3772,40 @@
       <c r="AE32" s="92"/>
       <c r="AF32" s="92"/>
       <c r="AG32" s="93"/>
-      <c r="AH32" s="133"/>
-      <c r="AI32" s="134"/>
-      <c r="AJ32" s="134"/>
-      <c r="AK32" s="134"/>
-      <c r="AL32" s="134"/>
-      <c r="AM32" s="134"/>
-      <c r="AN32" s="134"/>
-      <c r="AO32" s="134"/>
-      <c r="AP32" s="134"/>
-      <c r="AQ32" s="134"/>
-      <c r="AR32" s="134"/>
-      <c r="AS32" s="134"/>
-      <c r="AT32" s="134"/>
-      <c r="AU32" s="134"/>
-      <c r="AV32" s="134"/>
-      <c r="AW32" s="134"/>
-      <c r="AX32" s="134"/>
-      <c r="AY32" s="134"/>
-      <c r="AZ32" s="134"/>
-      <c r="BA32" s="134"/>
-      <c r="BB32" s="134"/>
-      <c r="BC32" s="134"/>
-      <c r="BD32" s="134"/>
-      <c r="BE32" s="134"/>
-      <c r="BF32" s="134"/>
-      <c r="BG32" s="134"/>
-      <c r="BH32" s="134"/>
-      <c r="BI32" s="134"/>
-      <c r="BJ32" s="134"/>
-      <c r="BK32" s="134"/>
-      <c r="BL32" s="134"/>
-      <c r="BM32" s="135"/>
+      <c r="AH32" s="64"/>
+      <c r="AI32" s="65"/>
+      <c r="AJ32" s="65"/>
+      <c r="AK32" s="65"/>
+      <c r="AL32" s="65"/>
+      <c r="AM32" s="65"/>
+      <c r="AN32" s="65"/>
+      <c r="AO32" s="65"/>
+      <c r="AP32" s="65"/>
+      <c r="AQ32" s="65"/>
+      <c r="AR32" s="65"/>
+      <c r="AS32" s="65"/>
+      <c r="AT32" s="65"/>
+      <c r="AU32" s="65"/>
+      <c r="AV32" s="65"/>
+      <c r="AW32" s="65"/>
+      <c r="AX32" s="65"/>
+      <c r="AY32" s="65"/>
+      <c r="AZ32" s="65"/>
+      <c r="BA32" s="65"/>
+      <c r="BB32" s="65"/>
+      <c r="BC32" s="65"/>
+      <c r="BD32" s="65"/>
+      <c r="BE32" s="65"/>
+      <c r="BF32" s="65"/>
+      <c r="BG32" s="65"/>
+      <c r="BH32" s="65"/>
+      <c r="BI32" s="65"/>
+      <c r="BJ32" s="65"/>
+      <c r="BK32" s="65"/>
+      <c r="BL32" s="65"/>
+      <c r="BM32" s="66"/>
       <c r="BO32" s="43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:68" ht="16" customHeight="1">
@@ -3844,229 +3844,229 @@
       <c r="AE33" s="92"/>
       <c r="AF33" s="92"/>
       <c r="AG33" s="93"/>
-      <c r="AH33" s="133"/>
-      <c r="AI33" s="134"/>
-      <c r="AJ33" s="134"/>
-      <c r="AK33" s="134"/>
-      <c r="AL33" s="134"/>
-      <c r="AM33" s="134"/>
-      <c r="AN33" s="134"/>
-      <c r="AO33" s="134"/>
-      <c r="AP33" s="134"/>
-      <c r="AQ33" s="134"/>
-      <c r="AR33" s="134"/>
-      <c r="AS33" s="134"/>
-      <c r="AT33" s="134"/>
-      <c r="AU33" s="134"/>
-      <c r="AV33" s="134"/>
-      <c r="AW33" s="134"/>
-      <c r="AX33" s="134"/>
-      <c r="AY33" s="134"/>
-      <c r="AZ33" s="134"/>
-      <c r="BA33" s="134"/>
-      <c r="BB33" s="134"/>
-      <c r="BC33" s="134"/>
-      <c r="BD33" s="134"/>
-      <c r="BE33" s="134"/>
-      <c r="BF33" s="134"/>
-      <c r="BG33" s="134"/>
-      <c r="BH33" s="134"/>
-      <c r="BI33" s="134"/>
-      <c r="BJ33" s="134"/>
-      <c r="BK33" s="134"/>
-      <c r="BL33" s="134"/>
-      <c r="BM33" s="135"/>
+      <c r="AH33" s="64"/>
+      <c r="AI33" s="65"/>
+      <c r="AJ33" s="65"/>
+      <c r="AK33" s="65"/>
+      <c r="AL33" s="65"/>
+      <c r="AM33" s="65"/>
+      <c r="AN33" s="65"/>
+      <c r="AO33" s="65"/>
+      <c r="AP33" s="65"/>
+      <c r="AQ33" s="65"/>
+      <c r="AR33" s="65"/>
+      <c r="AS33" s="65"/>
+      <c r="AT33" s="65"/>
+      <c r="AU33" s="65"/>
+      <c r="AV33" s="65"/>
+      <c r="AW33" s="65"/>
+      <c r="AX33" s="65"/>
+      <c r="AY33" s="65"/>
+      <c r="AZ33" s="65"/>
+      <c r="BA33" s="65"/>
+      <c r="BB33" s="65"/>
+      <c r="BC33" s="65"/>
+      <c r="BD33" s="65"/>
+      <c r="BE33" s="65"/>
+      <c r="BF33" s="65"/>
+      <c r="BG33" s="65"/>
+      <c r="BH33" s="65"/>
+      <c r="BI33" s="65"/>
+      <c r="BJ33" s="65"/>
+      <c r="BK33" s="65"/>
+      <c r="BL33" s="65"/>
+      <c r="BM33" s="66"/>
       <c r="BO33" s="43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:68" ht="16" customHeight="1">
       <c r="A34" s="4">
         <v>31</v>
       </c>
-      <c r="B34" s="154"/>
-      <c r="C34" s="155"/>
-      <c r="D34" s="155"/>
-      <c r="E34" s="155"/>
-      <c r="F34" s="155"/>
-      <c r="G34" s="155"/>
-      <c r="H34" s="155"/>
-      <c r="I34" s="155"/>
-      <c r="J34" s="155"/>
-      <c r="K34" s="155"/>
-      <c r="L34" s="155"/>
-      <c r="M34" s="155"/>
-      <c r="N34" s="155"/>
-      <c r="O34" s="155"/>
-      <c r="P34" s="155"/>
-      <c r="Q34" s="155"/>
-      <c r="R34" s="155"/>
-      <c r="S34" s="155"/>
-      <c r="T34" s="155"/>
-      <c r="U34" s="155"/>
-      <c r="V34" s="155"/>
-      <c r="W34" s="155"/>
-      <c r="X34" s="155"/>
-      <c r="Y34" s="155"/>
-      <c r="Z34" s="155"/>
-      <c r="AA34" s="155"/>
-      <c r="AB34" s="155"/>
-      <c r="AC34" s="155"/>
-      <c r="AD34" s="155"/>
-      <c r="AE34" s="155"/>
-      <c r="AF34" s="155"/>
-      <c r="AG34" s="156"/>
-      <c r="AH34" s="136"/>
-      <c r="AI34" s="137"/>
-      <c r="AJ34" s="137"/>
-      <c r="AK34" s="137"/>
-      <c r="AL34" s="137"/>
-      <c r="AM34" s="137"/>
-      <c r="AN34" s="137"/>
-      <c r="AO34" s="137"/>
-      <c r="AP34" s="137"/>
-      <c r="AQ34" s="137"/>
-      <c r="AR34" s="137"/>
-      <c r="AS34" s="137"/>
-      <c r="AT34" s="137"/>
-      <c r="AU34" s="137"/>
-      <c r="AV34" s="137"/>
-      <c r="AW34" s="137"/>
-      <c r="AX34" s="137"/>
-      <c r="AY34" s="137"/>
-      <c r="AZ34" s="137"/>
-      <c r="BA34" s="137"/>
-      <c r="BB34" s="137"/>
-      <c r="BC34" s="137"/>
-      <c r="BD34" s="137"/>
-      <c r="BE34" s="137"/>
-      <c r="BF34" s="137"/>
-      <c r="BG34" s="137"/>
-      <c r="BH34" s="137"/>
-      <c r="BI34" s="137"/>
-      <c r="BJ34" s="137"/>
-      <c r="BK34" s="137"/>
-      <c r="BL34" s="137"/>
-      <c r="BM34" s="138"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="95"/>
+      <c r="I34" s="95"/>
+      <c r="J34" s="95"/>
+      <c r="K34" s="95"/>
+      <c r="L34" s="95"/>
+      <c r="M34" s="95"/>
+      <c r="N34" s="95"/>
+      <c r="O34" s="95"/>
+      <c r="P34" s="95"/>
+      <c r="Q34" s="95"/>
+      <c r="R34" s="95"/>
+      <c r="S34" s="95"/>
+      <c r="T34" s="95"/>
+      <c r="U34" s="95"/>
+      <c r="V34" s="95"/>
+      <c r="W34" s="95"/>
+      <c r="X34" s="95"/>
+      <c r="Y34" s="95"/>
+      <c r="Z34" s="95"/>
+      <c r="AA34" s="95"/>
+      <c r="AB34" s="95"/>
+      <c r="AC34" s="95"/>
+      <c r="AD34" s="95"/>
+      <c r="AE34" s="95"/>
+      <c r="AF34" s="95"/>
+      <c r="AG34" s="96"/>
+      <c r="AH34" s="67"/>
+      <c r="AI34" s="68"/>
+      <c r="AJ34" s="68"/>
+      <c r="AK34" s="68"/>
+      <c r="AL34" s="68"/>
+      <c r="AM34" s="68"/>
+      <c r="AN34" s="68"/>
+      <c r="AO34" s="68"/>
+      <c r="AP34" s="68"/>
+      <c r="AQ34" s="68"/>
+      <c r="AR34" s="68"/>
+      <c r="AS34" s="68"/>
+      <c r="AT34" s="68"/>
+      <c r="AU34" s="68"/>
+      <c r="AV34" s="68"/>
+      <c r="AW34" s="68"/>
+      <c r="AX34" s="68"/>
+      <c r="AY34" s="68"/>
+      <c r="AZ34" s="68"/>
+      <c r="BA34" s="68"/>
+      <c r="BB34" s="68"/>
+      <c r="BC34" s="68"/>
+      <c r="BD34" s="68"/>
+      <c r="BE34" s="68"/>
+      <c r="BF34" s="68"/>
+      <c r="BG34" s="68"/>
+      <c r="BH34" s="68"/>
+      <c r="BI34" s="68"/>
+      <c r="BJ34" s="68"/>
+      <c r="BK34" s="68"/>
+      <c r="BL34" s="68"/>
+      <c r="BM34" s="69"/>
       <c r="BO34" s="43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:68">
       <c r="A35" s="4">
         <v>47</v>
       </c>
-      <c r="B35" s="76" t="s">
+      <c r="B35" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="79" t="s">
+      <c r="C35" s="140"/>
+      <c r="D35" s="140"/>
+      <c r="E35" s="141"/>
+      <c r="F35" s="142" t="s">
         <v>4</v>
       </c>
-      <c r="G35" s="80"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="81"/>
-      <c r="J35" s="82" t="s">
+      <c r="G35" s="143"/>
+      <c r="H35" s="143"/>
+      <c r="I35" s="144"/>
+      <c r="J35" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35" s="81"/>
+      <c r="L35" s="81"/>
+      <c r="M35" s="82"/>
+      <c r="N35" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="83"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="84"/>
-      <c r="N35" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="O35" s="83"/>
-      <c r="P35" s="83"/>
-      <c r="Q35" s="84"/>
-      <c r="R35" s="70" t="s">
-        <v>12</v>
-      </c>
-      <c r="S35" s="71"/>
-      <c r="T35" s="71"/>
-      <c r="U35" s="72"/>
-      <c r="V35" s="70" t="s">
+      <c r="O35" s="81"/>
+      <c r="P35" s="81"/>
+      <c r="Q35" s="82"/>
+      <c r="R35" s="133" t="s">
+        <v>11</v>
+      </c>
+      <c r="S35" s="134"/>
+      <c r="T35" s="134"/>
+      <c r="U35" s="135"/>
+      <c r="V35" s="133" t="s">
+        <v>15</v>
+      </c>
+      <c r="W35" s="134"/>
+      <c r="X35" s="134"/>
+      <c r="Y35" s="135"/>
+      <c r="Z35" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="W35" s="71"/>
-      <c r="X35" s="71"/>
-      <c r="Y35" s="72"/>
-      <c r="Z35" s="70" t="s">
+      <c r="AA35" s="134"/>
+      <c r="AB35" s="134"/>
+      <c r="AC35" s="135"/>
+      <c r="AD35" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="AA35" s="71"/>
-      <c r="AB35" s="71"/>
-      <c r="AC35" s="72"/>
-      <c r="AD35" s="73" t="s">
+      <c r="AE35" s="137"/>
+      <c r="AF35" s="137"/>
+      <c r="AG35" s="138"/>
+      <c r="AH35" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="AE35" s="74"/>
-      <c r="AF35" s="74"/>
-      <c r="AG35" s="75"/>
-      <c r="AH35" s="150" t="s">
+      <c r="AI35" s="84"/>
+      <c r="AJ35" s="84"/>
+      <c r="AK35" s="85"/>
+      <c r="AL35" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="AI35" s="151"/>
-      <c r="AJ35" s="151"/>
-      <c r="AK35" s="152"/>
-      <c r="AL35" s="82" t="s">
-        <v>20</v>
-      </c>
-      <c r="AM35" s="83"/>
-      <c r="AN35" s="83"/>
-      <c r="AO35" s="84"/>
-      <c r="AP35" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="AQ35" s="83"/>
-      <c r="AR35" s="83"/>
-      <c r="AS35" s="84"/>
-      <c r="AT35" s="148" t="s">
+      <c r="AM35" s="81"/>
+      <c r="AN35" s="81"/>
+      <c r="AO35" s="82"/>
+      <c r="AP35" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ35" s="81"/>
+      <c r="AR35" s="81"/>
+      <c r="AS35" s="82"/>
+      <c r="AT35" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="AU35" s="80"/>
+      <c r="AV35" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW35" s="82"/>
+      <c r="AX35" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY35" s="80"/>
+      <c r="AZ35" s="80"/>
+      <c r="BA35" s="87"/>
+      <c r="BB35" s="145" t="s">
+        <v>28</v>
+      </c>
+      <c r="BC35" s="146"/>
+      <c r="BD35" s="146"/>
+      <c r="BE35" s="147"/>
+      <c r="BF35" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="BG35" s="146"/>
+      <c r="BH35" s="146"/>
+      <c r="BI35" s="147"/>
+      <c r="BJ35" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="AU35" s="149"/>
-      <c r="AV35" s="83" t="s">
-        <v>31</v>
-      </c>
-      <c r="AW35" s="84"/>
-      <c r="AX35" s="148" t="s">
-        <v>28</v>
-      </c>
-      <c r="AY35" s="149"/>
-      <c r="AZ35" s="149"/>
-      <c r="BA35" s="153"/>
-      <c r="BB35" s="85" t="s">
-        <v>29</v>
-      </c>
-      <c r="BC35" s="86"/>
-      <c r="BD35" s="86"/>
-      <c r="BE35" s="87"/>
-      <c r="BF35" s="85" t="s">
-        <v>30</v>
-      </c>
-      <c r="BG35" s="86"/>
-      <c r="BH35" s="86"/>
-      <c r="BI35" s="87"/>
-      <c r="BJ35" s="139" t="s">
-        <v>32</v>
-      </c>
-      <c r="BK35" s="140"/>
-      <c r="BL35" s="140"/>
-      <c r="BM35" s="141"/>
+      <c r="BK35" s="71"/>
+      <c r="BL35" s="71"/>
+      <c r="BM35" s="72"/>
       <c r="BO35" s="43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:68">
       <c r="A36" s="44"/>
       <c r="BO36" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:68">
       <c r="A37" s="45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="46"/>
       <c r="C37" s="46"/>
@@ -4127,47 +4127,47 @@
       <c r="P38" s="49"/>
       <c r="Q38" s="49"/>
       <c r="BO38" s="43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:68" ht="18" customHeight="1">
       <c r="A39" s="4">
         <v>1</v>
       </c>
-      <c r="B39" s="121" t="s">
+      <c r="B39" s="115" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="116"/>
+      <c r="D39" s="116"/>
+      <c r="E39" s="116"/>
+      <c r="F39" s="117"/>
+      <c r="G39" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="122"/>
-      <c r="D39" s="122"/>
-      <c r="E39" s="122"/>
-      <c r="F39" s="123"/>
-      <c r="G39" s="121" t="s">
-        <v>36</v>
-      </c>
-      <c r="H39" s="122"/>
-      <c r="I39" s="122"/>
-      <c r="J39" s="122"/>
-      <c r="K39" s="123"/>
+      <c r="H39" s="116"/>
+      <c r="I39" s="116"/>
+      <c r="J39" s="116"/>
+      <c r="K39" s="117"/>
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
       <c r="BO39" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:68">
       <c r="A40" s="5">
         <v>2</v>
       </c>
-      <c r="B40" s="124"/>
-      <c r="C40" s="125"/>
-      <c r="D40" s="125"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="126"/>
-      <c r="G40" s="124"/>
-      <c r="H40" s="125"/>
-      <c r="I40" s="125"/>
-      <c r="J40" s="125"/>
-      <c r="K40" s="126"/>
+      <c r="B40" s="118"/>
+      <c r="C40" s="119"/>
+      <c r="D40" s="119"/>
+      <c r="E40" s="119"/>
+      <c r="F40" s="120"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="119"/>
+      <c r="I40" s="119"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="120"/>
       <c r="L40" s="28"/>
       <c r="M40" s="28"/>
       <c r="BO40" s="43"/>
@@ -4176,16 +4176,16 @@
       <c r="A41" s="4">
         <v>3</v>
       </c>
-      <c r="B41" s="124"/>
-      <c r="C41" s="125"/>
-      <c r="D41" s="125"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="126"/>
-      <c r="G41" s="124"/>
-      <c r="H41" s="125"/>
-      <c r="I41" s="125"/>
-      <c r="J41" s="125"/>
-      <c r="K41" s="126"/>
+      <c r="B41" s="118"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="119"/>
+      <c r="E41" s="119"/>
+      <c r="F41" s="120"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="119"/>
+      <c r="I41" s="119"/>
+      <c r="J41" s="119"/>
+      <c r="K41" s="120"/>
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
       <c r="BO41" s="43"/>
@@ -4194,16 +4194,16 @@
       <c r="A42" s="50">
         <v>2</v>
       </c>
-      <c r="B42" s="127"/>
-      <c r="C42" s="128"/>
-      <c r="D42" s="128"/>
-      <c r="E42" s="128"/>
-      <c r="F42" s="129"/>
-      <c r="G42" s="127"/>
-      <c r="H42" s="128"/>
-      <c r="I42" s="128"/>
-      <c r="J42" s="128"/>
-      <c r="K42" s="129"/>
+      <c r="B42" s="121"/>
+      <c r="C42" s="122"/>
+      <c r="D42" s="122"/>
+      <c r="E42" s="122"/>
+      <c r="F42" s="123"/>
+      <c r="G42" s="121"/>
+      <c r="H42" s="122"/>
+      <c r="I42" s="122"/>
+      <c r="J42" s="122"/>
+      <c r="K42" s="123"/>
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
       <c r="BO42" s="43"/>
@@ -8812,20 +8812,9 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="BO20:BP20"/>
-    <mergeCell ref="BO30:BP30"/>
-    <mergeCell ref="BO37:BP37"/>
-    <mergeCell ref="AH31:BM34"/>
-    <mergeCell ref="BJ35:BM35"/>
-    <mergeCell ref="B29:BM30"/>
-    <mergeCell ref="AT35:AU35"/>
-    <mergeCell ref="AV35:AW35"/>
-    <mergeCell ref="AH35:AK35"/>
-    <mergeCell ref="AL35:AO35"/>
-    <mergeCell ref="AP35:AS35"/>
-    <mergeCell ref="AX35:BA35"/>
-    <mergeCell ref="B31:AG34"/>
-    <mergeCell ref="B19:BM22"/>
+    <mergeCell ref="B3:BM6"/>
+    <mergeCell ref="B11:BM14"/>
+    <mergeCell ref="B15:BM18"/>
     <mergeCell ref="B7:BJ10"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B39:F42"/>
@@ -8842,10 +8831,21 @@
     <mergeCell ref="R35:U35"/>
     <mergeCell ref="BB35:BE35"/>
     <mergeCell ref="BF35:BI35"/>
+    <mergeCell ref="BO20:BP20"/>
+    <mergeCell ref="BO30:BP30"/>
+    <mergeCell ref="BO37:BP37"/>
+    <mergeCell ref="AH31:BM34"/>
+    <mergeCell ref="BJ35:BM35"/>
+    <mergeCell ref="B29:BM30"/>
+    <mergeCell ref="AT35:AU35"/>
+    <mergeCell ref="AV35:AW35"/>
+    <mergeCell ref="AH35:AK35"/>
+    <mergeCell ref="AL35:AO35"/>
+    <mergeCell ref="AP35:AS35"/>
+    <mergeCell ref="AX35:BA35"/>
+    <mergeCell ref="B31:AG34"/>
+    <mergeCell ref="B19:BM22"/>
     <mergeCell ref="B27:BM28"/>
-    <mergeCell ref="B3:BM6"/>
-    <mergeCell ref="B11:BM14"/>
-    <mergeCell ref="B15:BM18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>